<commit_message>
Updated the data processing procedure
</commit_message>
<xml_diff>
--- a/Dataset/Captions collection/final_captions_collection.xlsx
+++ b/Dataset/Captions collection/final_captions_collection.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About in TKN_Geo during TKN_Year. The values are reported using the FPPI (Farm product pridce index). It's clearly possible to see how the TKN_About is quite low from January to May, but then it rapidly increase from June to December, reaching its maximum value during September TKN_Year.</t>
+          <t>The following line chart is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported using the FPPI (Farm product pridce index). It's clearly possible to see how the TKN_About  is quite low from January to May, but then it rapidly increase from June to December, reaching its maximum value during September  TKN_Year .</t>
         </is>
       </c>
       <c r="W2" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About (units) in TKN_Geo during TKN_Year. It's possible to see how the highest value was during May, when almost 100 new motor vehicles have been producted. Furthermore, it's also clear that January and December are the months with less new motor vehicles producted over TKN_Year in TKN_Geo.</t>
+          <t>The following line chart is about the TKN_About  (units) in  TKN_Geo  during  TKN_Year . It's possible to see how the highest value was during May, when almost 100 new motor vehicles have been producted. Furthermore, it's also clear that January and December are the months with less new motor vehicles producted over  TKN_Year  in  TKN_Geo .</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -725,7 +725,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>The image reports a line chart about the TKN_About TKN_UOM metres) in Canda during TKN_Year. The values are fluctuating over the months, reaching a peak during May TKN_Year. At the same time it's clearly possible to see that December TKN_Year has been the month with less production.</t>
+          <t>The image reports a line chart about the TKN_About  TKN_UOM  metres) in Canda during  TKN_Year . The values are fluctuating over the months, reaching a peak during May  TKN_Year . At the same time it's clearly possible to see that December  TKN_Year  has been the month with less production.</t>
         </is>
       </c>
       <c r="W4" t="n">
@@ -809,7 +809,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>The line chart shows the TKN_About TKN_Geo during TKN_Year. It's clearly possible to see how during the summer months the amount of car entering TKN_Geo is way higher than the rest of the year, reaching the maximum value during the month of August with around 100 cars.</t>
+          <t>The line chart shows the total TKN_UOM  of vehicles entering  TKN_Geo  during  TKN_Year . It's clearly possible to see how during the summer months the amount of car entering  TKN_Geo  is way higher than the rest of the year, reaching the maximum value during the month of August with around 100 cars.</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>The following graph describes how TKN_UOM index) about TKN_About in TKN_Geo has been slowly increasing during TKN_Year. In particular, it increased from 0 in February to 100 in December.</t>
+          <t>The following graph describes how TKN_UOM  index) about TKN_About  in  TKN_Geo  has been slowly increasing during  TKN_Year . In particular, it increased from 0 in February to 100 in December.</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -977,7 +977,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>The line chart shows the TKN_UOM about TKN_About grain in TKN_Geo during TKN_Year. It's possible to see how the index has been quite steady from January to June, but then a relevant drop has been recorded from June to August, where the index dropped from 93 to 8. During the last few months of the year the index slowly started to increase again.</t>
+          <t>The line chart shows the TKN_UOM  about TKN_About  grain in  TKN_Geo  during  TKN_Year . It's possible to see how the index has been quite steady from January to June, but then a relevant drop has been recorded from June to August, where the index dropped from 93 to 8. During the last few months of the year the index slowly started to increase again.</t>
         </is>
       </c>
       <c r="W7" t="n">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>The chart shows the TKN_UOM about TKN_About in TKN_Geo during TKN_Year. The index has been quite steady during the first few months of the year, with a maximum value in March, but then it rapidly decreased from June over, reaching the minimum value during October which was around 1. The index started to slowly grow again during the months of November and December.</t>
+          <t>The chart shows the TKN_UOM  about TKN_About  in  TKN_Geo  during  TKN_Year . The index has been quite steady during the first few months of the year, with a maximum value in March, but then it rapidly decreased from June over, reaching the minimum value during October which was around 1. The index started to slowly grow again during the months of November and December.</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of May with a number of 100 in TKN_Geo. The biggest increase in production of poultry can be observed from February until May, while a drop from May to July takes place. From August until November the production remains quite stable at approximately 62 and starts decreasing until it reaches its minimum in February below 4.</t>
+          <t>Production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of May with a number of 100 in  TKN_Geo . The biggest increase in production of poultry can be observed from February until May, while a drop from May to July takes place. From August until November the production remains quite stable at approximately 62 and starts decreasing until it reaches its minimum in February below 4.</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About in TKN_UOM in TKN_Geo during TKN_Year. In general the production recorded its highes values during the spring and summer months, reaching a peak during May -118. The most significant jump of the values during TKN_Year is between the months of February and March.</t>
+          <t>The graph shows the TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year . In general the production recorded its highes values during the spring and summer months, reaching a peak during May 2019. The most significant jump of the values during  TKN_Year  is between the months of February and March.</t>
         </is>
       </c>
       <c r="W10" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>The line chart reports the values TKN_About TKN_UOM in TKN_Geo during TKN_Year. During the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of June and July. After that, it rapidly dropped from over 97 to less than 6 in the month of Setpember.</t>
+          <t>The line chart reports the values TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . During the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of June and July. After that, it rapidly dropped from over 97 to less than 6 in the month of Setpember.</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -1392,12 +1392,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately 1000 tonnes of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 8000 to 8500 tonnes. A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 11500 tonnes.</t>
+          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately 10000 tonnes of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 8000 to 8500 tonnes. A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 11500 tonnes.</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately -175 TKN_UOM of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 12 to 25 TKN_UOM. A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 105 TKN_UOM.</t>
+          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately 65 TKN_UOM  of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 12 to 25 TKN_UOM . A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 105 TKN_UOM .</t>
         </is>
       </c>
       <c r="W12" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>The figure shows a line chart about the production of what flour (in tonnes) in TKN_Geo during TKN_Year. The values have been mainly fluctuating during the year, without any significant trend or patterns. Even that, if it has been recorded a significant growth from November to December, where the TKN_About during TKN_Year reached its peak.</t>
+          <t>The figure shows a line chart about the production of what flour (in tonnes) in  TKN_Geo  during  TKN_Year . The values have been mainly fluctuating during the year, without any significant trend or patterns. Even that, if it has been recorded a significant growth from November to December, where the TKN_About  during  TKN_Year  reached its peak.</t>
         </is>
       </c>
       <c r="W13" t="n">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About in TKN_Geo. The price is the highest during the month of January at 100. From February until May the price starts fluctuating between roughly 50 to 79. Prices for laptop computers show a dramatic drop during the month of June. The minimum value lies at 0. The price starts oscillating again between July and December with prices between 64 to 43.</t>
+          <t>This graph represents the TKN_About  in  TKN_Geo . The price is the highest during the month of January at 100. From February until May the price starts fluctuating between roughly 50 to 79. Prices for laptop computers show a dramatic drop during the month of June. The minimum value lies at 0. The price starts oscillating again between July and December with prices between 64 to 43.</t>
         </is>
       </c>
       <c r="W14" t="n">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>The following graph is about the imports TKN_About (in tonnes) in TKN_Geo during TKN_Year. It's possible to see how the values are generally increasing over the year, with a substan raise from August until October, where the values basically tripled. The maximum value recorded over the year is during November TKN_Year, where the recorded production has been over 97 tonnes.</t>
+          <t>The following graph is about the imports TKN_About  (in tonnes) in  TKN_Geo  during  TKN_Year . It's possible to see how the values are generally increasing over the year, with a substan raise from August until October, where the values basically tripled. The maximum value recorded over the year is during November  TKN_Year , where the recorded production has been over 97 tonnes.</t>
         </is>
       </c>
       <c r="W15" t="n">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>This line chart represent TKN_About in TKN_Year. A slow, but steady increase is taking place from March until it reaches its peak in August with a total TKN_UOM of 97. After August the total TKN_UOM of Canadian vehicles returning starts decreasing until reaching its minimum value below 6 in February. This big difference may be due to holiday season during the warmer months of the year.</t>
+          <t>This line chart represent the TKN_UOM  of total Canadian vehicles returning in  TKN_Year . A slow, but steady increase is taking place from March until it reaches its peak in August with a total TKN_UOM  of 97. After August the total TKN_UOM  of Canadian vehicles returning starts decreasing until reaching its minimum value below 6 in February. This big difference may be due to holiday season during the warmer months of the year.</t>
         </is>
       </c>
       <c r="W16" t="n">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>The following line chart shows the TKN_UOM about the TKN_About in TKN_Geo during TKN_Year. The values are significantly fluctuating over the year, showing several peaks and falls. The highest values of the indexes have been recorded during February, July and October. The lower values of the indexes have been recorded during April, September and December.</t>
+          <t>The following line chart shows the TKN_UOM  about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are significantly fluctuating over the year, showing several peaks and falls. The highest values of the indexes have been recorded during February, July and October. The lower values of the indexes have been recorded during April, September and December.</t>
         </is>
       </c>
       <c r="W17" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>This line chart reflects the TKN_About in TKN_Geo during TKN_Year. From January until March the production remains unaltered at approximately 4. From March until July a steady increase of up to 40 can be observed. There is a rapid gain in production between July and August, reaching its highest production which will last until December.</t>
+          <t>This line chart reflects the TKN_About  in  TKN_Geo  during  TKN_Year . From January until March the production remains unaltered at approximately 4. From March until July a steady increase of up to 40 can be observed. There is a rapid gain in production between July and August, reaching its highest production which will last until December.</t>
         </is>
       </c>
       <c r="W18" t="n">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>It shows the TKN_UOM of TKN_About TKN_Geo during TKN_Year. It's clearly possible to see how this value rapidly increase from January until the end of the summer, reaching its maximum value in August. After that, the TKN_UOM of vehicles entering TKN_Geo decrease during the last few months of the year. The minimum value has been recorded during February.</t>
+          <t>It shows the TKN_UOM  of TKN_About   TKN_Geo  during  TKN_Year . It's clearly possible to see how this value rapidly increase from January until the end of the summer, reaching its maximum value in August. After that, the TKN_UOM  of vehicles entering  TKN_Geo  decrease during the last few months of the year. The minimum value has been recorded during February.</t>
         </is>
       </c>
       <c r="W19" t="n">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>This chart illustrates the land price index of Canada in 2016. A minimum of 982.25 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 987.5. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 1000.0.</t>
+          <t>This chart illustrates the land price index of Canada in 2016. A minimum of 982 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 987. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 1000.</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>This chart illustrates TKN_About TKN_UOM of TKN_Geo in TKN_Year. A minimum of 982.25 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 987.5. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 1000.0.</t>
+          <t>This chart illustrates TKN_About  TKN_UOM  of  TKN_Geo  in  TKN_Year . A minimum of 5 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 32. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 100.</t>
         </is>
       </c>
       <c r="W20" t="n">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>The line chart describes the TKN_UOM of TKN_About TKN_Geo during TKN_Year. It's clearly possible to observe that this value rapidly growed from January to August, showing the highest values during the summer months. During the last few months of the year the TKN_UOM of TKN_About TKN_Geo rapidly decreased.</t>
+          <t>The line chart describes the TKN_UOM  of TKN_About   TKN_Geo  during  TKN_Year . It's clearly possible to observe that this value rapidly growed from January to August, showing the highest values during the summer months. During the last few months of the year the TKN_UOM  of TKN_About   TKN_Geo  rapidly decreased.</t>
         </is>
       </c>
       <c r="W21" t="n">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo in TKN_Year is illustrated by this graph. Whereas the maximum of 100 can be observed during January, a slow drop can be seen until May. The graph depicts a sharp drop between May and June, reaching 21. For the following months the price index graph starts oscillating until reaching its minimum value in December at 0.</t>
+          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  is illustrated by this graph. Whereas the maximum of 100 can be observed during January, a slow drop can be seen until May. The graph depicts a sharp drop between May and June, reaching 21. For the following months the price index graph starts oscillating until reaching its minimum value in December at 0.</t>
         </is>
       </c>
       <c r="W22" t="n">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>The graph describes the TKN_About (in tonnes) in TKN_Geo during TKN_Year. As can be seen from the graph, the value reports two significant peaks during the month of March and June. The minimum value has been recorded during the month of September. It's also possible to see how the values during January and December do not differ so much from each other.</t>
+          <t>The graph describes the TKN_About  (in tonnes) in  TKN_Geo  during  TKN_Year . As can be seen from the graph, the value reports two significant peaks during the month of March and June. The minimum value has been recorded during the month of September. It's also possible to see how the values during January and December do not differ so much from each other.</t>
         </is>
       </c>
       <c r="W23" t="n">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>This graph illustrates the TKN_About in TKN_Geo in TKN_Year. Production mainly starts in March, with a slow increase throughout until June. Production sharply increases from June onwards, reaching a maximum of nearly 104 during August. A rapid drop follows between August and October, reaching a minimum of below 1. The graph depicts a short increase in production from October until December and comes back to nearly minimum during January and February.</t>
+          <t>This graph illustrates the TKN_About  in  TKN_Geo  in  TKN_Year . Production mainly starts in March, with a slow increase throughout until June. Production sharply increases from June onwards, reaching a maximum of nearly 104 during August. A rapid drop follows between August and October, reaching a minimum of below 1. The graph depicts a short increase in production from October until December and comes back to nearly minimum during January and February.</t>
         </is>
       </c>
       <c r="W24" t="n">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>This graph illustrates the Canadian TKN_About in TKN_Year. The unit used is TKN_UOM. Import reaches its maximum of over 97 TKN_UOM during June and its second highes import during the month of March with approximately 79. After June the import drastically decreases until reaching a minimum of approximately 3 in September. From the months of September until February the import oscillates between approximately 3 and 34.</t>
+          <t>This graph illustrates the Canadian TKN_About  in  TKN_Year . The unit used is TKN_UOM . Import reaches its maximum of over 97 TKN_UOM  during June and its second highes import during the month of March with approximately 79. After June the import drastically decreases until reaching a minimum of approximately 3 in September. From the months of September until February the import oscillates between approximately 3 and 34.</t>
         </is>
       </c>
       <c r="W25" t="n">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_UOM in TKN_Geo during TKN_Year. Production shows peaks in January and March, whereas it significantly drops after March, reaching its minimum of approximately 0 in May. For the following months production slightly increases until August. Between August and September a rapid increase in production can be observed, indicating the maximum of over 96 in September. Production slowly decreases throughout the following months until December.</t>
+          <t>This graph depicts the TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year . Production shows peaks in January and March, whereas it significantly drops after March, reaching its minimum of approximately 0 in May. For the following months production slightly increases until August. Between August and September a rapid increase in production can be observed, indicating the maximum of over 96 in September. Production slowly decreases throughout the following months until December.</t>
         </is>
       </c>
       <c r="W26" t="n">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>This graph indicates the TKN_UOM of TKN_About in TKN_Year. The lowest TKN_UOM of approximately 3 can be observed during the month of February. Over the following -144 months a steady increase takes place. As can be seen from the graph there is sharp rise of returning vehicles from June until August. After August the TKN_UOM steadily decreases until reaching its minimum in February.</t>
+          <t>This graph indicates the TKN_UOM  of TKN_About  in  TKN_Year . The lowest TKN_UOM  of approximately 3 can be observed during the month of February. Over the following 4 months a steady increase takes place. As can be seen from the graph there is sharp rise of returning vehicles from June until August. After August the TKN_UOM  steadily decreases until reaching its minimum in February.</t>
         </is>
       </c>
       <c r="W27" t="n">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>The following graph is about the TKN_About in TKN_Geo during TKN_Year; the values are in tonnes. It shows a clearly growth from January over, reaching its maximum value during October. Then it's possible to see a significant drop from October to November.</t>
+          <t>The following graph is about the TKN_About  in  TKN_Geo  during  TKN_Year ; the values are in tonnes. It shows a clearly growth from January over, reaching its maximum value during October. Then it's possible to see a significant drop from October to November.</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About in TKN_Geo during TKN_Year. The values are reported in tonnes. It shows how the production is actually falling down from January to August, when it reaches its minimum. From September to December the values are slowly rising up.</t>
+          <t>The following line chart is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported in tonnes. It shows how the production is actually falling down from January to August, when it reaches its minimum. From September to December the values are slowly rising up.</t>
         </is>
       </c>
       <c r="W29" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>In the following graph is described the monthly TKN_About in TKN_UOM about TKN_Geo during TKN_Year. The minimum value has been registered during the month of January and maximum during July. Furthermore, it's possible to see how the TKN_About is generally higher during spring and summer.</t>
+          <t>In the following graph is described the monthly TKN_About  in TKN_UOM  about  TKN_Geo  during  TKN_Year . The minimum value has been registered during the month of January and maximum during July. Furthermore, it's possible to see how the TKN_About  is generally higher during spring and summer.</t>
         </is>
       </c>
       <c r="W30" t="n">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About in TKN_Geo in the year of TKN_Year. There is one data entry for each month of the year. Production is measured TKN_UOM index. The x-axis shows the months, the y-axis the index ranging from 4 to 100. There is a high in May (index of 100) and a low in February (a bit below 4).</t>
+          <t>The graph shows the TKN_About  in  TKN_Geo  in the year of  TKN_Year . There is one data entry for each month of the year. Production is measured TKN_UOM  index. The x-axis shows the months, the y-axis the index ranging from 4 to 100. There is a high in May (index of 100) and a low in February (a bit below 4).</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About in TKN_Geo for the year TKN_Year. There are sharp decreases in production for the months of February, July and November.</t>
+          <t>The graph illustrates the TKN_About  in  TKN_Geo  for the year  TKN_Year . There are sharp decreases in production for the months of February, July and November.</t>
         </is>
       </c>
       <c r="W32" t="n">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>The graph shows the values TKN_About TKN_UOM in TKN_Geo during TKN_Year. It's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. The minimum value has been recorded during January and the maximum one during December.</t>
+          <t>The graph shows the values TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . It's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. The minimum value has been recorded during January and the maximum one during December.</t>
         </is>
       </c>
       <c r="W33" t="n">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_Geo in TKN_Year TKN_UOM meters. The values range from roughly 102 in March to -1 in December. January to March there is an increase in production, March to July production decreased and reached 36 in July. There is another high of about 102 cubic meters in November.</t>
+          <t>This graph depicts the TKN_About  in  TKN_Geo  in  TKN_Year  TKN_UOM  meters. The values range from roughly 102 in March to -1 in December. January to March there is an increase in production, March to July production decreased and reached 36 in July. There is another high of about 102 cubic meters in November.</t>
         </is>
       </c>
       <c r="W34" t="n">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>The graph indicates the number TKN_UOM meters of soft TKN_About in TKN_Geo for TKN_Year. Production is highest in spring time and drops to its lowest in December.</t>
+          <t>The graph indicates the number TKN_UOM  meters of soft TKN_About  in  TKN_Geo  for  TKN_Year . Production is highest in spring time and drops to its lowest in December.</t>
         </is>
       </c>
       <c r="W35" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>As can be seen from the graph the TKN_About in TKN_Geo during TKN_Year had a significant growth during the second half of the year. It decreased from January to June, when it has been recorded the minimum value of the year. But then it started to rapidly increase reaching its maximum value during November 742.</t>
+          <t>As can be seen from the graph the TKN_About  in  TKN_Geo  during  TKN_Year  had a significant growth during the second half of the year. It decreased from January to June, when it has been recorded the minimum value of the year. But then it started to rapidly increase reaching its maximum value during November 2019.</t>
         </is>
       </c>
       <c r="W36" t="n">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>As is shown form the graph, the TKN_About steadily increases in winter time, and steadily decreases in summer. The graph shows that production is highest in November and lowest in June.</t>
+          <t>As is shown form the graph, the TKN_About  steadily increases in winter time, and steadily decreases in summer. The graph shows that production is highest in November and lowest in June.</t>
         </is>
       </c>
       <c r="W37" t="n">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>The line chart illustrates the TKN_About in TKN_Geo during TKN_Year. The values are described using TKN_UOM (FPPI). It's clearly possible to see two main peaks over the year, one during February and one during October. At the same time, during the summer the production significantly decreased, reaching its minimum value during the month of July.</t>
+          <t>The line chart illustrates the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It's clearly possible to see two main peaks over the year, one during February and one during October. At the same time, during the summer the production significantly decreased, reaching its minimum value during the month of July.</t>
         </is>
       </c>
       <c r="W38" t="n">
@@ -3665,7 +3665,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>The graph illustrates the total TKN_UOM of TKN_About TKN_Geo. Data for every month of TKN_Year is shown. The TKN_UOMs vary for each month. A high is reached in July (about 110 vehicles), probably because of people going on vacation. Low values can be found for the winter months, e.g., less than 11 vehicles in January and February and roughly 11 vehicles in November and December.</t>
+          <t>The graph illustrates the total TKN_UOM  of TKN_About   TKN_Geo . Data for every month of  TKN_Year  is shown. The TKN_UOM s vary for each month. A high is reached in July (about 110 vehicles), probably because of people going on vacation. Low values can be found for the winter months, e.g., less than 11 vehicles in January and February and roughly 11 vehicles in November and December.</t>
         </is>
       </c>
       <c r="W39" t="n">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>The graph shows the the TKN_UOM of TKN_About TKN_Geo in TKN_Year. As illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. For the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
+          <t>The graph shows the the TKN_UOM  of TKN_About   TKN_Geo  in  TKN_Year . As illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. For the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
         </is>
       </c>
       <c r="W40" t="n">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About in TKN_Geo TKN_Year. The values are reported using TKN_UOM as unit of measure. It clearly possible to see several peaks and dips of production over the year. In particular, the maximum values have been recorded during March and July. It's also illustrated a significant fall of the production from July to August.</t>
+          <t>The following line chart is about the TKN_About  in  TKN_Geo   TKN_Year . The values are reported using TKN_UOM  as unit of measure. It clearly possible to see several peaks and dips of production over the year. In particular, the maximum values have been recorded during March and July. It's also illustrated a significant fall of the production from July to August.</t>
         </is>
       </c>
       <c r="W41" t="n">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>The line graph depicts the TKN_About in TKN_Geo for every month of TKN_Year. The overall trend for this year is a decrease. January recorded a high of 820, whereas November had a low of 1.</t>
+          <t>The line graph depicts the TKN_About  in  TKN_Geo  for every month of  TKN_Year . The overall trend for this year is a decrease. January recorded a high of 99, whereas November had a low of 1.</t>
         </is>
       </c>
       <c r="W42" t="n">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the TKN_About computer in TKN_Geo during TKN_Year slowly decreased over the year with several fluctuations. During January and February the values remain stable, without any changes. The minimum values have been recorded during August and October.</t>
+          <t>As it can be seen from the graph, the TKN_About  computer in  TKN_Geo  during  TKN_Year  slowly decreased over the year with several fluctuations. During January and February the values remain stable, without any changes. The minimum values have been recorded during August and October.</t>
         </is>
       </c>
       <c r="W43" t="n">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About in TKN_Geo for the year fo TKN_Year. The graph shows production steadily increasing till October and then declines in the months after. It is important to note that production at the end of the year in December is much higher than it was beginning the year in January.</t>
+          <t>The graph shows the TKN_About  in  TKN_Geo  for the year fo  TKN_Year . The graph shows production steadily increasing till October and then declines in the months after. It is important to note that production at the end of the year in December is much higher than it was beginning the year in January.</t>
         </is>
       </c>
       <c r="W44" t="n">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>The graph is a line chart, illustrating the TKN_About in TKN_Geo. The data used is from TKN_Year. The y-axis showing the index ranges from -11 to 108. The index increased over the months of the year, with some ups and downs in between. The lowest and highest values were found in January (1129) and December (1167), respectively.</t>
+          <t>The graph is a line chart, illustrating the TKN_About  in  TKN_Geo . The data used is from  TKN_Year . The y-axis showing the index ranges from -11 to 108. The index increased over the months of the year, with some ups and downs in between. The lowest and highest values were found in January (0) and December (100), respectively.</t>
         </is>
       </c>
       <c r="W45" t="n">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>From the graph it is clear TKN_About are cheapest during the months of August, September, and October for the TKN_Year year. They are the most expensive in February but see a steady decline until the month of September.</t>
+          <t>From the graph it is clear TKN_About  are cheapest during the months of August, September, and October for the  TKN_Year  year. They are the most expensive in February but see a steady decline until the month of September.</t>
         </is>
       </c>
       <c r="W46" t="n">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>This line graph illustrates the total TKN_UOM of TKN_About in TKN_Year. The x-axis shows the different months of the year, whereas the y-axis shows the TKN_UOM of vehicles. There is a rise in the first months of the year, reaching a high in August (2300000). TKN_UOMs decrease over the last months of the year.</t>
+          <t>This line graph illustrates the total TKN_UOM  of TKN_About  in  TKN_Year . The x-axis shows the different months of the year, whereas the y-axis shows the TKN_UOM  of vehicles. There is a rise in the first months of the year, reaching a high in August (101).  TKN_UOM s decrease over the last months of the year.</t>
         </is>
       </c>
       <c r="W47" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About TKN_UOM (index 347) in TKN_Geo in TKN_Year. Data entries are broken down into the months of the year. The graph's trend is a rise over the months. The value in January is 1006, the one for December is 103. The steepest incline can be found between March and May.</t>
+          <t>The graph shows TKN_About  TKN_UOM  (index 347) in  TKN_Geo  in  TKN_Year . Data entries are broken down into the months of the year. The graph's trend is a rise over the months. The value in January is 6, the one for December is 103. The steepest incline can be found between March and May.</t>
         </is>
       </c>
       <c r="W48" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>The chart is showing the values about the TKN_About in TKN_Geo during TKN_Year. The values are illustrated using TKN_UOM (FPPI). As can be seen from the graph, from January to May the values have been rapidly decreasing. Then, a peak has been recorded during the month of June, but after that the values started to decrease again until October. During the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of December.</t>
+          <t>The chart is showing the values about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are illustrated using TKN_UOM  (FPPI). As can be seen from the graph, from January to May the values have been rapidly decreasing. Then, a peak has been recorded during the month of June, but after that the values started to decrease again until October. During the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of December.</t>
         </is>
       </c>
       <c r="W49" t="n">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>The following graph shows information about TKN_About TKN_UOM in TKN_Geo during TKN_Year. As can be seen from the graph, the index have been steadily increasing its value over the year. There are few light fluctuations but no peaks or dips have been recorded.</t>
+          <t>The following graph shows information about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . As can be seen from the graph, the index have been steadily increasing its value over the year. There are few light fluctuations but no peaks or dips have been recorded.</t>
         </is>
       </c>
       <c r="W50" t="n">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>The land TKN_UOM for TKN_Geo during the year of TKN_Year increased from April to December. The TKN_UOM plateaued during the months of March through April, June through August, September through October and November through December.</t>
+          <t>The land TKN_UOM  for  TKN_Geo  during the year of  TKN_Year  increased from April to December. The TKN_UOM  plateaued during the months of March through April, June through August, September through October and November through December.</t>
         </is>
       </c>
       <c r="W51" t="n">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>The graph depicts a TKN_About in TKN_Geo. Data was taken from TKN_Year. One can observe a decline in the price index within the first months of the year, reaching a low of 0 in April. Throughout the following three months, the index increased to 100 in July. Values decreased steadily until October (1006) and stayed the same for November and December (1008).</t>
+          <t>The graph depicts a TKN_About  in  TKN_Geo . Data was taken from  TKN_Year . One can observe a decline in the price index within the first months of the year, reaching a low of 0 in April. Throughout the following three months, the index increased to 100 in July. Values decreased steadily until October (56) and stayed the same for November and December (69).</t>
         </is>
       </c>
       <c r="W52" t="n">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>The TKN_About for TKN_Geo in TKN_Year rapidly declined in July TKN_Year. The production then steadily recovered until October, and then fell again until December.</t>
+          <t>The TKN_About  for  TKN_Geo  in  TKN_Year  rapidly declined in July  TKN_Year . The production then steadily recovered until October, and then fell again until December.</t>
         </is>
       </c>
       <c r="W53" t="n">
@@ -4925,7 +4925,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>The following chart provides information about TKN_About TKN_UOM in TKN_Geo during TKN_Year. It's clearly possible to see how the index value significantly dropped down between January and February. Over the next few months the index value remained stable. It raised up again during the summer, reaching the same value of January during the month of June. From June to December the index value maintained the same level.</t>
+          <t>The following chart provides information about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . It's clearly possible to see how the index value significantly dropped down between January and February. Over the next few months the index value remained stable. It raised up again during the summer, reaching the same value of January during the month of June. From June to December the index value maintained the same level.</t>
         </is>
       </c>
       <c r="W54" t="n">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>This line chart depicts TKN_About TKN_UOM of houses in TKN_Geo in TKN_Year. It is broken down into the months of the year. Values are ranging from -3 to 103. The graph's overall trend is a continuous increase over the months. The lowest value was found for January (-3), whereas the highest value was recorded for November and December (103).</t>
+          <t>This line chart depicts TKN_About  TKN_UOM  of houses in  TKN_Geo  in  TKN_Year . It is broken down into the months of the year. Values are ranging from -3 to 103. The graph's overall trend is a continuous increase over the months. The lowest value was found for January (-3), whereas the highest value was recorded for November and December (103).</t>
         </is>
       </c>
       <c r="W55" t="n">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>The TKN_About reached its highest point in January of TKN_Year. Thereafter, production declined in February and then recovered in May. In the months following production steadily decreased until September. Thereafter, the graph fluctuated from October to December.</t>
+          <t>The TKN_About  reached its highest point in January of  TKN_Year . Thereafter, production declined in February and then recovered in May. In the months following production steadily decreased until September. Thereafter, the graph fluctuated from October to December.</t>
         </is>
       </c>
       <c r="W56" t="n">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>In this graph, one can see the TKN_About in TKN_Geo. Production of TKN_Year is measured TKN_UOM meters. The graph is M-shaped, with lows in January, July, and December and highs in March and November.</t>
+          <t>In this graph, one can see the TKN_About  in  TKN_Geo . Production of  TKN_Year  is measured TKN_UOM  meters. The graph is M-shaped, with lows in January, July, and December and highs in March and November.</t>
         </is>
       </c>
       <c r="W57" t="n">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>The following line chart is about TKN_About TKN_UOM in TKN_Geo during TKN_Year. From the graph it's clearly possible to see how the index values have been steadily growing during TKN_Year. Few light fluctuations have been reported during the summer months.</t>
+          <t>The following line chart is about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . From the graph it's clearly possible to see how the index values have been steadily growing during  TKN_Year . Few light fluctuations have been reported during the summer months.</t>
         </is>
       </c>
       <c r="W58" t="n">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>The graph illustrated the TKN_About in TKN_Geo in TKN_Year. The measurement used is TKN_UOM (FPPI): There is a clear peak in August, reaching an index of more than 96.</t>
+          <t>The graph illustrated the TKN_About  in  TKN_Geo  in  TKN_Year . The measurement used is TKN_UOM  (FPPI): There is a clear peak in August, reaching an index of more than 96.</t>
         </is>
       </c>
       <c r="W59" t="n">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>The TKN_About in 2994 rapidly fell from a high in January, to its lowest point in March of TKN_Year. After that the price index saw some fluctuation in the coming months until November, where it dropped again and did not change in December.</t>
+          <t>The TKN_About  in 2018 rapidly fell from a high in January, to its lowest point in March of  TKN_Year . After that the price index saw some fluctuation in the coming months until November, where it dropped again and did not change in December.</t>
         </is>
       </c>
       <c r="W60" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>The following line chart provides useful information about the TKN_About in TKN_Geo during TKN_Year. The production value is quantified using the number of TKN_UOM producted. During the first few months of the year the production rapidly increased, reaching the maximum value over TKN_Year in March. After that, over the next few months, the TKN_About slightly decreased until the end of the year.</t>
+          <t>The following line chart provides useful information about the TKN_About  in  TKN_Geo  during  TKN_Year . The production value is quantified using the number of TKN_UOM  producted. During the first few months of the year the production rapidly increased, reaching the maximum value over  TKN_Year  in March. After that, over the next few months, the TKN_About  slightly decreased until the end of the year.</t>
         </is>
       </c>
       <c r="W61" t="n">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>In this graph, the TKN_About can be seen. The data illustrated was collected in TKN_Geo in TKN_Year. The graph's line shows many ups and downs, with an overall high in February and May (index of 1010) and an overall low in August (index of 997).</t>
+          <t>In this graph, the TKN_About  can be seen. The data illustrated was collected in  TKN_Geo  in  TKN_Year . The graph's line shows many ups and downs, with an overall high in February and May (index of 100) and an overall low in August (index of 13).</t>
         </is>
       </c>
       <c r="W62" t="n">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>The graph shows TKN_UOM in TKN_Geo for the year TKN_Year. The graph reaches its highest point in June and then steadily drops each month until reaching its lowest point in October. Thereafter, it slowly recovers until December.</t>
+          <t>The graph shows TKN_UOM  in  TKN_Geo  for the year  TKN_Year . The graph reaches its highest point in June and then steadily drops each month until reaching its lowest point in October. Thereafter, it slowly recovers until December.</t>
         </is>
       </c>
       <c r="W63" t="n">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>The following graph shows information about the TKN_About index in TKN_Geo during TKN_Year. The overall trend is descending. It's clearly possible to see several fluctuations over the year, mainly during the summer months. The maximum value has been recorded during February and the minimum one during December.</t>
+          <t>The following graph shows information about the TKN_About  index in  TKN_Geo  during  TKN_Year . The overall trend is descending. It's clearly possible to see several fluctuations over the year, mainly during the summer months. The maximum value has been recorded during February and the minimum one during December.</t>
         </is>
       </c>
       <c r="W64" t="n">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>In this graph, the TKN_About in TKN_Geo is illustrated. The x-axis shows the months of the year of TKN_Year, whereas the y-axis depicts the production in tonnes. Values in August and September stand out, reaching almost 102 in September. During the remaining months of the year, production is comparably lower.</t>
+          <t>In this graph, the TKN_About  in  TKN_Geo  is illustrated. The x-axis shows the months of the year of  TKN_Year , whereas the y-axis depicts the production in tonnes. Values in August and September stand out, reaching almost 102 in September. During the remaining months of the year, production is comparably lower.</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>The graph depicts the fluctuation of TKN_About from January to November in TKN_Year. Production then sharply declined from November to December, reaching its lowest point.</t>
+          <t>The graph depicts the fluctuation of TKN_About  from January to November in  TKN_Year . Production then sharply declined from November to December, reaching its lowest point.</t>
         </is>
       </c>
       <c r="W66" t="n">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>The shown line chart provides information about the TKN_About in TKN_Geo during TKN_Year. The values are described using TKN_UOM (FPPI). It's clearly possible to see two significant peaks during the months of March and August. Then the overall value of production remain quite stable during the year.</t>
+          <t>The shown line chart provides information about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It's clearly possible to see two significant peaks during the months of March and August. Then the overall value of production remain quite stable during the year.</t>
         </is>
       </c>
       <c r="W67" t="n">
@@ -6101,7 +6101,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>This graph shows the TKN_About and poults, measured TKN_UOM index. The recorded data is from TKN_Geo, TKN_Year. The graph's line reaches its high in October, with an index of 100. The decline in the following month stands out, resulting in an index of 0 in November and December.</t>
+          <t>This graph shows the TKN_About  and poults, measured TKN_UOM  index. The recorded data is from  TKN_Geo ,  TKN_Year . The graph's line reaches its high in October, with an index of 100. The decline in the following month stands out, resulting in an index of 0 in November and December.</t>
         </is>
       </c>
       <c r="W68" t="n">
@@ -6185,7 +6185,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>A line TKN_About TKN_Geo each month in TKN_Year.  It indicates that travel was lowest during the winter months, reaching a minimum in February, and highest in the summer months, peaking in August (but with a slight dip in June).  The median TKN_UOM of returning vehicles is between 50 and 63.</t>
+          <t>A line TKN_About   TKN_Geo  each month in  TKN_Year .  It indicates that travel was lowest during the winter months, reaching a minimum in February, and highest in the summer months, peaking in August (but with a slight dip in June).  The median TKN_UOM  of returning vehicles is between 50 and 63.</t>
         </is>
       </c>
       <c r="W69" t="n">
@@ -6269,7 +6269,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>A figure indicating TKN_About in TKN_Geo each month in TKN_Year.  There do not seem to be any seasonal trends in the production.  The maximum production occurred in October, at over 97 TKN_UOM; and production fell below 10 TKN_UOM in February, August and September.</t>
+          <t>A figure indicating TKN_About  in  TKN_Geo  each month in  TKN_Year .  There do not seem to be any seasonal trends in the production.  The maximum production occurred in October, at over 97 TKN_UOM ; and production fell below 10 TKN_UOM  in February, August and September.</t>
         </is>
       </c>
       <c r="W70" t="n">
@@ -6353,7 +6353,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>Softwood and hardwood stock totals in TKN_Geo during each month of TKN_Year.  The total rose from slightly over TKN_UOM meters in January to over 97 cubic meters in April.  It then experienced a drop to less than 24 cubic meters from May to July, after which it continued to decline until reaching a minimum level in December of under 4 cubic meters.</t>
+          <t>Softwood and hardwood stock totals in  TKN_Geo  during each month of  TKN_Year .  The total rose from slightly over TKN_UOM  meters in January to over 97 cubic meters in April.  It then experienced a drop to less than 24 cubic meters from May to July, after which it continued to decline until reaching a minimum level in December of under 4 cubic meters.</t>
         </is>
       </c>
       <c r="W71" t="n">
@@ -6437,7 +6437,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>Tablet computer price index in TKN_Geo for TKN_Year.  The price index slowly trended downwards throughout the year but experienced three significant drops: in March, in September (possibly coinciding with back-to-school sales), and in December (possibly due to Boxing Day and Boxing Week sales).</t>
+          <t>Tablet computer price index in  TKN_Geo  for  TKN_Year .  The price index slowly trended downwards throughout the year but experienced three significant drops: in March, in September (possibly coinciding with back-to-school sales), and in December (possibly due to Boxing Day and Boxing Week sales).</t>
         </is>
       </c>
       <c r="W72" t="n">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>The following line chart provides information about the TKN_About of hardwood in TKN_Geo during TKN_Year. The production values have been described using TKN_UOM as unit of measure. The values have been strongly fluactuating over the year. It shows several peaks and dips over the year. Even that, the maximum value has been recorded during March and the minimum during July.</t>
+          <t>The following line chart provides information about the TKN_About  of hardwood in  TKN_Geo  during  TKN_Year . The production values have been described using TKN_UOM  as unit of measure. The values have been strongly fluactuating over the year. It shows several peaks and dips over the year. Even that, the maximum value has been recorded during March and the minimum during July.</t>
         </is>
       </c>
       <c r="W73" t="n">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>The line chart is describing the values about TKN_About in TKN_Geo during TKN_Year. The production amout is described using TKN_UOM (FPPI). The minimum recorded value is during February. The maximum recorded value is during August. Furthermore, there are several fluctuations over the year.</t>
+          <t>The line chart is describing the values about TKN_About  in  TKN_Geo  during  TKN_Year . The production amout is described using TKN_UOM  (FPPI). The minimum recorded value is during February. The maximum recorded value is during August. Furthermore, there are several fluctuations over the year.</t>
         </is>
       </c>
       <c r="W74" t="n">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>The shown graph is about the TKN_About in TKN_Geo during TKN_Year. The production values are quantified using TKN_UOM as unit of measure. As can be seen from the graph, the values are oscillating over the year. Just one significant peak has been recorded during August TKN_Year. The minimum value over the year was during December.</t>
+          <t>The shown graph is about the TKN_About  in  TKN_Geo  during  TKN_Year . The production values are quantified using TKN_UOM  as unit of measure. As can be seen from the graph, the values are oscillating over the year. Just one significant peak has been recorded during August  TKN_Year . The minimum value over the year was during December.</t>
         </is>
       </c>
       <c r="W75" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>Poultry production cost for each month in TKN_Geo in TKN_Year.  The cost index, at its lowest TKN_About year, steadily rose from less than 7 in March to over 93 August, then settled in September at roughly 71.</t>
+          <t>Poultry production cost for each month in  TKN_Geo  in  TKN_Year .  The cost index, at its lowest TKN_About  year, steadily rose from less than 7 in March to over 93 August, then settled in September at roughly 71.</t>
         </is>
       </c>
       <c r="W76" t="n">
@@ -6857,7 +6857,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>Hardwood production in TKN_Geo for each month of TKN_Year.  While production varied between less than 11 TKN_UOM and over 99 TKN_UOM in a given month, there do not seem to be any trends in the value over time.</t>
+          <t>Hardwood production in  TKN_Geo  for each month of  TKN_Year .  While production varied between less than 11 TKN_UOM  and over 99 TKN_UOM  in a given month, there do not seem to be any trends in the value over time.</t>
         </is>
       </c>
       <c r="W77" t="n">
@@ -6941,7 +6941,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>The graph describes the TKN_About in TKN_Geo during TKN_Year. The production value is described using TKN_UOM (FPPI). As it can be seen from the graph, the production rapidly increased from January until August. After that, from August to December the production slightly decreased. The maximum value has been registered in August and the minimum one during February.</t>
+          <t>The graph describes the TKN_About  in  TKN_Geo  during  TKN_Year . The production value is described using TKN_UOM  (FPPI). As it can be seen from the graph, the production rapidly increased from January until August. After that, from August to December the production slightly decreased. The maximum value has been registered in August and the minimum one during February.</t>
         </is>
       </c>
       <c r="W78" t="n">
@@ -7025,7 +7025,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>The following line chart is decribing the trend of the TKN_About in TKN_Geo during TKN_Year. The values are described using TKN_UOM (FPPI). It can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. The most significant peak was recorded during the month of July TKN_Year. The lowest values have been recorded during the months of September and December.</t>
+          <t>The following line chart is decribing the trend of the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. The most significant peak was recorded during the month of July  TKN_Year . The lowest values have been recorded during the months of September and December.</t>
         </is>
       </c>
       <c r="W79" t="n">
@@ -7109,7 +7109,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>Creamery butter imports into TKN_Geo in TKN_Year.  Imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 92 TKN_UOM in June, followed by an equally sharp drop to a minimum value of less than 7 TKN_UOM in July.</t>
+          <t>Creamery butter imports into  TKN_Geo  in  TKN_Year .  Imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 92 TKN_UOM  in June, followed by an equally sharp drop to a minimum value of less than 7 TKN_UOM  in July.</t>
         </is>
       </c>
       <c r="W80" t="n">
@@ -7193,7 +7193,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>The graph shows the values about the TKN_About in TKN_Geo over TKN_Year. The values are described using TKN_UOM as unit of measure. There is a drop from January to February. It's possible to see how the production value rapidly increased from February to April. Then from April to December the production value slightly decreased, showing few light fluctuations.</t>
+          <t>The graph shows the values about the TKN_About  in  TKN_Geo  over  TKN_Year . The values are described using TKN_UOM  as unit of measure. There is a drop from January to February. It's possible to see how the production value rapidly increased from February to April. Then from April to December the production value slightly decreased, showing few light fluctuations.</t>
         </is>
       </c>
       <c r="W81" t="n">
@@ -7277,7 +7277,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>Malt production in TKN_Geo in TKN_Year.  The production trends were fairly smooth for most of the year, rising from January to May, falling from August to November, and staying at or above 47 TKN_UOM until the end of the year.  By comparison, June and July showed strong fluctuations in production, and the value dropped to its all-year low of under 4 TKN_UOM in December.</t>
+          <t>Malt production in  TKN_Geo  in  TKN_Year .  The production trends were fairly smooth for most of the year, rising from January to May, falling from August to November, and staying at or above 47 TKN_UOM  until the end of the year.  By comparison, June and July showed strong fluctuations in production, and the value dropped to its all-year low of under 4 TKN_UOM  in December.</t>
         </is>
       </c>
       <c r="W82" t="n">
@@ -7356,12 +7356,12 @@
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>Production of vehicles in Canada in 2017.  The graph indicates much lower production during the winter months, with January, February and December totals more than 30000 units lower than any point during the rest of the year.  While the total peaked in may at 220000 units, it was consistently above 180000 units from March until September.</t>
+          <t>The provided graph displays the number of Canadian vehicles returning to Canada over the year 2016 divided by month. It starts out at around 150000 vehicles in January, falls to 135000 in February and rises continuously to over 220000 in August. The following month show a steady decrease to its second lowest point of just under 160000 in December.</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>Production of vehicles in TKN_Geo in TKN_Year.  The graph indicates much lower production during the winter months, with January, February and December totals more than -77 TKN_UOM lower than any point during the rest of the year.  While the total peaked in may at 100 TKN_UOM, it was consistently above 62 TKN_UOM from March until September.</t>
+          <t>The provided graph displays the TKN_About  returning to  TKN_Geo  over the year 2016 divided by month. It starts out at around 34 vehicles in January, falls to 20 in February and rises continuously to over 100 in August. The following month show a steady decrease to its second lowest point of just under 44 in December.</t>
         </is>
       </c>
       <c r="W83" t="n">
@@ -7445,7 +7445,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the total TKN_UOM of Unitated States vehicles entering in TKN_Geo during TKN_Year presented the highest values during the summer period. In particular, the maximum value has been reached during July. The month with less TKN_About TKN_Geo over the year has been February TKN_Year.</t>
+          <t>As it can be seen from the graph, the total TKN_UOM  of Unitated States vehicles entering in  TKN_Geo  during  TKN_Year  presented the highest values during the summer period. In particular, the maximum value has been reached during July. The month with less TKN_About   TKN_Geo  over the year has been February  TKN_Year .</t>
         </is>
       </c>
       <c r="W84" t="n">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>This chart shows how the TKN_UOM varies by month throughout TKN_Year. We see a distinctive TKN_About starts at a middling level in the first three months of the year, before a rapid increase from April to July, where it reaches a peak. A quick descent then follow into the fall, with a low point in September, a small rebound in October, and falling again in December.</t>
+          <t>This chart shows how the TKN_UOM  varies by month throughout  TKN_Year . We see a distinctive TKN_About  starts at a middling level in the first three months of the year, before a rapid increase from April to July, where it reaches a peak. A quick descent then follow into the fall, with a low point in September, a small rebound in October, and falling again in December.</t>
         </is>
       </c>
       <c r="W85" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About fruit, TKN_UOM index, in TKN_Geo in TKN_Year. We see a generally increasing pattern throughout the year. We start at a markedly low level of production from January until May, at which point production starts to increase until July. Production then falls for August to October, until surging in November and reaching a maximum in December.</t>
+          <t>This chart shows the TKN_About  fruit, TKN_UOM  index, in  TKN_Geo  in  TKN_Year . We see a generally increasing pattern throughout the year. We start at a markedly low level of production from January until May, at which point production starts to increase until July. Production then falls for August to October, until surging in November and reaching a maximum in December.</t>
         </is>
       </c>
       <c r="W86" t="n">
@@ -7697,7 +7697,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About malt, measures in tonnes, in TKN_Geo in TKN_Year. Product starts in January at its low point, before a steep increase in February. A mild decrease follows until April, before increasing to a maximum in June. Production then falls over the remainder of the year though with some fluctuation, with December levels almost as low as January.</t>
+          <t>This chart shows the TKN_About  malt, measures in tonnes, in  TKN_Geo  in  TKN_Year . Product starts in January at its low point, before a steep increase in February. A mild decrease follows until April, before increasing to a maximum in June. Production then falls over the remainder of the year though with some fluctuation, with December levels almost as low as January.</t>
         </is>
       </c>
       <c r="W87" t="n">
@@ -7781,7 +7781,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>This charts shows the TKN_About shell, as measured TKN_UOM index, in TKN_Geo in TKN_Year. Production in January starts at a relatively high level, before increasing in February. After this, a gradual decline follows, reaching a minimum in July. After this, production recovers over the remainder of the year, reaching near the maximum by Oct before reaching the maximum by November and December.</t>
+          <t>This charts shows the TKN_About  shell, as measured TKN_UOM  index, in  TKN_Geo  in  TKN_Year . Production in January starts at a relatively high level, before increasing in February. After this, a gradual decline follows, reaching a minimum in July. After this, production recovers over the remainder of the year, reaching near the maximum by Oct before reaching the maximum by November and December.</t>
         </is>
       </c>
       <c r="W88" t="n">
@@ -7865,7 +7865,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About oats, measured in TKN_UOM, in TKN_Geo. Generally, production fluctuates quite a lot month to month. Production starts at a middling level in January, with wide oscillations until July. After July, production increases consistently until reaching a maximum in September, before then gradually decreasing until reaching a level similiar to January in December.</t>
+          <t>This chart shows the TKN_About  oats, measured in  TKN_UOM , in  TKN_Geo . Generally, production fluctuates quite a lot month to month. Production starts at a middling level in January, with wide oscillations until July. After July, production increases consistently until reaching a maximum in September, before then gradually decreasing until reaching a level similiar to January in December.</t>
         </is>
       </c>
       <c r="W89" t="n">
@@ -7949,7 +7949,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>Line chart showing the increase of TKN_About TKN_UOM in TKN_Year in TKN_Geo.</t>
+          <t>Line chart showing the increase of TKN_About  TKN_UOM  in  TKN_Year  in  TKN_Geo .</t>
         </is>
       </c>
       <c r="W90" t="n">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>Line chart showing TKN_About TKN_UOM in TKN_Geo in TKN_Year.</t>
+          <t>Line chart showing TKN_About  TKN_UOM  in  TKN_Geo  in  TKN_Year .</t>
         </is>
       </c>
       <c r="W91" t="n">
@@ -8117,7 +8117,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About in TKN_Geo during TKN_Year. Production starts very low in January and undergoes a sharp increase until it reaches its peak of over 96 motor vehicles in April. The following months production decreases, being almost steady at 69 from July until September. Production gradually decreases until December.</t>
+          <t>This graph represents the TKN_About  in  TKN_Geo  during  TKN_Year . Production starts very low in January and undergoes a sharp increase until it reaches its peak of over 96 motor vehicles in April. The following months production decreases, being almost steady at 69 from July until September. Production gradually decreases until December.</t>
         </is>
       </c>
       <c r="W92" t="n">
@@ -8196,12 +8196,12 @@
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>The price index of servers in Canada during 2017 is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 103 in November. A small increase to 1010 is observed in December.</t>
+          <t>The price index of servers in Canada during 2017 is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 1007 in November. A small increase to 1010 is observed in December.</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately -3477 in November. A small increase to 12 is observed in December.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 0 in November. A small increase to 12 is observed in December.</t>
         </is>
       </c>
       <c r="W93" t="n">
@@ -8285,7 +8285,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_UOM in TKN_Geo during TKN_Year is shown in this line chart. Production sharply increases from January until March. During the following months production fluctuates in an overall decreasing manner until it reaches its minimum in August. There is a sharp gain in production of candle from August until reaching the maximum of over 95 in December.</t>
+          <t>The TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year  is shown in this line chart. Production sharply increases from January until March. During the following months production fluctuates in an overall decreasing manner until it reaches its minimum in August. There is a sharp gain in production of candle from August until reaching the maximum of over 95 in December.</t>
         </is>
       </c>
       <c r="W94" t="n">
@@ -8369,7 +8369,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About of TKN_Geo in TKN_Year.   The number of products experiences a sharp increase from January until reaching the maximum during June, whereas a small decline is observed in the month of April. From June until September the TKN_About rapidly decline and reach a minimum of under -856 in September. The following -856 months a small increase can be observed, before it drops again in December.</t>
+          <t>This graph represents the TKN_About  of  TKN_Geo  in  TKN_Year .   The number of products experiences a sharp increase from January until reaching the maximum during June, whereas a small decline is observed in the month of April. From June until September the TKN_About  rapidly decline and reach a minimum of under 2 in September. The following 2 months a small increase can be observed, before it drops again in December.</t>
         </is>
       </c>
       <c r="W95" t="n">
@@ -8453,7 +8453,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>This line chart describes the TKN_About of TKN_Geo in TKN_Year. In January a production of 19 can be observed. This decreases in the month of February and from then onwards a small, but constant increase is taking place until the maximum of over 97 can be seen in September. After September TKN_About steadily decreases again, with a small increase in November. A value of approximately 53 is observed in December.</t>
+          <t>This line chart describes the TKN_About  of  TKN_Geo  in  TKN_Year . In January a production of 19 can be observed. This decreases in the month of February and from then onwards a small, but constant increase is taking place until the maximum of over 97 can be seen in September. After September TKN_About  steadily decreases again, with a small increase in November. A value of approximately 53 is observed in December.</t>
         </is>
       </c>
       <c r="W96" t="n">
@@ -8537,7 +8537,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>This graph represents TKN_About TKN_UOM of TKN_Geo in TKN_Year. Overall a content increase can be observed throughout the year, starting at approximately 0 in January and increasing of uptimes to 100 in November where it plateaus like that until December.</t>
+          <t>This graph represents TKN_About  TKN_UOM  of  TKN_Geo  in  TKN_Year . Overall a content increase can be observed throughout the year, starting at approximately 0 in January and increasing of uptimes to 100 in November where it plateaus like that until December.</t>
         </is>
       </c>
       <c r="W97" t="n">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>This chart represents the TKN_About of TKN_Geo in TKN_Year. Whereas the production oscillates from January until June ranging from 34 until 53 a minimum value of below 9 is observed during July. The following three months a sharp increase is taking place and reaching a value of approximately 98. The production stays almost consistent from October until December.</t>
+          <t>This chart represents the TKN_About  of  TKN_Geo  in  TKN_Year . Whereas the production oscillates from January until June ranging from 34 until 53 a minimum value of below 9 is observed during July. The following three months a sharp increase is taking place and reaching a value of approximately 98. The production stays almost consistent from October until December.</t>
         </is>
       </c>
       <c r="W98" t="n">
@@ -8705,7 +8705,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>This line chart illustrates the TKN_About (in tonnes) of TKN_Geo in TKN_Year. Production starts very low in January at approximately 0 tonnes. From there on production starts oscillating a lot, having a peak during February, a low in March and reaching the maximum during April. There is a sharp decline from April until May, after which production starts fluctuating again until September. There is a rapid jump in October reaching almost 95 tonnes. A very slight increase can be observed for November, after which the production drops in December.</t>
+          <t>This line chart illustrates the TKN_About  (in tonnes) of  TKN_Geo  in  TKN_Year . Production starts very low in January at approximately 0 tonnes. From there on production starts oscillating a lot, having a peak during February, a low in March and reaching the maximum during April. There is a sharp decline from April until May, after which production starts fluctuating again until September. There is a rapid jump in October reaching almost 95 tonnes. A very slight increase can be observed for November, after which the production drops in December.</t>
         </is>
       </c>
       <c r="W99" t="n">
@@ -8789,7 +8789,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>This line chart depicts the TKN_About in TKN_UOM of TKN_Geo in TKN_Year. Production starts at approximately 59 TKN_UOM during January, after which a moderate increase can be observed until reaching about 95 in March. Production remains steady at 73 during April and May, after which the maximum production is achieved in June with 99 TKN_UOM. There is a sharp drop in July, a rapid increase until November until the minimum value of approximately 3 is reached in December.</t>
+          <t>This line chart depicts the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . Production starts at approximately 59 TKN_UOM  during January, after which a moderate increase can be observed until reaching about 95 in March. Production remains steady at 73 during April and May, after which the maximum production is achieved in June with 99 TKN_UOM . There is a sharp drop in July, a rapid increase until November until the minimum value of approximately 3 is reached in December.</t>
         </is>
       </c>
       <c r="W100" t="n">
@@ -8873,7 +8873,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>The chart shows the variation TKN_About prices in TKN_Geo during the year TKN_Year. Except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
+          <t>The chart shows the variation TKN_About  prices in  TKN_Geo  during the year  TKN_Year . Except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
         </is>
       </c>
       <c r="W101" t="n">
@@ -8957,7 +8957,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>Increase TKN_About TKN_UOM during TKN_Year months per months.</t>
+          <t>Increase TKN_About  TKN_UOM  during  TKN_Year  months per months.</t>
         </is>
       </c>
       <c r="W102" t="n">
@@ -9041,7 +9041,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About of softwood in TKN_Geo over the year of TKN_Year. The data is presented TKN_UOM meters. According to the graph TKN_About of softwood is the highest in March and the lowest in December.</t>
+          <t>The graph shows TKN_About  of softwood in  TKN_Geo  over the year of  TKN_Year . The data is presented TKN_UOM  meters. According to the graph TKN_About  of softwood is the highest in March and the lowest in December.</t>
         </is>
       </c>
       <c r="W103" t="n">
@@ -9125,7 +9125,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>The chart shows the variation of TKN_About in TKN_Geo during the year TKN_Year. The higher price was identify during the month of January, followed by a considerable decline till May, when it returns to rise rapidly. Prices remain steady in the last -20460 months of the year.</t>
+          <t>The chart shows the variation of TKN_About  in  TKN_Geo  during the year  TKN_Year . The higher price was identify during the month of January, followed by a considerable decline till May, when it returns to rise rapidly. Prices remain steady in the last 4 months of the year.</t>
         </is>
       </c>
       <c r="W104" t="n">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About value in TKN_Geo during TKN_Year. The values are described using TKN_UOM (FPPI). The products index shown several fluctuations. In particular, it's clearly possible to see several peaks and dips. In February, July and October the value reached its maximum values. During April and September the value reached its minimum values.</t>
+          <t>The graph shows the TKN_About  value in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). The products index shown several fluctuations. In particular, it's clearly possible to see several peaks and dips. In February, July and October the value reached its maximum values. During April and September the value reached its minimum values.</t>
         </is>
       </c>
       <c r="W105" t="n">
@@ -9293,7 +9293,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>The data presented in the graph shows the TKN_About in TKN_Geo over the year of TKN_Year in tonnes. The lowest TKN_About can be observed in January. The supply increases constantly over the next months and reaches its highest value in June, after which it decreases with a similar rate and reaches a local minimum in September.</t>
+          <t>The data presented in the graph shows the TKN_About  in  TKN_Geo  over the year of  TKN_Year  in tonnes. The lowest TKN_About  can be observed in January. The supply increases constantly over the next months and reaches its highest value in June, after which it decreases with a similar rate and reaches a local minimum in September.</t>
         </is>
       </c>
       <c r="W106" t="n">
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>The chart shows the variation of TKN_About in TKN_Geo during the year TKN_Year. The production reaches its top on March after which we observe an oscillating period until November, when there is a steeply fall.</t>
+          <t>The chart shows the variation of TKN_About  in  TKN_Geo  during the year  TKN_Year . The production reaches its top on March after which we observe an oscillating period until November, when there is a steeply fall.</t>
         </is>
       </c>
       <c r="W107" t="n">
@@ -9461,7 +9461,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>A line chart about the global growth and punctual drops TKN_About TKN_Geo, TKN_Year.</t>
+          <t>A line chart about the global growth and punctual drops TKN_About   TKN_Geo ,  TKN_Year .</t>
         </is>
       </c>
       <c r="W108" t="n">
@@ -9545,7 +9545,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>The diagramm showes TKN_UOM of TKN_Geo over the year TKN_Year. From January to TKN_About increase. in April there is a small  drop and afterwards a continous increase till June. It stays constant between June and July and decrase rapitly till September/October. At october the annual minimum is reached. In November there is a small increase and in December it drops again.</t>
+          <t>The diagramm showes TKN_UOM  of  TKN_Geo  over the year  TKN_Year . From January to TKN_About  increase. in April there is a small  drop and afterwards a continous increase till June. It stays constant between June and July and decrase rapitly till September/October. At october the annual minimum is reached. In November there is a small increase and in December it drops again.</t>
         </is>
       </c>
       <c r="W109" t="n">
@@ -9629,7 +9629,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>A line chart about the price TKN_About in TKN_Geo, TKN_Year. The index dropped from 100 to stabilizes around 23 by the month of April.</t>
+          <t>A line chart about the price TKN_About  in  TKN_Geo ,  TKN_Year . The index dropped from 100 to stabilizes around 23 by the month of April.</t>
         </is>
       </c>
       <c r="W110" t="n">
@@ -9713,7 +9713,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>The TKN_About was slightly increasing during the three first months of the year TKN_Year, then slightly decline for a month.  Afterwards it stayed constant for a month until a massive drop for -16-16357 months, to grow again for a month and then decrease again. The -1635 last months of the year the index surges again.</t>
+          <t>The TKN_About  was slightly increasing during the three first months of the year  TKN_Year , then slightly decline for a month.  Afterwards it stayed constant for a month until a massive drop for 2 months, to grow again for a month and then decrease again. The 3 last months of the year the index surges again.</t>
         </is>
       </c>
       <c r="W111" t="n">
@@ -9797,7 +9797,7 @@
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>The Diagramm showes the TKN_About of TKN_Geo over the year TKN_Year. The index is quite stable between Jannuary and May with a small peak in March. Then it drops suddenly till July. It increaes a little bit in August and drop again in September to the lowest point of the year (less then 1120). From September to December it increase slightly to 37.</t>
+          <t>The Diagramm showes the TKN_About  of  TKN_Geo  over the year  TKN_Year . The index is quite stable between Jannuary and May with a small peak in March. Then it drops suddenly till July. It increaes a little bit in August and drop again in September to the lowest point of the year (less then 7). From September to December it increase slightly to 37.</t>
         </is>
       </c>
       <c r="W112" t="n">
@@ -9881,7 +9881,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>The line chart about TKN_About in TKN_Geo, TKN_Year shows that there was a peak in the production during the period of June, July and August.  To drop during the month of October and then raise again. At the beginning of the year the production was growing until this boost in Summer.</t>
+          <t>The line chart about TKN_About  in  TKN_Geo ,  TKN_Year  shows that there was a peak in the production during the period of June, July and August.  To drop during the month of October and then raise again. At the beginning of the year the production was growing until this boost in Summer.</t>
         </is>
       </c>
       <c r="W113" t="n">
@@ -9965,7 +9965,7 @@
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>The diagramm showes the TKN_About in TKN_UOM over the year TKN_Year. The Graphe fluctuates a lot over the Year. Ther are peaks in January, April/May, October and December. The highest production is reached in October. There are also monthes with a low TKN_About: February, August and November. The lowst production is reached in August.</t>
+          <t>The diagramm showes the TKN_About  in TKN_UOM  over the year  TKN_Year . The Graphe fluctuates a lot over the Year. Ther are peaks in January, April/May, October and December. The highest production is reached in October. There are also monthes with a low TKN_About : February, August and November. The lowst production is reached in August.</t>
         </is>
       </c>
       <c r="W114" t="n">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>The diagram showes the TKN_About in Dollar  over the year TKN_Year in TKN_Geo. In januarry less than 6 vehicles were produced (lowest). Till April the production increase steadyly and reach the highest value. From April to December it decreases slowly with two small peaks in September and November.</t>
+          <t>The diagram showes the TKN_About  in Dollar  over the year  TKN_Year  in  TKN_Geo . In januarry less than 6 vehicles were produced (lowest). Till April the production increase steadyly and reach the highest value. From April to December it decreases slowly with two small peaks in September and November.</t>
         </is>
       </c>
       <c r="W115" t="n">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>Land TKN_UOM in TKN_Geo in the year of TKN_Year. The graphic shows the course of the TKN_About in TKN_Geo over the year TKN_Year. It is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. For the mounths of november and december the maximum value is reached with 100.</t>
+          <t>Land TKN_UOM  in  TKN_Geo  in the year of  TKN_Year . The graphic shows the course of the TKN_About   in  TKN_Geo  over the year  TKN_Year . It is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. For the mounths of november and december the maximum value is reached with 100.</t>
         </is>
       </c>
       <c r="W116" t="n">
@@ -10217,7 +10217,7 @@
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_UOM of TKN_Geo in TKN_Year. Production starts at approximately 64 TKN_UOM in January and increases to one of its maximum values of 102 TKN_UOM in March. The following months show first a slow decrease, but then a sharp decrease in July. From July until November production gradually increases again until it reaches its second maximum of 102 TKN_UOM in November. There is a sharp drop from November onwards, reaching its minimum value of -1 TKN_UOM in December.</t>
+          <t>This graph depicts the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . Production starts at approximately 64 TKN_UOM  in January and increases to one of its maximum values of 102 TKN_UOM  in March. The following months show first a slow decrease, but then a sharp decrease in July. From July until November production gradually increases again until it reaches its second maximum of 102 TKN_UOM  in November. There is a sharp drop from November onwards, reaching its minimum value of -1 TKN_UOM  in December.</t>
         </is>
       </c>
       <c r="W117" t="n">
@@ -10301,7 +10301,7 @@
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in TKN_Geo TKN_Year. The graphic shows the production of new motor vehicles ($) in TKN_Geo over the year TKN_Year. iT is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
+          <t>Production of new motor vehicles in  TKN_Geo   TKN_Year . The graphic shows the production of new motor vehicles ($) in  TKN_Geo  over the year  TKN_Year . iT is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
         </is>
       </c>
       <c r="W118" t="n">
@@ -10385,7 +10385,7 @@
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>This line chart represents the Canadian TKN_About in TKN_UOM in TKN_Year. The year starts with a minimum production value of -1 TKN_UOM in January and gradually increases until reaching its maximum in May with approximately 98. From May onwards the production starts fluctuating, having a low in July, but also an increased production in September. In the following three months a constant drop is observed, reaching a value of 24 TKN_UOM in December.</t>
+          <t>This line chart represents the Canadian TKN_About  in TKN_UOM  in  TKN_Year . The year starts with a minimum production value of -1 TKN_UOM  in January and gradually increases until reaching its maximum in May with approximately 98. From May onwards the production starts fluctuating, having a low in July, but also an increased production in September. In the following three months a constant drop is observed, reaching a value of 24 TKN_UOM  in December.</t>
         </is>
       </c>
       <c r="W119" t="n">
@@ -10469,7 +10469,7 @@
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>This chart represents the TKN_About in TKN_UOM of TKN_Geo in TKN_Year. The minimum supply can be observed during January with -1 TKN_UOM. From then onwards the supply steadily increases until May with 92 TKN_UOM. From May until July the supply is held about constant. A slow, but constant decrease is observed from July until December.</t>
+          <t>This chart represents the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . The minimum supply can be observed during January with -1 TKN_UOM . From then onwards the supply steadily increases until May with 92 TKN_UOM . From May until July the supply is held about constant. A slow, but constant decrease is observed from July until December.</t>
         </is>
       </c>
       <c r="W120" t="n">
@@ -10553,7 +10553,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About in TKN_Geo in TKN_Year. The maximum price of approximately 100 can be observed during January, whereas the price steadily decreases during the following months until May with 62. There is a sharp drop in June at a value of 21. The following months the price does not fluctuate too much, reaching a minimum of 0 in December.</t>
+          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year . The maximum price of approximately 100 can be observed during January, whereas the price steadily decreases during the following months until May with 62. There is a sharp drop in June at a value of 21. The following months the price does not fluctuate too much, reaching a minimum of 0 in December.</t>
         </is>
       </c>
       <c r="W121" t="n">
@@ -10637,7 +10637,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>The shown line chart illustrates the TKN_About hardwood in TKN_Geo during TKN_Year. The production is described using TKN_UOM as unit of measure. The values have been significantly oscillating over the year. In particular, the production reached its maximum value during the month of May and its minimum value during July. After July, it rapidly grown up again, reaching an another peak during October.</t>
+          <t>The shown line chart illustrates the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The production is described using TKN_UOM  as unit of measure. The values have been significantly oscillating over the year. In particular, the production reached its maximum value during the month of May and its minimum value during July. After July, it rapidly grown up again, reaching an another peak during October.</t>
         </is>
       </c>
       <c r="W122" t="n">
@@ -10721,7 +10721,7 @@
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>The following line chart describes the TKN_About hardwood in TKN_Geo during TKN_Year. The unit of measurement of the data TKN_UOM metres. The production showed several peaks during the year, mainly during March, June and November. Furthermore, a significant drop has been recorded between the months of June and July.</t>
+          <t>The following line chart describes the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The unit of measurement of the data TKN_UOM  metres. The production showed several peaks during the year, mainly during March, June and November. Furthermore, a significant drop has been recorded between the months of June and July.</t>
         </is>
       </c>
       <c r="W123" t="n">
@@ -10805,7 +10805,7 @@
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the production value of what flour in TKN_Geo during TKN_Year has been strongly fluctuating. The unit of measurement is tonnes. The graph shows several peaks, but the maximum values have been recorded during the months of April, Octoeber and November. At the same time, the months with less TKN_About have been January and July.</t>
+          <t>As it's shown in the graph, the production value of what flour in  TKN_Geo  during  TKN_Year  has been strongly fluctuating. The unit of measurement is tonnes. The graph shows several peaks, but the maximum values have been recorded during the months of April, Octoeber and November. At the same time, the months with less TKN_About  have been January and July.</t>
         </is>
       </c>
       <c r="W124" t="n">
@@ -10889,7 +10889,7 @@
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>This line graph displays TKN_About in TKN_UOM in TKN_Geo for TKN_Year. The amount fluctuates with an increase from January to March, followed by a slow decrease from March to June.  A steep reduction follows in July, matched by an equally steep increase in August.  A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of -1 TKN_UOM.</t>
+          <t>This line graph displays TKN_About  in TKN_UOM  in  TKN_Geo  for  TKN_Year . The amount fluctuates with an increase from January to March, followed by a slow decrease from March to June.  A steep reduction follows in July, matched by an equally steep increase in August.  A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of -1 TKN_UOM .</t>
         </is>
       </c>
       <c r="W125" t="n">
@@ -10973,7 +10973,7 @@
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>This line graph displays TKN_About TKN_UOM in TKN_Geo for TKN_Year.  The index is unchanged from January to April, where it rises steadily until August.  From August to November there is a steep increase, with the value remaining unchanged in December.</t>
+          <t>This line graph displays TKN_About  TKN_UOM  in  TKN_Geo  for  TKN_Year .  The index is unchanged from January to April, where it rises steadily until August.  From August to November there is a steep increase, with the value remaining unchanged in December.</t>
         </is>
       </c>
       <c r="W126" t="n">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>This line graph displays the TKN_About in TKN_Geo for TKN_Year TKN_UOM index.  A small decrease from January to February is followed by a steady increase until October, where the value again decreases for November and December.</t>
+          <t>This line graph displays the TKN_About  in  TKN_Geo  for  TKN_Year  TKN_UOM  index.  A small decrease from January to February is followed by a steady increase until October, where the value again decreases for November and December.</t>
         </is>
       </c>
       <c r="W127" t="n">
@@ -11141,7 +11141,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>This line graph displays the TKN_About in TKN_Geo for TKN_Year TKN_UOM index.  A slow but steady increase is observed from January to June, where a steep increase is seen from June to August.  A steep decrease follows from August to October, where the value again rises steadily from October to December.</t>
+          <t>This line graph displays the TKN_About  in  TKN_Geo  for  TKN_Year  TKN_UOM  index.  A slow but steady increase is observed from January to June, where a steep increase is seen from June to August.  A steep decrease follows from August to October, where the value again rises steadily from October to December.</t>
         </is>
       </c>
       <c r="W128" t="n">
@@ -11220,12 +11220,12 @@
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>A Graph showing the production of new motor vehicles by Canada in 2016. As you can see the production had a big climbing in Q1 2016. It stayed stable in Q2 and Q3, while fell down in Q4.it is a phisiologic trend for the motor vehicles market.</t>
+          <t>A Graph showing the production of new motor vehicles by Canada in 2016. As you can see the production had a big climbing in Q1 2016. It stayed stable in Q2 and Q3, while fell down in Q4. it is a phisiologic trend for the motor vehicles market.</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>A Graph showing the TKN_About by TKN_Geo in TKN_Year. As you can see the production had a big climbing in Q1 TKN_Year. It stayed stable in Q2 and Q3, while fell down in Q4.it is a phisiologic trend for the motor vehicles market.</t>
+          <t>A Graph showing the TKN_About  by  TKN_Geo  in  TKN_Year . As you can see the production had a big climbing in Q1  TKN_Year . It stayed stable in Q2 and Q3, while fell down in Q4. it is a phisiologic trend for the motor vehicles market.</t>
         </is>
       </c>
       <c r="W129" t="n">
@@ -11309,7 +11309,7 @@
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>Graphic of the market prices trend of Computers in TKN_Geo TKN_Year. This graphic shows TKN_About prices in TKN_Year for the canadian market. It immediatly affect you how the prices raise from january to february and then slowly decrease until July. We can see another drop from July to September, probably justified by people on holiday, not buying any Computer and the a slight raise again till the end of the year.</t>
+          <t>Graphic of the market prices trend of Computers in  TKN_Geo   TKN_Year . This graphic shows TKN_About  prices in  TKN_Year  for the canadian market. It immediatly affect you how the prices raise from january to february and then slowly decrease until July. We can see another drop from July to September, probably justified by people on holiday, not buying any Computer and the a slight raise again till the end of the year.</t>
         </is>
       </c>
       <c r="W130" t="n">
@@ -11561,7 +11561,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>Plot graph TKN_About bikes were produced in TKN_Year in TKN_Geo.</t>
+          <t>Plot graph TKN_About  bikes were produced in  TKN_Year  in  TKN_Geo .</t>
         </is>
       </c>
       <c r="W133" t="n">
@@ -11645,7 +11645,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>Servers price index in TKN_Year from April to July has sharply increased.</t>
+          <t>Servers price index in  TKN_Year  from April to July has sharply increased.</t>
         </is>
       </c>
       <c r="W134" t="n">
@@ -11897,7 +11897,7 @@
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>The best time to buy TKN_About in TKN_Geo in TKN_Year was between April and May.</t>
+          <t>The best time to buy TKN_About  in  TKN_Geo  in  TKN_Year  was between April and May.</t>
         </is>
       </c>
       <c r="W137" t="n">
@@ -11981,7 +11981,7 @@
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>In TKN_Year, TKN_About has suffered strong fluctuations.</t>
+          <t>In  TKN_Year , TKN_About  has suffered strong fluctuations.</t>
         </is>
       </c>
       <c r="W138" t="n">
@@ -12065,7 +12065,7 @@
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>A plot chart about TKN_About vehicles.</t>
+          <t>A plot chart about TKN_About  vehicles.</t>
         </is>
       </c>
       <c r="W139" t="n">
@@ -12233,7 +12233,7 @@
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>In June TKN_About has hugely decrease.</t>
+          <t>In June  TKN_Year  laptop price has hugely decrease.</t>
         </is>
       </c>
       <c r="W141" t="n">
@@ -12317,7 +12317,7 @@
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>Malt production incredibly decrease from July TKN_Year to August TKN_Year.</t>
+          <t>Malt production incredibly decrease from July  TKN_Year  to August  TKN_Year .</t>
         </is>
       </c>
       <c r="W142" t="n">
@@ -12485,7 +12485,7 @@
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>Amount TKN_About TKN_Geo in TKN_Year.</t>
+          <t>Amount TKN_About   TKN_Geo  in  TKN_Year .</t>
         </is>
       </c>
       <c r="W144" t="n">
@@ -12569,7 +12569,7 @@
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>Cars entering TKN_Geo in one year.</t>
+          <t>Cars entering  TKN_Geo  in one year.</t>
         </is>
       </c>
       <c r="W145" t="n">
@@ -12653,7 +12653,7 @@
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>Oats produzed in TKN_Geo in the year TKN_Year.</t>
+          <t>Oats produzed in  TKN_Geo  in the year  TKN_Year .</t>
         </is>
       </c>
       <c r="W146" t="n">
@@ -12737,7 +12737,7 @@
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>The FPPI TKN_About in TKN_Year fluctuates steadily between January and April. Then the FPPI start to decline, with its downwards slope increasing slightly after May. The FPPI drops dramatically in July, and reaches its lowest point in August. It then quickly starts raising, slowing slightly between September and October, and finishes its climb in November. The FPPI is close to its January value and is fairly steady until December.</t>
+          <t>The FPPI TKN_About  in  TKN_Year  fluctuates steadily between January and April. Then the FPPI start to decline, with its downwards slope increasing slightly after May. The FPPI drops dramatically in July, and reaches its lowest point in August. It then quickly starts raising, slowing slightly between September and October, and finishes its climb in November. The FPPI is close to its January value and is fairly steady until December.</t>
         </is>
       </c>
       <c r="W147" t="n">
@@ -12821,7 +12821,7 @@
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the TKN_UOM TKN_About TKN_Geo during TKN_Year has been much higher during the summer compared with the other months of the year. In particular, the maximum TKN_UOM TKN_About TKN_Geo in TKN_Year has been registered during August. At the same time, the minimum value during February.</t>
+          <t>As it's shown in the graph, the TKN_UOM  TKN_About   TKN_Geo  during  TKN_Year  has been much higher during the summer compared with the other months of the year. In particular, the maximum TKN_UOM  TKN_About   TKN_Geo  in  TKN_Year  has been registered during August. At the same time, the minimum value during February.</t>
         </is>
       </c>
       <c r="W148" t="n">
@@ -12905,7 +12905,7 @@
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the TKN_About index in TKN_Geo rapidly decreased over TKN_Year. Few fluctuations have been reported over the year. The maximum value has been recorded during March and the minimum during December TKN_Year.</t>
+          <t>As it's possible to see from the graph, the TKN_About  index in  TKN_Geo  rapidly decreased over  TKN_Year . Few fluctuations have been reported over the year. The maximum value has been recorded during March and the minimum during December  TKN_Year .</t>
         </is>
       </c>
       <c r="W149" t="n">
@@ -12989,7 +12989,7 @@
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>From the graph is clear that the TKN_About had a significant jump from the month of February to April. The values in the graph are described using TKN_UOM as unit of measurement. From July over the values started to slowly decrease until the end of the year.</t>
+          <t>From the graph is clear that the TKN_About  had a significant jump from the month of February to April. The values in the graph are described using TKN_UOM  as unit of measurement. From July over the values started to slowly decrease until the end of the year.</t>
         </is>
       </c>
       <c r="W150" t="n">
@@ -13073,7 +13073,7 @@
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About hardwood in TKN_Geo during TKN_Year. The described values are TKN_UOM metres. It's clearly possible to see how the production fluctuated over the year, with several peaks and dips. But at the end of the year, betwewen November and December, has been registered a significant drop of the value.</t>
+          <t>The following line chart is about the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The described values are TKN_UOM  metres. It's clearly possible to see how the production fluctuated over the year, with several peaks and dips. But at the end of the year, betwewen November and December, has been registered a significant drop of the value.</t>
         </is>
       </c>
       <c r="W151" t="n">
@@ -13157,7 +13157,7 @@
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About in TKN_Geo during TKN_Year maintained the same level for almost the whole year, but the summer months. During the summer months have been registered the highest values, in particular during August which was the highest peak of production. After that, the values dropped down form August to October.</t>
+          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  during  TKN_Year  maintained the same level for almost the whole year, but the summer months. During the summer months have been registered the highest values, in particular during August which was the highest peak of production. After that, the values dropped down form August to October.</t>
         </is>
       </c>
       <c r="W152" t="n">
@@ -13241,7 +13241,7 @@
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>A chart showing the TKN_UOM of TKN_About TKN_Geo sorted by month and showing the significant peak in the summer months.</t>
+          <t>A chart showing the TKN_UOM  of TKN_About   TKN_Geo  sorted by month and showing the significant peak in the summer months.</t>
         </is>
       </c>
       <c r="W153" t="n">
@@ -13320,12 +13320,12 @@
       </c>
       <c r="U154" t="inlineStr">
         <is>
-          <t>A line chart about the production of fresh vegetables in Canada in the year 2017. Values ​​are analyzed in the different months of the year.</t>
+          <t>A line chart about the production of fresh vegetables in Canada in the year 2017. Values   are analyzed in the different months of the year.</t>
         </is>
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About in TKN_Geo in the year TKN_Year. Values ​​are analyzed in the different months of the year.</t>
+          <t>A line chart about the TKN_About  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year.</t>
         </is>
       </c>
       <c r="W154" t="n">
@@ -13404,12 +13404,12 @@
       </c>
       <c r="U155" t="inlineStr">
         <is>
-          <t>A line chart about the price index of Desktop and similar computer in Canada in the year 2018. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 954 to 962.</t>
+          <t>A line chart about the price index of Desktop and similar computer in Canada in the year 2018. Values   are analyzed in the different months of the year. With index values   ranging from less than 954 to 962.</t>
         </is>
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About computer in TKN_Geo in the year TKN_Year. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 11 to 100.</t>
+          <t>A line chart about the TKN_About  computer in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 11 to 100.</t>
         </is>
       </c>
       <c r="W155" t="n">
@@ -13488,12 +13488,12 @@
       </c>
       <c r="U156" t="inlineStr">
         <is>
-          <t>A line chart about the Production of Malt in tonnes in Canada in the year 2016. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 45000 to more than 60000. The maximum value is reached in June.</t>
+          <t>A line chart about the Production of Malt in tonnes in Canada in the year 2016. Values   are analyzed in the different months of the year. With index values   ranging from less than 45000 to more than 60000. The maximum value is reached in June.</t>
         </is>
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About in TKN_UOM in TKN_Geo in the year TKN_Year. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 10 to more than 96. The maximum value is reached in June.</t>
+          <t>A line chart about the TKN_About  in TKN_UOM  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 10 to more than 96. The maximum value is reached in June.</t>
         </is>
       </c>
       <c r="W156" t="n">
@@ -13572,12 +13572,12 @@
       </c>
       <c r="U157" t="inlineStr">
         <is>
-          <t>A line chart about the Commercial software prince index in Canada in the year 2016. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 1180 to more than 1220. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
+          <t>A line chart about the Commercial software prince index in Canada in the year 2016. Values   are analyzed in the different months of the year. With index values   ranging from less than 1180 to more than 1220. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
         </is>
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About in TKN_Geo in the year TKN_Year. Values ​​are analyzed in the different months of the year. With index values ​​ranging from less than 12 to more than 105. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
+          <t>A line chart about the TKN_About  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 12 to more than 105. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
         </is>
       </c>
       <c r="W157" t="n">
@@ -13661,7 +13661,7 @@
       </c>
       <c r="V158" t="inlineStr">
         <is>
-          <t>A line chart about TKN_About per TKN_UOM in TKN_Geo in the year TKN_Year. The value grows until May and then decreases.</t>
+          <t>A line chart about TKN_About  per TKN_UOM  in  TKN_Geo  in the year  TKN_Year . The value grows until May and then decreases.</t>
         </is>
       </c>
       <c r="W158" t="n">
@@ -13745,7 +13745,7 @@
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About per TKN_UOM in TKN_Geo in the year TKN_Year. The minimum value is reached in September and the maximum in January.</t>
+          <t>A line chart about the TKN_About  per TKN_UOM  in  TKN_Geo  in the year  TKN_Year . The minimum value is reached in September and the maximum in January.</t>
         </is>
       </c>
       <c r="W159" t="n">
@@ -13829,7 +13829,7 @@
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>The chart represents the TKN_About (month vs. profit in dollars) in TKN_Year in TKN_Geo. The profit goes up rapidly in the first four months, then oscillates tending downward during May-September and finally plummets during September-December.</t>
+          <t>The chart represents the TKN_About  (month vs. profit in dollars) in  TKN_Year  in  TKN_Geo . The profit goes up rapidly in the first four months, then oscillates tending downward during May-September and finally plummets during September-December.</t>
         </is>
       </c>
       <c r="W160" t="n">
@@ -13913,7 +13913,7 @@
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About (month vs. tonnes) in TKN_Geo in TKN_Year. First the rapid growth is observed in January, followed by a sharp decline in February. The import then raises slightly in March, remaining constant from April to June. Falling slightly during June-August, it jumps high in August-November, with a small slip in December.</t>
+          <t>The graph shows the TKN_About  (month vs. tonnes) in  TKN_Geo  in  TKN_Year . First the rapid growth is observed in January, followed by a sharp decline in February. The import then raises slightly in March, remaining constant from April to June. Falling slightly during June-August, it jumps high in August-November, with a small slip in December.</t>
         </is>
       </c>
       <c r="W161" t="n">
@@ -13997,7 +13997,7 @@
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>Continuous increase of TKN_About TKN_UOM in TKN_Geo during the year TKN_Year.</t>
+          <t>Continuous increase of TKN_About  TKN_UOM  in  TKN_Geo  during the year  TKN_Year .</t>
         </is>
       </c>
       <c r="W162" t="n">
@@ -14081,7 +14081,7 @@
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>The TKN_About fluctuates in TKN_Geo during the year TKN_Year. From Januar until June it is remaining almost stable. From June until October it rises continuously and reaches the maximum value in october. In november and december it shows the smallest value.</t>
+          <t>The TKN_About  fluctuates in  TKN_Geo  during the year  TKN_Year . From Januar until June it is remaining almost stable. From June until October it rises continuously and reaches the maximum value in october. In november and december it shows the smallest value.</t>
         </is>
       </c>
       <c r="W163" t="n">
@@ -14165,7 +14165,7 @@
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>The graph shows the trend of TKN_About TKN_Geo during the year TKN_Year. The TKN_UOM drops between january and february and shows the minimum value in february. From february on it increases and shows the maximum value in august. Between august and december the TKN_UOM decreases continuously.</t>
+          <t>The graph shows the trend of the total TKN_UOM  of Canadian vehicles returning to  TKN_Geo  during the year  TKN_Year . The TKN_UOM  drops between january and february and shows the minimum value in february. From february on it increases and shows the maximum value in august. Between august and december the TKN_UOM  decreases continuously.</t>
         </is>
       </c>
       <c r="W164" t="n">
@@ -14249,7 +14249,7 @@
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>Graph that describes the TKN_About in TKN_Geo in TKN_Year. The production in October and February is the highest, while there is a significant drop the following two months of each. The production slightly rises in May but it then plunges until July, where the lowest value can be seen. After that month, there is a steady increase until October.</t>
+          <t>Graph that describes the TKN_About  in  TKN_Geo  in  TKN_Year . The production in October and February is the highest, while there is a significant drop the following two months of each. The production slightly rises in May but it then plunges until July, where the lowest value can be seen. After that month, there is a steady increase until October.</t>
         </is>
       </c>
       <c r="W165" t="n">
@@ -14333,7 +14333,7 @@
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>Total softwood production TKN_UOM meters in TKN_Geo in TKN_Year is shown in the graph. Production in January starts at roughly 88 m3, and it shrinks the next month. In March, this value goes back up and remains steady until May. It plunges until July to the same value as in February and then it oscilates between this value and the one in January until November to drop again to -2 m3 in December.</t>
+          <t>Total softwood production TKN_UOM  meters in  TKN_Geo  in  TKN_Year  is shown in the graph. Production in January starts at roughly 88 m3, and it shrinks the next month. In March, this value goes back up and remains steady until May. It plunges until July to the same value as in February and then it oscilates between this value and the one in January until November to drop again to -2 m3 in December.</t>
         </is>
       </c>
       <c r="W166" t="n">
@@ -14417,7 +14417,7 @@
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>The graph depicts the FPPI in TKN_Geo during TKN_Year. The highest was during August, where it was above 1220, whereas the lowest was in December, where it almost reached -4. From January to July, the values fluctuate between 15 and 1180, and after August, the values decrease until December.</t>
+          <t>The graph depicts the FPPI in  TKN_Geo  during  TKN_Year . The highest was during August, where it was above 89, whereas the lowest was in December, where it almost reached -4. From January to July, the values fluctuate between 15 and 52, and after August, the values decrease until December.</t>
         </is>
       </c>
       <c r="W167" t="n">
@@ -14501,7 +14501,7 @@
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>The graph shows a general downward trend of the TKN_About over the year TKN_Year in TKN_Geo. There was a slight price climb in the middle of the year. As this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
+          <t>The graph shows a general downward trend of the TKN_About  over the year  TKN_Year  in  TKN_Geo . There was a slight price climb in the middle of the year. As this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
         </is>
       </c>
       <c r="W168" t="n">
@@ -14585,7 +14585,7 @@
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>This graph shows the monthly amount TKN_About produced in TKN_Geo in TKN_Year in TKN_UOM. Oat production stayed within the range of 0 and 97 TKN_UOM each month. While most months averaged production at around 45 TKN_UOM, February, June and July saw dips in production to around 7 TKN_UOM and the fall months saw a higher harvest, -48 and above 90 TKN_UOM consecutively.</t>
+          <t>This graph shows the monthly amount TKN_About  produced in  TKN_Geo  in  TKN_Year  in TKN_UOM . Oat production stayed within the range of 0 and 97 TKN_UOM  each month. While most months averaged production at around 45 TKN_UOM , February, June and July saw dips in production to around 7 TKN_UOM  and the fall months saw a higher harvest, -48 and above 90 TKN_UOM  consecutively.</t>
         </is>
       </c>
       <c r="W169" t="n">
@@ -14669,7 +14669,7 @@
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>This graph shows a general upward trend in the price TKN_About in TKN_Geo in TKN_Year. While there were drops in the price index in April and August from their respective previous months, the graph obeyed an increasing trend.</t>
+          <t>This graph shows a general upward trend in the price TKN_About  in  TKN_Geo  in  TKN_Year . While there were drops in the price index in April and August from their respective previous months, the graph obeyed an increasing trend.</t>
         </is>
       </c>
       <c r="W170" t="n">
@@ -14753,7 +14753,7 @@
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>The given graph shows the average retail TKN_About in TKN_Geo in the year TKN_Year split into the different months. In january the price started out at 92 dollars, increased slightly and then plummeted to 25 dollars average in June. A short incline happend in July just for it falling back onto the June price in august. After a slight incline, the price fell to its lowest in december.</t>
+          <t>The given graph shows the average retail TKN_About  in  TKN_Geo  in the year  TKN_Year  split into the different months. In january the price started out at 92 dollars, increased slightly and then plummeted to 25 dollars average in June. A short incline happend in July just for it falling back onto the June price in august. After a slight incline, the price fell to its lowest in december.</t>
         </is>
       </c>
       <c r="W171" t="n">
@@ -14837,7 +14837,7 @@
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About fruits in TKN_Geo over the year of TKN_Year. In the first half of the year the production was nearly constant, until it fall dramatically in the mounth of August. Afterwards the fresh fruit production rises again over the index of 75.</t>
+          <t>The graph shows the TKN_About  fruits in  TKN_Geo  over the year of  TKN_Year . In the first half of the year the production was nearly constant, until it fall dramatically in the mounth of August. Afterwards the fresh fruit production rises again over the index of 75.</t>
         </is>
       </c>
       <c r="W172" t="n">
@@ -14921,7 +14921,7 @@
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>The graph showes the anual TKN_About in the year TKN_Year. The price in the first thre month is very high, especially in March. The following month ist drops and increase again in June and stays constant till July. Afterwards it decrease continusliy till December. Over the whole year there is a decreasing trend.</t>
+          <t>The graph showes the anual TKN_About  in the year  TKN_Year . The price in the first thre month is very high, especially in March. The following month ist drops and increase again in June and stays constant till July. Afterwards it decrease continusliy till December. Over the whole year there is a decreasing trend.</t>
         </is>
       </c>
       <c r="W173" t="n">
@@ -15005,7 +15005,7 @@
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>This graph shows the TKN_UOM of TKN_About in TKN_Year. The TKN_UOM of cars entering is about 11 at the start and end of the year. It increases towards summer. There is a peak in the middle of the year at 101 in July.</t>
+          <t>This graph shows the TKN_UOM  of TKN_About  in  TKN_Year . The TKN_UOM  of cars entering is about 11 at the start and end of the year. It increases towards summer. There is a peak in the middle of the year at 101 in July.</t>
         </is>
       </c>
       <c r="W174" t="n">
@@ -15084,12 +15084,12 @@
       </c>
       <c r="U175" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the yearly developement of wheat flower production in tonnes in 2018. The starting point in January is around 30.000 tons, with an increase to peak production  in April with over 43.000 tons and a following decline to just under 35.000 tons. After a slight increase the production plummited to just over 20.000 tons in September and fell to its lowest point of around 17.000 tons in December.</t>
+          <t>The accompanying graph shows the yearly developement of wheat flower production in tonnes in 2018. The starting point in January is around 30000 tons, with an increase to peak production  in April with over 43000 tons and a following decline to just under 35000 tons. After a slight increase the production plummited to just over 20000 tons in September and fell to its lowest point of around 17000 tons in December.</t>
         </is>
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the yearly developement TKN_About in TKN_UOM in TKN_Year. The starting point in January is around 30.000 tons, with an increase to peak production  in April with over 43.000 tons and a following decline to just under 35.000 tons. After a slight increase the production plummited to just over 20.000 tons in September and fell to its lowest point of around 17.000 tons in December.</t>
+          <t>The accompanying graph shows the yearly developement TKN_About  in TKN_UOM  in  TKN_Year . The starting point in January is around 50 tons, with an increase to peak production  in April with over 103 tons and a following decline to just under 71 tons. After a slight increase the production plummited to just over 9 tons in September and fell to its lowest point of around -3 tons in December.</t>
         </is>
       </c>
       <c r="W175" t="n">
@@ -15173,7 +15173,7 @@
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>The grapg shows the TKN_About in TKN_Geo in the year TKN_Year. It is noticeable that the price decreases almost continuously during the first third of the year. Afterwards, the price for the summer months remains constant, before falling massive in November.</t>
+          <t>The grapg shows the TKN_About  in  TKN_Geo  in the year  TKN_Year . It is noticeable that the price decreases almost continuously during the first third of the year. Afterwards, the price for the summer months remains constant, before falling massive in November.</t>
         </is>
       </c>
       <c r="W176" t="n">
@@ -15257,7 +15257,7 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About TKN_UOM development in TKN_Geo in TKN_Year. The starting point was just shy of 3 dollars in january but skyrocketed to over 79 dollars in May. A continouus, but a lot less steeper incline happend in between may and december, finishing at around 100 dollars in december.</t>
+          <t>The graph shows TKN_About  TKN_UOM  development in  TKN_Geo  in  TKN_Year . The starting point was just shy of 3 dollars in january but skyrocketed to over 79 dollars in May. A continouus, but a lot less steeper incline happend in between may and december, finishing at around 100 dollars in december.</t>
         </is>
       </c>
       <c r="W177" t="n">
@@ -15341,7 +15341,7 @@
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>The TKN_About from the year TKN_Year is showen by the graph. in Jannuary it starts increasing continously till March, decreas a little bit in April and increase again till it reach the annual maximum of  around 103 in June. The folowing monthes the index decrease rapidly till October and reaches the minimum value of about 0. in November and December it increases again.</t>
+          <t>The TKN_About  from the year  TKN_Year  is showen by the graph. in Jannuary it starts increasing continously till March, decreas a little bit in April and increase again till it reach the annual maximum of  around 103 in June. The folowing monthes the index decrease rapidly till October and reaches the minimum value of about 0. in November and December it increases again.</t>
         </is>
       </c>
       <c r="W178" t="n">
@@ -15425,7 +15425,7 @@
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>This is a TKN_About graph, showing the amount produced in TKN_UOM for the year TKN_Year. Production stayed within the range of 6 to about 99 TKN_UOM during the year. Production started just under 41 TKN_UOM in January and rose to above 77 TKN_UOM in March. It then dips to under 6 TKN_UOM in August, with acute increases in May and July, before experiencing a continuous rise to above 95 TKN_UOM in December.</t>
+          <t>This is a TKN_About  graph, showing the amount produced in TKN_UOM  for the year  TKN_Year . Production stayed within the range of 6 to about 99 TKN_UOM  during the year. Production started just under 41 TKN_UOM  in January and rose to above 77 TKN_UOM  in March. It then dips to under 6 TKN_UOM  in August, with acute increases in May and July, before experiencing a continuous rise to above 95 TKN_UOM  in December.</t>
         </is>
       </c>
       <c r="W179" t="n">
@@ -15504,12 +15504,12 @@
       </c>
       <c r="U180" t="inlineStr">
         <is>
-          <t>The graph shows the production of wheat flour (in tonnes) in Canada in the year 2018. Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 42.000 tonnes. This is followed by a more or less constant decline, until in December with 10.000 tonnes the minimum of production is reached.</t>
+          <t>The graph shows the production of wheat flour (in tonnes) in Canada in the year 2018. Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 42000 tonnes. This is followed by a more or less constant decline, until in December with 10000 tonnes the minimum of production is reached.</t>
         </is>
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About (in TKN_UOM) in TKN_Geo in the year TKN_Year. Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 42.000 TKN_UOM. This is followed by a more or less constant decline, until in December with 10.000 TKN_UOM the minimum of production is reached.</t>
+          <t>The graph shows the TKN_About  (in TKN_UOM ) in  TKN_Geo  in the year  TKN_Year . Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 99 TKN_UOM . This is followed by a more or less constant decline, until in December with -32 TKN_UOM  the minimum of production is reached.</t>
         </is>
       </c>
       <c r="W180" t="n">
@@ -15593,7 +15593,7 @@
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>The given graph shows TKN_About TKN_UOM development in TKN_Geo in the year TKN_Year, devided by month. The index started out at 100 january and then decreased to 0 in february and staying constant until may, giving way to a rise back to 100 between may and july, again staying at 100 dollars till the end of the year.</t>
+          <t>The given graph shows TKN_About  TKN_UOM  development in  TKN_Geo  in the year  TKN_Year , devided by month. The index started out at 100 january and then decreased to 0 in february and staying constant until may, giving way to a rise back to 100 between may and july, again staying at 100 dollars till the end of the year.</t>
         </is>
       </c>
       <c r="W181" t="n">
@@ -15677,7 +15677,7 @@
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>The graph showes the TKN_About in TKN_Year. It starts with the maximum value in January and falls massive till to the minimum in March. Afterwards it increases till June while dropping a little bit in May. In June it drops again and increase afterwards slowly till october. It fall again rapidly in November and stays constant in December.</t>
+          <t>The graph showes the TKN_About  in  TKN_Year . It starts with the maximum value in January and falls massive till to the minimum in March. Afterwards it increases till June while dropping a little bit in May. In June it drops again and increase afterwards slowly till october. It fall again rapidly in November and stays constant in December.</t>
         </is>
       </c>
       <c r="W182" t="n">
@@ -15756,12 +15756,12 @@
       </c>
       <c r="U183" t="inlineStr">
         <is>
-          <t>The graphs shows the total softwood and hardwood production in Canada in the year 2017. As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over 60.000 cubic meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
+          <t>The graphs shows the total softwood and hardwood production in Canada in the year 2017. As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over 60000 cubic meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
         </is>
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>The graphs shows the TKN_About in TKN_Geo in the year TKN_Year. As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over TKN_UOM meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
+          <t>The graphs shows the TKN_About  in  TKN_Geo  in the year  TKN_Year . As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over TKN_UOM  meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
         </is>
       </c>
       <c r="W183" t="n">
@@ -15845,7 +15845,7 @@
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>The graph showes TKN_About in TKN_UOM in the year TKN_Year. The highest production is in January with around 104 TKN_UOM. It decreases in February and stay nearly constant till April. Afterwards it drops constanously and rapidly till june. It increase agin in july till it drop again in August to the minimal TKN_About. Till the end of the year it increase beside a small drop in November.</t>
+          <t>The graph showes TKN_About  in TKN_UOM  in the year  TKN_Year . The highest production is in January with around 104 TKN_UOM . It decreases in February and stay nearly constant till April. Afterwards it drops constanously and rapidly till june. It increase agin in july till it drop again in August to the minimal TKN_About . Till the end of the year it increase beside a small drop in November.</t>
         </is>
       </c>
       <c r="W184" t="n">
@@ -15929,7 +15929,7 @@
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>This shows the TKN_About in TKN_Year. it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. There was also a dip in April. The price is an index that does not reflect absolute pricing.</t>
+          <t>This shows the TKN_About  in  TKN_Year . it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. There was also a dip in April. The price is an index that does not reflect absolute pricing.</t>
         </is>
       </c>
       <c r="W185" t="n">
@@ -16013,7 +16013,7 @@
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>The aforementioned graph shows the TKN_About in FPPI units divided by months of the year TKN_Year. Starting point is at 93 in January and after some slight ups and downs it increased to around 104 in May only to plummet over the next few months to its lowest point around 1 in September just to increase to 44 in December again.</t>
+          <t>The aforementioned graph shows the TKN_About  in FPPI units divided by months of the year  TKN_Year . Starting point is at 93 in January and after some slight ups and downs it increased to around 104 in May only to plummet over the next few months to its lowest point around 1 in September just to increase to 44 in December again.</t>
         </is>
       </c>
       <c r="W186" t="n">
@@ -16097,7 +16097,7 @@
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About TKN_UOM in canada in the year of TKN_Year. It is striking that the value only changes twice a year. It falls from January to February, and from May to July it rises back to the original amount of 100. For the rest of the year, the value remains constant.</t>
+          <t>The graph shows TKN_About  TKN_UOM  in canada in the year of  TKN_Year . It is striking that the value only changes twice a year. It falls from January to February, and from May to July it rises back to the original amount of 100. For the rest of the year, the value remains constant.</t>
         </is>
       </c>
       <c r="W187" t="n">
@@ -16181,7 +16181,7 @@
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>The accompanying shows the monthly development of TKN_About production in the year TKN_Year in TKN_Geo, measured in FPPI. It starts out at 90 in January, increases slightly to just shy of 102 in March, falls to 80 in April and increases again to 95 in June. After that it constantly decreases until reaching its lowest point of -3 in October. It continues to rise afterwards.</t>
+          <t>The accompanying shows the monthly development of TKN_About  production in the year  TKN_Year  in  TKN_Geo , measured in FPPI. It starts out at 90 in January, increases slightly to just shy of 102 in March, falls to 80 in April and increases again to 95 in June. After that it constantly decreases until reaching its lowest point of -3 in October. It continues to rise afterwards.</t>
         </is>
       </c>
       <c r="W188" t="n">
@@ -16260,12 +16260,12 @@
       </c>
       <c r="U189" t="inlineStr">
         <is>
-          <t>The grapg shows the production of rye in canada in the year of 2016. While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 25.000 tonnes is reached. A lot of work for the farmers in this season of the year I guess.</t>
+          <t>The grapg shows the production of rye in canada in the year of 2016. While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 25000 tonnes is reached. A lot of work for the farmers in this season of the year I guess.</t>
         </is>
       </c>
       <c r="V189" t="inlineStr">
         <is>
-          <t>The grapg shows the TKN_About in canada in the year of TKN_Year. While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 25.000 TKN_UOM is reached. A lot of work for the farmers in this season of the year I guess.</t>
+          <t>The grapg shows the TKN_About  in canada in the year of  TKN_Year . While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 102 TKN_UOM  is reached. A lot of work for the farmers in this season of the year I guess.</t>
         </is>
       </c>
       <c r="W189" t="n">
@@ -16349,7 +16349,7 @@
       </c>
       <c r="V190" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About in TKN_Geo in in TKN_Year. The first few monthes till May the production fluctuate at around 93. In june it starts to decrease a little bit and in july and august there is a massive drop. In September the graph keeps going decreasing and reach the annual minimum. The last monthes of the year the graph is increasing again.</t>
+          <t>The graph illustrates the TKN_About  in  TKN_Geo  in in  TKN_Year . The first few monthes till May the production fluctuate at around 93. In june it starts to decrease a little bit and in july and august there is a massive drop. In September the graph keeps going decreasing and reach the annual minimum. The last monthes of the year the graph is increasing again.</t>
         </is>
       </c>
       <c r="W190" t="n">
@@ -16433,7 +16433,7 @@
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>The TKN_About of wood in TKN_Year. It stayed at within above 61 and about TKN_UOM meters except for two dips in July with 34 cubic meters and December with below 7 cubic meters.</t>
+          <t>The TKN_About  of wood in  TKN_Year . It stayed at within above 61 and about TKN_UOM  meters except for two dips in July with 34 cubic meters and December with below 7 cubic meters.</t>
         </is>
       </c>
       <c r="W191" t="n">
@@ -16517,7 +16517,7 @@
       </c>
       <c r="V192" t="inlineStr">
         <is>
-          <t>The given graph shows the monthly development of the TKN_About TKN_UOM in TKN_Year in TKN_Geo. After starting out at 88 in January it immediately starts falling to 25 in May, rising again to 48 in June and then falling to 0 in August. After staying pretty flat until October it starts skyrocketing to its highest point of 100 in December.</t>
+          <t>The given graph shows the monthly development of the TKN_About  TKN_UOM  in  TKN_Year  in  TKN_Geo . After starting out at 88 in January it immediately starts falling to 25 in May, rising again to 48 in June and then falling to 0 in August. After staying pretty flat until October it starts skyrocketing to its highest point of 100 in December.</t>
         </is>
       </c>
       <c r="W192" t="n">
@@ -16601,7 +16601,7 @@
       </c>
       <c r="V193" t="inlineStr">
         <is>
-          <t>Graph elucidates the TKN_About in the year TKN_Year. Production experienced a general increase over the year, with a sharp spike in August and dips in the months of February, July and November.</t>
+          <t>Graph elucidates the TKN_About  in the year  TKN_Year . Production experienced a general increase over the year, with a sharp spike in August and dips in the months of February, July and November.</t>
         </is>
       </c>
       <c r="W193" t="n">
@@ -16685,7 +16685,7 @@
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>The graph illustrates the productioin TKN_About in TKN_UOM in TKN_Year. The first few montes till May the graph stays quite constant at a low level of about 2 TKN_UOM, besides a small peak in March up to nearly 27 TKN_UOM. The graph starts to increase continusly from May to July. Afterwards it increase rapidly till the maxumum value in September. The next few monthes till the end of the year ithe graph decreases.</t>
+          <t>The graph illustrates the productioin TKN_About  in TKN_UOM  in  TKN_Year . The first few montes till May the graph stays quite constant at a low level of about 2 TKN_UOM , besides a small peak in March up to nearly 27 TKN_UOM . The graph starts to increase continusly from May to July. Afterwards it increase rapidly till the maxumum value in September. The next few monthes till the end of the year ithe graph decreases.</t>
         </is>
       </c>
       <c r="W194" t="n">
@@ -16769,7 +16769,7 @@
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>The graph highlights the TKN_About over the course of a year. It follow a "U" shape with a local increase in the month of June.</t>
+          <t>The graph highlights the TKN_About  over the course of a year. It follow a "U" shape with a local increase in the month of June.</t>
         </is>
       </c>
       <c r="W195" t="n">
@@ -16853,7 +16853,7 @@
       </c>
       <c r="V196" t="inlineStr">
         <is>
-          <t>The provided graph depicts the development of the TKN_About in TKN_Geo in TKN_Year, divided by month. After a slow decline from 100 in January to 92 in February it crashes, reaching a low point of 30 in March. Afterwards it rises to 71 in April and then slowly but constantly declines to -2 in December.</t>
+          <t>The provided graph depicts the development of the TKN_About  in  TKN_Geo  in  TKN_Year , divided by month. After a slow decline from 100 in January to 92 in February it crashes, reaching a low point of 30 in March. Afterwards it rises to 71 in April and then slowly but constantly declines to -2 in December.</t>
         </is>
       </c>
       <c r="W196" t="n">
@@ -16937,7 +16937,7 @@
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About TKN_UOM increasing over the year. It stayed the same for the mon of May and September but was increasing continuously throughout the year otherwise.</t>
+          <t>The graph shows TKN_About  TKN_UOM  increasing over the year. It stayed the same for the mon of May and September but was increasing continuously throughout the year otherwise.</t>
         </is>
       </c>
       <c r="W197" t="n">
@@ -17021,7 +17021,7 @@
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>The graph showes the TKN_About in TKN_Year. The graph decreases in February. From february till August it starts to increase continously and reaches the maximum of over 94. From August till December the graph decrease continuslie till a total TKN_UOM of 28 in December.</t>
+          <t>The graph showes the TKN_About  in  TKN_Year . The graph decreases in February. From february till August it starts to increase continously and reaches the maximum of over 94. From August till December the graph decrease continuslie till a total TKN_UOM  of 28 in December.</t>
         </is>
       </c>
       <c r="W198" t="n">
@@ -17105,7 +17105,7 @@
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>The provided graph depicts the changes in the TKN_About in TKN_Geo in TKN_Year. The first value sits at 34 in January, giving way to a slight increase to 56 that is followed by a decline back to 35 in April. A short rise follows in may but its crashing to -1 in July. The following months show a steep increase till October, followed by a slow and steady rise till December.</t>
+          <t>The provided graph depicts the changes in the TKN_About  in  TKN_Geo  in  TKN_Year . The first value sits at 34 in January, giving way to a slight increase to 56 that is followed by a decline back to 35 in April. A short rise follows in may but its crashing to -1 in July. The following months show a steep increase till October, followed by a slow and steady rise till December.</t>
         </is>
       </c>
       <c r="W199" t="n">
@@ -17184,12 +17184,12 @@
       </c>
       <c r="U200" t="inlineStr">
         <is>
-          <t>The graph illustrates the production of rye in canada in the year 2017. The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 20.000 tonnes. Then the production decrease again for the remaining months of the year.</t>
+          <t>The graph illustrates the production of rye in canada in the year 2017. The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 20000 tonnes. Then the production decrease again for the remaining months of the year.</t>
         </is>
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About in canada in the year TKN_Year. The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 20.000 tonnes. Then the production decrease again for the remaining months of the year.</t>
+          <t>The graph illustrates the TKN_About  in canada in the year  TKN_Year . The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 100 tonnes. Then the production decrease again for the remaining months of the year.</t>
         </is>
       </c>
       <c r="W200" t="n">
@@ -17273,7 +17273,7 @@
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>It describes the TKN_About computer in TKN_Geo during TKN_Year. It's clearly possible to see how the values are strongly fluctuating over the year. The maximum values have been recorded during the may of February and May. The minimum value was in August TKN_Year.</t>
+          <t>It describes the TKN_About  computer in  TKN_Geo  during  TKN_Year . It's clearly possible to see how the values are strongly fluctuating over the year. The maximum values have been recorded during the may of February and May. The minimum value was in August  TKN_Year .</t>
         </is>
       </c>
       <c r="W201" t="n">
@@ -17357,7 +17357,7 @@
       </c>
       <c r="V202" t="inlineStr">
         <is>
-          <t>The graph shoes the overall TKN_About computer prices throughout the year. The months of March, June, September and December experienced more sharp drops than the others. The price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
+          <t>The graph shoes the overall TKN_About  computer prices throughout the year. The months of March, June, September and December experienced more sharp drops than the others. The price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
         </is>
       </c>
       <c r="W202" t="n">
@@ -17441,7 +17441,7 @@
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About in TKN_UOM in TKN_Geo in TKN_Year. The lowest production is in Jannuary. From February till July the graph oscillate. in August it drops and rise again in September. It stay constant in October before it decrease in November again. In december it jump to the highest production of around 101.</t>
+          <t>The graph shows the TKN_About  in TKN_UOM  in  TKN_Geo  in  TKN_Year . The lowest production is in Jannuary. From February till July the graph oscillate. in August it drops and rise again in September. It stay constant in October before it decrease in November again. In december it jump to the highest production of around 101.</t>
         </is>
       </c>
       <c r="W203" t="n">
@@ -17520,12 +17520,12 @@
       </c>
       <c r="U204" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the fluctuation in oat production in tons in Canada in the year 2016 divided by months. Between January and July it fluctuates heavily followed by a rise to over 200.000 tons in September. The next few months show a continuous decline to the end point at 140.000 tons in December.</t>
+          <t>The accompanying graph shows the fluctuation in oat production in tons in Canada in the year 2016 divided by months. Between January and July it fluctuates heavily followed by a rise to over 200000 tons in September. The next few months show a continuous decline to the end point at 140000 tons in December.</t>
         </is>
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the fluctuation in TKN_About in tons in TKN_Geo in the year TKN_Year divided by months. Between January and July it fluctuates heavily followed by a rise to over 200.000 tons in September. The next few months show a continuous decline to the end point at 140.000 tons in December.</t>
+          <t>The accompanying graph shows the fluctuation in TKN_About  in tons in  TKN_Geo  in the year  TKN_Year  divided by months. Between January and July it fluctuates heavily followed by a rise to over 94 tons in September. The next few months show a continuous decline to the end point at 48 tons in December.</t>
         </is>
       </c>
       <c r="W204" t="n">
@@ -17609,7 +17609,7 @@
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>It shows the data about TKN_About in TKN_Geo during TKN_Year. The displayed values are in tones. It's possible to see how the value rapidly increase from January over, reaching its peaks during the month of July with approximately 101 tonnes. After that, the values decrease until September and then rise up again during last -262 months of the year.</t>
+          <t>It shows the data about TKN_About  in  TKN_Geo  during  TKN_Year . The displayed values are in tones. It's possible to see how the value rapidly increase from January over, reaching its peaks during the month of July with approximately 101 tonnes. After that, the values decrease until September and then rise up again during last 3 months of the year.</t>
         </is>
       </c>
       <c r="W205" t="n">
@@ -17688,12 +17688,12 @@
       </c>
       <c r="U206" t="inlineStr">
         <is>
-          <t>The graph indicates the house price index in canada in the year 2016. As shown the index increases during the hole year until he reaches the maximum of 1.000 in December. Unfortunately, you can not say more about this graph.</t>
+          <t>The graph indicates the house price index in canada in the year 2016. As shown the index increases during the hole year until he reaches the maximum of 1000 in December. Unfortunately, you can not say more about this graph.</t>
         </is>
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>The graph indicates TKN_About TKN_UOM in canada in the year TKN_Year. As shown the index increases during the hole year until he reaches the maximum of 1.000 in December. Unfortunately, you can not say more about this graph.</t>
+          <t>The graph indicates TKN_About  TKN_UOM  in canada in the year  TKN_Year . As shown the index increases during the hole year until he reaches the maximum of 100 in December. Unfortunately, you can not say more about this graph.</t>
         </is>
       </c>
       <c r="W206" t="n">
@@ -17777,7 +17777,7 @@
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About computer in the year TKN_Year in TKN_Geo. The price index fluctuates hugely the first four monthes and reach the maximum in May. It falls in June and July and drop massivly in August. it rise again in September and October and stays constant in Novermber. In December it drop again.</t>
+          <t>The graph shows the TKN_About  computer in the year  TKN_Year  in  TKN_Geo . The price index fluctuates hugely the first four monthes and reach the maximum in May. It falls in June and July and drop massivly in August. it rise again in September and October and stays constant in Novermber. In December it drop again.</t>
         </is>
       </c>
       <c r="W207" t="n">
@@ -17856,12 +17856,12 @@
       </c>
       <c r="U208" t="inlineStr">
         <is>
-          <t>The provided graph displays the number of Canadian vehicles returning to Canada over the year 2016 divided by month. It starts out at around 150.000 vehicles in January, falls to 135.000 in February and rises continuously to over 220.000 in August. The following month show a steady decrease to its second lowest point of just under 160.000 in December.</t>
+          <t>The provided graph displays the number of Canadian vehicles returning to Canada over the year 2016 divided by month. It starts out at around 1500000 vehicles in January, falls to 1350000 in February and rises continuously to over 2200000 in August. The following month show a steady decrease to its second lowest point of just under 1600000 in December.</t>
         </is>
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>The provided graph displays TKN_About TKN_Geo over the year TKN_Year divided by month. It starts out at around 150.000 vehicles in January, falls to 135.000 in February and rises continuously to over 220.000 in August. The following month show a steady decrease to its second lowest point of just under 160.000 in December.</t>
+          <t>The provided graph displays the TKN_UOM  of Canadian vehicles returning to  TKN_Geo  over the year  TKN_Year  divided by month. It starts out at around 18 vehicles in January, falls to 1 in February and rises continuously to over 97 in August. The following month show a steady decrease to its second lowest point of just under 29 in December.</t>
         </is>
       </c>
       <c r="W208" t="n">
@@ -17945,7 +17945,7 @@
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About in TKN_Year. The graph follows an uphill climb from January until August, except for dips in the months of Feburary and June. After August, the graph has a falling trend to the end of the year.</t>
+          <t>The graph shows the TKN_UOM  of Canadian vehicles returning in  TKN_Year . The graph follows an uphill climb from January until August, except for dips in the months of Feburary and June. After August, the graph has a falling trend to the end of the year.</t>
         </is>
       </c>
       <c r="W209" t="n">
@@ -18029,7 +18029,7 @@
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>The line chart is displaying the recorded data about TKN_About in TKN_Geo during TKN_Year. The minimum value of production have been recorded during the months of January, August and November. From January to February has been recorded a significant growth. The maximum value of production over the year was recorded during December.</t>
+          <t>The line chart is displaying the recorded data about TKN_About  in  TKN_Geo  during  TKN_Year . The minimum value of production have been recorded during the months of January, August and November. From January to February has been recorded a significant growth. The maximum value of production over the year was recorded during December.</t>
         </is>
       </c>
       <c r="W210" t="n">
@@ -18113,7 +18113,7 @@
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>The graph indicates the TKN_About in canada in the year of TKN_Year. As the graph rises from January to February, it drops sharply until July, before reaching a minimum of 4. Subsequently, the value rises continuously until the end of the year, reaching a maximum of 96 in December.</t>
+          <t>The graph indicates the TKN_About  in canada in the year of  TKN_Year . As the graph rises from January to February, it drops sharply until July, before reaching a minimum of 4. Subsequently, the value rises continuously until the end of the year, reaching a maximum of 96 in December.</t>
         </is>
       </c>
       <c r="W211" t="n">
@@ -18197,7 +18197,7 @@
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>The displayed chart shows the TKN_About TKN_Geo during TKN_Year. It's possible to see how the highest values have been recorded during the spring and summer months. In particular, the maximum TKN_UOM of cars entering TKN_Geo has been reached July and a August. The months with minimum values have been January and February.</t>
+          <t>The displayed chart shows the total TKN_UOM  of vehicles entering  TKN_Geo  during  TKN_Year . It's possible to see how the highest values have been recorded during the spring and summer months. In particular, the maximum TKN_UOM  of cars entering  TKN_Geo  has been reached July and a August. The months with minimum values have been January and February.</t>
         </is>
       </c>
       <c r="W212" t="n">
@@ -18281,7 +18281,7 @@
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About over the year of TKN_Year. The graph stayed in the range of about 2 and 94 tonnes. It has a zig-zag waveform from January to August, before a last peak in September and then decreasing in the last quarter of the year.</t>
+          <t>The graph shows the TKN_About  over the year of  TKN_Year . The graph stayed in the range of about 2 and 94 tonnes. It has a zig-zag waveform from January to August, before a last peak in September and then decreasing in the last quarter of the year.</t>
         </is>
       </c>
       <c r="W213" t="n">
@@ -18360,12 +18360,12 @@
       </c>
       <c r="U214" t="inlineStr">
         <is>
-          <t>The given graph shows the malt production in tons in Canada in 2017. The Graph continuously rises from 52.000 tons in January to 60.000 in May, falls back to 53.000 in June and rises to 63.000 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 40.000 tons.</t>
+          <t>The given graph shows the malt production in tons in Canada in 2017. The Graph continuously rises from 52000 tons in January to 60000 in May, falls back to 53000 in June and rises to 63000 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 40000 tons.</t>
         </is>
       </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>The given graph shows the TKN_About in tons in TKN_Geo in TKN_Year. The Graph continuously rises from 52.000 tons in January to 60.000 in May, falls back to 53.000 in June and rises to 63.000 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 40.000 tons.</t>
+          <t>The given graph shows the TKN_About  in tons in  TKN_Geo  in  TKN_Year . The Graph continuously rises from 56 tons in January to 91 in May, falls back to 60 in June and rises to 104 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 4 tons.</t>
         </is>
       </c>
       <c r="W214" t="n">
@@ -18449,7 +18449,7 @@
       </c>
       <c r="V215" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About in TKN_Geo in TKN_Year. The first five monthes of the year it oscillates at around 4. the next two months the production increase. It drop a little bit in August and rise again in September to the annual maximum of 105. in October, November and December there is a slightly and continously decrease.</t>
+          <t>The graph shows the TKN_About  in  TKN_Geo  in  TKN_Year . The first five monthes of the year it oscillates at around 4. the next two months the production increase. It drop a little bit in August and rise again in September to the annual maximum of 105. in October, November and December there is a slightly and continously decrease.</t>
         </is>
       </c>
       <c r="W215" t="n">
@@ -18528,12 +18528,12 @@
       </c>
       <c r="U216" t="inlineStr">
         <is>
-          <t>The graph indicates the entering vehicles from the united states in canada in the year of 2018. It is noticeable that the number is rising sharply by the middle of the year, reaching a maximum of 1.200.000 in August. Then the value is strong again until the end of the year.</t>
+          <t>The graph indicates the entering vehicles from the united states in canada in the year of 2018. It is noticeable that the number is rising sharply by the middle of the year, reaching a maximum of 1200000 in August. Then the value is strong again until the end of the year.</t>
         </is>
       </c>
       <c r="V216" t="inlineStr">
         <is>
-          <t>The graph indicates the TKN_About in canada in the year of TKN_Year. It is noticeable that the TKN_UOM is rising sharply by the middle of the year, reaching a maximum of 1.200.000 in August. Then the value is strong again until the end of the year.</t>
+          <t>The graph indicates the TKN_About  in canada in the year of  TKN_Year . It is noticeable that the TKN_UOM  is rising sharply by the middle of the year, reaching a maximum of 101 in August. Then the value is strong again until the end of the year.</t>
         </is>
       </c>
       <c r="W216" t="n">
@@ -18617,7 +18617,7 @@
       </c>
       <c r="V217" t="inlineStr">
         <is>
-          <t>The grain TKN_About the year TKN_Year saw a zig-zag pattern from January to May before increasing in July and remained relatively stable for the rest of the year at the increased price.</t>
+          <t>The grain TKN_About  the year  TKN_Year  saw a zig-zag pattern from January to May before increasing in July and remained relatively stable for the rest of the year at the increased price.</t>
         </is>
       </c>
       <c r="W217" t="n">
@@ -18701,7 +18701,7 @@
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>The graph is showing the production's trend TKN_About hardwood in TKN_Geo during TKN_Year. The values are TKN_UOM metres. It's clearly possible to see how the values are strongly fluctuating over the year. There are several peaks, in particular during March, May and Novembe. At the same time, the minimum values have been recorded during the months of January, July and August.</t>
+          <t>The graph is showing the production's trend TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The values are TKN_UOM  metres. It's clearly possible to see how the values are strongly fluctuating over the year. There are several peaks, in particular during March, May and Novembe. At the same time, the minimum values have been recorded during the months of January, July and August.</t>
         </is>
       </c>
       <c r="W218" t="n">
@@ -18785,7 +18785,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>The following graph is showing the recorded values about TKN_About in TKN_Geo during TKN_Year. The values have been reported using TKN_UOM (FPPI). As it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of August. After the summer, the production value drop, reaching its minimum value in October.</t>
+          <t>The following graph is showing the recorded values about TKN_About  in  TKN_Geo  during  TKN_Year . The values have been reported using TKN_UOM  (FPPI). As it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of August. After the summer, the production value drop, reaching its minimum value in October.</t>
         </is>
       </c>
       <c r="W219" t="n">
@@ -18869,7 +18869,7 @@
       </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>It illustrates the TKN_About hardwood in TKN_Geo during TKN_Year using TKN_UOM as unit of measurement. From January to April has been recorded a slightly increase. The value significantly dropped from May to July, and then it remain steady for the last months of the year. The minimum value has been recorded during the month of December.</t>
+          <t>It illustrates the TKN_About  hardwood in  TKN_Geo  during  TKN_Year  using TKN_UOM  as unit of measurement. From January to April has been recorded a slightly increase. The value significantly dropped from May to July, and then it remain steady for the last months of the year. The minimum value has been recorded during the month of December.</t>
         </is>
       </c>
       <c r="W220" t="n">
@@ -18953,7 +18953,7 @@
       </c>
       <c r="V221" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year has been increasing over the year. Even that, several fluctuations have been recorded, in particular during the first months of the year. The maximum values have been recorded during November and December. During the first months of the year, from January to May, have been recorded the minimum production values.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  has been increasing over the year. Even that, several fluctuations have been recorded, in particular during the first months of the year. The maximum values have been recorded during November and December. During the first months of the year, from January to May, have been recorded the minimum production values.</t>
         </is>
       </c>
       <c r="W221" t="n">
@@ -19037,7 +19037,7 @@
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>A graph showing TKN_UOM over TKN_About the year TKN_Year in TKN_Geo. It shows a significant price drop in July followed by a steady increase of the FPPPI until October.</t>
+          <t>A graph showing TKN_UOM  over TKN_About  the year  TKN_Year  in  TKN_Geo . It shows a significant price drop in July followed by a steady increase of the FPPPI until October.</t>
         </is>
       </c>
       <c r="W222" t="n">
@@ -19121,7 +19121,7 @@
       </c>
       <c r="V223" t="inlineStr">
         <is>
-          <t>A graph showing the Canadian TKN_About in TKN_UOM over the course of the year TKN_Year. The production was highest in August and then steadily decreased.</t>
+          <t>A graph showing the Canadian TKN_About  in TKN_UOM  over the course of the year  TKN_Year . The production was highest in August and then steadily decreased.</t>
         </is>
       </c>
       <c r="W223" t="n">
@@ -19205,7 +19205,7 @@
       </c>
       <c r="V224" t="inlineStr">
         <is>
-          <t>A graph showing the TKN_About poultry in TKN_Geo over the course of the year TKN_Year. The FPPI has risen steadily until August and then dropped slowly.</t>
+          <t>A graph showing the TKN_About  poultry in  TKN_Geo  over the course of the year  TKN_Year . The FPPI has risen steadily until August and then dropped slowly.</t>
         </is>
       </c>
       <c r="W224" t="n">
@@ -19289,7 +19289,7 @@
       </c>
       <c r="V225" t="inlineStr">
         <is>
-          <t>the TKN_About TKN_Geo in TKN_Year were about 1 in Jan and Feb. then, they increased linearly until Aug, reaching 94. The they decreased considerably to 2400000, almost back to where they started from.</t>
+          <t>the TKN_About   TKN_Geo  in  TKN_Year  were about 1 in Jan and Feb. then, they increased linearly until Aug, reaching 94. The they decreased considerably to 28, almost back to where they started from.</t>
         </is>
       </c>
       <c r="W225" t="n">
@@ -19373,7 +19373,7 @@
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo increased constantly in TKN_Year (from 11 to 96 FPPI), with the exception of the October-December period when it decreased to 74.</t>
+          <t>The TKN_About  in  TKN_Geo  increased constantly in  TKN_Year  (from 11 to 96 FPPI), with the exception of the October-December period when it decreased to 74.</t>
         </is>
       </c>
       <c r="W226" t="n">
@@ -19452,12 +19452,12 @@
       </c>
       <c r="U227" t="inlineStr">
         <is>
-          <t>Production of creamery decreased sharply in Canada in the period January-June from 11500 to about 8000. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching 1000 by the end of the year.</t>
+          <t>Production of creamery decreased sharply in Canada in the period January-June from 11500 to about 8000. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching 10000 by the end of the year.</t>
         </is>
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>Production of creamery decreased sharply in TKN_Geo in the period January-June from 105 to about 12. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching -175 by the end of the year.</t>
+          <t>Production of creamery decreased sharply in  TKN_Geo  in the period January-June from 105 to about 12. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching 65 by the end of the year.</t>
         </is>
       </c>
       <c r="W227" t="n">
@@ -19536,12 +19536,12 @@
       </c>
       <c r="U228" t="inlineStr">
         <is>
-          <t>The supply of creamery in Canada in 2017 grew rapidly from Jan (2400 tons) to May (38000). Then it was stable until July, when it started to drop, reaching 34000 by the end of the year.</t>
+          <t>The supply of creamery in Canada in 2017 grew rapidly from Jan (24000 tons) to May (38000). Then it was stable until July, when it started to drop, reaching 34000 by the end of the year.</t>
         </is>
       </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo in TKN_Year grew rapidly from Jan (2400 tons) to May (38000). Then it was stable until July, when it started to drop, reaching 66 by the end of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  grew rapidly from Jan (-1 tons) to May (92). Then it was stable until July, when it started to drop, reaching 66 by the end of the year.</t>
         </is>
       </c>
       <c r="W228" t="n">
@@ -19625,7 +19625,7 @@
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>The TKN_About vehicle in TKN_Geo in TKN_Year climbed from 7 to 100 from Jan to May. Then it dropped until Jul, was stable until Sep. with a final further decline to 16 at the end of the year.</t>
+          <t>The TKN_About  vehicle in  TKN_Geo  in  TKN_Year  climbed from 7 to 100 from Jan to May. Then it dropped until Jul, was stable until Sep. with a final further decline to 16 at the end of the year.</t>
         </is>
       </c>
       <c r="W229" t="n">
@@ -19709,7 +19709,7 @@
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo in TKN_Year rose sharply until May, from 2 to 100 units. Then it started decreasing, reaching the same January level of 2 in December, at the end of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  rose sharply until May, from 2 to 100 units. Then it started decreasing, reaching the same January level of 2 in December, at the end of the year.</t>
         </is>
       </c>
       <c r="W230" t="n">
@@ -19793,7 +19793,7 @@
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>Production of fresh vegetables for TKN_Year in whole TKN_Geo, represented TKN_UOM index. It can be seen, that the production rises in the months from february until october and then drops.</t>
+          <t>Production of fresh vegetables for  TKN_Year  in whole  TKN_Geo , represented TKN_UOM  index. It can be seen, that the production rises in the months from february until october and then drops.</t>
         </is>
       </c>
       <c r="W231" t="n">
@@ -19877,7 +19877,7 @@
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>TKN_Year: TKN_About in TKN_Geo, with a peak in may and the lowest production in february.</t>
+          <t>TKN_Year : TKN_About  in  TKN_Geo , with a peak in may and the lowest production in february.</t>
         </is>
       </c>
       <c r="W232" t="n">
@@ -19961,7 +19961,7 @@
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>This is a line graph showing the total TKN_Year imports TKN_About to TKN_Geo in TKN_UOM. The graph has significant fluctuations between each month. There is a substantial spike in June, which was the peak month at over 97 tonnes. There is also a clear dip in September, which was the lowest month at under 4 tonnes.</t>
+          <t>This is a line graph showing the total  TKN_Year  imports TKN_About  to  TKN_Geo  in  TKN_UOM . The graph has significant fluctuations between each month. There is a substantial spike in June, which was the peak month at over 97 tonnes. There is also a clear dip in September, which was the lowest month at under 4 tonnes.</t>
         </is>
       </c>
       <c r="W233" t="n">
@@ -20045,7 +20045,7 @@
       </c>
       <c r="V234" t="inlineStr">
         <is>
-          <t>This is a line graph showing TKN_About index of laptops in TKN_Geo. There is a declining trend throughout the year, with a slight spike in October. The graph's peak is in February at 994, and the graph's trough is in December at 0.</t>
+          <t>This is a line graph showing the  TKN_Year  price index of laptops in  TKN_Geo . There is a declining trend throughout the year, with a slight spike in October. The graph's peak is in February at 100, and the graph's trough is in December at 0.</t>
         </is>
       </c>
       <c r="W234" t="n">
@@ -20129,7 +20129,7 @@
       </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>This is a line graph showing the TKN_About TKN_UOM in TKN_Geo. There is a stable increase from the graph's bottom at under 3 in January, and peaking at over 94 in December.</t>
+          <t>This is a line graph showing the  TKN_Year  house TKN_UOM  in  TKN_Geo . There is a stable increase from the graph's bottom at under 3 in January, and peaking at over 94 in December.</t>
         </is>
       </c>
       <c r="W235" t="n">
@@ -20213,7 +20213,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>The maximum value of TKN_About during TKN_Year has been reached during the month of August. In particular, the value started to grow in March reaching its peak in August. After that, it slowly decreased. The minimum value was during February TKN_Year.</t>
+          <t>The maximum value of TKN_About  during  TKN_Year  has been reached during the month of August. In particular, the value started to grow in March reaching its peak in August. After that, it slowly decreased. The minimum value was during February  TKN_Year .</t>
         </is>
       </c>
       <c r="W236" t="n">
@@ -20297,7 +20297,7 @@
       </c>
       <c r="V237" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About in TKN_Geo during TKN_Year rapidly increased from January over. In particular, it reached its peak during the month of June TKN_Year. After that, it started to decline until September. The last three months of the year it remained quite stable.</t>
+          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  during  TKN_Year  rapidly increased from January over. In particular, it reached its peak during the month of June  TKN_Year . After that, it started to decline until September. The last three months of the year it remained quite stable.</t>
         </is>
       </c>
       <c r="W237" t="n">
@@ -20381,7 +20381,7 @@
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year showed several fluctuations during the year. The production values have been displayed using TKN_UOM as unit of measurement. The most relevant peaks have been recorded during the months of February and June. At the same time, the minimum values were recorded in January and September TKN_Year.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  showed several fluctuations during the year. The production values have been displayed using  TKN_UOM  as unit of measurement. The most relevant peaks have been recorded during the months of February and June. At the same time, the minimum values were recorded in January and September  TKN_Year .</t>
         </is>
       </c>
       <c r="W238" t="n">
@@ -20465,7 +20465,7 @@
       </c>
       <c r="V239" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo decreased over TKN_Year. It's clearly possible to see how it rapidly drop from January to April. After that, the price index values have been fluctuating for most of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  decreased over  TKN_Year . It's clearly possible to see how it rapidly drop from January to April. After that, the price index values have been fluctuating for most of the year.</t>
         </is>
       </c>
       <c r="W239" t="n">
@@ -20549,7 +20549,7 @@
       </c>
       <c r="V240" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year reached its maximum values during the months of July, August and September. In particular, the maximum value over the year has been registered during the month of August. It's clearly possible to see how the TKN_About is way higher during the summer months than during the winter one.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  reached its maximum values during the months of July, August and September. In particular, the maximum value over the year has been registered during the month of August. It's clearly possible to see how the TKN_About  is way higher during the summer months than during the winter one.</t>
         </is>
       </c>
       <c r="W240" t="n">
@@ -20633,7 +20633,7 @@
       </c>
       <c r="V241" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year reported several fluctations. Even that, it shows a significant peak during the month of August. The minimum value has been registered during the month of February.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  reported several fluctations. Even that, it shows a significant peak during the month of August. The minimum value has been registered during the month of February.</t>
         </is>
       </c>
       <c r="W241" t="n">
@@ -20717,7 +20717,7 @@
       </c>
       <c r="V242" t="inlineStr">
         <is>
-          <t>The line chart describes the TKN_About index trend in TKN_Geo during TKN_Year. It considerably oscillated over the year, with several peaks and dips. The highest values have been recorded during January and June. The minimum value was recorded in November TKN_Year.</t>
+          <t>The line chart describes the TKN_About  index trend in  TKN_Geo  during  TKN_Year . It considerably oscillated over the year, with several peaks and dips. The highest values have been recorded during January and June. The minimum value was recorded in November  TKN_Year .</t>
         </is>
       </c>
       <c r="W242" t="n">
@@ -20801,7 +20801,7 @@
       </c>
       <c r="V243" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo TKN_Year shows the highest values during the summer months. In particular, the production reports its maximum value during the month of August. It remain quite steady during the other months of the year. The minimum value was during October TKN_Year.</t>
+          <t>The TKN_About  in  TKN_Geo   TKN_Year  shows the highest values during the summer months. In particular, the production reports its maximum value during the month of August. It remain quite steady during the other months of the year. The minimum value was during October  TKN_Year .</t>
         </is>
       </c>
       <c r="W243" t="n">
@@ -20885,7 +20885,7 @@
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo slipped down during the TKN_Year. The highest value has been recorded during March. Then, it significantly dropped between May and September. The minimu value was recorded during the month of September. During last -1635 months of the year it slightly started to increase again.</t>
+          <t>The TKN_About  in  TKN_Geo  slipped down during the  TKN_Year . The highest value has been recorded during March. Then, it significantly dropped between May and September. The minimu value was recorded during the month of September. During last 3 months of the year it slightly started to increase again.</t>
         </is>
       </c>
       <c r="W244" t="n">
@@ -20969,7 +20969,7 @@
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>The graph is showing the trend about TKN_About in TKN_Geo during TKN_Year. The values are illustrated using TKN_UOM (FPPI). The values have been fluactuating over the year, with several dips and peaks. The maximum value was in October TKN_Year. During the last two months of the year, Nov and Dec, was recorded the minimum production of the TKN_Year.</t>
+          <t>The graph is showing the trend about TKN_About  in  TKN_Geo  during  TKN_Year . The values are illustrated using TKN_UOM  (FPPI). The values have been fluactuating over the year, with several dips and peaks. The maximum value was in October  TKN_Year . During the last two months of the year, Nov and Dec, was recorded the minimum production of the  TKN_Year .</t>
         </is>
       </c>
       <c r="W245" t="n">
@@ -21053,7 +21053,7 @@
       </c>
       <c r="V246" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the TKN_About in TKN_Geo during TKN_Year rapidly increased fom January to April. After that, it slowly slide down from April until the end of the year. The maximum number of new motor vehicles in TKN_Geo during TKN_Year was in April.</t>
+          <t>As it's shown in the graph, the TKN_About  in  TKN_Geo  during  TKN_Year  rapidly increased fom January to April. After that, it slowly slide down from April until the end of the year. The maximum number of new motor vehicles in  TKN_Geo  during  TKN_Year  was in April.</t>
         </is>
       </c>
       <c r="W246" t="n">
@@ -21137,7 +21137,7 @@
       </c>
       <c r="V247" t="inlineStr">
         <is>
-          <t>It shows the TKN_About in TKN_Geo during TKN_Year. The values are described using TKN_UOM as UOM. It rapidly increase from January for the first half of the year. It reach its maximum value during the month of June. After that, it starts to decline til September. The TKN_About fluctuated over the last few months of TKN_Year.</t>
+          <t>It shows the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using  TKN_UOM  as UOM. It rapidly increase from January for the first half of the year. It reach its maximum value during the month of June. After that, it starts to decline til September. The TKN_About  fluctuated over the last few months of  TKN_Year .</t>
         </is>
       </c>
       <c r="W247" t="n">
@@ -21221,7 +21221,7 @@
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>As it's possible to see, the following graph is about the TKN_About in TKN_Geo during TKN_Year. The values are reported using TKN_UOM (FPPI). The production slightly increase over the first half of the year, so from January until July. After that, it has been recorded a significant jump of the values between July and August. During the last few months of the year it remained steady.</t>
+          <t>As it's possible to see, the following graph is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported using TKN_UOM  (FPPI). The production slightly increase over the first half of the year, so from January until July. After that, it has been recorded a significant jump of the values between July and August. During the last few months of the year it remained steady.</t>
         </is>
       </c>
       <c r="W248" t="n">
@@ -21305,7 +21305,7 @@
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>Production of rye in TKN_Geo during TKN_Year got a considerable peak during August. During most of the year the values have been fluctuating up and down, with several peaks and dips. Even that, the minimum value over TKN_Year has been recorded in December.</t>
+          <t>Production of rye in  TKN_Geo  during  TKN_Year  got a considerable peak during August. During most of the year the values have been fluctuating up and down, with several peaks and dips. Even that, the minimum value over  TKN_Year  has been recorded in December.</t>
         </is>
       </c>
       <c r="W249" t="n">
@@ -21389,7 +21389,7 @@
       </c>
       <c r="V250" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in TKN_Geo during TKN_Year showed a massive climb from February to March. The production value kept raising up. it reached its maximum value during the month of May. After that, the production of new motor vehicles slightly started to decline, reaching a dip during the month of December TKN_Year.</t>
+          <t>Production of new motor vehicles in  TKN_Geo  during  TKN_Year  showed a massive climb from February to March. The production value kept raising up. it reached its maximum value during the month of May. After that, the production of new motor vehicles slightly started to decline, reaching a dip during the month of December  TKN_Year .</t>
         </is>
       </c>
       <c r="W250" t="n">
@@ -21473,7 +21473,7 @@
       </c>
       <c r="V251" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo strongly oscillated over TKN_Year. It's clearly possible to see how it reported several peaks and dips. The highest value was during October TKN_Year. The minimum value was in August TKN_Year.</t>
+          <t>The TKN_About  in  TKN_Geo  strongly oscillated over  TKN_Year . It's clearly possible to see how it reported several peaks and dips. The highest value was during October  TKN_Year . The minimum value was in August  TKN_Year .</t>
         </is>
       </c>
       <c r="W251" t="n">
@@ -21557,7 +21557,7 @@
       </c>
       <c r="V252" t="inlineStr">
         <is>
-          <t>The following graph shows the TKN_About value in TKN_Geo during TKN_Year, and the values are described using the TKN_UOM as UOM. It's possible to see how the production value considerably increased from January until July. After that, it dropped between July and September.</t>
+          <t>The following graph shows the TKN_About  value in  TKN_Geo  during  TKN_Year , and the values are described using the TKN_UOM  as UOM. It's possible to see how the production value considerably increased from January until July. After that, it dropped between July and September.</t>
         </is>
       </c>
       <c r="W252" t="n">
@@ -21641,7 +21641,7 @@
       </c>
       <c r="V253" t="inlineStr">
         <is>
-          <t>The TKN_About strongly fluctuated over the TKN_Year in TKN_Geo. It doesn't really have an ascendant or descendant trend. The most significant dip has been recorded in May. The most considerable peak was recorded in September TKN_Year.</t>
+          <t>The TKN_About  strongly fluctuated over the  TKN_Year  in  TKN_Geo . It doesn't really have an ascendant or descendant trend. The most significant dip has been recorded in May. The most considerable peak was recorded in September  TKN_Year .</t>
         </is>
       </c>
       <c r="W253" t="n">
@@ -21725,7 +21725,7 @@
       </c>
       <c r="V254" t="inlineStr">
         <is>
-          <t>The TKN_UOM TKN_About TKN_Geo during TKN_Year substantially increased over the summer months. In particular, the maximum value was reached during August. The minimum TKN_UOM of vehicles enterin TKN_Geo was during February.</t>
+          <t>The TKN_UOM  TKN_About   TKN_Geo  during  TKN_Year  substantially increased over the summer months. In particular, the maximum value was reached during August. The minimum TKN_UOM  of vehicles enterin  TKN_Geo  was during February.</t>
         </is>
       </c>
       <c r="W254" t="n">
@@ -21809,7 +21809,7 @@
       </c>
       <c r="V255" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year considerably oscillated up and down over the year.  The maximum value was recorded in May TKN_Year. But at the same time, two other peaks were in May and October. The minimum value over the whole TKN_Year was during December TKN_Year, with less than 9 TKN_UOM producted.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  considerably oscillated up and down over the year.  The maximum value was recorded in May  TKN_Year . But at the same time, two other peaks were in May and October. The minimum value over the whole  TKN_Year  was during December  TKN_Year , with less than 9 TKN_UOM  producted.</t>
         </is>
       </c>
       <c r="W255" t="n">
@@ -21893,7 +21893,7 @@
       </c>
       <c r="V256" t="inlineStr">
         <is>
-          <t>The graph shows the trend about TKN_About index in TKN_Geo over TKN_Year. After a significantly steep rise from January to February, the values started to slightly decline. They have been decreasing from February til September. A significant drop was registered between July and August. The minimum value over the year was in September TKN_Year. During last few months of the year the price index started to slightly grow again.</t>
+          <t>The graph shows the trend about TKN_About  index in  TKN_Geo  over  TKN_Year . After a significantly steep rise from January to February, the values started to slightly decline. They have been decreasing from February til September. A significant drop was registered between July and August. The minimum value over the year was in September  TKN_Year . During last few months of the year the price index started to slightly grow again.</t>
         </is>
       </c>
       <c r="W256" t="n">
@@ -21977,7 +21977,7 @@
       </c>
       <c r="V257" t="inlineStr">
         <is>
-          <t>Production of creamery butter in TKN_Geo has been rapidly decreasing over from January until August TKN_Year. Even that, couple of peaks have been recorded during that period, in particular April and July. During the last few months of year, the production started to considerably grow again. The minimum value over the year was registered in August TKN_Year.</t>
+          <t>Production of creamery butter in  TKN_Geo  has been rapidly decreasing over from January until August  TKN_Year . Even that, couple of peaks have been recorded during that period, in particular April and July. During the last few months of year, the production started to considerably grow again. The minimum value over the year was registered in August  TKN_Year .</t>
         </is>
       </c>
       <c r="W257" t="n">
@@ -22061,7 +22061,7 @@
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About index of serves in TKN_Geo during TKN_Year. At the beginning of the year, between January and March, the index considerably dropped down. After that, it has been oscillating over the rest of the year. A peak was recorded in June. The values strongly declined also between October and November.</t>
+          <t>The graph shows TKN_About  index of serves in  TKN_Geo  during  TKN_Year . At the beginning of the year, between January and March, the index considerably dropped down. After that, it has been oscillating over the rest of the year. A peak was recorded in June. The values strongly declined also between October and November.</t>
         </is>
       </c>
       <c r="W258" t="n">
@@ -22145,7 +22145,7 @@
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>As it's possible to see in the shown graph, the TKN_About reported the highest values during the first half of the year. In particular, the maximum value was recorded during June TKN_Year. After that, it rapidly decreased from June until September. The minimum value was during September TKN_Year.</t>
+          <t>As it's possible to see in the shown graph, the TKN_About  reported the highest values during the first half of the year. In particular, the maximum value was recorded during June  TKN_Year . After that, it rapidly decreased from June until September. The minimum value was during September  TKN_Year .</t>
         </is>
       </c>
       <c r="W259" t="n">
@@ -22229,7 +22229,7 @@
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo has been strongly fluctuating over TKN_Year. It's clearly possible to identify several peaks and dips. The maximum value was during May. Even that, the production value strongly dropped down from October to December, reaching its minimum value of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  has been strongly fluctuating over  TKN_Year . It's clearly possible to identify several peaks and dips. The maximum value was during May. Even that, the production value strongly dropped down from October to December, reaching its minimum value of the year.</t>
         </is>
       </c>
       <c r="W260" t="n">
@@ -22313,7 +22313,7 @@
       </c>
       <c r="V261" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo has been quite steady during the first few months of the TKN_Year. After that, it rapidly declined from June until October. During last three months of the year it started to slightly increase again. The highest value of the year was recorded in March and the lowest in October.</t>
+          <t>The TKN_About  in  TKN_Geo  has been quite steady during the first few months of the  TKN_Year . After that, it rapidly declined from June until October. During last three months of the year it started to slightly increase again. The highest value of the year was recorded in March and the lowest in October.</t>
         </is>
       </c>
       <c r="W261" t="n">
@@ -22397,7 +22397,7 @@
       </c>
       <c r="V262" t="inlineStr">
         <is>
-          <t>This figure depicts the TKN_About in TKN_UOM of TKN_Year. Whereas it starts off in January at approximately 63 TKN_UOM, production fluctuates until reaching its maximum in May at around 104. There is a sudden drop, reaching the minimum annual value in July at below 11 TKN_UOM. Production then again rises from July until October and experiences a drop from October until December.</t>
+          <t>This figure depicts the TKN_About  in TKN_UOM  of  TKN_Year . Whereas it starts off in January at approximately 63 TKN_UOM , production fluctuates until reaching its maximum in May at around 104. There is a sudden drop, reaching the minimum annual value in July at below 11 TKN_UOM . Production then again rises from July until October and experiences a drop from October until December.</t>
         </is>
       </c>
       <c r="W262" t="n">
@@ -22476,12 +22476,12 @@
       </c>
       <c r="U263" t="inlineStr">
         <is>
-          <t>The production of new motor vehicles in Canada of 2018 is shown in this figure. The unit given is dollars. Production shows its lowest value in January at 0.5. Following this production experiences a sharp increase, until reaching its maximum of approximately 0.93 in May. Production gradually decreases from May until July, plateauing from July until September around 0.75. There is a steady decline from September until December, reaching a value of around 0.54.</t>
+          <t>The production of new motor vehicles in Canada of 2018 is shown in this figure. The unit given is dollars. Production shows its lowest value in January. Following this production experiences a sharp increase, until reaching its maximum in May. Production gradually decreases from May until July, plateauing from July until September. There is a steady decline from September until December.</t>
         </is>
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo of TKN_Year is shown in this figure. The unit given is dollars. Production shows its lowest value in January at 0.5. Following this production experiences a sharp increase, until reaching its maximum of approximately 0.93 in May. Production gradually decreases from May until July, plateauing from July until September around 0.75. There is a steady decline from September until December, reaching a value of around 0.54.</t>
+          <t>The TKN_About  in  TKN_Geo  of  TKN_Year  is shown in this figure. The unit given is dollars. Production shows its lowest value in January. Following this production experiences a sharp increase, until reaching its maximum in May. Production gradually decreases from May until July, plateauing from July until September. There is a steady decline from September until December.</t>
         </is>
       </c>
       <c r="W263" t="n">
@@ -22565,7 +22565,7 @@
       </c>
       <c r="V264" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About during TKN_Year. Maximum production is reached in the months of January and February at 100. From then on production oscillates in a decreasing manner, plateauing at 67 during April and May and at 33 during June and July. The minimum production is observed during August and October. There is a rise from October until December, reaching a value of 44.</t>
+          <t>This figure represents the Canadian TKN_About  during  TKN_Year . Maximum production is reached in the months of January and February at 100. From then on production oscillates in a decreasing manner, plateauing at 67 during April and May and at 33 during June and July. The minimum production is observed during August and October. There is a rise from October until December, reaching a value of 44.</t>
         </is>
       </c>
       <c r="W264" t="n">
@@ -22649,7 +22649,7 @@
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>The TKN_UOM of TKN_About TKN_Geo in TKN_Year is depicted in this graph. During January approximately 8 vehicles enter. These TKN_UOMs slightly decrease to 1 in February, the lowest value of the year. From then on a steady increase in entering vehicles can be observed, until the maximum value is reached in August at approxiamtely 100. From August until December the TKN_UOM of vehicles entering TKN_Geo experience a steady decrease, reaching a TKN_UOM of 22 at the end of the year.</t>
+          <t>The TKN_UOM  of TKN_About   TKN_Geo  in  TKN_Year  is depicted in this graph. During January approximately 8 vehicles enter. These TKN_UOM s slightly decrease to 1 in February, the lowest value of the year. From then on a steady increase in entering vehicles can be observed, until the maximum value is reached in August at approxiamtely 100. From August until December the TKN_UOM  of vehicles entering  TKN_Geo  experience a steady decrease, reaching a TKN_UOM  of 22 at the end of the year.</t>
         </is>
       </c>
       <c r="W265" t="n">
@@ -22733,7 +22733,7 @@
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>This graph depicts the total TKN_UOM of TKN_About in TKN_Geo during TKN_Year. The lowest TKN_UOM of vehicles is observed in January, at approximately 1. During the following months TKN_UOMs of entering vehicles steadily increase until reaching the maximum TKN_UOM the year TKN_Year in July with approximately 101. From July until November a sharp drop is experienced, with TKN_UOMs of around 11 in November. The TKN_UOM hardly changes in December.</t>
+          <t>This graph depicts the total TKN_UOM  of TKN_About  in  TKN_Geo  during  TKN_Year . The lowest TKN_UOM  of vehicles is observed in January, at approximately 1. During the following months TKN_UOM s of entering vehicles steadily increase until reaching the maximum TKN_UOM  the year  TKN_Year  in July with approximately 101. From July until November a sharp drop is experienced, with TKN_UOM s of around 11 in November. The TKN_UOM  hardly changes in December.</t>
         </is>
       </c>
       <c r="W266" t="n">
@@ -22817,7 +22817,7 @@
       </c>
       <c r="V267" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_UOM in TKN_Year. The unit given is TKN_UOM. Production starts at around 85 in January and drops to approximately 59 in February. It then fluctuates around 98 between the months of March and May, until it drops back to same production numbers of February during July. Production of softwood fluctuates between July until October, reaching around 85. Afterwards a sharp decline can be observed until December, which marks the lowest production numbers for this year at around -2.</t>
+          <t>This graph depicts the TKN_About  in TKN_UOM  in  TKN_Year . The unit given is TKN_UOM . Production starts at around 85 in January and drops to approximately 59 in February. It then fluctuates around 98 between the months of March and May, until it drops back to same production numbers of February during July. Production of softwood fluctuates between July until October, reaching around 85. Afterwards a sharp decline can be observed until December, which marks the lowest production numbers for this year at around -2.</t>
         </is>
       </c>
       <c r="W267" t="n">
@@ -22901,7 +22901,7 @@
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>This figure shows the Canadian TKN_About of TKN_Year. Production is measured in tonnes. Production is the lowest during the month of January at approximately 0. There is a sharp increase for February, reaching 59 tonnes, after which a drop is experienced during March. The maximum TKN_About is taking place in April at above 100 tonnes. Production is rather low during May. During the following months production fluctuates until a sharp increase in observed for October, reaching nearly 95 tonnes. Production remains nearly steady throughout November and drops back to 50 during December.</t>
+          <t>This figure shows the Canadian TKN_About  of  TKN_Year . Production is measured in tonnes. Production is the lowest during the month of January at approximately 0. There is a sharp increase for February, reaching 59 tonnes, after which a drop is experienced during March. The maximum TKN_About  is taking place in April at above 100 tonnes. Production is rather low during May. During the following months production fluctuates until a sharp increase in observed for October, reaching nearly 95 tonnes. Production remains nearly steady throughout November and drops back to 50 during December.</t>
         </is>
       </c>
       <c r="W268" t="n">
@@ -22985,7 +22985,7 @@
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About of TKN_Year. The unit used TKN_UOM metres. Production during January lies at approximately 61 and experiences an increase until reaching the maximum value in March at above 99. From then production slowly declines until June, after which a sharp drop can be observed in July at approximately 34. From July until November production levels increase again, reaching a value of nearly 98. There is a rapid decline of production in December, which marks the lowest production of the year at -2 cubic metres.</t>
+          <t>This graph depicts the TKN_About  of  TKN_Year . The unit used TKN_UOM  metres. Production during January lies at approximately 61 and experiences an increase until reaching the maximum value in March at above 99. From then production slowly declines until June, after which a sharp drop can be observed in July at approximately 34. From July until November production levels increase again, reaching a value of nearly 98. There is a rapid decline of production in December, which marks the lowest production of the year at -2 cubic metres.</t>
         </is>
       </c>
       <c r="W269" t="n">
@@ -23069,7 +23069,7 @@
       </c>
       <c r="V270" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo has been substantially growing over TKN_Year. In particular, during the first few months of the year the values have been slightly decreasing. But then from June over it rapidly increased, reaching it peaks on November TKN_Year. The minimum production value during TKN_Year has been reported during June.</t>
+          <t>The TKN_About  in  TKN_Geo  has been substantially growing over  TKN_Year . In particular, during the first few months of the year the values have been slightly decreasing. But then from June over it rapidly increased, reaching it peaks on November  TKN_Year . The minimum production value during  TKN_Year  has been reported during June.</t>
         </is>
       </c>
       <c r="W270" t="n">
@@ -23153,7 +23153,7 @@
       </c>
       <c r="V271" t="inlineStr">
         <is>
-          <t>The house TKN_UOM in TKN_Geo during TKN_Year presents a quite ambiguous trend. Firstly, during the first few months, it slowly decrease. But then, from May to July, it recorded a considerable growth. During the last few months of the year the house TKN_UOM mainted the same level.</t>
+          <t>The house TKN_UOM  in  TKN_Geo  during  TKN_Year  presents a quite ambiguous trend. Firstly, during the first few months, it slowly decrease. But then, from May to July, it recorded a considerable growth. During the last few months of the year the house TKN_UOM  mainted the same level.</t>
         </is>
       </c>
       <c r="W271" t="n">
@@ -23237,7 +23237,7 @@
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About in TKN_Geo has been significantly decreasing over TKN_Year. Few fluctuations of the value have been recorded, but without any significant peaks or dips. The highest value was in January. The minimum value was in December TKN_Year.</t>
+          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  has been significantly decreasing over  TKN_Year . Few fluctuations of the value have been recorded, but without any significant peaks or dips. The highest value was in January. The minimum value was in December  TKN_Year .</t>
         </is>
       </c>
       <c r="W272" t="n">
@@ -23321,7 +23321,7 @@
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>The graph shows how TKN_About TKN_UOM in TKN_Geo rapidly increased during TKN_Year. In particular, it started in January around -12 and ended up in December with more than 94. The most significant increase was recorded between March and May.</t>
+          <t>The graph shows how TKN_About  TKN_UOM  in  TKN_Geo  rapidly increased during  TKN_Year . In particular, it started in January around -12 and ended up in December with more than 94. The most significant increase was recorded between March and May.</t>
         </is>
       </c>
       <c r="W273" t="n">
@@ -23405,7 +23405,7 @@
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>Total Canadian livestock and animal products in TKN_Year are shown in this graph. The unit given is TKN_UOM (FPPI). During January products lie at 63 and the second highes value of the year can be observed in February at approximately 76. There is a sharp decline from February onwards, reaching a low of 1 in April. During the following months there is a steep rise, reaching the maximum of 99 in July. Again, a huge decrease follows until reaching the lowest value in September, which is followed by a significant rise for October. Following this, a rapid drop can be observed until December.</t>
+          <t>Total Canadian livestock and animal products in  TKN_Year  are shown in this graph. The unit given is TKN_UOM  (FPPI). During January products lie at 63 and the second highes value of the year can be observed in February at approximately 76. There is a sharp decline from February onwards, reaching a low of 1 in April. During the following months there is a steep rise, reaching the maximum of 99 in July. Again, a huge decrease follows until reaching the lowest value in September, which is followed by a significant rise for October. Following this, a rapid drop can be observed until December.</t>
         </is>
       </c>
       <c r="W274" t="n">
@@ -23489,7 +23489,7 @@
       </c>
       <c r="V275" t="inlineStr">
         <is>
-          <t>It's possible to see how the TKN_About in TKN_Geo presented several fluctuations over the year. In particular during the first few months different peaks and dips have been recorded. Then the import value rapidly increased from August to November. It reached its maximum value during the month of November. The minimum value was in January TKN_Year.</t>
+          <t>It's possible to see how the TKN_About  in  TKN_Geo  presented several fluctuations over the year. In particular during the first few months different peaks and dips have been recorded. Then the import value rapidly increased from August to November. It reached its maximum value during the month of November. The minimum value was in January  TKN_Year .</t>
         </is>
       </c>
       <c r="W275" t="n">
@@ -23573,7 +23573,7 @@
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>The values about TKN_About in TKN_Geo during TKN_Year show a quite interesting trend. The production remained stable for most of the year. But two big peaks of production have been recorded, one in March and one in August. Even that, the most significant peak was definetely in August TKN_Year. The month with less production was December.</t>
+          <t>The values about TKN_About  in  TKN_Geo  during  TKN_Year  show a quite interesting trend. The production remained stable for most of the year. But two big peaks of production have been recorded, one in March and one in August. Even that, the most significant peak was definetely in August  TKN_Year . The month with less production was December.</t>
         </is>
       </c>
       <c r="W276" t="n">
@@ -23657,7 +23657,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_Geo during TKN_Year. The given unit is TKN_UOM (FPPI). The graph represents a parable throughout the year. It starts at 34 during January, after which a steady decline can be observed, reaching the lowest production value in June at 0. During the following months production rapidly increases until the maximum is reached in November at approximately 100. There is a small decrease in December.</t>
+          <t>This graph depicts the TKN_About  in  TKN_Geo  during  TKN_Year . The given unit is TKN_UOM  (FPPI). The graph represents a parable throughout the year. It starts at 34 during January, after which a steady decline can be observed, reaching the lowest production value in June at 0. During the following months production rapidly increases until the maximum is reached in November at approximately 100. There is a small decrease in December.</t>
         </is>
       </c>
       <c r="W277" t="n">
@@ -23741,7 +23741,7 @@
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>This graph illustrates values about the TKN_About in TKN_Geo during TKN_Year. Those values are described using TKN_UOM (FPPI). It's clearly possible to see how the maximum values of production are registered during the summer months. In particular, the highest production value was during July TKN_Year. At the same time, the lowest one was in December.</t>
+          <t>This graph illustrates values about the TKN_About  in  TKN_Geo  during  TKN_Year . Those values are described using TKN_UOM  (FPPI). It's clearly possible to see how the maximum values of production are registered during the summer months. In particular, the highest production value was during July  TKN_Year . At the same time, the lowest one was in December.</t>
         </is>
       </c>
       <c r="W278" t="n">
@@ -23820,12 +23820,12 @@
       </c>
       <c r="U279" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian production of rye during 2017. The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 6000 to 8000 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 15000 tonnes. The highest production can be observed during October with nearly 20000. Rye production experiences a sharp drop in November, reaching around 75000 tonnes. There is a minimal increase during December.</t>
+          <t>This figure represents the Canadian production of rye during 2017. The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 6000 to 8000 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 15000 tonnes. The highest production can be observed during October with nearly 20000. Rye production experiences a sharp drop in November, reaching around 7500 tonnes. There is a minimal increase during December.</t>
         </is>
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About during TKN_Year. The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 3 to 17 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 65 tonnes. The highest production can be observed during October with nearly 100. Rye production experiences a sharp drop in November, reaching around 481 tonnes. There is a minimal increase during December.</t>
+          <t>This figure represents the Canadian TKN_About  during  TKN_Year . The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 3 to 17 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 65 tonnes. The highest production can be observed during October with nearly 100. Rye production experiences a sharp drop in November, reaching around 13 tonnes. There is a minimal increase during December.</t>
         </is>
       </c>
       <c r="W279" t="n">
@@ -23909,7 +23909,7 @@
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo clearly showed an ascendant trend during TKN_Year. The values have been oscillating up and down several times over the year, even if the trend kept growing up. The production reached its maximum value during the month of December, and its minimum values during the first months of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  clearly showed an ascendant trend during  TKN_Year . The values have been oscillating up and down several times over the year, even if the trend kept growing up. The production reached its maximum value during the month of December, and its minimum values during the first months of the year.</t>
         </is>
       </c>
       <c r="W280" t="n">
@@ -23993,7 +23993,7 @@
       </c>
       <c r="V281" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from this graph how the TKN_About in TKN_Geo had a big drop from June to August TKN_Year. During the first few months, from January to June, the value remained quite stable. But then it dramatically dropped down. Even that, during the last few months of the year the production of value slightly started to grow up again.</t>
+          <t>It's clearly possible to see from this graph how the TKN_About  in  TKN_Geo  had a big drop from June to August  TKN_Year . During the first few months, from January to June, the value remained quite stable. But then it dramatically dropped down. Even that, during the last few months of the year the production of value slightly started to grow up again.</t>
         </is>
       </c>
       <c r="W281" t="n">
@@ -24077,7 +24077,7 @@
       </c>
       <c r="V282" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About in TKN_Geo during TKN_Year. The unit TKN_UOM (FPPI). Production starts off at approximately 11 in January and goes down to the lowest production at 0 during February. During the months of March and May the production remains unchanged at 33. There is a slight increase of production during June, until it remain stable throughout July until September at 56. Then, a small drop can be observed, which is followed by a sharp increase, until it peaks during December at 100.</t>
+          <t>This graph depicts the TKN_About  in  TKN_Geo  during  TKN_Year . The unit TKN_UOM  (FPPI). Production starts off at approximately 11 in January and goes down to the lowest production at 0 during February. During the months of March and May the production remains unchanged at 33. There is a slight increase of production during June, until it remain stable throughout July until September at 56. Then, a small drop can be observed, which is followed by a sharp increase, until it peaks during December at 100.</t>
         </is>
       </c>
       <c r="W282" t="n">
@@ -24161,7 +24161,7 @@
       </c>
       <c r="V283" t="inlineStr">
         <is>
-          <t>The land TKN_UOM in TKN_Geo during TKN_Year has been showing a slight but constant ascendant trend. In particular, from January to April the index value remained exactly the same. But then, after that, it started to grow up with few fluctuations in between. The maximum values were reached during the months of November and December TKN_Year.</t>
+          <t>The land TKN_UOM  in  TKN_Geo  during  TKN_Year  has been showing a slight but constant ascendant trend. In particular, from January to April the index value remained exactly the same. But then, after that, it started to grow up with few fluctuations in between. The maximum values were reached during the months of November and December  TKN_Year .</t>
         </is>
       </c>
       <c r="W283" t="n">
@@ -24245,7 +24245,7 @@
       </c>
       <c r="V284" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from the graph that the TKN_About in TKN_Geo during TKN_Year reached its maximum values during the summer months. In particular, the most significant peak of the values was registered during August TKN_Year. Despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
+          <t>It's clearly possible to see from the graph that the TKN_About  in  TKN_Geo  during  TKN_Year  reached its maximum values during the summer months. In particular, the most significant peak of the values was registered during August  TKN_Year . Despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
         </is>
       </c>
       <c r="W284" t="n">
@@ -24329,7 +24329,7 @@
       </c>
       <c r="V285" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian TKN_About in TKN_Year. The given unit are tonnes. Production starts off at approximately 70 during January, after which a sharp decline is observed during February, reaching below 10. Production fluctuates between March and June, after which a rapid decline takes place again, reaching the lowest production values of the year in August at -1. Staying mostly constant in September, there is a significant rise peaking in October above 97. Production of Canola declines again during November, and hardly changes for December at around 42.</t>
+          <t>This graph represents the Canadian TKN_About  in  TKN_Year . The given unit are tonnes. Production starts off at approximately 70 during January, after which a sharp decline is observed during February, reaching below 10. Production fluctuates between March and June, after which a rapid decline takes place again, reaching the lowest production values of the year in August at -1. Staying mostly constant in September, there is a significant rise peaking in October above 97. Production of Canola declines again during November, and hardly changes for December at around 42.</t>
         </is>
       </c>
       <c r="W285" t="n">
@@ -24413,7 +24413,7 @@
       </c>
       <c r="V286" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About in TKN_Year. The price index starts off at 81 during January, and keeps decreasing throughout the following months, until it reaches its minimum value of below 6 in April. From then on there is a sharp increase, peaking in July at above 94. During the following months a moderate decrease is experienced until October. The price index remains unchanged during November and December at 69.</t>
+          <t>This figure represents the Canadian TKN_About  in  TKN_Year . The price index starts off at 81 during January, and keeps decreasing throughout the following months, until it reaches its minimum value of below 6 in April. From then on there is a sharp increase, peaking in July at above 94. During the following months a moderate decrease is experienced until October. The price index remains unchanged during November and December at 69.</t>
         </is>
       </c>
       <c r="W286" t="n">
@@ -24497,7 +24497,7 @@
       </c>
       <c r="V287" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo considerably increased over TKN_Year. The minimum value was in January around 3. The maximum value was in December around 100. All over the year there were reported several fluctuations of the index value.</t>
+          <t>The TKN_About  in  TKN_Geo  considerably increased over  TKN_Year . The minimum value was in January around 3. The maximum value was in December around 100. All over the year there were reported several fluctuations of the index value.</t>
         </is>
       </c>
       <c r="W287" t="n">
@@ -24581,7 +24581,7 @@
       </c>
       <c r="V288" t="inlineStr">
         <is>
-          <t>It shows the TKN_About in TKN_Geo during TKN_Year. It's possible to see how it considerably declined over the year.  Over the year the values ahs been oscillating several times, in particular during the summer months. Even that, the maximum value was recorded in January and the minimum one in November TKN_Year.</t>
+          <t>It shows the TKN_About  in  TKN_Geo  during  TKN_Year . It's possible to see how it considerably declined over the year.  Over the year the values ahs been oscillating several times, in particular during the summer months. Even that, the maximum value was recorded in January and the minimum one in November  TKN_Year .</t>
         </is>
       </c>
       <c r="W288" t="n">
@@ -24665,7 +24665,7 @@
       </c>
       <c r="V289" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo reported some strong oscillations of the value during TKN_Year. As it's possible to see from the graph, several peaks and dips have been registered. The most significant peaks were during March and July. The most considerable dips during September and December. Furthermore, a marked drop of the production value was registered between July and August TKN_Year.</t>
+          <t>The TKN_About  in  TKN_Geo  reported some strong oscillations of the value during  TKN_Year . As it's possible to see from the graph, several peaks and dips have been registered. The most significant peaks were during March and July. The most considerable dips during September and December. Furthermore, a marked drop of the production value was registered between July and August  TKN_Year .</t>
         </is>
       </c>
       <c r="W289" t="n">
@@ -24744,12 +24744,12 @@
       </c>
       <c r="U290" t="inlineStr">
         <is>
-          <t>This figure represents the land price index in Canada in 2018. Overall the price index increases throughout the year. During January a value of 1037.0 can be observed, after which it rises up to 1038.5 during February. It falls back to 1037.0 during March and April. During the following 2 months there is a steady increase, after which the land price index remains unchanged at 1039.0 throughout June until August. Also, it remains steady during September and October at 1040.0. Moreover, the land price index stays constant at the peak value of the year during November and December, reaching up to 1041.0.</t>
+          <t>This figure represents the land price index in Canada in 2018. Overall the price index increases throughout the year. During January a value of 1037 can be observed, after which it rises up to 1038 during February. It falls back to 1037 during March and April. During the following 2 months there is a steady increase, after which the land price index remains unchanged at 1039 throughout June until August. Also, it remains steady during September and October at 1040. Moreover, the land price index stays constant at the peak value of the year during November and December, reaching up to 1041.</t>
         </is>
       </c>
       <c r="V290" t="inlineStr">
         <is>
-          <t>This figure represents TKN_About TKN_UOM in TKN_Geo in TKN_Year. Overall the TKN_UOM increases throughout the year. During January a value of 1037.0 can be observed, after which it rises up to 1038.5 during February. It falls back to 1037.0 during March and April. During the following -25875 months there is a steady increase, after which TKN_About TKN_UOM remains unchanged at 1039.0 throughout June until August. Also, it remains steady during September and October at 1040.0. Moreover, TKN_About TKN_UOM stays constant at the peak value of the year during November and December, reaching up to 1041.0.</t>
+          <t>This figure represents TKN_About  TKN_UOM  in  TKN_Geo  in  TKN_Year . Overall the TKN_UOM  increases throughout the year. During January a value of 0 can be observed, after which it rises up to 25 during February. It falls back to 0 during March and April. During the following 2 months there is a steady increase, after which TKN_About  TKN_UOM  remains unchanged at 50 throughout June until August. Also, it remains steady during September and October at 75. Moreover, TKN_About  TKN_UOM  stays constant at the peak value of the year during November and December, reaching up to 100.</t>
         </is>
       </c>
       <c r="W290" t="n">
@@ -24833,7 +24833,7 @@
       </c>
       <c r="V291" t="inlineStr">
         <is>
-          <t>The TKN_About returning presents a steep growth over the first half of the year. In particular, it starts to grow during the month of February until reaching its peak during July TKN_Year. After that, it slightly start to decrease over the last few months of the year. The lowest value of the year was registered during February TKN_Year.</t>
+          <t>The total TKN_UOM  of United States vehicles returning presents a steep growth over the first half of the year. In particular, it starts to grow during the month of February until reaching its peak during July  TKN_Year . After that, it slightly start to decrease over the last few months of the year. The lowest value of the year was registered during February  TKN_Year .</t>
         </is>
       </c>
       <c r="W291" t="n">
@@ -24917,7 +24917,7 @@
       </c>
       <c r="V292" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About in TKN_Geo in TKN_Year. The peak value can be observed during January at 100. During the following months the price index fluctuates, until there is a sharp decline from May to June, reaching the lowest value of 0. There is a sharp increase during the month of July to 64. The price index fluctuates again from August until December.</t>
+          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year . The peak value can be observed during January at 100. During the following months the price index fluctuates, until there is a sharp decline from May to June, reaching the lowest value of 0. There is a sharp increase during the month of July to 64. The price index fluctuates again from August until December.</t>
         </is>
       </c>
       <c r="W292" t="n">
@@ -25001,7 +25001,7 @@
       </c>
       <c r="V293" t="inlineStr">
         <is>
-          <t>The amount TKN_About in TKN_Geo during TKN_Year presented strong variations in its values over the year. It's possible to identify several peaks, dips and curves. During June and July has been recorded a massive drop of the import value. At the same time, the most significant peak was registered during June. The most considerable dip was reported during July.</t>
+          <t>The amount TKN_About  in  TKN_Geo  during  TKN_Year  presented strong variations in its values over the year. It's possible to identify several peaks, dips and curves. During June and July has been recorded a massive drop of the import value. At the same time, the most significant peak was registered during June. The most considerable dip was reported during July.</t>
         </is>
       </c>
       <c r="W293" t="n">
@@ -25085,7 +25085,7 @@
       </c>
       <c r="V294" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo showed an oscillating trend over TKN_Year. In particular, couple of peaks have been registered, mainly during the months of March and May. At the same time, the production value showed its minimum values during the months of July and December. The most considerable drop of the value was registered between the months of November and December.</t>
+          <t>The TKN_About  in  TKN_Geo  showed an oscillating trend over  TKN_Year . In particular, couple of peaks have been registered, mainly during the months of March and May. At the same time, the production value showed its minimum values during the months of July and December. The most considerable drop of the value was registered between the months of November and December.</t>
         </is>
       </c>
       <c r="W294" t="n">
@@ -25169,7 +25169,7 @@
       </c>
       <c r="V295" t="inlineStr">
         <is>
-          <t>The following graph depicts the Canadian TKN_About in TKN_UOM during TKN_Year. In January approximately 60 TKN_UOM were produced, after which a sharp drop can be observed for February, reaching slightly below 15. Production remain mostly stable throughout March to May, with the lowest production coming up in July at 0. Production sharply increases during the following months, until it peaks in October at approximately 97. Following this there is a drop, and production remains almost unchanged during November and December at 45.</t>
+          <t>The following graph depicts the Canadian TKN_About  in TKN_UOM  during  TKN_Year . In January approximately 60 TKN_UOM  were produced, after which a sharp drop can be observed for February, reaching slightly below 15. Production remain mostly stable throughout March to May, with the lowest production coming up in July at 0. Production sharply increases during the following months, until it peaks in October at approximately 97. Following this there is a drop, and production remains almost unchanged during November and December at 45.</t>
         </is>
       </c>
       <c r="W295" t="n">
@@ -25253,7 +25253,7 @@
       </c>
       <c r="V296" t="inlineStr">
         <is>
-          <t>The values about TKN_About in TKN_Geo have been strongly flactuating over the TKN_Year. The most significant peak was recorded during June. At the same time, the lower value was during December.  It's also possible to see a huge drop of the production value between the months of June and July.</t>
+          <t>The values about TKN_About  in  TKN_Geo  have been strongly flactuating over the  TKN_Year . The most significant peak was recorded during June. At the same time, the lower value was during December.  It's also possible to see a huge drop of the production value between the months of June and July.</t>
         </is>
       </c>
       <c r="W296" t="n">
@@ -25337,7 +25337,7 @@
       </c>
       <c r="V297" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About in TKN_Geo in TKN_Year (in tonnes). The lowest production is during January. There is a sharp increase during February and during the following months production levels off between 4-116 and 61. A decrease can be observed in August. For the following -116 months TKN_About remains steady at approximately 47. After a drop in November, production peaks in December with up to 101 tonnes.</t>
+          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year  (in tonnes). The lowest production is during January. There is a sharp increase during February and during the following months production levels off between 42 and 61. A decrease can be observed in August. For the following 2 months TKN_About  remains steady at approximately 47. After a drop in November, production peaks in December with up to 101 tonnes.</t>
         </is>
       </c>
       <c r="W297" t="n">
@@ -25421,7 +25421,7 @@
       </c>
       <c r="V298" t="inlineStr">
         <is>
-          <t>The shown data values are about the TKN_About in TKN_Geo during TKN_Year. They are described using TKN_UOM (FPPI). The values slightly increased from January to February. After that, from February over it steeply declined until reaching the minimum value of the year in July. Then, the production value started to rise again until the end of the year. During the last three months the value remained quite stable.</t>
+          <t>The shown data values are about the TKN_About  in  TKN_Geo  during  TKN_Year . They are described using TKN_UOM  (FPPI). The values slightly increased from January to February. After that, from February over it steeply declined until reaching the minimum value of the year in July. Then, the production value started to rise again until the end of the year. During the last three months the value remained quite stable.</t>
         </is>
       </c>
       <c r="W298" t="n">
@@ -25500,12 +25500,12 @@
       </c>
       <c r="U299" t="inlineStr">
         <is>
-          <t>This figure represents the production of Canola in Canada during 2016. The unit given is tonnes. In January production lies at approximately 780000 tonnes. During the following 2 months the production increases. From March until August the production fluctuates until reaching the minimum during August with 58000. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 1130000 tonnes.</t>
+          <t>This figure represents the production of Canola in Canada during 2016. The unit given is tonnes. In January production lies at approximately 780000 tonnes. During the following 2 months the production increases. From March until August the production fluctuates until reaching the minimum during August with 580000. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 1130000 tonnes.</t>
         </is>
       </c>
       <c r="V299" t="inlineStr">
         <is>
-          <t>This figure represents the TKN_About in TKN_Geo during TKN_Year. The unit given is tonnes. In January production lies at approximately 38 tonnes. During the following -101 months the production increases. From March until August the production fluctuates until reaching the minimum during August with -91. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 100 tonnes.</t>
+          <t>This figure represents the TKN_About  in  TKN_Geo  during  TKN_Year . The unit given is tonnes. In January production lies at approximately 38 tonnes. During the following 2 months the production increases. From March until August the production fluctuates until reaching the minimum during August with 2. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 100 tonnes.</t>
         </is>
       </c>
       <c r="W299" t="n">
@@ -25589,7 +25589,7 @@
       </c>
       <c r="V300" t="inlineStr">
         <is>
-          <t>The TKN_UOM of TKN_About during TKN_Year registered the highest values during the summer months. In particular, the maximum TKN_UOM was recorded during August TKN_Year. At the same time, the lowest value of the year was during the month of February. During the last few months of the year the TKN_UOM of vehicles returning to the country slowly decreased.</t>
+          <t>The TKN_UOM  of TKN_About  during  TKN_Year  registered the highest values during the summer months. In particular, the maximum TKN_UOM  was recorded during August  TKN_Year . At the same time, the lowest value of the year was during the month of February. During the last few months of the year the TKN_UOM  of vehicles returning to the country slowly decreased.</t>
         </is>
       </c>
       <c r="W300" t="n">
@@ -25673,7 +25673,7 @@
       </c>
       <c r="V301" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how TKN_About TKN_UOM in TKN_Geo has been slowly but constantly increasing over TKN_Year. It presented few fluactuations, but none of them are significant.</t>
+          <t>It's clearly possible to see how TKN_About  TKN_UOM  in  TKN_Geo  has been slowly but constantly increasing over  TKN_Year . It presented few fluactuations, but none of them are significant.</t>
         </is>
       </c>
       <c r="W301" t="n">
@@ -25757,7 +25757,7 @@
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian TKN_About (in tonnes) during TKN_Year. The lowest value can be observed in January with 1 tonnes. Supply increases during February, remains almost unchanged throughout March and sharply increases during the following months until it reaches its peak in July with 101 tonnes. There is a sharp decline in TKN_About from July until September. The supply remains stable during October and experiences a small rise during November.</t>
+          <t>This graph represents the Canadian TKN_About  (in tonnes) during  TKN_Year . The lowest value can be observed in January with 1 tonnes. Supply increases during February, remains almost unchanged throughout March and sharply increases during the following months until it reaches its peak in July with 101 tonnes. There is a sharp decline in TKN_About  from July until September. The supply remains stable during October and experiences a small rise during November.</t>
         </is>
       </c>
       <c r="W302" t="n">
@@ -25841,7 +25841,7 @@
       </c>
       <c r="V303" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo reported a not homogeneous trend over TKN_Year. The maximum value was recorded during January. After that, several oscillations have been recorded over the year. In particular, a big drop was recorded between the months of April and June. The value keep fluactuating over the last few months of the year.</t>
+          <t>The TKN_About  in  TKN_Geo  reported a not homogeneous trend over  TKN_Year . The maximum value was recorded during January. After that, several oscillations have been recorded over the year. In particular, a big drop was recorded between the months of April and June. The value keep fluactuating over the last few months of the year.</t>
         </is>
       </c>
       <c r="W303" t="n">
@@ -25925,7 +25925,7 @@
       </c>
       <c r="V304" t="inlineStr">
         <is>
-          <t>The TKN_About in TKN_Geo during TKN_Year is represented in the following graph. The unit given is tonnes. Production remains mainly stable throughout January to March at approximately 16 tonnes. There is a small increase during April and May, followed by a minor decline during June and July. The maximum TKN_About takes place during August with approximately 101 tonnes. From August to December the production drastically decreases until it reaches its minimum of -1 in December.</t>
+          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  is represented in the following graph. The unit given is tonnes. Production remains mainly stable throughout January to March at approximately 16 tonnes. There is a small increase during April and May, followed by a minor decline during June and July. The maximum TKN_About  takes place during August with approximately 101 tonnes. From August to December the production drastically decreases until it reaches its minimum of -1 in December.</t>
         </is>
       </c>
       <c r="W304" t="n">
@@ -26009,7 +26009,7 @@
       </c>
       <c r="V305" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the TKN_About in TKN_Geo reported two significant peaks during TKN_Year, one in February and one in October. Futhermore, from February to July the production value strongly decrease, reaching the yearly minimum value during July. It's clearly possible to see how the summer months are the period with the least TKN_About.</t>
+          <t>As it's possible to see from the graph, the TKN_About  in  TKN_Geo  reported two significant peaks during  TKN_Year , one in February and one in October. Futhermore, from February to July the production value strongly decrease, reaching the yearly minimum value during July. It's clearly possible to see how the summer months are the period with the least TKN_About .</t>
         </is>
       </c>
       <c r="W305" t="n">
@@ -26093,7 +26093,7 @@
       </c>
       <c r="V306" t="inlineStr">
         <is>
-          <t>The shown data are about TKN_UOM in TKN_Geo during TKN_Year. The maximum value was recorded during the month of June. After that, a big drop has been registered between June and September. During the last few months of the TKN_About value slightly increased.</t>
+          <t>The shown data are about TKN_UOM  in  TKN_Geo  during  TKN_Year . The maximum value was recorded during the month of June. After that, a big drop has been registered between June and September. During the last few months of the TKN_About  value slightly increased.</t>
         </is>
       </c>
       <c r="W306" t="n">
@@ -26177,7 +26177,7 @@
       </c>
       <c r="V307" t="inlineStr">
         <is>
-          <t>The value about TKN_About in TKN_Geo rapidly increased during the first months of TKN_Year. After that, a considerable drop was recorded between the months of May and July. During the last months of the year the softwood and hardwood stocks slowly declined. The minimum value has been reached during the month of December.</t>
+          <t>The value about TKN_About  in  TKN_Geo  rapidly increased during the first months of  TKN_Year . After that, a considerable drop was recorded between the months of May and July. During the last months of the year the softwood and hardwood stocks slowly declined. The minimum value has been reached during the month of December.</t>
         </is>
       </c>
       <c r="W307" t="n">

</xml_diff>

<commit_message>
Stable and working version.
</commit_message>
<xml_diff>
--- a/Dataset/Captions collection/final_captions_collection.xlsx
+++ b/Dataset/Captions collection/final_captions_collection.xlsx
@@ -552,12 +552,12 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>The following line chart is about the production of grains in Canada during 2017. The values are reported using the FPPI (Farm product pridce index). It's clearly possible to see how the production of grains is quite low from January to May, but then it rapidly increase from June to December, reaching its maximum value during September 2017.</t>
+          <t>the following line chart is about the production of grains in canada during 2017. the values are reported using the fppi (farm product pridce index). it's clearly possible to see how the production of grains is quite low from january to may, but then it rapidly increase from june to december, reaching its maximum value during september 2017.</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported using the FPPI (Farm product pridce index). It's clearly possible to see how the TKN_About  is quite low from January to May, but then it rapidly increase from June to December, reaching its maximum value during September  TKN_Year .</t>
+          <t>the following line chart is about the TKN_About  in canada during  TKN_Year . the values are reported using the fppi (farm product pridce index). it's clearly possible to see how the TKN_About  is quite low from january to may, but then it rapidly increase from june to december, reaching its maximum value during september  TKN_Year .</t>
         </is>
       </c>
       <c r="W2" t="n">
@@ -636,12 +636,12 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>The following line chart is about the production of new motor vehicles (units) in Canada during 2018. It's possible to see how the highest value was during May, when almost 220000 new motor vehicles have been producted. Furthermore, it's also clear that January and December are the months with less new motor vehicles producted over 2018 in Canada.</t>
+          <t>the following line chart is about the production of new motor vehicles (units) in canada during 2018. it's possible to see how the highest value was during may, when almost 220000 new motor vehicles have been producted. furthermore, it's also clear that january and december are the months with less new motor vehicles producted over 2018 in canada.</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About  (units) in  TKN_Geo  during  TKN_Year . It's possible to see how the highest value was during May, when almost 100 new motor vehicles have been producted. Furthermore, it's also clear that January and December are the months with less new motor vehicles producted over  TKN_Year  in  TKN_Geo .</t>
+          <t>the following line chart is about the TKN_About  (units) in canada during  TKN_Year . it's possible to see how the highest value was during may, when almost 100 new motor vehicles have been producted. furthermore, it's also clear that january and december are the months with less new motor vehicles producted over  TKN_Year  in canada.</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -720,12 +720,12 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>The image reports a line chart about the total softwood and hardwood production (in cubic metres) in Canda during 2018. The values are fluctuating over the months, reaching a peak during May 2018. At the same time it's clearly possible to see that December 2018 has been the month with less production.</t>
+          <t>the image reports a line chart about the total softwood and hardwood production (in cubic metres) in canda during 2018. the values are fluctuating over the months, reaching a peak during may 2018. at the same time it's clearly possible to see that december 2018 has been the month with less production.</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>The image reports a line chart about the TKN_About  TKN_UOM  metres) in Canda during  TKN_Year . The values are fluctuating over the months, reaching a peak during May  TKN_Year . At the same time it's clearly possible to see that December  TKN_Year  has been the month with less production.</t>
+          <t>the image reports a line chart about the TKN_About  TKN_UOM  metres) in canda during  TKN_Year . the values are fluctuating over the months, reaching a peak during may  TKN_Year . at the same time it's clearly possible to see that december  TKN_Year  has been the month with less production.</t>
         </is>
       </c>
       <c r="W4" t="n">
@@ -804,12 +804,12 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>The line chart shows the total number of vehicles entering Canada during 2016. It's clearly possible to see how during the summer months the amount of car entering Canada is way higher than the rest of the year, reaching the maximum value during the month of August with around 3400000 cars.</t>
+          <t>the line chart shows the total number of vehicles entering canada during 2016. it's clearly possible to see how during the summer months the amount of car entering canada is way higher than the rest of the year, reaching the maximum value during the month of august with around 3400000 cars.</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>The line chart shows the total TKN_UOM  of vehicles entering  TKN_Geo  during  TKN_Year . It's clearly possible to see how during the summer months the amount of car entering  TKN_Geo  is way higher than the rest of the year, reaching the maximum value during the month of August with around 100 cars.</t>
+          <t>the line chart shows the total TKN_UOM  of TKN_About  during  TKN_Year . it's clearly possible to see how during the summer months the amount of car entering canada is way higher than the rest of the year, reaching the maximum value during the month of august with around 100 cars.</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -888,12 +888,12 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>The following graph describes how the FPPI (farm product price index) about production of eggs in shell in Canada has been slowly increasing during 2017. In particular, it increased from 1362 in February to 1371 in December.</t>
+          <t>the following graph describes how the fppi (farm product price index) about production of eggs in shell in canada has been slowly increasing during 2017. in particular, it increased from 1362 in february to 1371 in december.</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>The following graph describes how TKN_UOM  index) about TKN_About  in  TKN_Geo  has been slowly increasing during  TKN_Year . In particular, it increased from 0 in February to 100 in December.</t>
+          <t>the following graph describes how TKN_UOM  index) about TKN_About  in canada has been slowly increasing during  TKN_Year . in particular, it increased from 0 in february to 100 in december.</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -972,12 +972,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>The line chart shows the farm product price index (FPPI) about production of grain in Canada during 2016. It's possible to see how the index has been quite steady from January to June, but then a relevant drop has been recorded from June to August, where the index dropped from 1100 to 980. During the last few months of the year the index slowly started to increase again.</t>
+          <t>the line chart shows the farm product price index (fppi) about production of grain in canada during 2016. it's possible to see how the index has been quite steady from january to june, but then a relevant drop has been recorded from june to august, where the index dropped from 1100 to 980. during the last few months of the year the index slowly started to increase again.</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>The line chart shows the TKN_UOM  about TKN_About  grain in  TKN_Geo  during  TKN_Year . It's possible to see how the index has been quite steady from January to June, but then a relevant drop has been recorded from June to August, where the index dropped from 93 to 8. During the last few months of the year the index slowly started to increase again.</t>
+          <t>the line chart shows the TKN_UOM  about TKN_About  grain in canada during  TKN_Year . it's possible to see how the index has been quite steady from january to june, but then a relevant drop has been recorded from june to august, where the index dropped from 93 to 8. during the last few months of the year the index slowly started to increase again.</t>
         </is>
       </c>
       <c r="W7" t="n">
@@ -1056,12 +1056,12 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>The chart shows the farm product price index (FPPI) about total livestock and animal products in Canada during 2016. The index has been quite steady during the first few months of the year, with a maximum value in March, but then it rapidly decreased from June over, reaching the minimum value during October which was around 1270. The index started to slowly grow again during the months of November and December.</t>
+          <t>the chart shows the farm product price index (fppi) about total livestock and animal products in canada during 2016. the index has been quite steady during the first few months of the year, with a maximum value in march, but then it rapidly decreased from june over, reaching the minimum value during october which was around 1270. the index started to slowly grow again during the months of november and december.</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>The chart shows the TKN_UOM  about TKN_About  in  TKN_Geo  during  TKN_Year . The index has been quite steady during the first few months of the year, with a maximum value in March, but then it rapidly decreased from June over, reaching the minimum value during October which was around 1. The index started to slowly grow again during the months of November and December.</t>
+          <t>the chart shows the TKN_UOM  about TKN_About  in canada during  TKN_Year . the index has been quite steady during the first few months of the year, with a maximum value in march, but then it rapidly decreased from june over, reaching the minimum value during october which was around 1. the index started to slowly grow again during the months of november and december.</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -1140,12 +1140,12 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of May with a number of 1215 in Canada. The biggest increase in production of poultry can be observed from February until May, while a drop from May to July takes place. From August until November the production remains quite stable at approximately 1205 and starts decreasing until it reaches its minimum in February below 1190.</t>
+          <t>production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of may with a number of 1215 in canada. the biggest increase in production of poultry can be observed from february until may, while a drop from may to july takes place. from august until november the production remains quite stable at approximately 1205 and starts decreasing until it reaches its minimum in february below 1190.</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of May with a number of 100 in  TKN_Geo . The biggest increase in production of poultry can be observed from February until May, while a drop from May to July takes place. From August until November the production remains quite stable at approximately 62 and starts decreasing until it reaches its minimum in February below 4.</t>
+          <t>production of poultry including chickens, turkeys, chicks and poults reaches its maximum during the month of may with a number of 100 in canada. the biggest increase in production of poultry can be observed from february until may, while a drop from may to july takes place. from august until november the production remains quite stable at approximately 62 and starts decreasing until it reaches its minimum in february below 4.</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>The graph shows the production of new motor vehicles in dollars in Canada during 2018. In general the production recorded its highes values during the spring and summer months, reaching a peak during May 2019. The most significant jump of the values during 2018 is between the months of February and March.</t>
+          <t>the graph shows the production of new motor vehicles in dollars in canada during 2018. in general the production recorded its highes values during the spring and summer months, reaching a peak during may 2019. the most significant jump of the values during 2018 is between the months of february and march.</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year . In general the production recorded its highes values during the spring and summer months, reaching a peak during May 2019. The most significant jump of the values during  TKN_Year  is between the months of February and March.</t>
+          <t>the graph shows the TKN_About  in TKN_UOM  in canada during  TKN_Year . in general the production recorded its highes values during the spring and summer months, reaching a peak during may 2019. the most significant jump of the values during  TKN_Year  is between the months of february and march.</t>
         </is>
       </c>
       <c r="W10" t="n">
@@ -1308,12 +1308,12 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>The line chart reports the values about the total farm production price index (FPPI) in Canada during 2017. During the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of June and July. After that, it rapidly dropped from over 1360 to less than 1290 in the month of Setpember.</t>
+          <t>the line chart reports the values about the total farm production price index (fppi) in canada during 2017. during the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of june and july. after that, it rapidly dropped from over 1360 to less than 1290 in the month of setpember.</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>The line chart reports the values TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . During the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of June and July. After that, it rapidly dropped from over 97 to less than 6 in the month of Setpember.</t>
+          <t>the line chart reports the values TKN_About  TKN_UOM  in canada during  TKN_Year . during the first half of the hear the index shown an ascendant trend, reaching its maximum value during the months of june and july. after that, it rapidly dropped from over 97 to less than 6 in the month of setpember.</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -1392,12 +1392,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately 10000 tonnes of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 8000 to 8500 tonnes. A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 11500 tonnes.</t>
+          <t>production of creamery butter varies a lot throughout the year. being mostly stable from february until april with approximately 10000 tonnes of creamery butter, a drop is observed from april until june. the production starts oscillating between june and november, whereas production varies between 8000 to 8500 tonnes. a sharp increase in creamery butter production is taking place from november onwards, reaching its maximum in january with almost 11500 tonnes.</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>Production of creamery butter varies a lot throughout the year. Being mostly stable from February until April with approximately 65 TKN_UOM  of creamery butter, a drop is observed from April until June. The production starts oscillating between June and November, whereas production varies between 12 to 25 TKN_UOM . A sharp increase in creamery butter production is taking place from November onwards, reaching its maximum in January with almost 105 TKN_UOM .</t>
+          <t>production of creamery butter varies a lot throughout the year. being mostly stable from february until april with approximately 65 TKN_UOM  of creamery butter, a drop is observed from april until june. the production starts oscillating between june and november, whereas production varies between 12 to 25 TKN_UOM . a sharp increase in creamery butter production is taking place from november onwards, reaching its maximum in january with almost 105 TKN_UOM .</t>
         </is>
       </c>
       <c r="W12" t="n">
@@ -1476,12 +1476,12 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>The figure shows a line chart about the production of what flour (in tonnes) in Canada during 2017. The values have been mainly fluctuating during the year, without any significant trend or patterns. Even that, if it has been recorded a significant growth from November to December, where the production of wheat flour during 2017 reached its peak.</t>
+          <t>the figure shows a line chart about the production of what flour (in tonnes) in canada during 2017. the values have been mainly fluctuating during the year, without any significant trend or patterns. even that, if it has been recorded a significant growth from november to december, where the production of wheat flour during 2017 reached its peak.</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>The figure shows a line chart about the production of what flour (in tonnes) in  TKN_Geo  during  TKN_Year . The values have been mainly fluctuating during the year, without any significant trend or patterns. Even that, if it has been recorded a significant growth from November to December, where the TKN_About  during  TKN_Year  reached its peak.</t>
+          <t>the figure shows a line chart about the production of what flour (in tonnes) in canada during  TKN_Year . the values have been mainly fluctuating during the year, without any significant trend or patterns. even that, if it has been recorded a significant growth from november to december, where the TKN_About  during  TKN_Year  reached its peak.</t>
         </is>
       </c>
       <c r="W13" t="n">
@@ -1560,12 +1560,12 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>This graph represents the price index of laptop computers in Canada. The price is the highest during the month of January at 966. From February until May the price starts fluctuating between roughly 959 to 963. Prices for laptop computers show a dramatic drop during the month of June. The minimum value lies at 952. The price starts oscillating again between July and December with prices between 961 to 958.</t>
+          <t>this graph represents the price index of laptop computers in canada. the price is the highest during the month of january at 966. from february until may the price starts fluctuating between roughly 959 to 963. prices for laptop computers show a dramatic drop during the month of june. the minimum value lies at 952. the price starts oscillating again between july and december with prices between 961 to 958.</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  in  TKN_Geo . The price is the highest during the month of January at 100. From February until May the price starts fluctuating between roughly 50 to 79. Prices for laptop computers show a dramatic drop during the month of June. The minimum value lies at 0. The price starts oscillating again between July and December with prices between 64 to 43.</t>
+          <t>this graph represents the TKN_About  in canada. the price is the highest during the month of january at 100. from february until may the price starts fluctuating between roughly 50 to 79. prices for laptop computers show a dramatic drop during the month of june. the minimum value lies at 0. the price starts oscillating again between july and december with prices between 64 to 43.</t>
         </is>
       </c>
       <c r="W14" t="n">
@@ -1644,12 +1644,12 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>The following graph is about the imports of creamery butter (in tonnes) in Canada during 2016. It's possible to see how the values are generally increasing over the year, with a substan raise from August until October, where the values basically tripled. The maximum value recorded over the year is during November 2016, where the recorded production has been over 3000 tonnes.</t>
+          <t>the following graph is about the imports of creamery butter (in tonnes) in canada during 2016. it's possible to see how the values are generally increasing over the year, with a substan raise from august until october, where the values basically tripled. the maximum value recorded over the year is during november 2016, where the recorded production has been over 3000 tonnes.</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>The following graph is about the imports TKN_About  (in tonnes) in  TKN_Geo  during  TKN_Year . It's possible to see how the values are generally increasing over the year, with a substan raise from August until October, where the values basically tripled. The maximum value recorded over the year is during November  TKN_Year , where the recorded production has been over 97 tonnes.</t>
+          <t>the following graph is about the imports TKN_About  (in tonnes) in canada during  TKN_Year . it's possible to see how the values are generally increasing over the year, with a substan raise from august until october, where the values basically tripled. the maximum value recorded over the year is during november  TKN_Year , where the recorded production has been over 97 tonnes.</t>
         </is>
       </c>
       <c r="W15" t="n">
@@ -1728,12 +1728,12 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>This line chart represent the number of total Canadian vehicles returning in 2016. A slow, but steady increase is taking place from March until it reaches its peak in August with a total number of 2200000. After August the total number of Canadian vehicles returning starts decreasing until reaching its minimum value below 1400000 in February. This big difference may be due to holiday season during the warmer months of the year.</t>
+          <t>this line chart represent the number of total canadian vehicles returning in 2016. a slow, but steady increase is taking place from march until it reaches its peak in august with a total number of 2200000. after august the total number of canadian vehicles returning starts decreasing until reaching its minimum value below 1400000 in february. this big difference may be due to holiday season during the warmer months of the year.</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>This line chart represent the TKN_UOM  of total Canadian vehicles returning in  TKN_Year . A slow, but steady increase is taking place from March until it reaches its peak in August with a total TKN_UOM  of 97. After August the total TKN_UOM  of Canadian vehicles returning starts decreasing until reaching its minimum value below 6 in February. This big difference may be due to holiday season during the warmer months of the year.</t>
+          <t>this line chart represent the TKN_UOM  of total canadian vehicles returning in  TKN_Year . a slow, but steady increase is taking place from march until it reaches its peak in august with a total TKN_UOM  of 97. after august the total TKN_UOM  of canadian vehicles returning starts decreasing until reaching its minimum value below 6 in february. this big difference may be due to holiday season during the warmer months of the year.</t>
         </is>
       </c>
       <c r="W16" t="n">
@@ -1812,12 +1812,12 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>The following line chart shows the farm product price index (FPPI) about the total livestock and animal products in Canada during 2018. The values are significantly fluctuating over the year, showing several peaks and falls. The highest values of the indexes have been recorded during February, July and October. The lower values of the indexes have been recorded during April, September and December.</t>
+          <t>the following line chart shows the farm product price index (fppi) about the total livestock and animal products in canada during 2018. the values are significantly fluctuating over the year, showing several peaks and falls. the highest values of the indexes have been recorded during february, july and october. the lower values of the indexes have been recorded during april, september and december.</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>The following line chart shows the TKN_UOM  about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are significantly fluctuating over the year, showing several peaks and falls. The highest values of the indexes have been recorded during February, July and October. The lower values of the indexes have been recorded during April, September and December.</t>
+          <t>the following line chart shows the TKN_UOM  about the TKN_About  in canada during  TKN_Year . the values are significantly fluctuating over the year, showing several peaks and falls. the highest values of the indexes have been recorded during february, july and october. the lower values of the indexes have been recorded during april, september and december.</t>
         </is>
       </c>
       <c r="W17" t="n">
@@ -1896,12 +1896,12 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>This line chart reflects the production of eggs in a shell in Canada during 2018. From January until March the production remains unaltered at approximately 1375. From March until July a steady increase of up to 1405 can be observed. There is a rapid gain in production between July and August, reaching its highest production which will last until December.</t>
+          <t>this line chart reflects the production of eggs in a shell in canada during 2018. from january until march the production remains unaltered at approximately 1375. from march until july a steady increase of up to 1405 can be observed. there is a rapid gain in production between july and august, reaching its highest production which will last until december.</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>This line chart reflects the TKN_About  in  TKN_Geo  during  TKN_Year . From January until March the production remains unaltered at approximately 4. From March until July a steady increase of up to 40 can be observed. There is a rapid gain in production between July and August, reaching its highest production which will last until December.</t>
+          <t>this line chart reflects the TKN_About  in canada during  TKN_Year . from january until march the production remains unaltered at approximately 4. from march until july a steady increase of up to 40 can be observed. there is a rapid gain in production between july and august, reaching its highest production which will last until december.</t>
         </is>
       </c>
       <c r="W18" t="n">
@@ -1980,12 +1980,12 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>It shows the number of total vehicles entering Canada during 2017. It's clearly possible to see how this value rapidly increase from January until the end of the summer, reaching its maximum value in August. After that, the number of vehicles entering Canada decrease during the last few months of the year. The minimum value has been recorded during February.</t>
+          <t>it shows the number of total vehicles entering canada during 2017. it's clearly possible to see how this value rapidly increase from january until the end of the summer, reaching its maximum value in august. after that, the number of vehicles entering canada decrease during the last few months of the year. the minimum value has been recorded during february.</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>It shows the TKN_UOM  of TKN_About   TKN_Geo  during  TKN_Year . It's clearly possible to see how this value rapidly increase from January until the end of the summer, reaching its maximum value in August. After that, the TKN_UOM  of vehicles entering  TKN_Geo  decrease during the last few months of the year. The minimum value has been recorded during February.</t>
+          <t>it shows the TKN_UOM  of TKN_About  during  TKN_Year . it's clearly possible to see how this value rapidly increase from january until the end of the summer, reaching its maximum value in august. after that, the TKN_UOM  of vehicles entering canada decrease during the last few months of the year. the minimum value has been recorded during february.</t>
         </is>
       </c>
       <c r="W19" t="n">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>This chart illustrates the land price index of Canada in 2016. A minimum of 982 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 987. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 1000.</t>
+          <t>this chart illustrates the land price index of canada in 2016. a minimum of 982 can be observed throughout the months of january until april. a slow, but constant increase takes place from april until august, reaching a value of almost 987. from august onwards a sharp increase can be seen, until reaching its maximum during november and december at 1000.</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>This chart illustrates TKN_About  TKN_UOM  of  TKN_Geo  in  TKN_Year . A minimum of 5 can be observed throughout the months of January until April. A slow, but constant increase takes place from April until August, reaching a value of almost 32. From August onwards a sharp increase can be seen, until reaching its maximum during November and December at 100.</t>
+          <t>this chart illustrates TKN_About  TKN_UOM  of canada in  TKN_Year . a minimum of 5 can be observed throughout the months of january until april. a slow, but constant increase takes place from april until august, reaching a value of almost 32. from august onwards a sharp increase can be seen, until reaching its maximum during november and december at 100.</t>
         </is>
       </c>
       <c r="W20" t="n">
@@ -2148,12 +2148,12 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>The line chart describes the number of total vehicles entering Canada during 2018. It's clearly possible to observe that this value rapidly growed from January to August, showing the highest values during the summer months. During the last few months of the year the number of total vehicles entering Canada rapidly decreased.</t>
+          <t>the line chart describes the number of total vehicles entering canada during 2018. it's clearly possible to observe that this value rapidly growed from january to august, showing the highest values during the summer months. during the last few months of the year the number of total vehicles entering canada rapidly decreased.</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>The line chart describes the TKN_UOM  of TKN_About   TKN_Geo  during  TKN_Year . It's clearly possible to observe that this value rapidly growed from January to August, showing the highest values during the summer months. During the last few months of the year the TKN_UOM  of TKN_About   TKN_Geo  rapidly decreased.</t>
+          <t>the line chart describes the TKN_UOM  of TKN_About  during  TKN_Year . it's clearly possible to observe that this value rapidly growed from january to august, showing the highest values during the summer months. during the last few months of the year the TKN_UOM  of TKN_About  rapidly decreased.</t>
         </is>
       </c>
       <c r="W21" t="n">
@@ -2232,12 +2232,12 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>The price index of desktop and similar computers in Canada in 2017 is illustrated by this graph. Whereas the maximum of 1004 can be observed during January, a slow drop can be seen until May. The graph depicts a sharp drop between May and June, reaching 973. For the following months the price index graph starts oscillating until reaching its minimum value in December at 965.</t>
+          <t>the price index of desktop and similar computers in canada in 2017 is illustrated by this graph. whereas the maximum of 1004 can be observed during january, a slow drop can be seen until may. the graph depicts a sharp drop between may and june, reaching 973. for the following months the price index graph starts oscillating until reaching its minimum value in december at 965.</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  is illustrated by this graph. Whereas the maximum of 100 can be observed during January, a slow drop can be seen until May. The graph depicts a sharp drop between May and June, reaching 21. For the following months the price index graph starts oscillating until reaching its minimum value in December at 0.</t>
+          <t>the TKN_About  in canada in  TKN_Year  is illustrated by this graph. whereas the maximum of 100 can be observed during january, a slow drop can be seen until may. the graph depicts a sharp drop between may and june, reaching 21. for the following months the price index graph starts oscillating until reaching its minimum value in december at 0.</t>
         </is>
       </c>
       <c r="W22" t="n">
@@ -2316,12 +2316,12 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>The graph describes the import of creamery butter (in tonnes) in Canada during 2017. As can be seen from the graph, the value reports two significant peaks during the month of March and June. The minimum value has been recorded during the month of September. It's also possible to see how the values during January and December do not differ so much from each other.</t>
+          <t>the graph describes the import of creamery butter (in tonnes) in canada during 2017. as can be seen from the graph, the value reports two significant peaks during the month of march and june. the minimum value has been recorded during the month of september. it's also possible to see how the values during january and december do not differ so much from each other.</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>The graph describes the TKN_About  (in tonnes) in  TKN_Geo  during  TKN_Year . As can be seen from the graph, the value reports two significant peaks during the month of March and June. The minimum value has been recorded during the month of September. It's also possible to see how the values during January and December do not differ so much from each other.</t>
+          <t>the graph describes the TKN_About  (in tonnes) in canada during  TKN_Year . as can be seen from the graph, the value reports two significant peaks during the month of march and june. the minimum value has been recorded during the month of september. it's also possible to see how the values during january and december do not differ so much from each other.</t>
         </is>
       </c>
       <c r="W23" t="n">
@@ -2400,12 +2400,12 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>This graph illustrates the production of fresh potatoes in Canada in 2016. Production mainly starts in March, with a slow increase throughout until June. Production sharply increases from June onwards, reaching a maximum of nearly 1700 during August. A rapid drop follows between August and October, reaching a minimum of below 1350. The graph depicts a short increase in production from October until December and comes back to nearly minimum during January and February.</t>
+          <t>this graph illustrates the production of fresh potatoes in canada in 2016. production mainly starts in march, with a slow increase throughout until june. production sharply increases from june onwards, reaching a maximum of nearly 1700 during august. a rapid drop follows between august and october, reaching a minimum of below 1350. the graph depicts a short increase in production from october until december and comes back to nearly minimum during january and february.</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>This graph illustrates the TKN_About  in  TKN_Geo  in  TKN_Year . Production mainly starts in March, with a slow increase throughout until June. Production sharply increases from June onwards, reaching a maximum of nearly 104 during August. A rapid drop follows between August and October, reaching a minimum of below 1. The graph depicts a short increase in production from October until December and comes back to nearly minimum during January and February.</t>
+          <t>this graph illustrates the TKN_About  in canada in  TKN_Year . production mainly starts in march, with a slow increase throughout until june. production sharply increases from june onwards, reaching a maximum of nearly 104 during august. a rapid drop follows between august and october, reaching a minimum of below 1. the graph depicts a short increase in production from october until december and comes back to nearly minimum during january and february.</t>
         </is>
       </c>
       <c r="W24" t="n">
@@ -2484,12 +2484,12 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>This graph illustrates the Canadian import of creamery butter in 2017. The unit used is tonnes. Import reaches its maximum of over 2500 tonnes during June and its second highes import during the month of March with approximately 2150. After June the import drastically decreases until reaching a minimum of approximately 730 in September. From the months of September until February the import oscillates between approximately 730 and 1300.</t>
+          <t>this graph illustrates the canadian import of creamery butter in 2017. the unit used is tonnes. import reaches its maximum of over 2500 tonnes during june and its second highes import during the month of march with approximately 2150. after june the import drastically decreases until reaching a minimum of approximately 730 in september. from the months of september until february the import oscillates between approximately 730 and 1300.</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>This graph illustrates the Canadian TKN_About  in  TKN_Year . The unit used is TKN_UOM . Import reaches its maximum of over 97 TKN_UOM  during June and its second highes import during the month of March with approximately 79. After June the import drastically decreases until reaching a minimum of approximately 3 in September. From the months of September until February the import oscillates between approximately 3 and 34.</t>
+          <t>this graph illustrates the canadian TKN_About  in  TKN_Year . the unit used is TKN_UOM . import reaches its maximum of over 97 TKN_UOM  during june and its second highes import during the month of march with approximately 79. after june the import drastically decreases until reaching a minimum of approximately 3 in september. from the months of september until february the import oscillates between approximately 3 and 34.</t>
         </is>
       </c>
       <c r="W25" t="n">
@@ -2568,12 +2568,12 @@
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>This graph depicts the production of oats in tonnes in Canada during 2017. Production shows peaks in January and March, whereas it significantly drops after March, reaching its minimum of approximately 65000 in May. For the following months production slightly increases until August. Between August and September a rapid increase in production can be observed, indicating the maximum of over 200000 in September. Production slowly decreases throughout the following months until December.</t>
+          <t>this graph depicts the production of oats in tonnes in canada during 2017. production shows peaks in january and march, whereas it significantly drops after march, reaching its minimum of approximately 65000 in may. for the following months production slightly increases until august. between august and september a rapid increase in production can be observed, indicating the maximum of over 200000 in september. production slowly decreases throughout the following months until december.</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year . Production shows peaks in January and March, whereas it significantly drops after March, reaching its minimum of approximately 0 in May. For the following months production slightly increases until August. Between August and September a rapid increase in production can be observed, indicating the maximum of over 96 in September. Production slowly decreases throughout the following months until December.</t>
+          <t>this graph depicts the TKN_About  in TKN_UOM  in canada during  TKN_Year . production shows peaks in january and march, whereas it significantly drops after march, reaching its minimum of approximately 0 in may. for the following months production slightly increases until august. between august and september a rapid increase in production can be observed, indicating the maximum of over 96 in september. production slowly decreases throughout the following months until december.</t>
         </is>
       </c>
       <c r="W26" t="n">
@@ -2652,12 +2652,12 @@
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>This graph indicates the number of total Canadian vehicles returning to the country in 2017. The lowest number of approximately 1400000 can be observed during the month of February. Over the following 4 months a steady increase takes place. As can be seen from the graph there is sharp rise of returning vehicles from June until August. After August the number steadily decreases until reaching its minimum in February.</t>
+          <t>this graph indicates the number of total canadian vehicles returning to the country in 2017. the lowest number of approximately 1400000 can be observed during the month of february. over the following 4 months a steady increase takes place. as can be seen from the graph there is sharp rise of returning vehicles from june until august. after august the number steadily decreases until reaching its minimum in february.</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>This graph indicates the TKN_UOM  of TKN_About  in  TKN_Year . The lowest TKN_UOM  of approximately 3 can be observed during the month of February. Over the following 4 months a steady increase takes place. As can be seen from the graph there is sharp rise of returning vehicles from June until August. After August the TKN_UOM  steadily decreases until reaching its minimum in February.</t>
+          <t>this graph indicates the TKN_UOM  of TKN_About  in  TKN_Year . the lowest TKN_UOM  of approximately 3 can be observed during the month of february. over the following 4 months a steady increase takes place. as can be seen from the graph there is sharp rise of returning vehicles from june until august. after august the TKN_UOM  steadily decreases until reaching its minimum in february.</t>
         </is>
       </c>
       <c r="W27" t="n">
@@ -2736,12 +2736,12 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>The following graph is about the production of rye in Canada during 2017; the values are in tonnes. It shows a clearly growth from January over, reaching its maximum value during October. Then it's possible to see a significant drop from October to November.</t>
+          <t>the following graph is about the production of rye in canada during 2017; the values are in tonnes. it shows a clearly growth from january over, reaching its maximum value during october. then it's possible to see a significant drop from october to november.</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>The following graph is about the TKN_About  in  TKN_Geo  during  TKN_Year ; the values are in tonnes. It shows a clearly growth from January over, reaching its maximum value during October. Then it's possible to see a significant drop from October to November.</t>
+          <t>the following graph is about the TKN_About  in canada during  TKN_Year ; the values are in tonnes. it shows a clearly growth from january over, reaching its maximum value during october. then it's possible to see a significant drop from october to november.</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -2820,12 +2820,12 @@
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>The following line chart is about the production of creamery butter in Canada during 2016. The values are reported in tonnes. It shows how the production is actually falling down from January to August, when it reaches its minimum. From September to December the values are slowly rising up.</t>
+          <t>the following line chart is about the production of creamery butter in canada during 2016. the values are reported in tonnes. it shows how the production is actually falling down from january to august, when it reaches its minimum. from september to december the values are slowly rising up.</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported in tonnes. It shows how the production is actually falling down from January to August, when it reaches its minimum. From September to December the values are slowly rising up.</t>
+          <t>the following line chart is about the TKN_About  in canada during  TKN_Year . the values are reported in tonnes. it shows how the production is actually falling down from january to august, when it reaches its minimum. from september to december the values are slowly rising up.</t>
         </is>
       </c>
       <c r="W29" t="n">
@@ -2904,12 +2904,12 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>In the following graph is described the monthly supply of creamery butter in tonnes about Canada during 2016. The minimum value has been registered during the month of January and maximum during July. Furthermore, it's possible to see how the supply of creamery butter is generally higher during spring and summer.</t>
+          <t>in the following graph is described the monthly supply of creamery butter in tonnes about canada during 2016. the minimum value has been registered during the month of january and maximum during july. furthermore, it's possible to see how the supply of creamery butter is generally higher during spring and summer.</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>In the following graph is described the monthly TKN_About  in TKN_UOM  about  TKN_Geo  during  TKN_Year . The minimum value has been registered during the month of January and maximum during July. Furthermore, it's possible to see how the TKN_About  is generally higher during spring and summer.</t>
+          <t>in the following graph is described the monthly TKN_About  in TKN_UOM  about canada during  TKN_Year . the minimum value has been registered during the month of january and maximum during july. furthermore, it's possible to see how the TKN_About  is generally higher during spring and summer.</t>
         </is>
       </c>
       <c r="W30" t="n">
@@ -2988,12 +2988,12 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>The graph shows the production of chickens, turkeys, chicks, and poults in Canada in the year of 2017. There is one data entry for each month of the year. Production is measured by the farm product price index. The x-axis shows the months, the y-axis the index ranging from 1190 to 1215. There is a high in May (index of 1215) and a low in February (a bit below 1190).</t>
+          <t>the graph shows the production of chickens, turkeys, chicks, and poults in canada in the year of 2017. there is one data entry for each month of the year. production is measured by the farm product price index. the x-axis shows the months, the y-axis the index ranging from 1190 to 1215. there is a high in may (index of 1215) and a low in february (a bit below 1190).</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  in  TKN_Geo  in the year of  TKN_Year . There is one data entry for each month of the year. Production is measured TKN_UOM  index. The x-axis shows the months, the y-axis the index ranging from 4 to 100. There is a high in May (index of 100) and a low in February (a bit below 4).</t>
+          <t>the graph shows the TKN_About  in canada in the year of  TKN_Year . there is one data entry for each month of the year. production is measured TKN_UOM  index. the x-axis shows the months, the y-axis the index ranging from 4 to 100. there is a high in may (index of 100) and a low in february (a bit below 4).</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -3072,12 +3072,12 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>The graph illustrates the production of oats in Canada for the year 2018. There are sharp decreases in production for the months of February, July and November.</t>
+          <t>the graph illustrates the production of oats in canada for the year 2018. there are sharp decreases in production for the months of february, july and november.</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About  in  TKN_Geo  for the year  TKN_Year . There are sharp decreases in production for the months of February, July and November.</t>
+          <t>the graph illustrates the TKN_About  in canada for the year  TKN_Year . there are sharp decreases in production for the months of february, july and november.</t>
         </is>
       </c>
       <c r="W32" t="n">
@@ -3156,12 +3156,12 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>The graph shows the values of House price index in Canada during 2016. It's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. The minimum value has been recorded during January and the maximum one during December.</t>
+          <t>the graph shows the values of house price index in canada during 2016. it's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. the minimum value has been recorded during january and the maximum one during december.</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>The graph shows the values TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . It's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. The minimum value has been recorded during January and the maximum one during December.</t>
+          <t>the graph shows the values TKN_About  TKN_UOM  in canada during  TKN_Year . it's clearly possible to see how it rapidly increased over the year, with really few and light fluctuations. the minimum value has been recorded during january and the maximum one during december.</t>
         </is>
       </c>
       <c r="W33" t="n">
@@ -3240,12 +3240,12 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>This graph depicts the total softwood production in Canada in 2016 in cubic meters. The values range from roughly 57000 in March to 46000 in December. January to March there is an increase in production, March to July production decreased and reached 50000 in July. There is another high of about 57000 cubic meters in November.</t>
+          <t>this graph depicts the total softwood production in canada in 2016 in cubic meters. the values range from roughly 57000 in march to 46000 in december. january to march there is an increase in production, march to july production decreased and reached 50000 in july. there is another high of about 57000 cubic meters in november.</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in  TKN_Geo  in  TKN_Year  TKN_UOM  meters. The values range from roughly 102 in March to -1 in December. January to March there is an increase in production, March to July production decreased and reached 36 in July. There is another high of about 102 cubic meters in November.</t>
+          <t>this graph depicts the TKN_About  in canada in  TKN_Year  TKN_UOM  meters. the values range from roughly 102 in march to -1 in december. january to march there is an increase in production, march to july production decreased and reached 36 in july. there is another high of about 102 cubic meters in november.</t>
         </is>
       </c>
       <c r="W34" t="n">
@@ -3324,12 +3324,12 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>The graph indicates the number of cubic meters of soft wood production in Canada for 2018. Production is highest in spring time and drops to its lowest in December.</t>
+          <t>the graph indicates the number of cubic meters of soft wood production in canada for 2018. production is highest in spring time and drops to its lowest in december.</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>The graph indicates the number TKN_UOM  meters of soft TKN_About  in  TKN_Geo  for  TKN_Year . Production is highest in spring time and drops to its lowest in December.</t>
+          <t>the graph indicates the number TKN_UOM  meters of soft TKN_About  in canada for  TKN_Year . production is highest in spring time and drops to its lowest in december.</t>
         </is>
       </c>
       <c r="W35" t="n">
@@ -3408,12 +3408,12 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>As can be seen from the graph the production of unprocessed milk in Canada during 2018 had a significant growth during the second half of the year. It decreased from January to June, when it has been recorded the minimum value of the year. But then it started to rapidly increase reaching its maximum value during November 2019.</t>
+          <t>as can be seen from the graph the production of unprocessed milk in canada during 2018 had a significant growth during the second half of the year. it decreased from january to june, when it has been recorded the minimum value of the year. but then it started to rapidly increase reaching its maximum value during november 2019.</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>As can be seen from the graph the TKN_About  in  TKN_Geo  during  TKN_Year  had a significant growth during the second half of the year. It decreased from January to June, when it has been recorded the minimum value of the year. But then it started to rapidly increase reaching its maximum value during November 2019.</t>
+          <t>as can be seen from the graph the TKN_About  in canada during  TKN_Year  had a significant growth during the second half of the year. it decreased from january to june, when it has been recorded the minimum value of the year. but then it started to rapidly increase reaching its maximum value during november 2019.</t>
         </is>
       </c>
       <c r="W36" t="n">
@@ -3492,12 +3492,12 @@
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>As is shown form the graph, the production of unprocessed milk steadily increases in winter time, and steadily decreases in summer. The graph shows that production is highest in November and lowest in June.</t>
+          <t>as is shown form the graph, the production of unprocessed milk steadily increases in winter time, and steadily decreases in summer. the graph shows that production is highest in november and lowest in june.</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>As is shown form the graph, the TKN_About  steadily increases in winter time, and steadily decreases in summer. The graph shows that production is highest in November and lowest in June.</t>
+          <t>as is shown form the graph, the TKN_About  steadily increases in winter time, and steadily decreases in summer. the graph shows that production is highest in november and lowest in june.</t>
         </is>
       </c>
       <c r="W37" t="n">
@@ -3576,12 +3576,12 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>The line chart illustrates the production of unprocessed milk in Canada during 2017. The values are described using the farm product price index (FPPI). It's clearly possible to see two main peaks over the year, one during February and one during October. At the same time, during the summer the production significantly decreased, reaching its minimum value during the month of July.</t>
+          <t>the line chart illustrates the production of unprocessed milk in canada during 2017. the values are described using the farm product price index (fppi). it's clearly possible to see two main peaks over the year, one during february and one during october. at the same time, during the summer the production significantly decreased, reaching its minimum value during the month of july.</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>The line chart illustrates the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It's clearly possible to see two main peaks over the year, one during February and one during October. At the same time, during the summer the production significantly decreased, reaching its minimum value during the month of July.</t>
+          <t>the line chart illustrates the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it's clearly possible to see two main peaks over the year, one during february and one during october. at the same time, during the summer the production significantly decreased, reaching its minimum value during the month of july.</t>
         </is>
       </c>
       <c r="W38" t="n">
@@ -3660,12 +3660,12 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>The graph illustrates the total number of vehicles from the United States entering Canada. Data for every month of 2016 is shown. The numbers vary for each month. A high is reached in July (about 1300000 vehicles), probably because of people going on vacation. Low values can be found for the winter months, e.g., less than 700000 vehicles in January and February and roughly 700000 vehicles in November and December.</t>
+          <t>the graph illustrates the total number of vehicles from the united states entering canada. data for every month of 2016 is shown. the numbers vary for each month. a high is reached in july (about 1300000 vehicles), probably because of people going on vacation. low values can be found for the winter months, e.g., less than 700000 vehicles in january and february and roughly 700000 vehicles in november and december.</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>The graph illustrates the total TKN_UOM  of TKN_About   TKN_Geo . Data for every month of  TKN_Year  is shown. The TKN_UOM s vary for each month. A high is reached in July (about 110 vehicles), probably because of people going on vacation. Low values can be found for the winter months, e.g., less than 11 vehicles in January and February and roughly 11 vehicles in November and December.</t>
+          <t>the graph illustrates the total TKN_UOM  of TKN_About  canada. data for every month of  TKN_Year  is shown. the TKN_UOM s vary for each month. a high is reached in july (about 110 vehicles), probably because of people going on vacation. low values can be found for the winter months, e.g., less than 11 vehicles in january and february and roughly 11 vehicles in november and december.</t>
         </is>
       </c>
       <c r="W39" t="n">
@@ -3744,12 +3744,12 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>The graph shows the the number of United States vehicles entering Canada in 2018. As illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. For the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
+          <t>the graph shows the the number of united states vehicles entering canada in 2018. as illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. for the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>The graph shows the the TKN_UOM  of TKN_About   TKN_Geo  in  TKN_Year . As illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. For the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
+          <t>the graph shows the the TKN_UOM  of TKN_About  canada in  TKN_Year . as illustrated form the graph, the spring months show the amount of cars steadily increasing and reaching their highest point in summer. for the following months, in fall, the amount of cars entering decline and reach their lowest point in winter.</t>
         </is>
       </c>
       <c r="W40" t="n">
@@ -3828,12 +3828,12 @@
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>The following line chart is about the production of malt in Canada 2018. The values are reported using tonnes as unit of measure. It clearly possible to see several peaks and dips of production over the year. In particular, the maximum values have been recorded during March and July. It's also illustrated a significant fall of the production from July to August.</t>
+          <t>the following line chart is about the production of malt in canada 2018. the values are reported using tonnes as unit of measure. it clearly possible to see several peaks and dips of production over the year. in particular, the maximum values have been recorded during march and july. it's also illustrated a significant fall of the production from july to august.</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About  in  TKN_Geo   TKN_Year . The values are reported using TKN_UOM  as unit of measure. It clearly possible to see several peaks and dips of production over the year. In particular, the maximum values have been recorded during March and July. It's also illustrated a significant fall of the production from July to August.</t>
+          <t>the following line chart is about the TKN_About  in canada  TKN_Year . the values are reported using TKN_UOM  as unit of measure. it clearly possible to see several peaks and dips of production over the year. in particular, the maximum values have been recorded during march and july. it's also illustrated a significant fall of the production from july to august.</t>
         </is>
       </c>
       <c r="W41" t="n">
@@ -3912,12 +3912,12 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>The line graph depicts the price index of tablet computers in Canada for every month of 2018. The overall trend for this year is a decrease. January recorded a high of 820, whereas November had a low of 755.</t>
+          <t>the line graph depicts the price index of tablet computers in canada for every month of 2018. the overall trend for this year is a decrease. january recorded a high of 820, whereas november had a low of 755.</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>The line graph depicts the TKN_About  in  TKN_Geo  for every month of  TKN_Year . The overall trend for this year is a decrease. January recorded a high of 99, whereas November had a low of 1.</t>
+          <t>the line graph depicts the TKN_About  in canada for every month of  TKN_Year . the overall trend for this year is a decrease. january recorded a high of 99, whereas november had a low of 1.</t>
         </is>
       </c>
       <c r="W42" t="n">
@@ -3996,12 +3996,12 @@
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the price index about desktop and similar computer in Canada during 2018 slowly decreased over the year with several fluctuations. During January and February the values remain stable, without any changes. The minimum values have been recorded during August and October.</t>
+          <t>as it can be seen from the graph, the price index about desktop and similar computer in canada during 2018 slowly decreased over the year with several fluctuations. during january and february the values remain stable, without any changes. the minimum values have been recorded during august and october.</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the TKN_About  computer in  TKN_Geo  during  TKN_Year  slowly decreased over the year with several fluctuations. During January and February the values remain stable, without any changes. The minimum values have been recorded during August and October.</t>
+          <t>as it can be seen from the graph, the TKN_About  computer in canada during  TKN_Year  slowly decreased over the year with several fluctuations. during january and february the values remain stable, without any changes. the minimum values have been recorded during august and october.</t>
         </is>
       </c>
       <c r="W43" t="n">
@@ -4080,12 +4080,12 @@
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>The graph shows the production of fresh vegetables in Canada for the year fo 2018. The graph shows production steadily increasing till October and then declines in the months after. It is important to note that production at the end of the year in December is much higher than it was beginning the year in January.</t>
+          <t>the graph shows the production of fresh vegetables in canada for the year fo 2018. the graph shows production steadily increasing till october and then declines in the months after. it is important to note that production at the end of the year in december is much higher than it was beginning the year in january.</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  in  TKN_Geo  for the year fo  TKN_Year . The graph shows production steadily increasing till October and then declines in the months after. It is important to note that production at the end of the year in December is much higher than it was beginning the year in January.</t>
+          <t>the graph shows the TKN_About  in canada for the year fo  TKN_Year . the graph shows production steadily increasing till october and then declines in the months after. it is important to note that production at the end of the year in december is much higher than it was beginning the year in january.</t>
         </is>
       </c>
       <c r="W44" t="n">
@@ -4164,12 +4164,12 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>The graph is a line chart, illustrating the commercial software price index in Canada. The data used is from 2018. The y-axis showing the index ranges from 1125 to 1170. The index increased over the months of the year, with some ups and downs in between. The lowest and highest values were found in January (1129) and December (1167), respectively.</t>
+          <t>the graph is a line chart, illustrating the commercial software price index in canada. the data used is from 2018. the y-axis showing the index ranges from 1125 to 1170. the index increased over the months of the year, with some ups and downs in between. the lowest and highest values were found in january (1129) and december (1167), respectively.</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>The graph is a line chart, illustrating the TKN_About  in  TKN_Geo . The data used is from  TKN_Year . The y-axis showing the index ranges from -11 to 108. The index increased over the months of the year, with some ups and downs in between. The lowest and highest values were found in January (0) and December (100), respectively.</t>
+          <t>the graph is a line chart, illustrating the TKN_About  in canada. the data used is from  TKN_Year . the y-axis showing the index ranges from -11 to 108. the index increased over the months of the year, with some ups and downs in between. the lowest and highest values were found in january (0) and december (100), respectively.</t>
         </is>
       </c>
       <c r="W45" t="n">
@@ -4248,12 +4248,12 @@
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>From the graph it is clear that desktop and similar computers are cheapest during the months of August, September, and October for the 2016 year. They are the most expensive in February but see a steady decline until the month of September.</t>
+          <t>from the graph it is clear that desktop and similar computers are cheapest during the months of august, september, and october for the 2016 year. they are the most expensive in february but see a steady decline until the month of september.</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>From the graph it is clear TKN_About  are cheapest during the months of August, September, and October for the  TKN_Year  year. They are the most expensive in February but see a steady decline until the month of September.</t>
+          <t>from the graph it is clear TKN_About  are cheapest during the months of august, september, and october for the  TKN_Year  year. they are the most expensive in february but see a steady decline until the month of september.</t>
         </is>
       </c>
       <c r="W46" t="n">
@@ -4332,12 +4332,12 @@
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>This line graph illustrates the total number of Canadian vehicles that returned to the country in 2018. The x-axis shows the different months of the year, whereas the y-axis shows the number of vehicles. There is a rise in the first months of the year, reaching a high in August (2300000). Numbers decrease over the last months of the year.</t>
+          <t>this line graph illustrates the total number of canadian vehicles that returned to the country in 2018. the x-axis shows the different months of the year, whereas the y-axis shows the number of vehicles. there is a rise in the first months of the year, reaching a high in august (2300000). numbers decrease over the last months of the year.</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>This line graph illustrates the total TKN_UOM  of TKN_About  in  TKN_Year . The x-axis shows the different months of the year, whereas the y-axis shows the TKN_UOM  of vehicles. There is a rise in the first months of the year, reaching a high in August (101).  TKN_UOM s decrease over the last months of the year.</t>
+          <t>this line graph illustrates the total TKN_UOM  of TKN_About  in  TKN_Year . the x-axis shows the different months of the year, whereas the y-axis shows the TKN_UOM  of vehicles. there is a rise in the first months of the year, reaching a high in august (101). TKN_UOM s decrease over the last months of the year.</t>
         </is>
       </c>
       <c r="W47" t="n">
@@ -4416,12 +4416,12 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>The graph shows the land price index (index 347) in Canada in 2017. Data entries are broken down into the months of the year. The graph's trend is a rise over the months. The value in January is 1006, the one for December is 1038. The steepest incline can be found between March and May.</t>
+          <t>the graph shows the land price index (index 347) in canada in 2017. data entries are broken down into the months of the year. the graph's trend is a rise over the months. the value in january is 1006, the one for december is 1038. the steepest incline can be found between march and may.</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  TKN_UOM  (index 347) in  TKN_Geo  in  TKN_Year . Data entries are broken down into the months of the year. The graph's trend is a rise over the months. The value in January is 6, the one for December is 103. The steepest incline can be found between March and May.</t>
+          <t>the graph shows TKN_About  TKN_UOM  (index 347) in canada in  TKN_Year . data entries are broken down into the months of the year. the graph's trend is a rise over the months. the value in january is 6, the one for december is 103. the steepest incline can be found between march and may.</t>
         </is>
       </c>
       <c r="W48" t="n">
@@ -4500,12 +4500,12 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>The chart is showing the values about the production of fresh vegetables in Canada during 2016. The values are illustrated using the farm product price index (FPPI). As can be seen from the graph, from January to May the values have been rapidly decreasing. Then, a peak has been recorded during the month of June, but after that the values started to decrease again until October. During the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of December.</t>
+          <t>the chart is showing the values about the production of fresh vegetables in canada during 2016. the values are illustrated using the farm product price index (fppi). as can be seen from the graph, from january to may the values have been rapidly decreasing. then, a peak has been recorded during the month of june, but after that the values started to decrease again until october. during the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of december.</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>The chart is showing the values about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are illustrated using TKN_UOM  (FPPI). As can be seen from the graph, from January to May the values have been rapidly decreasing. Then, a peak has been recorded during the month of June, but after that the values started to decrease again until October. During the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of December.</t>
+          <t>the chart is showing the values about the TKN_About  in canada during  TKN_Year . the values are illustrated using TKN_UOM  (fppi). as can be seen from the graph, from january to may the values have been rapidly decreasing. then, a peak has been recorded during the month of june, but after that the values started to decrease again until october. during the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of december.</t>
         </is>
       </c>
       <c r="W49" t="n">
@@ -4584,12 +4584,12 @@
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>The following graph shows information about the house and land price index in Canada during 2017. As can be seen from the graph, the index have been steadily increasing its value over the year. There are few light fluctuations but no peaks or dips have been recorded.</t>
+          <t>the following graph shows information about the house and land price index in canada during 2017. as can be seen from the graph, the index have been steadily increasing its value over the year. there are few light fluctuations but no peaks or dips have been recorded.</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>The following graph shows information about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . As can be seen from the graph, the index have been steadily increasing its value over the year. There are few light fluctuations but no peaks or dips have been recorded.</t>
+          <t>the following graph shows information about TKN_About  TKN_UOM  in canada during  TKN_Year . as can be seen from the graph, the index have been steadily increasing its value over the year. there are few light fluctuations but no peaks or dips have been recorded.</t>
         </is>
       </c>
       <c r="W50" t="n">
@@ -4668,12 +4668,12 @@
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>The land price index for Canada during the year of 2018 increased from April to December. The price index plateaued during the months of March through April, June through August, September through October and November through December.</t>
+          <t>the land price index for canada during the year of 2018 increased from april to december. the price index plateaued during the months of march through april, june through august, september through october and november through december.</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>The land TKN_UOM  for  TKN_Geo  during the year of  TKN_Year  increased from April to December. The TKN_UOM  plateaued during the months of March through April, June through August, September through October and November through December.</t>
+          <t>the land TKN_UOM  for canada during the year of  TKN_Year  increased from april to december. the TKN_UOM  plateaued during the months of march through april, june through august, september through october and november through december.</t>
         </is>
       </c>
       <c r="W51" t="n">
@@ -4752,12 +4752,12 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>The graph depicts a price index of servers in Canada. Data was taken from 2018. One can observe a decline in the price index within the first months of the year, reaching a low of 997 in April. Throughout the following three months, the index increased to 1013 in July. Values decreased steadily until October (1006) and stayed the same for November and December (1008).</t>
+          <t>the graph depicts a price index of servers in canada. data was taken from 2018. one can observe a decline in the price index within the first months of the year, reaching a low of 997 in april. throughout the following three months, the index increased to 1013 in july. values decreased steadily until october (1006) and stayed the same for november and december (1008).</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>The graph depicts a TKN_About  in  TKN_Geo . Data was taken from  TKN_Year . One can observe a decline in the price index within the first months of the year, reaching a low of 0 in April. Throughout the following three months, the index increased to 100 in July. Values decreased steadily until October (56) and stayed the same for November and December (69).</t>
+          <t>the graph depicts a TKN_About  in canada. data was taken from  TKN_Year . one can observe a decline in the price index within the first months of the year, reaching a low of 0 in april. throughout the following three months, the index increased to 100 in july. values decreased steadily until october (56) and stayed the same for november and december (69).</t>
         </is>
       </c>
       <c r="W52" t="n">
@@ -4836,12 +4836,12 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>The hardwood production for Canada in 2018 rapidly declined in July 2018. The production then steadily recovered until October, and then fell again until December.</t>
+          <t>the hardwood production for canada in 2018 rapidly declined in july 2018. the production then steadily recovered until october, and then fell again until december.</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>The TKN_About  for  TKN_Geo  in  TKN_Year  rapidly declined in July  TKN_Year . The production then steadily recovered until October, and then fell again until December.</t>
+          <t>the TKN_About  for canada in  TKN_Year  rapidly declined in july  TKN_Year . the production then steadily recovered until october, and then fell again until december.</t>
         </is>
       </c>
       <c r="W53" t="n">
@@ -4920,12 +4920,12 @@
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>The following chart provides information about the house and land price index in Canada during 2018. It's clearly possible to see how the index value significantly dropped down between January and February. Over the next few months the index value remained stable. It raised up again during the summer, reaching the same value of January during the month of June. From June to December the index value maintained the same level.</t>
+          <t>the following chart provides information about the house and land price index in canada during 2018. it's clearly possible to see how the index value significantly dropped down between january and february. over the next few months the index value remained stable. it raised up again during the summer, reaching the same value of january during the month of june. from june to december the index value maintained the same level.</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>The following chart provides information about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . It's clearly possible to see how the index value significantly dropped down between January and February. Over the next few months the index value remained stable. It raised up again during the summer, reaching the same value of January during the month of June. From June to December the index value maintained the same level.</t>
+          <t>the following chart provides information about TKN_About  TKN_UOM  in canada during  TKN_Year . it's clearly possible to see how the index value significantly dropped down between january and february. over the next few months the index value remained stable. it raised up again during the summer, reaching the same value of january during the month of june. from june to december the index value maintained the same level.</t>
         </is>
       </c>
       <c r="W54" t="n">
@@ -5004,12 +5004,12 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>This line chart depicts the house price index of houses in Canada in 2017. It is broken down into the months of the year. Values are ranging from 998 to 1033. The graph's overall trend is a continuous increase over the months. The lowest value was found for January (998), whereas the highest value was recorded for November and December (1033).</t>
+          <t>this line chart depicts the house price index of houses in canada in 2017. it is broken down into the months of the year. values are ranging from 998 to 1033. the graph's overall trend is a continuous increase over the months. the lowest value was found for january (998), whereas the highest value was recorded for november and december (1033).</t>
         </is>
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>This line chart depicts TKN_About  TKN_UOM  of houses in  TKN_Geo  in  TKN_Year . It is broken down into the months of the year. Values are ranging from -3 to 103. The graph's overall trend is a continuous increase over the months. The lowest value was found for January (-3), whereas the highest value was recorded for November and December (103).</t>
+          <t>this line chart depicts TKN_About  TKN_UOM  of houses in canada in  TKN_Year . it is broken down into the months of the year. values are ranging from -3 to 103. the graph's overall trend is a continuous increase over the months. the lowest value was found for january (-3), whereas the highest value was recorded for november and december (103).</t>
         </is>
       </c>
       <c r="W55" t="n">
@@ -5088,12 +5088,12 @@
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>The production of creamy butter reached its highest point in January of 2018. Thereafter, production declined in February and then recovered in May. In the months following production steadily decreased until September. Thereafter, the graph fluctuated from October to December.</t>
+          <t>the production of creamy butter reached its highest point in january of 2018. thereafter, production declined in february and then recovered in may. in the months following production steadily decreased until september. thereafter, the graph fluctuated from october to december.</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>The TKN_About  reached its highest point in January of  TKN_Year . Thereafter, production declined in February and then recovered in May. In the months following production steadily decreased until September. Thereafter, the graph fluctuated from October to December.</t>
+          <t>the TKN_About  reached its highest point in january of  TKN_Year . thereafter, production declined in february and then recovered in may. in the months following production steadily decreased until september. thereafter, the graph fluctuated from october to december.</t>
         </is>
       </c>
       <c r="W56" t="n">
@@ -5172,12 +5172,12 @@
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>In this graph, one can see the total softwood and hardwood production in Canada. Production of 2016 is measured in cubic meters. The graph is M-shaped, with lows in January, July, and December and highs in March and November.</t>
+          <t>in this graph, one can see the total softwood and hardwood production in canada. production of 2016 is measured in cubic meters. the graph is m-shaped, with lows in january, july, and december and highs in march and november.</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>In this graph, one can see the TKN_About  in  TKN_Geo . Production of  TKN_Year  is measured TKN_UOM  meters. The graph is M-shaped, with lows in January, July, and December and highs in March and November.</t>
+          <t>in this graph, one can see the TKN_About  in canada. production of  TKN_Year  is measured TKN_UOM  meters. the graph is m-shaped, with lows in january, july, and december and highs in march and november.</t>
         </is>
       </c>
       <c r="W57" t="n">
@@ -5256,12 +5256,12 @@
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>The following line chart is about the house and land price index in Canada during 2016. From the graph it's clearly possible to see how the index values have been steadily growing during 2016. Few light fluctuations have been reported during the summer months.</t>
+          <t>the following line chart is about the house and land price index in canada during 2016. from the graph it's clearly possible to see how the index values have been steadily growing during 2016. few light fluctuations have been reported during the summer months.</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>The following line chart is about TKN_About  TKN_UOM  in  TKN_Geo  during  TKN_Year . From the graph it's clearly possible to see how the index values have been steadily growing during  TKN_Year . Few light fluctuations have been reported during the summer months.</t>
+          <t>the following line chart is about TKN_About  TKN_UOM  in canada during  TKN_Year . from the graph it's clearly possible to see how the index values have been steadily growing during  TKN_Year . few light fluctuations have been reported during the summer months.</t>
         </is>
       </c>
       <c r="W58" t="n">
@@ -5340,12 +5340,12 @@
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>The graph illustrated the production of fresh potatoes in Canada in 2017. The measurement used is the farm product price index (FPPI): There is a clear peak in August, reaching an index of more than 1800.</t>
+          <t>the graph illustrated the production of fresh potatoes in canada in 2017. the measurement used is the farm product price index (fppi): there is a clear peak in august, reaching an index of more than 1800.</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>The graph illustrated the TKN_About  in  TKN_Geo  in  TKN_Year . The measurement used is TKN_UOM  (FPPI): There is a clear peak in August, reaching an index of more than 96.</t>
+          <t>the graph illustrated the TKN_About  in canada in  TKN_Year . the measurement used is TKN_UOM  (fppi): there is a clear peak in august, reaching an index of more than 96.</t>
         </is>
       </c>
       <c r="W59" t="n">
@@ -5424,12 +5424,12 @@
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>The price index for servers in 2018 rapidly fell from a high in January, to its lowest point in March of 2016. After that the price index saw some fluctuation in the coming months until November, where it dropped again and did not change in December.</t>
+          <t>the price index for servers in 2018 rapidly fell from a high in january, to its lowest point in march of 2016. after that the price index saw some fluctuation in the coming months until november, where it dropped again and did not change in december.</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>The TKN_About  in 2018 rapidly fell from a high in January, to its lowest point in March of  TKN_Year . After that the price index saw some fluctuation in the coming months until November, where it dropped again and did not change in December.</t>
+          <t>the TKN_About  in 2018 rapidly fell from a high in january, to its lowest point in march of  TKN_Year . after that the price index saw some fluctuation in the coming months until november, where it dropped again and did not change in december.</t>
         </is>
       </c>
       <c r="W60" t="n">
@@ -5508,12 +5508,12 @@
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>The following line chart provides useful information about the production of new motor vehicles in Canada during 2016. The production value is quantified using the number of units producted. During the first few months of the year the production rapidly increased, reaching the maximum value over 2016 in March. After that, over the next few months, the production of new motor vehicles slightly decreased until the end of the year.</t>
+          <t>the following line chart provides useful information about the production of new motor vehicles in canada during 2016. the production value is quantified using the number of units producted. during the first few months of the year the production rapidly increased, reaching the maximum value over 2016 in march. after that, over the next few months, the production of new motor vehicles slightly decreased until the end of the year.</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>The following line chart provides useful information about the TKN_About  in  TKN_Geo  during  TKN_Year . The production value is quantified using the number of TKN_UOM  producted. During the first few months of the year the production rapidly increased, reaching the maximum value over  TKN_Year  in March. After that, over the next few months, the TKN_About  slightly decreased until the end of the year.</t>
+          <t>the following line chart provides useful information about the TKN_About  in canada during  TKN_Year . the production value is quantified using the number of TKN_UOM  producted. during the first few months of the year the production rapidly increased, reaching the maximum value over  TKN_Year  in march. after that, over the next few months, the TKN_About  slightly decreased until the end of the year.</t>
         </is>
       </c>
       <c r="W61" t="n">
@@ -5592,12 +5592,12 @@
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>In this graph, the price index of laptop computers can be seen. The data illustrated was collected in Canada in 2016. The graph's line shows many ups and downs, with an overall high in February and May (index of 1010) and an overall low in August (index of 997).</t>
+          <t>in this graph, the price index of laptop computers can be seen. the data illustrated was collected in canada in 2016. the graph's line shows many ups and downs, with an overall high in february and may (index of 1010) and an overall low in august (index of 997).</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>In this graph, the TKN_About  can be seen. The data illustrated was collected in  TKN_Geo  in  TKN_Year . The graph's line shows many ups and downs, with an overall high in February and May (index of 100) and an overall low in August (index of 13).</t>
+          <t>in this graph, the TKN_About  can be seen. the data illustrated was collected in canada in  TKN_Year . the graph's line shows many ups and downs, with an overall high in february and may (index of 100) and an overall low in august (index of 13).</t>
         </is>
       </c>
       <c r="W62" t="n">
@@ -5676,12 +5676,12 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>The graph shows the total farm production index in Canada for the year 2016. The graph reaches its highest point in June and then steadily drops each month until reaching its lowest point in October. Thereafter, it slowly recovers until December.</t>
+          <t>the graph shows the total farm production index in canada for the year 2016. the graph reaches its highest point in june and then steadily drops each month until reaching its lowest point in october. thereafter, it slowly recovers until december.</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>The graph shows TKN_UOM  in  TKN_Geo  for the year  TKN_Year . The graph reaches its highest point in June and then steadily drops each month until reaching its lowest point in October. Thereafter, it slowly recovers until December.</t>
+          <t>the graph shows TKN_UOM  in canada for the year  TKN_Year . the graph reaches its highest point in june and then steadily drops each month until reaching its lowest point in october. thereafter, it slowly recovers until december.</t>
         </is>
       </c>
       <c r="W63" t="n">
@@ -5760,12 +5760,12 @@
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>The following graph shows information about the laptop computer price index in Canada during 2017. The overall trend is descending. It's clearly possible to see several fluctuations over the year, mainly during the summer months. The maximum value has been recorded during February and the minimum one during December.</t>
+          <t>the following graph shows information about the laptop computer price index in canada during 2017. the overall trend is descending. it's clearly possible to see several fluctuations over the year, mainly during the summer months. the maximum value has been recorded during february and the minimum one during december.</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>The following graph shows information about the TKN_About  index in  TKN_Geo  during  TKN_Year . The overall trend is descending. It's clearly possible to see several fluctuations over the year, mainly during the summer months. The maximum value has been recorded during February and the minimum one during December.</t>
+          <t>the following graph shows information about the TKN_About  index in canada during  TKN_Year . the overall trend is descending. it's clearly possible to see several fluctuations over the year, mainly during the summer months. the maximum value has been recorded during february and the minimum one during december.</t>
         </is>
       </c>
       <c r="W64" t="n">
@@ -5844,12 +5844,12 @@
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>In this graph, the production of rye in Canada is illustrated. The x-axis shows the months of the year of 2016, whereas the y-axis depicts the production in tonnes. Values in August and September stand out, reaching almost 25000 in September. During the remaining months of the year, production is comparably lower.</t>
+          <t>in this graph, the production of rye in canada is illustrated. the x-axis shows the months of the year of 2016, whereas the y-axis depicts the production in tonnes. values in august and september stand out, reaching almost 25000 in september. during the remaining months of the year, production is comparably lower.</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>In this graph, the TKN_About  in  TKN_Geo  is illustrated. The x-axis shows the months of the year of  TKN_Year , whereas the y-axis depicts the production in tonnes. Values in August and September stand out, reaching almost 102 in September. During the remaining months of the year, production is comparably lower.</t>
+          <t>in this graph, the TKN_About  in canada is illustrated. the x-axis shows the months of the year of  TKN_Year , whereas the y-axis depicts the production in tonnes. values in august and september stand out, reaching almost 102 in september. during the remaining months of the year, production is comparably lower.</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -5928,12 +5928,12 @@
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>The graph depicts the fluctuation of softwood and hard wood production from January to November in 2017. Production then sharply declined from November to December, reaching its lowest point.</t>
+          <t>the graph depicts the fluctuation of softwood and hard wood production from january to november in 2017. production then sharply declined from november to december, reaching its lowest point.</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>The graph depicts the fluctuation of TKN_About  from January to November in  TKN_Year . Production then sharply declined from November to December, reaching its lowest point.</t>
+          <t>the graph depicts the fluctuation of TKN_About  from january to november in  TKN_Year . production then sharply declined from november to december, reaching its lowest point.</t>
         </is>
       </c>
       <c r="W66" t="n">
@@ -6012,12 +6012,12 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>The shown line chart provides information about the production of fresh fruit in Canada during 2018. The values are described using the farm product price index (FPPI). It's clearly possible to see two significant peaks during the months of March and August. Then the overall value of production remain quite stable during the year.</t>
+          <t>the shown line chart provides information about the production of fresh fruit in canada during 2018. the values are described using the farm product price index (fppi). it's clearly possible to see two significant peaks during the months of march and august. then the overall value of production remain quite stable during the year.</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>The shown line chart provides information about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It's clearly possible to see two significant peaks during the months of March and August. Then the overall value of production remain quite stable during the year.</t>
+          <t>the shown line chart provides information about the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it's clearly possible to see two significant peaks during the months of march and august. then the overall value of production remain quite stable during the year.</t>
         </is>
       </c>
       <c r="W67" t="n">
@@ -6096,12 +6096,12 @@
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>This graph shows the production of chickens, turkeys, chicks, and poults, measured by the farm product price index. The recorded data is from Canada, 2016. The graph's line reaches its high in October, with an index of 1243. The decline in the following month stands out, resulting in an index of 1201 in November and December.</t>
+          <t>this graph shows the production of chickens, turkeys, chicks, and poults, measured by the farm product price index. the recorded data is from canada, 2016. the graph's line reaches its high in october, with an index of 1243. the decline in the following month stands out, resulting in an index of 1201 in november and december.</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>This graph shows the TKN_About  and poults, measured TKN_UOM  index. The recorded data is from  TKN_Geo ,  TKN_Year . The graph's line reaches its high in October, with an index of 100. The decline in the following month stands out, resulting in an index of 0 in November and December.</t>
+          <t>this graph shows the TKN_About  and poults, measured TKN_UOM  index. the recorded data is from canada,  TKN_Year . the graph's line reaches its high in october, with an index of 100. the decline in the following month stands out, resulting in an index of 0 in november and december.</t>
         </is>
       </c>
       <c r="W68" t="n">
@@ -6180,12 +6180,12 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>A line chart displaying Canadian vehicles returning to Canada each month in 2018.  It indicates that travel was lowest during the winter months, reaching a minimum in February, and highest in the summer months, peaking in August (but with a slight dip in June).  The median number of returning vehicles is between 1900000 and 2000000.</t>
+          <t>a line chart displaying canadian vehicles returning to canada each month in 2018.  it indicates that travel was lowest during the winter months, reaching a minimum in february, and highest in the summer months, peaking in august (but with a slight dip in june).  the median number of returning vehicles is between 1900000 and 2000000.</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>A line TKN_About   TKN_Geo  each month in  TKN_Year .  It indicates that travel was lowest during the winter months, reaching a minimum in February, and highest in the summer months, peaking in August (but with a slight dip in June).  The median TKN_UOM  of returning vehicles is between 50 and 63.</t>
+          <t>a line TKN_About  canada each month in  TKN_Year .  it indicates that travel was lowest during the winter months, reaching a minimum in february, and highest in the summer months, peaking in august (but with a slight dip in june).  the median TKN_UOM  of returning vehicles is between 50 and 63.</t>
         </is>
       </c>
       <c r="W69" t="n">
@@ -6264,12 +6264,12 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>A figure indicating canola production in Canada each month in 2018.  There do not seem to be any seasonal trends in the production.  The maximum production occurred in October, at over 1400000 tonnes; and production fell below 600000 tonnes in February, August and September.</t>
+          <t>a figure indicating canola production in canada each month in 2018.  there do not seem to be any seasonal trends in the production.  the maximum production occurred in october, at over 1400000 tonnes; and production fell below 600000 tonnes in february, august and september.</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>A figure indicating TKN_About  in  TKN_Geo  each month in  TKN_Year .  There do not seem to be any seasonal trends in the production.  The maximum production occurred in October, at over 97 TKN_UOM ; and production fell below 10 TKN_UOM  in February, August and September.</t>
+          <t>a figure indicating TKN_About  in canada each month in  TKN_Year .  there do not seem to be any seasonal trends in the production.  the maximum production occurred in october, at over 97 TKN_UOM ; and production fell below 10 TKN_UOM  in february, august and september.</t>
         </is>
       </c>
       <c r="W70" t="n">
@@ -6348,12 +6348,12 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>Softwood and hardwood stock totals in Canada during each month of 2016.  The total rose from slightly over 72000 cubic meters in January to over 75000 cubic meters in April.  It then experienced a drop to less than 68000 cubic meters from May to July, after which it continued to decline until reaching a minimum level in December of under 66000 cubic meters.</t>
+          <t>softwood and hardwood stock totals in canada during each month of 2016.  the total rose from slightly over 72000 cubic meters in january to over 75000 cubic meters in april.  it then experienced a drop to less than 68000 cubic meters from may to july, after which it continued to decline until reaching a minimum level in december of under 66000 cubic meters.</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>Softwood and hardwood stock totals in  TKN_Geo  during each month of  TKN_Year .  The total rose from slightly over TKN_UOM  meters in January to over 97 cubic meters in April.  It then experienced a drop to less than 24 cubic meters from May to July, after which it continued to decline until reaching a minimum level in December of under 4 cubic meters.</t>
+          <t>softwood and hardwood stock totals in canada during each month of  TKN_Year .  the total rose from slightly over TKN_UOM  meters in january to over 97 cubic meters in april.  it then experienced a drop to less than 24 cubic meters from may to july, after which it continued to decline until reaching a minimum level in december of under 4 cubic meters.</t>
         </is>
       </c>
       <c r="W71" t="n">
@@ -6432,12 +6432,12 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>Tablet computer price index in Canada for 2016.  The price index slowly trended downwards throughout the year but experienced three significant drops: in March, in September (possibly coinciding with back-to-school sales), and in December (possibly due to Boxing Day and Boxing Week sales).</t>
+          <t>tablet computer price index in canada for 2016.  the price index slowly trended downwards throughout the year but experienced three significant drops: in march, in september (possibly coinciding with back-to-school sales), and in december (possibly due to boxing day and boxing week sales).</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>Tablet computer price index in  TKN_Geo  for  TKN_Year .  The price index slowly trended downwards throughout the year but experienced three significant drops: in March, in September (possibly coinciding with back-to-school sales), and in December (possibly due to Boxing Day and Boxing Week sales).</t>
+          <t>tablet computer price index in canada for  TKN_Year .  the price index slowly trended downwards throughout the year but experienced three significant drops: in march, in september (possibly coinciding with back-to-school sales), and in december (possibly due to boxing day and boxing week sales).</t>
         </is>
       </c>
       <c r="W72" t="n">
@@ -6516,12 +6516,12 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>The following line chart provides information about the total production of hardwood in Canada during 2017. The production values have been described using cubic metres as unit of measure. The values have been strongly fluactuating over the year. It shows several peaks and dips over the year. Even that, the maximum value has been recorded during March and the minimum during July.</t>
+          <t>the following line chart provides information about the total production of hardwood in canada during 2017. the production values have been described using cubic metres as unit of measure. the values have been strongly fluactuating over the year. it shows several peaks and dips over the year. even that, the maximum value has been recorded during march and the minimum during july.</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>The following line chart provides information about the TKN_About  of hardwood in  TKN_Geo  during  TKN_Year . The production values have been described using TKN_UOM  as unit of measure. The values have been strongly fluactuating over the year. It shows several peaks and dips over the year. Even that, the maximum value has been recorded during March and the minimum during July.</t>
+          <t>the following line chart provides information about the TKN_About  of hardwood in canada during  TKN_Year . the production values have been described using TKN_UOM  as unit of measure. the values have been strongly fluactuating over the year. it shows several peaks and dips over the year. even that, the maximum value has been recorded during march and the minimum during july.</t>
         </is>
       </c>
       <c r="W73" t="n">
@@ -6600,12 +6600,12 @@
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>The line chart is describing the values about production of grains in Canada during 2018. The production amout is described using the farm product price index (FPPI). The minimum recorded value is during February. The maximum recorded value is during August. Furthermore, there are several fluctuations over the year.</t>
+          <t>the line chart is describing the values about production of grains in canada during 2018. the production amout is described using the farm product price index (fppi). the minimum recorded value is during february. the maximum recorded value is during august. furthermore, there are several fluctuations over the year.</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>The line chart is describing the values about TKN_About  in  TKN_Geo  during  TKN_Year . The production amout is described using TKN_UOM  (FPPI). The minimum recorded value is during February. The maximum recorded value is during August. Furthermore, there are several fluctuations over the year.</t>
+          <t>the line chart is describing the values about TKN_About  in canada during  TKN_Year . the production amout is described using TKN_UOM  (fppi). the minimum recorded value is during february. the maximum recorded value is during august. furthermore, there are several fluctuations over the year.</t>
         </is>
       </c>
       <c r="W74" t="n">
@@ -6684,12 +6684,12 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>The shown graph is about the production of rye in Canada during 2018. The production values are quantified using tonnes as unit of measure. As can be seen from the graph, the values are oscillating over the year. Just one significant peak has been recorded during August 2018. The minimum value over the year was during December.</t>
+          <t>the shown graph is about the production of rye in canada during 2018. the production values are quantified using tonnes as unit of measure. as can be seen from the graph, the values are oscillating over the year. just one significant peak has been recorded during august 2018. the minimum value over the year was during december.</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>The shown graph is about the TKN_About  in  TKN_Geo  during  TKN_Year . The production values are quantified using TKN_UOM  as unit of measure. As can be seen from the graph, the values are oscillating over the year. Just one significant peak has been recorded during August  TKN_Year . The minimum value over the year was during December.</t>
+          <t>the shown graph is about the TKN_About  in canada during  TKN_Year . the production values are quantified using TKN_UOM  as unit of measure. as can be seen from the graph, the values are oscillating over the year. just one significant peak has been recorded during august  TKN_Year . the minimum value over the year was during december.</t>
         </is>
       </c>
       <c r="W75" t="n">
@@ -6768,12 +6768,12 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>Poultry production cost for each month in Canada in 2018.  The cost index, at its lowest near the beginning of the year, steadily rose from less than 1180 in March to over 1260 August, then settled in September at roughly 1240.</t>
+          <t>poultry production cost for each month in canada in 2018.  the cost index, at its lowest near the beginning of the year, steadily rose from less than 1180 in march to over 1260 august, then settled in september at roughly 1240.</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>Poultry production cost for each month in  TKN_Geo  in  TKN_Year .  The cost index, at its lowest TKN_About  year, steadily rose from less than 7 in March to over 93 August, then settled in September at roughly 71.</t>
+          <t>poultry production cost for each month in canada in  TKN_Year .  the cost index, at its lowest TKN_About  year, steadily rose from less than 7 in march to over 93 august, then settled in september at roughly 71.</t>
         </is>
       </c>
       <c r="W76" t="n">
@@ -6852,12 +6852,12 @@
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>Hardwood production in Canada for each month of 2017.  While production varied between less than 1100 cubic metres and over 1500 cubic metres in a given month, there do not seem to be any trends in the value over time.</t>
+          <t>hardwood production in canada for each month of 2017.  while production varied between less than 1100 cubic metres and over 1500 cubic metres in a given month, there do not seem to be any trends in the value over time.</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>Hardwood production in  TKN_Geo  for each month of  TKN_Year .  While production varied between less than 11 TKN_UOM  and over 99 TKN_UOM  in a given month, there do not seem to be any trends in the value over time.</t>
+          <t>hardwood production in canada for each month of  TKN_Year .  while production varied between less than 11 TKN_UOM  and over 99 TKN_UOM  in a given month, there do not seem to be any trends in the value over time.</t>
         </is>
       </c>
       <c r="W77" t="n">
@@ -6936,12 +6936,12 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>The graph describes the production of chickens, turkeys, chicks and poults in Canada during 2018. The production value is described using the farm product price index (FPPI). As it can be seen from the graph, the production rapidly increased from January until August. After that, from August to December the production slightly decreased. The maximum value has been registered in August and the minimum one during February.</t>
+          <t>the graph describes the production of chickens, turkeys, chicks and poults in canada during 2018. the production value is described using the farm product price index (fppi). as it can be seen from the graph, the production rapidly increased from january until august. after that, from august to december the production slightly decreased. the maximum value has been registered in august and the minimum one during february.</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>The graph describes the TKN_About  in  TKN_Geo  during  TKN_Year . The production value is described using TKN_UOM  (FPPI). As it can be seen from the graph, the production rapidly increased from January until August. After that, from August to December the production slightly decreased. The maximum value has been registered in August and the minimum one during February.</t>
+          <t>the graph describes the TKN_About  in canada during  TKN_Year . the production value is described using TKN_UOM  (fppi). as it can be seen from the graph, the production rapidly increased from january until august. after that, from august to december the production slightly decreased. the maximum value has been registered in august and the minimum one during february.</t>
         </is>
       </c>
       <c r="W78" t="n">
@@ -7020,12 +7020,12 @@
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>The following line chart is decribing the trend of the total farm production index in Canada during 2018. The values are described using the farm product price index (FPPI). It can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. The most significant peak was recorded during the month of July 2018. The lowest values have been recorded during the months of September and December.</t>
+          <t>the following line chart is decribing the trend of the total farm production index in canada during 2018. the values are described using the farm product price index (fppi). it can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. the most significant peak was recorded during the month of july 2018. the lowest values have been recorded during the months of september and december.</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>The following line chart is decribing the trend of the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). It can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. The most significant peak was recorded during the month of July  TKN_Year . The lowest values have been recorded during the months of September and December.</t>
+          <t>the following line chart is decribing the trend of the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. the most significant peak was recorded during the month of july  TKN_Year . the lowest values have been recorded during the months of september and december.</t>
         </is>
       </c>
       <c r="W79" t="n">
@@ -7104,12 +7104,12 @@
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>Creamery butter imports into Canada in 2018.  Imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 1700 tonnes in June, followed by an equally sharp drop to a minimum value of less than 1100 tonnes in July.</t>
+          <t>creamery butter imports into canada in 2018.  imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 1700 tonnes in june, followed by an equally sharp drop to a minimum value of less than 1100 tonnes in july.</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>Creamery butter imports into  TKN_Geo  in  TKN_Year .  Imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 92 TKN_UOM  in June, followed by an equally sharp drop to a minimum value of less than 7 TKN_UOM  in July.</t>
+          <t>creamery butter imports into canada in  TKN_Year .  imports were higher overall during the second half of the year; however, the most noticeable feature is the sharp rise to a maximum value of over 92 TKN_UOM  in june, followed by an equally sharp drop to a minimum value of less than 7 TKN_UOM  in july.</t>
         </is>
       </c>
       <c r="W80" t="n">
@@ -7188,12 +7188,12 @@
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>The graph shows the values about the production of Wheat flour in Canada over 2018. The values are described using tonnes as unit of measure. There is a drop from January to February. It's possible to see how the production value rapidly increased from February to April. Then from April to December the production value slightly decreased, showing few light fluctuations.</t>
+          <t>the graph shows the values about the production of wheat flour in canada over 2018. the values are described using tonnes as unit of measure. there is a drop from january to february. it's possible to see how the production value rapidly increased from february to april. then from april to december the production value slightly decreased, showing few light fluctuations.</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>The graph shows the values about the TKN_About  in  TKN_Geo  over  TKN_Year . The values are described using TKN_UOM  as unit of measure. There is a drop from January to February. It's possible to see how the production value rapidly increased from February to April. Then from April to December the production value slightly decreased, showing few light fluctuations.</t>
+          <t>the graph shows the values about the TKN_About  in canada over  TKN_Year . the values are described using TKN_UOM  as unit of measure. there is a drop from january to february. it's possible to see how the production value rapidly increased from february to april. then from april to december the production value slightly decreased, showing few light fluctuations.</t>
         </is>
       </c>
       <c r="W81" t="n">
@@ -7272,12 +7272,12 @@
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>Malt production in Canada in 2017.  The production trends were fairly smooth for most of the year, rising from January to May, falling from August to November, and staying at or above 50000 tonnes until the end of the year.  By comparison, June and July showed strong fluctuations in production, and the value dropped to its all-year low of under 40000 tonnes in December.</t>
+          <t>malt production in canada in 2017.  the production trends were fairly smooth for most of the year, rising from january to may, falling from august to november, and staying at or above 50000 tonnes until the end of the year.  by comparison, june and july showed strong fluctuations in production, and the value dropped to its all-year low of under 40000 tonnes in december.</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>Malt production in  TKN_Geo  in  TKN_Year .  The production trends were fairly smooth for most of the year, rising from January to May, falling from August to November, and staying at or above 47 TKN_UOM  until the end of the year.  By comparison, June and July showed strong fluctuations in production, and the value dropped to its all-year low of under 4 TKN_UOM  in December.</t>
+          <t>malt production in canada in  TKN_Year .  the production trends were fairly smooth for most of the year, rising from january to may, falling from august to november, and staying at or above 47 TKN_UOM  until the end of the year.  by comparison, june and july showed strong fluctuations in production, and the value dropped to its all-year low of under 4 TKN_UOM  in december.</t>
         </is>
       </c>
       <c r="W82" t="n">
@@ -7356,12 +7356,12 @@
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>The provided graph displays the number of Canadian vehicles returning to Canada over the year 2016 divided by month. It starts out at around 150000 vehicles in January, falls to 135000 in February and rises continuously to over 220000 in August. The following month show a steady decrease to its second lowest point of just under 160000 in December.</t>
+          <t>the provided graph displays the number of canadian vehicles returning to canada over the year 2016 divided by month. it starts out at around 150000 vehicles in january, falls to 135000 in february and rises continuously to over 220000 in august. the following month show a steady decrease to its second lowest point of just under 160000 in december.</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>The provided graph displays the TKN_About  returning to  TKN_Geo  over the year 2016 divided by month. It starts out at around 34 vehicles in January, falls to 20 in February and rises continuously to over 100 in August. The following month show a steady decrease to its second lowest point of just under 44 in December.</t>
+          <t>the provided graph displays the TKN_About  returning to canada over the year 2016 divided by month. it starts out at around 34 vehicles in january, falls to 20 in february and rises continuously to over 100 in august. the following month show a steady decrease to its second lowest point of just under 44 in december.</t>
         </is>
       </c>
       <c r="W83" t="n">
@@ -7440,12 +7440,12 @@
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the total number of Unitated States vehicles entering in Canada during 2017 presented the highest values during the summer period. In particular, the maximum value has been reached during July. The month with less United States vehicles entering Canada over the year has been February 2017.</t>
+          <t>as it can be seen from the graph, the total number of unitated states vehicles entering in canada during 2017 presented the highest values during the summer period. in particular, the maximum value has been reached during july. the month with less united states vehicles entering canada over the year has been february 2017.</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>As it can be seen from the graph, the total TKN_UOM  of Unitated States vehicles entering in  TKN_Geo  during  TKN_Year  presented the highest values during the summer period. In particular, the maximum value has been reached during July. The month with less TKN_About   TKN_Geo  over the year has been February  TKN_Year .</t>
+          <t>as it can be seen from the graph, the total TKN_UOM  of unitated states vehicles entering in canada during  TKN_Year  presented the highest values during the summer period. in particular, the maximum value has been reached during july. the month with less TKN_About  canada over the year has been february  TKN_Year .</t>
         </is>
       </c>
       <c r="W84" t="n">
@@ -7524,12 +7524,12 @@
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>This chart shows how the Canadian total farm production index varies by month throughout 2018. We see a distinctive season pattern. Production starts at a middling level in the first three months of the year, before a rapid increase from April to July, where it reaches a peak. A quick descent then follow into the fall, with a low point in September, a small rebound in October, and falling again in December.</t>
+          <t>this chart shows how the canadian total farm production index varies by month throughout 2018. we see a distinctive season pattern. production starts at a middling level in the first three months of the year, before a rapid increase from april to july, where it reaches a peak. a quick descent then follow into the fall, with a low point in september, a small rebound in october, and falling again in december.</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>This chart shows how the TKN_UOM  varies by month throughout  TKN_Year . We see a distinctive TKN_About  starts at a middling level in the first three months of the year, before a rapid increase from April to July, where it reaches a peak. A quick descent then follow into the fall, with a low point in September, a small rebound in October, and falling again in December.</t>
+          <t>this chart shows how the TKN_UOM  varies by month throughout  TKN_Year . we see a distinctive TKN_About  starts at a middling level in the first three months of the year, before a rapid increase from april to july, where it reaches a peak. a quick descent then follow into the fall, with a low point in september, a small rebound in october, and falling again in december.</t>
         </is>
       </c>
       <c r="W85" t="n">
@@ -7608,12 +7608,12 @@
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>This chart shows the production of fresh fruit, by the farm product price index, in Canada in 2017. We see a generally increasing pattern throughout the year. We start at a markedly low level of production from January until May, at which point production starts to increase until July. Production then falls for August to October, until surging in November and reaching a maximum in December.</t>
+          <t>this chart shows the production of fresh fruit, by the farm product price index, in canada in 2017. we see a generally increasing pattern throughout the year. we start at a markedly low level of production from january until may, at which point production starts to increase until july. production then falls for august to october, until surging in november and reaching a maximum in december.</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About  fruit, TKN_UOM  index, in  TKN_Geo  in  TKN_Year . We see a generally increasing pattern throughout the year. We start at a markedly low level of production from January until May, at which point production starts to increase until July. Production then falls for August to October, until surging in November and reaching a maximum in December.</t>
+          <t>this chart shows the TKN_About  fruit, TKN_UOM  index, in canada in  TKN_Year . we see a generally increasing pattern throughout the year. we start at a markedly low level of production from january until may, at which point production starts to increase until july. production then falls for august to october, until surging in november and reaching a maximum in december.</t>
         </is>
       </c>
       <c r="W86" t="n">
@@ -7692,12 +7692,12 @@
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>This chart shows the production of malt, measures in tonnes, in Canada in 2016. Product starts in January at its low point, before a steep increase in February. A mild decrease follows until April, before increasing to a maximum in June. Production then falls over the remainder of the year though with some fluctuation, with December levels almost as low as January.</t>
+          <t>this chart shows the production of malt, measures in tonnes, in canada in 2016. product starts in january at its low point, before a steep increase in february. a mild decrease follows until april, before increasing to a maximum in june. production then falls over the remainder of the year though with some fluctuation, with december levels almost as low as january.</t>
         </is>
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About  malt, measures in tonnes, in  TKN_Geo  in  TKN_Year . Product starts in January at its low point, before a steep increase in February. A mild decrease follows until April, before increasing to a maximum in June. Production then falls over the remainder of the year though with some fluctuation, with December levels almost as low as January.</t>
+          <t>this chart shows the TKN_About  malt, measures in tonnes, in canada in  TKN_Year . product starts in january at its low point, before a steep increase in february. a mild decrease follows until april, before increasing to a maximum in june. production then falls over the remainder of the year though with some fluctuation, with december levels almost as low as january.</t>
         </is>
       </c>
       <c r="W87" t="n">
@@ -7776,12 +7776,12 @@
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>This charts shows the production of eggs in shell, as measured by the farm product price index, in Canada in 2016. Production in January starts at a relatively high level, before increasing in February. After this, a gradual decline follows, reaching a minimum in July. After this, production recovers over the remainder of the year, reaching near the maximum by Oct before reaching the maximum by November and December.</t>
+          <t>this charts shows the production of eggs in shell, as measured by the farm product price index, in canada in 2016. production in january starts at a relatively high level, before increasing in february. after this, a gradual decline follows, reaching a minimum in july. after this, production recovers over the remainder of the year, reaching near the maximum by oct before reaching the maximum by november and december.</t>
         </is>
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>This charts shows the TKN_About  shell, as measured TKN_UOM  index, in  TKN_Geo  in  TKN_Year . Production in January starts at a relatively high level, before increasing in February. After this, a gradual decline follows, reaching a minimum in July. After this, production recovers over the remainder of the year, reaching near the maximum by Oct before reaching the maximum by November and December.</t>
+          <t>this charts shows the TKN_About  shell, as measured TKN_UOM  index, in canada in  TKN_Year . production in january starts at a relatively high level, before increasing in february. after this, a gradual decline follows, reaching a minimum in july. after this, production recovers over the remainder of the year, reaching near the maximum by oct before reaching the maximum by november and december.</t>
         </is>
       </c>
       <c r="W88" t="n">
@@ -7860,12 +7860,12 @@
       </c>
       <c r="U89" t="inlineStr">
         <is>
-          <t>This chart shows the production of oats, measured in Tonnes, in Canada. Generally, production fluctuates quite a lot month to month. Production starts at a middling level in January, with wide oscillations until July. After July, production increases consistently until reaching a maximum in September, before then gradually decreasing until reaching a level similiar to January in December.</t>
+          <t>this chart shows the production of oats, measured in tonnes, in canada. generally, production fluctuates quite a lot month to month. production starts at a middling level in january, with wide oscillations until july. after july, production increases consistently until reaching a maximum in september, before then gradually decreasing until reaching a level similiar to january in december.</t>
         </is>
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>This chart shows the TKN_About  oats, measured in  TKN_UOM , in  TKN_Geo . Generally, production fluctuates quite a lot month to month. Production starts at a middling level in January, with wide oscillations until July. After July, production increases consistently until reaching a maximum in September, before then gradually decreasing until reaching a level similiar to January in December.</t>
+          <t>this chart shows the TKN_About  oats, measured in tonnes, in canada. generally, production fluctuates quite a lot month to month. production starts at a middling level in january, with wide oscillations until july. after july, production increases consistently until reaching a maximum in september, before then gradually decreasing until reaching a level similiar to january in december.</t>
         </is>
       </c>
       <c r="W89" t="n">
@@ -7944,12 +7944,12 @@
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>Line chart showing the increase of the House and land price index in 2016 in Canada.</t>
+          <t>line chart showing the increase of the house and land price index in 2016 in canada.</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>Line chart showing the increase of TKN_About  TKN_UOM  in  TKN_Year  in  TKN_Geo .</t>
+          <t>line chart showing the increase of TKN_About  TKN_UOM  in  TKN_Year  in canada.</t>
         </is>
       </c>
       <c r="W90" t="n">
@@ -8028,12 +8028,12 @@
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>Line chart showing the evolution of the Farm product price index in Canada in 2016.</t>
+          <t>line chart showing the evolution of the farm product price index in canada in 2016.</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>Line chart showing TKN_About  TKN_UOM  in  TKN_Geo  in  TKN_Year .</t>
+          <t>line chart showing TKN_About  TKN_UOM  in canada in  TKN_Year .</t>
         </is>
       </c>
       <c r="W91" t="n">
@@ -8112,12 +8112,12 @@
       </c>
       <c r="U92" t="inlineStr">
         <is>
-          <t>This graph represents the production of new motor vehicles in Canada during 2016. Production starts very low in January and undergoes a sharp increase until it reaches its peak of over 200000 motor vehicles in April. The following months production decreases, being almost steady at 175000 from July until September. Production gradually decreases until December.</t>
+          <t>this graph represents the production of new motor vehicles in canada during 2016. production starts very low in january and undergoes a sharp increase until it reaches its peak of over 200000 motor vehicles in april. the following months production decreases, being almost steady at 175000 from july until september. production gradually decreases until december.</t>
         </is>
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  in  TKN_Geo  during  TKN_Year . Production starts very low in January and undergoes a sharp increase until it reaches its peak of over 96 motor vehicles in April. The following months production decreases, being almost steady at 69 from July until September. Production gradually decreases until December.</t>
+          <t>this graph represents the TKN_About  in canada during  TKN_Year . production starts very low in january and undergoes a sharp increase until it reaches its peak of over 96 motor vehicles in april. the following months production decreases, being almost steady at 69 from july until september. production gradually decreases until december.</t>
         </is>
       </c>
       <c r="W92" t="n">
@@ -8196,12 +8196,12 @@
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>The price index of servers in Canada during 2017 is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 1007 in November. A small increase to 1010 is observed in December.</t>
+          <t>the price index of servers in canada during 2017 is depicted in this line chart. two maxima are reached during the months of january and june. between aforementioned months the price varies and reaches a low point during april, from which there is a sharp increase until june. from june onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 1007 in november. a small increase to 1010 is observed in december.</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  is depicted in this line chart. Two maxima are reached during the months of January and June. Between aforementioned months the price varies and reaches a low point during April, from which there is a sharp increase until June. From June onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 0 in November. A small increase to 12 is observed in December.</t>
+          <t>the TKN_About  in canada during  TKN_Year  is depicted in this line chart. two maxima are reached during the months of january and june. between aforementioned months the price varies and reaches a low point during april, from which there is a sharp increase until june. from june onwards the price decreases in an oscillating manner until it reaches its minimum of approximately 0 in november. a small increase to 12 is observed in december.</t>
         </is>
       </c>
       <c r="W93" t="n">
@@ -8280,12 +8280,12 @@
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>The production of canola in tonnes in Canada during 2016 is shown in this line chart. Production sharply increases from January until March. During the following months production fluctuates in an overall decreasing manner until it reaches its minimum in August. There is a sharp gain in production of candle from August until reaching the maximum of over 1100000 in December.</t>
+          <t>the production of canola in tonnes in canada during 2016 is shown in this line chart. production sharply increases from january until march. during the following months production fluctuates in an overall decreasing manner until it reaches its minimum in august. there is a sharp gain in production of candle from august until reaching the maximum of over 1100000 in december.</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>The TKN_About  in TKN_UOM  in  TKN_Geo  during  TKN_Year  is shown in this line chart. Production sharply increases from January until March. During the following months production fluctuates in an overall decreasing manner until it reaches its minimum in August. There is a sharp gain in production of candle from August until reaching the maximum of over 95 in December.</t>
+          <t>the TKN_About  in TKN_UOM  in canada during  TKN_Year  is shown in this line chart. production sharply increases from january until march. during the following months production fluctuates in an overall decreasing manner until it reaches its minimum in august. there is a sharp gain in production of candle from august until reaching the maximum of over 95 in december.</t>
         </is>
       </c>
       <c r="W94" t="n">
@@ -8364,12 +8364,12 @@
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>This graph represents the total livestock and animal products of Canada in 2017.   The number of products experiences a sharp increase from January until reaching the maximum during June, whereas a small decline is observed in the month of April. From June until September the total livestock and animal products rapidly decline and reach a minimum of under 1340 in September. The following 2 months a small increase can be observed, before it drops again in December.</t>
+          <t>this graph represents the total livestock and animal products of canada in 2017.   the number of products experiences a sharp increase from january until reaching the maximum during june, whereas a small decline is observed in the month of april. from june until september the total livestock and animal products rapidly decline and reach a minimum of under 1340 in september. the following 2 months a small increase can be observed, before it drops again in december.</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  of  TKN_Geo  in  TKN_Year .   The number of products experiences a sharp increase from January until reaching the maximum during June, whereas a small decline is observed in the month of April. From June until September the TKN_About  rapidly decline and reach a minimum of under 2 in September. The following 2 months a small increase can be observed, before it drops again in December.</t>
+          <t>this graph represents the TKN_About  of canada in  TKN_Year .   the number of products experiences a sharp increase from january until reaching the maximum during june, whereas a small decline is observed in the month of april. from june until september the TKN_About  rapidly decline and reach a minimum of under 2 in september. the following 2 months a small increase can be observed, before it drops again in december.</t>
         </is>
       </c>
       <c r="W95" t="n">
@@ -8448,12 +8448,12 @@
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>This line chart describes the production of fresh vegetables of Canada in 2017. In January a production of 1385 can be observed. This decreases in the month of February and from then onwards a small, but constant increase is taking place until the maximum of over 1410 can be seen in September. After September production of fresh vegetables steadily decreases again, with a small increase in November. A value of approximately 1396 is observed in December.</t>
+          <t>this line chart describes the production of fresh vegetables of canada in 2017. in january a production of 1385 can be observed. this decreases in the month of february and from then onwards a small, but constant increase is taking place until the maximum of over 1410 can be seen in september. after september production of fresh vegetables steadily decreases again, with a small increase in november. a value of approximately 1396 is observed in december.</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>This line chart describes the TKN_About  of  TKN_Geo  in  TKN_Year . In January a production of 19 can be observed. This decreases in the month of February and from then onwards a small, but constant increase is taking place until the maximum of over 97 can be seen in September. After September TKN_About  steadily decreases again, with a small increase in November. A value of approximately 53 is observed in December.</t>
+          <t>this line chart describes the TKN_About  of canada in  TKN_Year . in january a production of 19 can be observed. this decreases in the month of february and from then onwards a small, but constant increase is taking place until the maximum of over 97 can be seen in september. after september TKN_About  steadily decreases again, with a small increase in november. a value of approximately 53 is observed in december.</t>
         </is>
       </c>
       <c r="W96" t="n">
@@ -8532,12 +8532,12 @@
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>This graph represents the house and land price index of Canada in 2017. Overall a content increase can be observed throughout the year, starting at approximately 1001 in January and increasing of uptimes to 1033 in November where it plateaus like that until December.</t>
+          <t>this graph represents the house and land price index of canada in 2017. overall a content increase can be observed throughout the year, starting at approximately 1001 in january and increasing of uptimes to 1033 in november where it plateaus like that until december.</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>This graph represents TKN_About  TKN_UOM  of  TKN_Geo  in  TKN_Year . Overall a content increase can be observed throughout the year, starting at approximately 0 in January and increasing of uptimes to 100 in November where it plateaus like that until December.</t>
+          <t>this graph represents TKN_About  TKN_UOM  of canada in  TKN_Year . overall a content increase can be observed throughout the year, starting at approximately 0 in january and increasing of uptimes to 100 in november where it plateaus like that until december.</t>
         </is>
       </c>
       <c r="W97" t="n">
@@ -8616,12 +8616,12 @@
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>This chart represents the production of unprocessed milk of Canada in 2016. Whereas the production oscillates from January until June ranging from 1045 until 1065 a minimum value of below 1020 is observed during July. The following three months a sharp increase is taking place and reaching a value of approximately 1110. The production stays almost consistent from October until December.</t>
+          <t>this chart represents the production of unprocessed milk of canada in 2016. whereas the production oscillates from january until june ranging from 1045 until 1065 a minimum value of below 1020 is observed during july. the following three months a sharp increase is taking place and reaching a value of approximately 1110. the production stays almost consistent from october until december.</t>
         </is>
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>This chart represents the TKN_About  of  TKN_Geo  in  TKN_Year . Whereas the production oscillates from January until June ranging from 34 until 53 a minimum value of below 9 is observed during July. The following three months a sharp increase is taking place and reaching a value of approximately 98. The production stays almost consistent from October until December.</t>
+          <t>this chart represents the TKN_About  of canada in  TKN_Year . whereas the production oscillates from january until june ranging from 34 until 53 a minimum value of below 9 is observed during july. the following three months a sharp increase is taking place and reaching a value of approximately 98. the production stays almost consistent from october until december.</t>
         </is>
       </c>
       <c r="W98" t="n">
@@ -8700,12 +8700,12 @@
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>This line chart illustrates the production of wheat flour (in tonnes) of Canada in 2016. Production starts very low in January at approximately 19500 tonnes. From there on production starts oscillating a lot, having a peak during February, a low in March and reaching the maximum during April. There is a sharp decline from April until May, after which production starts fluctuating again until September. There is a rapid jump in October reaching almost 30000 tonnes. A very slight increase can be observed for November, after which the production drops in December.</t>
+          <t>this line chart illustrates the production of wheat flour (in tonnes) of canada in 2016. production starts very low in january at approximately 19500 tonnes. from there on production starts oscillating a lot, having a peak during february, a low in march and reaching the maximum during april. there is a sharp decline from april until may, after which production starts fluctuating again until september. there is a rapid jump in october reaching almost 30000 tonnes. a very slight increase can be observed for november, after which the production drops in december.</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>This line chart illustrates the TKN_About  (in tonnes) of  TKN_Geo  in  TKN_Year . Production starts very low in January at approximately 0 tonnes. From there on production starts oscillating a lot, having a peak during February, a low in March and reaching the maximum during April. There is a sharp decline from April until May, after which production starts fluctuating again until September. There is a rapid jump in October reaching almost 95 tonnes. A very slight increase can be observed for November, after which the production drops in December.</t>
+          <t>this line chart illustrates the TKN_About  (in tonnes) of canada in  TKN_Year . production starts very low in january at approximately 0 tonnes. from there on production starts oscillating a lot, having a peak during february, a low in march and reaching the maximum during april. there is a sharp decline from april until may, after which production starts fluctuating again until september. there is a rapid jump in october reaching almost 95 tonnes. a very slight increase can be observed for november, after which the production drops in december.</t>
         </is>
       </c>
       <c r="W99" t="n">
@@ -8784,12 +8784,12 @@
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>This line chart depicts the total hardwood production in cubic metres of Canada in 2016. Production starts at approximately 1370 cubic metres during January, after which a moderate increase can be observed until reaching about 1580 in March. Production remains steady at 1450 during April and May, after which the maximum production is achieved in June with 1600 cubic metres. There is a sharp drop in July, a rapid increase until November until the minimum value of approximately 1050 is reached in December.</t>
+          <t>this line chart depicts the total hardwood production in cubic metres of canada in 2016. production starts at approximately 1370 cubic metres during january, after which a moderate increase can be observed until reaching about 1580 in march. production remains steady at 1450 during april and may, after which the maximum production is achieved in june with 1600 cubic metres. there is a sharp drop in july, a rapid increase until november until the minimum value of approximately 1050 is reached in december.</t>
         </is>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>This line chart depicts the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . Production starts at approximately 59 TKN_UOM  during January, after which a moderate increase can be observed until reaching about 95 in March. Production remains steady at 73 during April and May, after which the maximum production is achieved in June with 99 TKN_UOM . There is a sharp drop in July, a rapid increase until November until the minimum value of approximately 3 is reached in December.</t>
+          <t>this line chart depicts the TKN_About  in TKN_UOM  of canada in  TKN_Year . production starts at approximately 59 TKN_UOM  during january, after which a moderate increase can be observed until reaching about 95 in march. production remains steady at 73 during april and may, after which the maximum production is achieved in june with 99 TKN_UOM . there is a sharp drop in july, a rapid increase until november until the minimum value of approximately 3 is reached in december.</t>
         </is>
       </c>
       <c r="W100" t="n">
@@ -8868,12 +8868,12 @@
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>The chart shows the variation of tablet computers prices in Canada during the year 2017. Except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
+          <t>the chart shows the variation of tablet computers prices in canada during the year 2017. except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
         </is>
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>The chart shows the variation TKN_About  prices in  TKN_Geo  during the year  TKN_Year . Except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
+          <t>the chart shows the variation TKN_About  prices in canada during the year  TKN_Year . except for some punctual oscillations, the overall trend is of price reduction throughout the period considered.</t>
         </is>
       </c>
       <c r="W101" t="n">
@@ -8952,12 +8952,12 @@
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>Increase of house price index during 2017 months per months.</t>
+          <t>increase of house price index during 2017 months per months.</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>Increase TKN_About  TKN_UOM  during  TKN_Year  months per months.</t>
+          <t>increase TKN_About  TKN_UOM  during  TKN_Year  months per months.</t>
         </is>
       </c>
       <c r="W102" t="n">
@@ -9036,12 +9036,12 @@
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>The graph shows the production of softwood in Canada over the year of 2017. The data is presented in cubic meters. According to the graph the production of softwood is the highest in March and the lowest in December.</t>
+          <t>the graph shows the production of softwood in canada over the year of 2017. the data is presented in cubic meters. according to the graph the production of softwood is the highest in march and the lowest in december.</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  of softwood in  TKN_Geo  over the year of  TKN_Year . The data is presented TKN_UOM  meters. According to the graph TKN_About  of softwood is the highest in March and the lowest in December.</t>
+          <t>the graph shows TKN_About  of softwood in canada over the year of  TKN_Year . the data is presented TKN_UOM  meters. according to the graph TKN_About  of softwood is the highest in march and the lowest in december.</t>
         </is>
       </c>
       <c r="W103" t="n">
@@ -9120,12 +9120,12 @@
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>The chart shows the variation of house price in Canada during the year 2018. The higher price was identify during the month of January, followed by a considerable decline till May, when it returns to rise rapidly. Prices remain steady in the last 4 months of the year.</t>
+          <t>the chart shows the variation of house price in canada during the year 2018. the higher price was identify during the month of january, followed by a considerable decline till may, when it returns to rise rapidly. prices remain steady in the last 4 months of the year.</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>The chart shows the variation of TKN_About  in  TKN_Geo  during the year  TKN_Year . The higher price was identify during the month of January, followed by a considerable decline till May, when it returns to rise rapidly. Prices remain steady in the last 4 months of the year.</t>
+          <t>the chart shows the variation of TKN_About  in canada during the year  TKN_Year . the higher price was identify during the month of january, followed by a considerable decline till may, when it returns to rise rapidly. prices remain steady in the last 4 months of the year.</t>
         </is>
       </c>
       <c r="W104" t="n">
@@ -9204,12 +9204,12 @@
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>The graph shows the livestock and animal products value in Canada during 2018. The values are described using the farm product price index (FPPI). The products index shown several fluctuations. In particular, it's clearly possible to see several peaks and dips. In February, July and October the value reached its maximum values. During April and September the value reached its minimum values.</t>
+          <t>the graph shows the livestock and animal products value in canada during 2018. the values are described using the farm product price index (fppi). the products index shown several fluctuations. in particular, it's clearly possible to see several peaks and dips. in february, july and october the value reached its maximum values. during april and september the value reached its minimum values.</t>
         </is>
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  value in  TKN_Geo  during  TKN_Year . The values are described using TKN_UOM  (FPPI). The products index shown several fluctuations. In particular, it's clearly possible to see several peaks and dips. In February, July and October the value reached its maximum values. During April and September the value reached its minimum values.</t>
+          <t>the graph shows the TKN_About  value in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). the products index shown several fluctuations. in particular, it's clearly possible to see several peaks and dips. in february, july and october the value reached its maximum values. during april and september the value reached its minimum values.</t>
         </is>
       </c>
       <c r="W105" t="n">
@@ -9288,12 +9288,12 @@
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>The data presented in the graph shows the supply of creamery butter in Canada over the year of 2018 in tonnes. The lowest supply of creamery butter can be observed in January. The supply increases constantly over the next months and reaches its highest value in June, after which it decreases with a similar rate and reaches a local minimum in September.</t>
+          <t>the data presented in the graph shows the supply of creamery butter in canada over the year of 2018 in tonnes. the lowest supply of creamery butter can be observed in january. the supply increases constantly over the next months and reaches its highest value in june, after which it decreases with a similar rate and reaches a local minimum in september.</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>The data presented in the graph shows the TKN_About  in  TKN_Geo  over the year of  TKN_Year  in tonnes. The lowest TKN_About  can be observed in January. The supply increases constantly over the next months and reaches its highest value in June, after which it decreases with a similar rate and reaches a local minimum in September.</t>
+          <t>the data presented in the graph shows the TKN_About  in canada over the year of  TKN_Year  in tonnes. the lowest TKN_About  can be observed in january. the supply increases constantly over the next months and reaches its highest value in june, after which it decreases with a similar rate and reaches a local minimum in september.</t>
         </is>
       </c>
       <c r="W106" t="n">
@@ -9372,12 +9372,12 @@
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>The chart shows the variation of softwood production in Canada during the year 2017. The production reaches its top on March after which we observe an oscillating period until November, when there is a steeply fall.</t>
+          <t>the chart shows the variation of softwood production in canada during the year 2017. the production reaches its top on march after which we observe an oscillating period until november, when there is a steeply fall.</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>The chart shows the variation of TKN_About  in  TKN_Geo  during the year  TKN_Year . The production reaches its top on March after which we observe an oscillating period until November, when there is a steeply fall.</t>
+          <t>the chart shows the variation of TKN_About  in canada during the year  TKN_Year . the production reaches its top on march after which we observe an oscillating period until november, when there is a steeply fall.</t>
         </is>
       </c>
       <c r="W107" t="n">
@@ -9456,12 +9456,12 @@
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>A line chart about the global growth and punctual drops of the monthly egg production in Canada, 2017.</t>
+          <t>a line chart about the global growth and punctual drops of the monthly egg production in canada, 2017.</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>A line chart about the global growth and punctual drops TKN_About   TKN_Geo ,  TKN_Year .</t>
+          <t>a line chart about the global growth and punctual drops TKN_About  canada,  TKN_Year .</t>
         </is>
       </c>
       <c r="W108" t="n">
@@ -9540,12 +9540,12 @@
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>The diagramm showes the toatal farm production index of Canada over the year 2017. From January to March the index increase. in April there is a small  drop and afterwards a continous increase till June. It stays constant between June and July and decrase rapitly till September/October. At october the annual minimum is reached. In November there is a small increase and in December it drops again.</t>
+          <t>the diagramm showes the toatal farm production index of canada over the year 2017. from january to march the index increase. in april there is a small  drop and afterwards a continous increase till june. it stays constant between june and july and decrase rapitly till september/october. at october the annual minimum is reached. in november there is a small increase and in december it drops again.</t>
         </is>
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>The diagramm showes TKN_UOM  of  TKN_Geo  over the year  TKN_Year . From January to TKN_About  increase. in April there is a small  drop and afterwards a continous increase till June. It stays constant between June and July and decrase rapitly till September/October. At october the annual minimum is reached. In November there is a small increase and in December it drops again.</t>
+          <t>the diagramm showes TKN_UOM  of canada over the year  TKN_Year . from january to TKN_About  increase. in april there is a small  drop and afterwards a continous increase till june. it stays constant between june and july and decrase rapitly till september/october. at october the annual minimum is reached. in november there is a small increase and in december it drops again.</t>
         </is>
       </c>
       <c r="W109" t="n">
@@ -9624,12 +9624,12 @@
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>A line chart about the price index concerning the commercial software in Canada, 2016. The index dropped from 1218 to stabilizes around 1185 by the month of April.</t>
+          <t>a line chart about the price index concerning the commercial software in canada, 2016. the index dropped from 1218 to stabilizes around 1185 by the month of april.</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>A line chart about the price TKN_About  in  TKN_Geo ,  TKN_Year . The index dropped from 100 to stabilizes around 23 by the month of April.</t>
+          <t>a line chart about the price TKN_About  in canada,  TKN_Year . the index dropped from 100 to stabilizes around 23 by the month of april.</t>
         </is>
       </c>
       <c r="W110" t="n">
@@ -9708,12 +9708,12 @@
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>The commercial software price index was slightly increasing during the three first months of the year 2017, then slightly decline for a month.  Afterwards it stayed constant for a month until a massive drop for 2 months, to grow again for a month and then decrease again. The 3 last months of the year the index surges again.</t>
+          <t>the commercial software price index was slightly increasing during the three first months of the year 2017, then slightly decline for a month.  afterwards it stayed constant for a month until a massive drop for 2 months, to grow again for a month and then decrease again. the 3 last months of the year the index surges again.</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>The TKN_About  was slightly increasing during the three first months of the year  TKN_Year , then slightly decline for a month.  Afterwards it stayed constant for a month until a massive drop for 2 months, to grow again for a month and then decrease again. The 3 last months of the year the index surges again.</t>
+          <t>the TKN_About  was slightly increasing during the three first months of the year  TKN_Year , then slightly decline for a month.  afterwards it stayed constant for a month until a massive drop for 2 months, to grow again for a month and then decrease again. the 3 last months of the year the index surges again.</t>
         </is>
       </c>
       <c r="W111" t="n">
@@ -9792,12 +9792,12 @@
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>The Diagramm showes the commercial software prince index of Canada over the year 2017. The index is quite stable between Jannuary and May with a small peak in March. Then it drops suddenly till July. It increaes a little bit in August and drop again in September to the lowest point of the year (less then 1120). From September to December it increase slightly to 1140.</t>
+          <t>the diagramm showes the commercial software prince index of canada over the year 2017. the index is quite stable between jannuary and may with a small peak in march. then it drops suddenly till july. it increaes a little bit in august and drop again in september to the lowest point of the year (less then 1120). from september to december it increase slightly to 1140.</t>
         </is>
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>The Diagramm showes the TKN_About  of  TKN_Geo  over the year  TKN_Year . The index is quite stable between Jannuary and May with a small peak in March. Then it drops suddenly till July. It increaes a little bit in August and drop again in September to the lowest point of the year (less then 7). From September to December it increase slightly to 37.</t>
+          <t>the diagramm showes the TKN_About  of canada over the year  TKN_Year . the index is quite stable between jannuary and may with a small peak in march. then it drops suddenly till july. it increaes a little bit in august and drop again in september to the lowest point of the year (less then 7). from september to december it increase slightly to 37.</t>
         </is>
       </c>
       <c r="W112" t="n">
@@ -9876,12 +9876,12 @@
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>The line chart about fresh potato production in Canada, 2018 shows that there was a peak in the production during the period of June, July and August.  To drop during the month of October and then raise again. At the beginning of the year the production was growing until this boost in Summer.</t>
+          <t>the line chart about fresh potato production in canada, 2018 shows that there was a peak in the production during the period of june, july and august.  to drop during the month of october and then raise again. at the beginning of the year the production was growing until this boost in summer.</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>The line chart about TKN_About  in  TKN_Geo ,  TKN_Year  shows that there was a peak in the production during the period of June, July and August.  To drop during the month of October and then raise again. At the beginning of the year the production was growing until this boost in Summer.</t>
+          <t>the line chart about TKN_About  in canada,  TKN_Year  shows that there was a peak in the production during the period of june, july and august.  to drop during the month of october and then raise again. at the beginning of the year the production was growing until this boost in summer.</t>
         </is>
       </c>
       <c r="W113" t="n">
@@ -9960,12 +9960,12 @@
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>The diagramm showes the production of Canola in tonnes over the year 2017. The Graphe fluctuates a lot over the Year. Ther are peaks in January, April/May, October and December. The highest production is reached in October. There are also monthes with a low production of Canola: February, August and November. The lowst production is reached in August.</t>
+          <t>the diagramm showes the production of canola in tonnes over the year 2017. the graphe fluctuates a lot over the year. ther are peaks in january, april/may, october and december. the highest production is reached in october. there are also monthes with a low production of canola: february, august and november. the lowst production is reached in august.</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>The diagramm showes the TKN_About  in TKN_UOM  over the year  TKN_Year . The Graphe fluctuates a lot over the Year. Ther are peaks in January, April/May, October and December. The highest production is reached in October. There are also monthes with a low TKN_About : February, August and November. The lowst production is reached in August.</t>
+          <t>the diagramm showes the TKN_About  in TKN_UOM  over the year  TKN_Year . the graphe fluctuates a lot over the year. ther are peaks in january, april/may, october and december. the highest production is reached in october. there are also monthes with a low TKN_About : february, august and november. the lowst production is reached in august.</t>
         </is>
       </c>
       <c r="W114" t="n">
@@ -10044,12 +10044,12 @@
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>The diagram showes the Production of new motor vehicles in Dollar  over the year 2016 in Canada. In januarry less than 4500000 vehicles were produced (lowest). Till April the production increase steadyly and reach the highest value. From April to December it decreases slowly with two small peaks in September and November.</t>
+          <t>the diagram showes the production of new motor vehicles in dollar  over the year 2016 in canada. in januarry less than 4500000 vehicles were produced (lowest). till april the production increase steadyly and reach the highest value. from april to december it decreases slowly with two small peaks in september and november.</t>
         </is>
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>The diagram showes the TKN_About  in Dollar  over the year  TKN_Year  in  TKN_Geo . In januarry less than 6 vehicles were produced (lowest). Till April the production increase steadyly and reach the highest value. From April to December it decreases slowly with two small peaks in September and November.</t>
+          <t>the diagram showes the TKN_About  in dollar  over the year  TKN_Year  in canada. in januarry less than 6 vehicles were produced (lowest). till april the production increase steadyly and reach the highest value. from april to december it decreases slowly with two small peaks in september and november.</t>
         </is>
       </c>
       <c r="W115" t="n">
@@ -10128,12 +10128,12 @@
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>Land Price Index in Canada in the year of 2018. The graphic shows the course of the Land Price Index in Canada over the year 2018. It is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. For the mounths of november and december the maximum value is reached with 1041.</t>
+          <t>land price index in canada in the year of 2018. the graphic shows the course of the land price index in canada over the year 2018. it is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. for the mounths of november and december the maximum value is reached with 1041.</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>Land TKN_UOM  in  TKN_Geo  in the year of  TKN_Year . The graphic shows the course of the TKN_About   in  TKN_Geo  over the year  TKN_Year . It is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. For the mounths of november and december the maximum value is reached with 100.</t>
+          <t>land TKN_UOM  in canada in the year of  TKN_Year . the graphic shows the course of the TKN_About   in canada over the year  TKN_Year . it is noticeable that the index initially remains constant for the beginning of the year and then rises sharply towards the end of the year. for the mounths of november and december the maximum value is reached with 100.</t>
         </is>
       </c>
       <c r="W116" t="n">
@@ -10212,12 +10212,12 @@
       </c>
       <c r="U117" t="inlineStr">
         <is>
-          <t>This graph depicts the total softwood production in cubic metres of Canada in 2016. Production starts at approximately 53000 cubic metres in January and increases to one of its maximum values of 57000 cubic metres in March. The following months show first a slow decrease, but then a sharp decrease in July. From July until November production gradually increases again until it reaches its second maximum of 57000 cubic metres in November. There is a sharp drop from November onwards, reaching its minimum value of 46000 cubic metres in December.</t>
+          <t>this graph depicts the total softwood production in cubic metres of canada in 2016. production starts at approximately 53000 cubic metres in january and increases to one of its maximum values of 57000 cubic metres in march. the following months show first a slow decrease, but then a sharp decrease in july. from july until november production gradually increases again until it reaches its second maximum of 57000 cubic metres in november. there is a sharp drop from november onwards, reaching its minimum value of 46000 cubic metres in december.</t>
         </is>
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . Production starts at approximately 64 TKN_UOM  in January and increases to one of its maximum values of 102 TKN_UOM  in March. The following months show first a slow decrease, but then a sharp decrease in July. From July until November production gradually increases again until it reaches its second maximum of 102 TKN_UOM  in November. There is a sharp drop from November onwards, reaching its minimum value of -1 TKN_UOM  in December.</t>
+          <t>this graph depicts the TKN_About  in TKN_UOM  of canada in  TKN_Year . production starts at approximately 64 TKN_UOM  in january and increases to one of its maximum values of 102 TKN_UOM  in march. the following months show first a slow decrease, but then a sharp decrease in july. from july until november production gradually increases again until it reaches its second maximum of 102 TKN_UOM  in november. there is a sharp drop from november onwards, reaching its minimum value of -1 TKN_UOM  in december.</t>
         </is>
       </c>
       <c r="W117" t="n">
@@ -10296,12 +10296,12 @@
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in Canada 2017. The graphic shows the production of new motor vehicles ($) in Canada over the year 2017. iT is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
+          <t>production of new motor vehicles in canada 2017. the graphic shows the production of new motor vehicles ($) in canada over the year 2017. it is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in  TKN_Geo   TKN_Year . The graphic shows the production of new motor vehicles ($) in  TKN_Geo  over the year  TKN_Year . iT is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
+          <t>production of new motor vehicles in canada  TKN_Year . the graphic shows the TKN_About  ($) in canada over the year  TKN_Year . it is noticeable that in the spring and summer months significantly more money is spent on the production of new vehicel as in the winter.</t>
         </is>
       </c>
       <c r="W118" t="n">
@@ -10380,12 +10380,12 @@
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>This line chart represents the Canadian production of new motor vehicles in dollars in 2017. The year starts with a minimum production value of 4500000 dollars in January and gradually increases until reaching its maximum in May with approximately 8500000. From May onwards the production starts fluctuating, having a low in July, but also an increased production in September. In the following three months a constant drop is observed, reaching a value of 5500000 dollars in December.</t>
+          <t>this line chart represents the canadian production of new motor vehicles in dollars in 2017. the year starts with a minimum production value of 4500000 dollars in january and gradually increases until reaching its maximum in may with approximately 8500000. from may onwards the production starts fluctuating, having a low in july, but also an increased production in september. in the following three months a constant drop is observed, reaching a value of 5500000 dollars in december.</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>This line chart represents the Canadian TKN_About  in TKN_UOM  in  TKN_Year . The year starts with a minimum production value of -1 TKN_UOM  in January and gradually increases until reaching its maximum in May with approximately 98. From May onwards the production starts fluctuating, having a low in July, but also an increased production in September. In the following three months a constant drop is observed, reaching a value of 24 TKN_UOM  in December.</t>
+          <t>this line chart represents the canadian TKN_About  in TKN_UOM  in  TKN_Year . the year starts with a minimum production value of -1 TKN_UOM  in january and gradually increases until reaching its maximum in may with approximately 98. from may onwards the production starts fluctuating, having a low in july, but also an increased production in september. in the following three months a constant drop is observed, reaching a value of 24 TKN_UOM  in december.</t>
         </is>
       </c>
       <c r="W119" t="n">
@@ -10464,12 +10464,12 @@
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>This chart represents the supply of creamery butter in tonnes of Canada in 2017. The minimum supply can be observed during January with 24000 tonnes. From then onwards the supply steadily increases until May with 38000 tonnes. From May until July the supply is held about constant. A slow, but constant decrease is observed from July until December.</t>
+          <t>this chart represents the supply of creamery butter in tonnes of canada in 2017. the minimum supply can be observed during january with 24000 tonnes. from then onwards the supply steadily increases until may with 38000 tonnes. from may until july the supply is held about constant. a slow, but constant decrease is observed from july until december.</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>This chart represents the TKN_About  in TKN_UOM  of  TKN_Geo  in  TKN_Year . The minimum supply can be observed during January with -1 TKN_UOM . From then onwards the supply steadily increases until May with 92 TKN_UOM . From May until July the supply is held about constant. A slow, but constant decrease is observed from July until December.</t>
+          <t>this chart represents the TKN_About  in TKN_UOM  of canada in  TKN_Year . the minimum supply can be observed during january with -1 TKN_UOM . from then onwards the supply steadily increases until may with 92 TKN_UOM . from may until july the supply is held about constant. a slow, but constant decrease is observed from july until december.</t>
         </is>
       </c>
       <c r="W120" t="n">
@@ -10548,12 +10548,12 @@
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>This graph represents the price index of Desktop and similar computers in Canada in 2017. The maximum price of approximately 1004 can be observed during January, whereas the price steadily decreases during the following months until May with 989. There is a sharp drop in June at a value of 973. The following months the price does not fluctuate too much, reaching a minimum of 965 in December.</t>
+          <t>this graph represents the price index of desktop and similar computers in canada in 2017. the maximum price of approximately 1004 can be observed during january, whereas the price steadily decreases during the following months until may with 989. there is a sharp drop in june at a value of 973. the following months the price does not fluctuate too much, reaching a minimum of 965 in december.</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year . The maximum price of approximately 100 can be observed during January, whereas the price steadily decreases during the following months until May with 62. There is a sharp drop in June at a value of 21. The following months the price does not fluctuate too much, reaching a minimum of 0 in December.</t>
+          <t>this graph represents the TKN_About  in canada in  TKN_Year . the maximum price of approximately 100 can be observed during january, whereas the price steadily decreases during the following months until may with 62. there is a sharp drop in june at a value of 21. the following months the price does not fluctuate too much, reaching a minimum of 0 in december.</t>
         </is>
       </c>
       <c r="W121" t="n">
@@ -10632,12 +10632,12 @@
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>The shown line chart illustrates the production values about total hardwood in Canada during 2018. The production is described using cubic metres as unit of measure. The values have been significantly oscillating over the year. In particular, the production reached its maximum value during the month of May and its minimum value during July. After July, it rapidly grown up again, reaching an another peak during October.</t>
+          <t>the shown line chart illustrates the production values about total hardwood in canada during 2018. the production is described using cubic metres as unit of measure. the values have been significantly oscillating over the year. in particular, the production reached its maximum value during the month of may and its minimum value during july. after july, it rapidly grown up again, reaching an another peak during october.</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>The shown line chart illustrates the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The production is described using TKN_UOM  as unit of measure. The values have been significantly oscillating over the year. In particular, the production reached its maximum value during the month of May and its minimum value during July. After July, it rapidly grown up again, reaching an another peak during October.</t>
+          <t>the shown line chart illustrates the TKN_About  hardwood in canada during  TKN_Year . the production is described using TKN_UOM  as unit of measure. the values have been significantly oscillating over the year. in particular, the production reached its maximum value during the month of may and its minimum value during july. after july, it rapidly grown up again, reaching an another peak during october.</t>
         </is>
       </c>
       <c r="W122" t="n">
@@ -10716,12 +10716,12 @@
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>The following line chart describes the production values of total hardwood in Canada during 2016. The unit of measurement of the data is cubic metres. The production showed several peaks during the year, mainly during March, June and November. Furthermore, a significant drop has been recorded between the months of June and July.</t>
+          <t>the following line chart describes the production values of total hardwood in canada during 2016. the unit of measurement of the data is cubic metres. the production showed several peaks during the year, mainly during march, june and november. furthermore, a significant drop has been recorded between the months of june and july.</t>
         </is>
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>The following line chart describes the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The unit of measurement of the data TKN_UOM  metres. The production showed several peaks during the year, mainly during March, June and November. Furthermore, a significant drop has been recorded between the months of June and July.</t>
+          <t>the following line chart describes the TKN_About  hardwood in canada during  TKN_Year . the unit of measurement of the data TKN_UOM  metres. the production showed several peaks during the year, mainly during march, june and november. furthermore, a significant drop has been recorded between the months of june and july.</t>
         </is>
       </c>
       <c r="W123" t="n">
@@ -10800,12 +10800,12 @@
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the production value of what flour in Canada during 2016 has been strongly fluctuating. The unit of measurement is tonnes. The graph shows several peaks, but the maximum values have been recorded during the months of April, Octoeber and November. At the same time, the months with less production of what flour have been January and July.</t>
+          <t>as it's shown in the graph, the production value of what flour in canada during 2016 has been strongly fluctuating. the unit of measurement is tonnes. the graph shows several peaks, but the maximum values have been recorded during the months of april, octoeber and november. at the same time, the months with less production of what flour have been january and july.</t>
         </is>
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the production value of what flour in  TKN_Geo  during  TKN_Year  has been strongly fluctuating. The unit of measurement is tonnes. The graph shows several peaks, but the maximum values have been recorded during the months of April, Octoeber and November. At the same time, the months with less TKN_About  have been January and July.</t>
+          <t>as it's shown in the graph, the production value of what flour in canada during  TKN_Year  has been strongly fluctuating. the unit of measurement is tonnes. the graph shows several peaks, but the maximum values have been recorded during the months of april, octoeber and november. at the same time, the months with less TKN_About  have been january and july.</t>
         </is>
       </c>
       <c r="W124" t="n">
@@ -10884,12 +10884,12 @@
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>This line graph displays total softwood production in cubic metres in Canada for 2016. The amount fluctuates with an increase from January to March, followed by a slow decrease from March to June.  A steep reduction follows in July, matched by an equally steep increase in August.  A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of 46000 cubic metres.</t>
+          <t>this line graph displays total softwood production in cubic metres in canada for 2016. the amount fluctuates with an increase from january to march, followed by a slow decrease from march to june.  a steep reduction follows in july, matched by an equally steep increase in august.  a steady increase from august to november is followed by a dramatic reduction in december to a yearly low of 46000 cubic metres.</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>This line graph displays TKN_About  in TKN_UOM  in  TKN_Geo  for  TKN_Year . The amount fluctuates with an increase from January to March, followed by a slow decrease from March to June.  A steep reduction follows in July, matched by an equally steep increase in August.  A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of -1 TKN_UOM .</t>
+          <t>this line graph displays TKN_About  in TKN_UOM  in canada for  TKN_Year . the amount fluctuates with an increase from january to march, followed by a slow decrease from march to june.  a steep reduction follows in july, matched by an equally steep increase in august.  a steady increase from august to november is followed by a dramatic reduction in december to a yearly low of -1 TKN_UOM .</t>
         </is>
       </c>
       <c r="W125" t="n">
@@ -10968,12 +10968,12 @@
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>This line graph displays the land price index in Canada for 2016.  The index is unchanged from January to April, where it rises steadily until August.  From August to November there is a steep increase, with the value remaining unchanged in December.</t>
+          <t>this line graph displays the land price index in canada for 2016.  the index is unchanged from january to april, where it rises steadily until august.  from august to november there is a steep increase, with the value remaining unchanged in december.</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>This line graph displays TKN_About  TKN_UOM  in  TKN_Geo  for  TKN_Year .  The index is unchanged from January to April, where it rises steadily until August.  From August to November there is a steep increase, with the value remaining unchanged in December.</t>
+          <t>this line graph displays TKN_About  TKN_UOM  in canada for  TKN_Year .  the index is unchanged from january to april, where it rises steadily until august.  from august to november there is a steep increase, with the value remaining unchanged in december.</t>
         </is>
       </c>
       <c r="W126" t="n">
@@ -11052,12 +11052,12 @@
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>This line graph displays the production of fresh vegetables in Canada for 2018 using the farm product price index.  A small decrease from January to February is followed by a steady increase until October, where the value again decreases for November and December.</t>
+          <t>this line graph displays the production of fresh vegetables in canada for 2018 using the farm product price index.  a small decrease from january to february is followed by a steady increase until october, where the value again decreases for november and december.</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>This line graph displays the TKN_About  in  TKN_Geo  for  TKN_Year  TKN_UOM  index.  A small decrease from January to February is followed by a steady increase until October, where the value again decreases for November and December.</t>
+          <t>this line graph displays the TKN_About  in canada for  TKN_Year  TKN_UOM  index.  a small decrease from january to february is followed by a steady increase until october, where the value again decreases for november and december.</t>
         </is>
       </c>
       <c r="W127" t="n">
@@ -11136,12 +11136,12 @@
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>This line graph displays the production of fresh potatoes in Canada for 2018 using the farm product price index.  A slow but steady increase is observed from January to June, where a steep increase is seen from June to August.  A steep decrease follows from August to October, where the value again rises steadily from October to December.</t>
+          <t>this line graph displays the production of fresh potatoes in canada for 2018 using the farm product price index.  a slow but steady increase is observed from january to june, where a steep increase is seen from june to august.  a steep decrease follows from august to october, where the value again rises steadily from october to december.</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>This line graph displays the TKN_About  in  TKN_Geo  for  TKN_Year  TKN_UOM  index.  A slow but steady increase is observed from January to June, where a steep increase is seen from June to August.  A steep decrease follows from August to October, where the value again rises steadily from October to December.</t>
+          <t>this line graph displays the TKN_About  in canada for  TKN_Year  TKN_UOM  index.  a slow but steady increase is observed from january to june, where a steep increase is seen from june to august.  a steep decrease follows from august to october, where the value again rises steadily from october to december.</t>
         </is>
       </c>
       <c r="W128" t="n">
@@ -11220,12 +11220,12 @@
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>A Graph showing the production of new motor vehicles by Canada in 2016. As you can see the production had a big climbing in Q1 2016. It stayed stable in Q2 and Q3, while fell down in Q4. it is a phisiologic trend for the motor vehicles market.</t>
+          <t>a graph showing the production of new motor vehicles by canada in 2016. as you can see the production had a big climbing in q1 2016. it stayed stable in q2 and q3, while fell down in q4. it is a phisiologic trend for the motor vehicles market.</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>A Graph showing the TKN_About  by  TKN_Geo  in  TKN_Year . As you can see the production had a big climbing in Q1  TKN_Year . It stayed stable in Q2 and Q3, while fell down in Q4. it is a phisiologic trend for the motor vehicles market.</t>
+          <t>a graph showing the TKN_About  by canada in  TKN_Year . as you can see the production had a big climbing in q1  TKN_Year . it stayed stable in q2 and q3, while fell down in q4. it is a phisiologic trend for the motor vehicles market.</t>
         </is>
       </c>
       <c r="W129" t="n">
@@ -11304,12 +11304,12 @@
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>Graphic of the market prices trend of Computers in Canada 2016. This graphic shows the trend of the computers prices in 2016 for the canadian market. It immediatly affect you how the prices raise from january to february and then slowly decrease until July. We can see another drop from July to September, probably justified by people on holiday, not buying any Computer and the a slight raise again till the end of the year.</t>
+          <t>graphic of the market prices trend of computers in canada 2016. this graphic shows the trend of the computers prices in 2016 for the canadian market. it immediatly affect you how the prices raise from january to february and then slowly decrease until july. we can see another drop from july to september, probably justified by people on holiday, not buying any computer and the a slight raise again till the end of the year.</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>Graphic of the market prices trend of Computers in  TKN_Geo   TKN_Year . This graphic shows TKN_About  prices in  TKN_Year  for the canadian market. It immediatly affect you how the prices raise from january to february and then slowly decrease until July. We can see another drop from July to September, probably justified by people on holiday, not buying any Computer and the a slight raise again till the end of the year.</t>
+          <t>graphic of the market prices trend of computers in canada  TKN_Year . this graphic shows TKN_About  prices in  TKN_Year  for the canadian market. it immediatly affect you how the prices raise from january to february and then slowly decrease until july. we can see another drop from july to september, probably justified by people on holiday, not buying any computer and the a slight raise again till the end of the year.</t>
         </is>
       </c>
       <c r="W130" t="n">
@@ -11556,12 +11556,12 @@
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>Plot graph describing how many motor bikes were produced in 2017 in Canada.</t>
+          <t>plot graph describing how many motor bikes were produced in 2017 in canada.</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>Plot graph TKN_About  bikes were produced in  TKN_Year  in  TKN_Geo .</t>
+          <t>plot graph TKN_About  bikes were produced in  TKN_Year  in canada.</t>
         </is>
       </c>
       <c r="W133" t="n">
@@ -11640,12 +11640,12 @@
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>Servers price index in 2018 from April to July has sharply increased.</t>
+          <t>servers price index in 2018 from april to july has sharply increased.</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>Servers price index in  TKN_Year  from April to July has sharply increased.</t>
+          <t>servers price index in  TKN_Year  from april to july has sharply increased.</t>
         </is>
       </c>
       <c r="W134" t="n">
@@ -11724,12 +11724,12 @@
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>Canola oil production fluctuate significantly over short periods of time.</t>
+          <t>canola oil production fluctuate significantly over short periods of time.</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>Canola oil production fluctuate significantly over short periods of time.</t>
+          <t>canola oil production fluctuate significantly over short periods of time.</t>
         </is>
       </c>
       <c r="W135" t="n">
@@ -11808,12 +11808,12 @@
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>Eggs production greatly increases during the second half of the year.</t>
+          <t>eggs production greatly increases during the second half of the year.</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>Eggs production greatly increases during the second half of the year.</t>
+          <t>eggs production greatly increases during the second half of the year.</t>
         </is>
       </c>
       <c r="W136" t="n">
@@ -11892,12 +11892,12 @@
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>The best time to buy a house in Canada in 2018 was between April and May.</t>
+          <t>the best time to buy a house in canada in 2018 was between april and may.</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>The best time to buy TKN_About  in  TKN_Geo  in  TKN_Year  was between April and May.</t>
+          <t>the best time to buy TKN_About  in canada in  TKN_Year  was between april and may.</t>
         </is>
       </c>
       <c r="W137" t="n">
@@ -11976,12 +11976,12 @@
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>In 2017, Canola oil production has suffered strong fluctuations.</t>
+          <t>in 2017, canola oil production has suffered strong fluctuations.</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>In  TKN_Year , TKN_About  has suffered strong fluctuations.</t>
+          <t>in  TKN_Year , TKN_About  has suffered strong fluctuations.</t>
         </is>
       </c>
       <c r="W138" t="n">
@@ -12060,12 +12060,12 @@
       </c>
       <c r="U139" t="inlineStr">
         <is>
-          <t>A plot chart about production of new motor vehicles.</t>
+          <t>a plot chart about production of new motor vehicles.</t>
         </is>
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>A plot chart about TKN_About  vehicles.</t>
+          <t>a plot chart about TKN_About  vehicles.</t>
         </is>
       </c>
       <c r="W139" t="n">
@@ -12144,12 +12144,12 @@
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>Fresh vegetables production start to increase from April.</t>
+          <t>fresh vegetables production start to increase from april.</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>Fresh vegetables production start to increase from April.</t>
+          <t>fresh vegetables production start to increase from april.</t>
         </is>
       </c>
       <c r="W140" t="n">
@@ -12228,12 +12228,12 @@
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>In June 2018 laptop price has hugely decrease.</t>
+          <t>in june 2018 laptop price has hugely decrease.</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>In June  TKN_Year  laptop price has hugely decrease.</t>
+          <t>in june  TKN_Year  laptop price has hugely decrease.</t>
         </is>
       </c>
       <c r="W141" t="n">
@@ -12312,12 +12312,12 @@
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>Malt production incredibly decrease from July 2018 to August 2018.</t>
+          <t>malt production incredibly decrease from july 2018 to august 2018.</t>
         </is>
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>Malt production incredibly decrease from July  TKN_Year  to August  TKN_Year .</t>
+          <t>malt production incredibly decrease from july  TKN_Year  to august  TKN_Year .</t>
         </is>
       </c>
       <c r="W142" t="n">
@@ -12396,12 +12396,12 @@
       </c>
       <c r="U143" t="inlineStr">
         <is>
-          <t>Production of creamery butter significantly increase near Christmas.</t>
+          <t>production of creamery butter significantly increase near christmas.</t>
         </is>
       </c>
       <c r="V143" t="inlineStr">
         <is>
-          <t>Production of creamery butter significantly increase near Christmas.</t>
+          <t>production of creamery butter significantly increase near christmas.</t>
         </is>
       </c>
       <c r="W143" t="n">
@@ -12480,12 +12480,12 @@
       </c>
       <c r="U144" t="inlineStr">
         <is>
-          <t>Amount of vehicles entering Canada in 2018.</t>
+          <t>amount of vehicles entering canada in 2018.</t>
         </is>
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>Amount TKN_About   TKN_Geo  in  TKN_Year .</t>
+          <t>amount of TKN_About  in  TKN_Year .</t>
         </is>
       </c>
       <c r="W144" t="n">
@@ -12564,12 +12564,12 @@
       </c>
       <c r="U145" t="inlineStr">
         <is>
-          <t>Cars entering Canada in one year.</t>
+          <t>cars entering canada in one year.</t>
         </is>
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>Cars entering  TKN_Geo  in one year.</t>
+          <t>cars entering canada in one year.</t>
         </is>
       </c>
       <c r="W145" t="n">
@@ -12648,12 +12648,12 @@
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>Oats produzed in Canada in the year 2017.</t>
+          <t>oats produzed in canada in the year 2017.</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>Oats produzed in  TKN_Geo  in the year  TKN_Year .</t>
+          <t>oats produzed in canada in the year  TKN_Year .</t>
         </is>
       </c>
       <c r="W146" t="n">
@@ -12732,12 +12732,12 @@
       </c>
       <c r="U147" t="inlineStr">
         <is>
-          <t>The FPPI of Canadian fresh fruit in 2016 fluctuates steadily between January and April. Then the FPPI start to decline, with its downwards slope increasing slightly after May. The FPPI drops dramatically in July, and reaches its lowest point in August. It then quickly starts raising, slowing slightly between September and October, and finishes its climb in November. The FPPI is close to its January value and is fairly steady until December.</t>
+          <t>the fppi of canadian fresh fruit in 2016 fluctuates steadily between january and april. then the fppi start to decline, with its downwards slope increasing slightly after may. the fppi drops dramatically in july, and reaches its lowest point in august. it then quickly starts raising, slowing slightly between september and october, and finishes its climb in november. the fppi is close to its january value and is fairly steady until december.</t>
         </is>
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>The FPPI TKN_About  in  TKN_Year  fluctuates steadily between January and April. Then the FPPI start to decline, with its downwards slope increasing slightly after May. The FPPI drops dramatically in July, and reaches its lowest point in August. It then quickly starts raising, slowing slightly between September and October, and finishes its climb in November. The FPPI is close to its January value and is fairly steady until December.</t>
+          <t>the fppi TKN_About  in  TKN_Year  fluctuates steadily between january and april. then the fppi start to decline, with its downwards slope increasing slightly after may. the fppi drops dramatically in july, and reaches its lowest point in august. it then quickly starts raising, slowing slightly between september and october, and finishes its climb in november. the fppi is close to its january value and is fairly steady until december.</t>
         </is>
       </c>
       <c r="W147" t="n">
@@ -12816,12 +12816,12 @@
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the number of vehicles entering Canada during 2016 has been much higher during the summer compared with the other months of the year. In particular, the maximum number of vehicles entering Canada in 2016 has been registered during August. At the same time, the minimum value during February.</t>
+          <t>as it's shown in the graph, the number of vehicles entering canada during 2016 has been much higher during the summer compared with the other months of the year. in particular, the maximum number of vehicles entering canada in 2016 has been registered during august. at the same time, the minimum value during february.</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the TKN_UOM  TKN_About   TKN_Geo  during  TKN_Year  has been much higher during the summer compared with the other months of the year. In particular, the maximum TKN_UOM  TKN_About   TKN_Geo  in  TKN_Year  has been registered during August. At the same time, the minimum value during February.</t>
+          <t>as it's shown in the graph, the TKN_UOM  of TKN_About  during  TKN_Year  has been much higher during the summer compared with the other months of the year. in particular, the maximum TKN_UOM  of TKN_About  in  TKN_Year  has been registered during august. at the same time, the minimum value during february.</t>
         </is>
       </c>
       <c r="W148" t="n">
@@ -12900,12 +12900,12 @@
       </c>
       <c r="U149" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the tablet computers price index in Canada rapidly decreased over 2017. Few fluctuations have been reported over the year. The maximum value has been recorded during March and the minimum during December 2017.</t>
+          <t>as it's possible to see from the graph, the tablet computers price index in canada rapidly decreased over 2017. few fluctuations have been reported over the year. the maximum value has been recorded during march and the minimum during december 2017.</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the TKN_About  index in  TKN_Geo  rapidly decreased over  TKN_Year . Few fluctuations have been reported over the year. The maximum value has been recorded during March and the minimum during December  TKN_Year .</t>
+          <t>as it's possible to see from the graph, the TKN_About  index in canada rapidly decreased over  TKN_Year . few fluctuations have been reported over the year. the maximum value has been recorded during march and the minimum during december  TKN_Year .</t>
         </is>
       </c>
       <c r="W149" t="n">
@@ -12984,12 +12984,12 @@
       </c>
       <c r="U150" t="inlineStr">
         <is>
-          <t>From the graph is clear that the supply of creamery butter had a significant jump from the month of February to April. The values in the graph are described using tonnes as unit of measurement. From July over the values started to slowly decrease until the end of the year.</t>
+          <t>from the graph is clear that the supply of creamery butter had a significant jump from the month of february to april. the values in the graph are described using tonnes as unit of measurement. from july over the values started to slowly decrease until the end of the year.</t>
         </is>
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>From the graph is clear that the TKN_About  had a significant jump from the month of February to April. The values in the graph are described using TKN_UOM  as unit of measurement. From July over the values started to slowly decrease until the end of the year.</t>
+          <t>from the graph is clear that the TKN_About  had a significant jump from the month of february to april. the values in the graph are described using TKN_UOM  as unit of measurement. from july over the values started to slowly decrease until the end of the year.</t>
         </is>
       </c>
       <c r="W150" t="n">
@@ -13068,12 +13068,12 @@
       </c>
       <c r="U151" t="inlineStr">
         <is>
-          <t>The following line chart is about the production of softwood and hardwood in Canada during 2018. The described values are in cubic metres. It's clearly possible to see how the production fluctuated over the year, with several peaks and dips. But at the end of the year, betwewen November and December, has been registered a significant drop of the value.</t>
+          <t>the following line chart is about the production of softwood and hardwood in canada during 2018. the described values are in cubic metres. it's clearly possible to see how the production fluctuated over the year, with several peaks and dips. but at the end of the year, betwewen november and december, has been registered a significant drop of the value.</t>
         </is>
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>The following line chart is about the TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The described values are TKN_UOM  metres. It's clearly possible to see how the production fluctuated over the year, with several peaks and dips. But at the end of the year, betwewen November and December, has been registered a significant drop of the value.</t>
+          <t>the following line chart is about the TKN_About  hardwood in canada during  TKN_Year . the described values are TKN_UOM  metres. it's clearly possible to see how the production fluctuated over the year, with several peaks and dips. but at the end of the year, betwewen november and december, has been registered a significant drop of the value.</t>
         </is>
       </c>
       <c r="W151" t="n">
@@ -13152,12 +13152,12 @@
       </c>
       <c r="U152" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the production of fresh potatoes in Canada during 2017 maintained the same level for almost the whole year, but the summer months. During the summer months have been registered the highest values, in particular during August which was the highest peak of production. After that, the values dropped down form August to October.</t>
+          <t>it's clearly possible to see how the production of fresh potatoes in canada during 2017 maintained the same level for almost the whole year, but the summer months. during the summer months have been registered the highest values, in particular during august which was the highest peak of production. after that, the values dropped down form august to october.</t>
         </is>
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  during  TKN_Year  maintained the same level for almost the whole year, but the summer months. During the summer months have been registered the highest values, in particular during August which was the highest peak of production. After that, the values dropped down form August to October.</t>
+          <t>it's clearly possible to see how the TKN_About  in canada during  TKN_Year  maintained the same level for almost the whole year, but the summer months. during the summer months have been registered the highest values, in particular during august which was the highest peak of production. after that, the values dropped down form august to october.</t>
         </is>
       </c>
       <c r="W152" t="n">
@@ -13236,12 +13236,12 @@
       </c>
       <c r="U153" t="inlineStr">
         <is>
-          <t>A chart showing the number of vehicles from the United States entering Canada sorted by month and showing the significant peak in the summer months.</t>
+          <t>a chart showing the number of vehicles from the united states entering canada sorted by month and showing the significant peak in the summer months.</t>
         </is>
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>A chart showing the TKN_UOM  of TKN_About   TKN_Geo  sorted by month and showing the significant peak in the summer months.</t>
+          <t>a chart showing the TKN_UOM  of TKN_About  canada sorted by month and showing the significant peak in the summer months.</t>
         </is>
       </c>
       <c r="W153" t="n">
@@ -13320,12 +13320,12 @@
       </c>
       <c r="U154" t="inlineStr">
         <is>
-          <t>A line chart about the production of fresh vegetables in Canada in the year 2017. Values   are analyzed in the different months of the year.</t>
+          <t>a line chart about the production of fresh vegetables in canada in the year 2017. values   are analyzed in the different months of the year.</t>
         </is>
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year.</t>
+          <t>a line chart about the TKN_About  in canada in the year  TKN_Year . values   are analyzed in the different months of the year.</t>
         </is>
       </c>
       <c r="W154" t="n">
@@ -13404,12 +13404,12 @@
       </c>
       <c r="U155" t="inlineStr">
         <is>
-          <t>A line chart about the price index of Desktop and similar computer in Canada in the year 2018. Values   are analyzed in the different months of the year. With index values   ranging from less than 954 to 962.</t>
+          <t>a line chart about the price index of desktop and similar computer in canada in the year 2018. values   are analyzed in the different months of the year. with index values   ranging from less than 954 to 962.</t>
         </is>
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About  computer in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 11 to 100.</t>
+          <t>a line chart about the TKN_About  computer in canada in the year  TKN_Year . values   are analyzed in the different months of the year. with index values   ranging from less than 11 to 100.</t>
         </is>
       </c>
       <c r="W155" t="n">
@@ -13488,12 +13488,12 @@
       </c>
       <c r="U156" t="inlineStr">
         <is>
-          <t>A line chart about the Production of Malt in tonnes in Canada in the year 2016. Values   are analyzed in the different months of the year. With index values   ranging from less than 45000 to more than 60000. The maximum value is reached in June.</t>
+          <t>a line chart about the production of malt in tonnes in canada in the year 2016. values   are analyzed in the different months of the year. with index values   ranging from less than 45000 to more than 60000. the maximum value is reached in june.</t>
         </is>
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About  in TKN_UOM  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 10 to more than 96. The maximum value is reached in June.</t>
+          <t>a line chart about the TKN_About  in TKN_UOM  in canada in the year  TKN_Year . values   are analyzed in the different months of the year. with index values   ranging from less than 10 to more than 96. the maximum value is reached in june.</t>
         </is>
       </c>
       <c r="W156" t="n">
@@ -13572,12 +13572,12 @@
       </c>
       <c r="U157" t="inlineStr">
         <is>
-          <t>A line chart about the Commercial software prince index in Canada in the year 2016. Values   are analyzed in the different months of the year. With index values   ranging from less than 1180 to more than 1220. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
+          <t>a line chart about the commercial software prince index in canada in the year 2016. values   are analyzed in the different months of the year. with index values   ranging from less than 1180 to more than 1220. the maximum value is reached in at the beginning of the year (jan) and then decreasing.</t>
         </is>
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About  in  TKN_Geo  in the year  TKN_Year . Values   are analyzed in the different months of the year. With index values   ranging from less than 12 to more than 105. The maximum value is reached in at the beginning of the year (Jan) and then decreasing.</t>
+          <t>a line chart about the TKN_About  in canada in the year  TKN_Year . values   are analyzed in the different months of the year. with index values   ranging from less than 12 to more than 105. the maximum value is reached in at the beginning of the year (jan) and then decreasing.</t>
         </is>
       </c>
       <c r="W157" t="n">
@@ -13656,12 +13656,12 @@
       </c>
       <c r="U158" t="inlineStr">
         <is>
-          <t>A line chart about Production of new motor vehicles per units in Canada in the year 2018. The value grows until May and then decreases.</t>
+          <t>a line chart about production of new motor vehicles per units in canada in the year 2018. the value grows until may and then decreases.</t>
         </is>
       </c>
       <c r="V158" t="inlineStr">
         <is>
-          <t>A line chart about TKN_About  per TKN_UOM  in  TKN_Geo  in the year  TKN_Year . The value grows until May and then decreases.</t>
+          <t>a line chart about TKN_About  per TKN_UOM  in canada in the year  TKN_Year . the value grows until may and then decreases.</t>
         </is>
       </c>
       <c r="W158" t="n">
@@ -13740,12 +13740,12 @@
       </c>
       <c r="U159" t="inlineStr">
         <is>
-          <t>A line chart about the Production of creamery butter per tonnes in Canada in the year 2018. The minimum value is reached in September and the maximum in January.</t>
+          <t>a line chart about the production of creamery butter per tonnes in canada in the year 2018. the minimum value is reached in september and the maximum in january.</t>
         </is>
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>A line chart about the TKN_About  per TKN_UOM  in  TKN_Geo  in the year  TKN_Year . The minimum value is reached in September and the maximum in January.</t>
+          <t>a line chart about the TKN_About  per TKN_UOM  in canada in the year  TKN_Year . the minimum value is reached in september and the maximum in january.</t>
         </is>
       </c>
       <c r="W159" t="n">
@@ -13824,12 +13824,12 @@
       </c>
       <c r="U160" t="inlineStr">
         <is>
-          <t>The chart represents the production of new motor vehicles (month vs. profit in dollars) in 2016 in Canada. The profit goes up rapidly in the first four months, then oscillates tending downward during May-September and finally plummets during September-December.</t>
+          <t>the chart represents the production of new motor vehicles (month vs. profit in dollars) in 2016 in canada. the profit goes up rapidly in the first four months, then oscillates tending downward during may-september and finally plummets during september-december.</t>
         </is>
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>The chart represents the TKN_About  (month vs. profit in dollars) in  TKN_Year  in  TKN_Geo . The profit goes up rapidly in the first four months, then oscillates tending downward during May-September and finally plummets during September-December.</t>
+          <t>the chart represents the TKN_About  (month vs. profit in dollars) in  TKN_Year  in canada. the profit goes up rapidly in the first four months, then oscillates tending downward during may-september and finally plummets during september-december.</t>
         </is>
       </c>
       <c r="W160" t="n">
@@ -13908,12 +13908,12 @@
       </c>
       <c r="U161" t="inlineStr">
         <is>
-          <t>The graph shows the import of creamery butter (month vs. tonnes) in Canada in 2016. First the rapid growth is observed in January, followed by a sharp decline in February. The import then raises slightly in March, remaining constant from April to June. Falling slightly during June-August, it jumps high in August-November, with a small slip in December.</t>
+          <t>the graph shows the import of creamery butter (month vs. tonnes) in canada in 2016. first the rapid growth is observed in january, followed by a sharp decline in february. the import then raises slightly in march, remaining constant from april to june. falling slightly during june-august, it jumps high in august-november, with a small slip in december.</t>
         </is>
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  (month vs. tonnes) in  TKN_Geo  in  TKN_Year . First the rapid growth is observed in January, followed by a sharp decline in February. The import then raises slightly in March, remaining constant from April to June. Falling slightly during June-August, it jumps high in August-November, with a small slip in December.</t>
+          <t>the graph shows the TKN_About  (month vs. tonnes) in canada in  TKN_Year . first the rapid growth is observed in january, followed by a sharp decline in february. the import then raises slightly in march, remaining constant from april to june. falling slightly during june-august, it jumps high in august-november, with a small slip in december.</t>
         </is>
       </c>
       <c r="W161" t="n">
@@ -13992,12 +13992,12 @@
       </c>
       <c r="U162" t="inlineStr">
         <is>
-          <t>Continuous increase of the house and land price index in Canada during the year 2017.</t>
+          <t>continuous increase of the house and land price index in canada during the year 2017.</t>
         </is>
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>Continuous increase of TKN_About  TKN_UOM  in  TKN_Geo  during the year  TKN_Year .</t>
+          <t>continuous increase of TKN_About  TKN_UOM  in canada during the year  TKN_Year .</t>
         </is>
       </c>
       <c r="W162" t="n">
@@ -14076,12 +14076,12 @@
       </c>
       <c r="U163" t="inlineStr">
         <is>
-          <t>The production of chickens, turkeys, chicks and poults fluctuates in Canada during the year 2016. From Januar until June it is remaining almost stable. From June until October it rises continuously and reaches the maximum value in october. In november and december it shows the smallest value.</t>
+          <t>the production of chickens, turkeys, chicks and poults fluctuates in canada during the year 2016. from januar until june it is remaining almost stable. from june until october it rises continuously and reaches the maximum value in october. in november and december it shows the smallest value.</t>
         </is>
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>The TKN_About  fluctuates in  TKN_Geo  during the year  TKN_Year . From Januar until June it is remaining almost stable. From June until October it rises continuously and reaches the maximum value in october. In november and december it shows the smallest value.</t>
+          <t>the TKN_About  fluctuates in canada during the year  TKN_Year . from januar until june it is remaining almost stable. from june until october it rises continuously and reaches the maximum value in october. in november and december it shows the smallest value.</t>
         </is>
       </c>
       <c r="W163" t="n">
@@ -14160,12 +14160,12 @@
       </c>
       <c r="U164" t="inlineStr">
         <is>
-          <t>The graph shows the trend of the total number of Canadian vehicles returning to Canada during the year 2017. The number drops between january and february and shows the minimum value in february. From february on it increases and shows the maximum value in august. Between august and december the number decreases continuously.</t>
+          <t>the graph shows the trend of the total number of canadian vehicles returning to canada during the year 2017. the number drops between january and february and shows the minimum value in february. from february on it increases and shows the maximum value in august. between august and december the number decreases continuously.</t>
         </is>
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>The graph shows the trend of the total TKN_UOM  of Canadian vehicles returning to  TKN_Geo  during the year  TKN_Year . The TKN_UOM  drops between january and february and shows the minimum value in february. From february on it increases and shows the maximum value in august. Between august and december the TKN_UOM  decreases continuously.</t>
+          <t>the graph shows the trend of the total TKN_UOM  of canadian vehicles returning to canada during the year  TKN_Year . the TKN_UOM  drops between january and february and shows the minimum value in february. from february on it increases and shows the maximum value in august. between august and december the TKN_UOM  decreases continuously.</t>
         </is>
       </c>
       <c r="W164" t="n">
@@ -14244,12 +14244,12 @@
       </c>
       <c r="U165" t="inlineStr">
         <is>
-          <t>Graph that describes the production of unprocessed milk in Canada in 2017. The production in October and February is the highest, while there is a significant drop the following two months of each. The production slightly rises in May but it then plunges until July, where the lowest value can be seen. After that month, there is a steady increase until October.</t>
+          <t>graph that describes the production of unprocessed milk in canada in 2017. the production in october and february is the highest, while there is a significant drop the following two months of each. the production slightly rises in may but it then plunges until july, where the lowest value can be seen. after that month, there is a steady increase until october.</t>
         </is>
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>Graph that describes the TKN_About  in  TKN_Geo  in  TKN_Year . The production in October and February is the highest, while there is a significant drop the following two months of each. The production slightly rises in May but it then plunges until July, where the lowest value can be seen. After that month, there is a steady increase until October.</t>
+          <t>graph that describes the TKN_About  in canada in  TKN_Year . the production in october and february is the highest, while there is a significant drop the following two months of each. the production slightly rises in may but it then plunges until july, where the lowest value can be seen. after that month, there is a steady increase until october.</t>
         </is>
       </c>
       <c r="W165" t="n">
@@ -14328,12 +14328,12 @@
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>Total softwood production in cubic meters in Canada in 2018 is shown in the graph. Production in January starts at roughly 5650 m3, and it shrinks the next month. In March, this value goes back up and remains steady until May. It plunges until July to the same value as in February and then it oscilates between this value and the one in January until November to drop again to 4200 m3 in December.</t>
+          <t>total softwood production in cubic meters in canada in 2018 is shown in the graph. production in january starts at roughly 5650 m3, and it shrinks the next month. in march, this value goes back up and remains steady until may. it plunges until july to the same value as in february and then it oscilates between this value and the one in january until november to drop again to 4200 m3 in december.</t>
         </is>
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>Total softwood production TKN_UOM  meters in  TKN_Geo  in  TKN_Year  is shown in the graph. Production in January starts at roughly 88 m3, and it shrinks the next month. In March, this value goes back up and remains steady until May. It plunges until July to the same value as in February and then it oscilates between this value and the one in January until November to drop again to -2 m3 in December.</t>
+          <t>total softwood production TKN_UOM  meters in canada in  TKN_Year  is shown in the graph. production in january starts at roughly 88 m3, and it shrinks the next month. in march, this value goes back up and remains steady until may. it plunges until july to the same value as in february and then it oscilates between this value and the one in january until november to drop again to -2 m3 in december.</t>
         </is>
       </c>
       <c r="W166" t="n">
@@ -14412,12 +14412,12 @@
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>The graph depicts the FPPI in Canada during 2018. The highest was during August, where it was above 1220, whereas the lowest was in December, where it almost reached 1120. From January to July, the values fluctuate between 1140 and 1180, and after August, the values decrease until December.</t>
+          <t>the graph depicts the fppi in canada during 2018. the highest was during august, where it was above 1220, whereas the lowest was in december, where it almost reached 1120. from january to july, the values fluctuate between 1140 and 1180, and after august, the values decrease until december.</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>The graph depicts the FPPI in  TKN_Geo  during  TKN_Year . The highest was during August, where it was above 89, whereas the lowest was in December, where it almost reached -4. From January to July, the values fluctuate between 15 and 52, and after August, the values decrease until December.</t>
+          <t>the graph depicts the fppi in canada during  TKN_Year . the highest was during august, where it was above 89, whereas the lowest was in december, where it almost reached -4. from january to july, the values fluctuate between 15 and 52, and after august, the values decrease until december.</t>
         </is>
       </c>
       <c r="W167" t="n">
@@ -14496,12 +14496,12 @@
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>The graph shows a general downward trend of the price of Tablet computers over the year 2017 in Canada. There was a slight price climb in the middle of the year. As this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
+          <t>the graph shows a general downward trend of the price of tablet computers over the year 2017 in canada. there was a slight price climb in the middle of the year. as this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>The graph shows a general downward trend of the TKN_About  over the year  TKN_Year  in  TKN_Geo . There was a slight price climb in the middle of the year. As this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
+          <t>the graph shows a general downward trend of the TKN_About  over the year  TKN_Year  in canada. there was a slight price climb in the middle of the year. as this is a price index and the y-axis is missing, one can only assume a relative decrease in price.</t>
         </is>
       </c>
       <c r="W168" t="n">
@@ -14580,12 +14580,12 @@
       </c>
       <c r="U169" t="inlineStr">
         <is>
-          <t>This graph shows the monthly amount of oats produced in Canada in 2018 in tonnes. Oat production stayed within the range of 80000 and 210000 tonnes each month. While most months averaged production at around 140000 tonnes, February, June and July saw dips in production to around 90000 tonnes and the fall months saw a higher harvest, 16000 and above 200000 tonnes consecutively.</t>
+          <t>this graph shows the monthly amount of oats produced in canada in 2018 in tonnes. oat production stayed within the range of 80000 and 210000 tonnes each month. while most months averaged production at around 140000 tonnes, february, june and july saw dips in production to around 90000 tonnes and the fall months saw a higher harvest, 16000 and above 200000 tonnes consecutively.</t>
         </is>
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>This graph shows the monthly amount TKN_About  produced in  TKN_Geo  in  TKN_Year  in TKN_UOM . Oat production stayed within the range of 0 and 97 TKN_UOM  each month. While most months averaged production at around 45 TKN_UOM , February, June and July saw dips in production to around 7 TKN_UOM  and the fall months saw a higher harvest, -48 and above 90 TKN_UOM  consecutively.</t>
+          <t>this graph shows the monthly amount TKN_About  produced in canada in  TKN_Year  in TKN_UOM . oat production stayed within the range of 0 and 97 TKN_UOM  each month. while most months averaged production at around 45 TKN_UOM , february, june and july saw dips in production to around 7 TKN_UOM  and the fall months saw a higher harvest, -48 and above 90 TKN_UOM  consecutively.</t>
         </is>
       </c>
       <c r="W169" t="n">
@@ -14664,12 +14664,12 @@
       </c>
       <c r="U170" t="inlineStr">
         <is>
-          <t>This graph shows a general upward trend in the price index of commercial software in Canada in 2018. While there were drops in the price index in April and August from their respective previous months, the graph obeyed an increasing trend.</t>
+          <t>this graph shows a general upward trend in the price index of commercial software in canada in 2018. while there were drops in the price index in april and august from their respective previous months, the graph obeyed an increasing trend.</t>
         </is>
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>This graph shows a general upward trend in the price TKN_About  in  TKN_Geo  in  TKN_Year . While there were drops in the price index in April and August from their respective previous months, the graph obeyed an increasing trend.</t>
+          <t>this graph shows a general upward trend in the price TKN_About  in canada in  TKN_Year . while there were drops in the price index in april and august from their respective previous months, the graph obeyed an increasing trend.</t>
         </is>
       </c>
       <c r="W170" t="n">
@@ -14748,12 +14748,12 @@
       </c>
       <c r="U171" t="inlineStr">
         <is>
-          <t>The given graph shows the average retail price developement of laptop computers in Canada in the year 2017 split into the different months. In january the price started out at 992 dollars, increased slightly and then plummeted to 976 dollars average in June. A short incline happend in July just for it falling back onto the June price in august. After a slight incline, the price fell to its lowest in december.</t>
+          <t>the given graph shows the average retail price developement of laptop computers in canada in the year 2017 split into the different months. in january the price started out at 992 dollars, increased slightly and then plummeted to 976 dollars average in june. a short incline happend in july just for it falling back onto the june price in august. after a slight incline, the price fell to its lowest in december.</t>
         </is>
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>The given graph shows the average retail TKN_About  in  TKN_Geo  in the year  TKN_Year  split into the different months. In january the price started out at 92 dollars, increased slightly and then plummeted to 25 dollars average in June. A short incline happend in July just for it falling back onto the June price in august. After a slight incline, the price fell to its lowest in december.</t>
+          <t>the given graph shows the average retail TKN_About  in canada in the year  TKN_Year  split into the different months. in january the price started out at 92 dollars, increased slightly and then plummeted to 25 dollars average in june. a short incline happend in july just for it falling back onto the june price in august. after a slight incline, the price fell to its lowest in december.</t>
         </is>
       </c>
       <c r="W171" t="n">
@@ -14832,12 +14832,12 @@
       </c>
       <c r="U172" t="inlineStr">
         <is>
-          <t>The graph shows the production of fresh fruits in Canada over the year of 2016. In the first half of the year the production was nearly constant, until it fall dramatically in the mounth of August. Afterwards the fresh fruit production rises again over the index of 1100.</t>
+          <t>the graph shows the production of fresh fruits in canada over the year of 2016. in the first half of the year the production was nearly constant, until it fall dramatically in the mounth of august. afterwards the fresh fruit production rises again over the index of 1100.</t>
         </is>
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  fruits in  TKN_Geo  over the year of  TKN_Year . In the first half of the year the production was nearly constant, until it fall dramatically in the mounth of August. Afterwards the fresh fruit production rises again over the index of 75.</t>
+          <t>the graph shows the TKN_About  fruits in canada over the year of  TKN_Year . in the first half of the year the production was nearly constant, until it fall dramatically in the mounth of august. afterwards the fresh fruit production rises again over the index of 75.</t>
         </is>
       </c>
       <c r="W172" t="n">
@@ -14916,12 +14916,12 @@
       </c>
       <c r="U173" t="inlineStr">
         <is>
-          <t>The graph showes the anual price index of tablet computers in the year 2017. The price in the first thre month is very high, especially in March. The following month ist drops and increase again in June and stays constant till July. Afterwards it decrease continusliy till December. Over the whole year there is a decreasing trend.</t>
+          <t>the graph showes the anual price index of tablet computers in the year 2017. the price in the first thre month is very high, especially in march. the following month ist drops and increase again in june and stays constant till july. afterwards it decrease continusliy till december. over the whole year there is a decreasing trend.</t>
         </is>
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>The graph showes the anual TKN_About  in the year  TKN_Year . The price in the first thre month is very high, especially in March. The following month ist drops and increase again in June and stays constant till July. Afterwards it decrease continusliy till December. Over the whole year there is a decreasing trend.</t>
+          <t>the graph showes the anual TKN_About  in the year  TKN_Year . the price in the first thre month is very high, especially in march. the following month ist drops and increase again in june and stays constant till july. afterwards it decrease continusliy till december. over the whole year there is a decreasing trend.</t>
         </is>
       </c>
       <c r="W173" t="n">
@@ -15000,12 +15000,12 @@
       </c>
       <c r="U174" t="inlineStr">
         <is>
-          <t>This graph shows the number of vehicles entering the United States in 2016. The number of cars entering is about 700000 at the start and end of the year. It increases towards summer. There is a peak in the middle of the year at 1250000 in July.</t>
+          <t>this graph shows the number of vehicles entering the united states in 2016. the number of cars entering is about 700000 at the start and end of the year. it increases towards summer. there is a peak in the middle of the year at 1250000 in july.</t>
         </is>
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>This graph shows the TKN_UOM  of TKN_About  in  TKN_Year . The TKN_UOM  of cars entering is about 11 at the start and end of the year. It increases towards summer. There is a peak in the middle of the year at 101 in July.</t>
+          <t>this graph shows the TKN_UOM  of TKN_About  in  TKN_Year . the TKN_UOM  of cars entering is about 11 at the start and end of the year. it increases towards summer. there is a peak in the middle of the year at 101 in july.</t>
         </is>
       </c>
       <c r="W174" t="n">
@@ -15084,12 +15084,12 @@
       </c>
       <c r="U175" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the yearly developement of wheat flower production in tonnes in 2018. The starting point in January is around 30000 tons, with an increase to peak production  in April with over 43000 tons and a following decline to just under 35000 tons. After a slight increase the production plummited to just over 20000 tons in September and fell to its lowest point of around 17000 tons in December.</t>
+          <t>the accompanying graph shows the yearly developement of wheat flower production in tonnes in 2018. the starting point in january is around 30000 tons, with an increase to peak production  in april with over 43000 tons and a following decline to just under 35000 tons. after a slight increase the production plummited to just over 20000 tons in september and fell to its lowest point of around 17000 tons in december.</t>
         </is>
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the yearly developement TKN_About  in TKN_UOM  in  TKN_Year . The starting point in January is around 50 tons, with an increase to peak production  in April with over 103 tons and a following decline to just under 71 tons. After a slight increase the production plummited to just over 9 tons in September and fell to its lowest point of around -3 tons in December.</t>
+          <t>the accompanying graph shows the yearly developement TKN_About  in TKN_UOM  in  TKN_Year . the starting point in january is around 50 tons, with an increase to peak production  in april with over 103 tons and a following decline to just under 71 tons. after a slight increase the production plummited to just over 9 tons in september and fell to its lowest point of around -3 tons in december.</t>
         </is>
       </c>
       <c r="W175" t="n">
@@ -15168,12 +15168,12 @@
       </c>
       <c r="U176" t="inlineStr">
         <is>
-          <t>The grapg shows the price index of tablet computers in Canada in the year 2018. It is noticeable that the price decreases almost continuously during the first third of the year. Afterwards, the price for the summer months remains constant, before falling massive in November.</t>
+          <t>the grapg shows the price index of tablet computers in canada in the year 2018. it is noticeable that the price decreases almost continuously during the first third of the year. afterwards, the price for the summer months remains constant, before falling massive in november.</t>
         </is>
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>The grapg shows the TKN_About  in  TKN_Geo  in the year  TKN_Year . It is noticeable that the price decreases almost continuously during the first third of the year. Afterwards, the price for the summer months remains constant, before falling massive in November.</t>
+          <t>the grapg shows the TKN_About  in canada in the year  TKN_Year . it is noticeable that the price decreases almost continuously during the first third of the year. afterwards, the price for the summer months remains constant, before falling massive in november.</t>
         </is>
       </c>
       <c r="W176" t="n">
@@ -15252,12 +15252,12 @@
       </c>
       <c r="U177" t="inlineStr">
         <is>
-          <t>The graph shows the land price index development in Canada in 2017. The starting point was just shy of 1005 dollars in january but skyrocketed to over 1030 dollars in May. A continouus, but a lot less steeper incline happend in between may and december, finishing at around 1037 dollars in december.</t>
+          <t>the graph shows the land price index development in canada in 2017. the starting point was just shy of 1005 dollars in january but skyrocketed to over 1030 dollars in may. a continouus, but a lot less steeper incline happend in between may and december, finishing at around 1037 dollars in december.</t>
         </is>
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  TKN_UOM  development in  TKN_Geo  in  TKN_Year . The starting point was just shy of 3 dollars in january but skyrocketed to over 79 dollars in May. A continouus, but a lot less steeper incline happend in between may and december, finishing at around 100 dollars in december.</t>
+          <t>the graph shows TKN_About  TKN_UOM  development in canada in  TKN_Year . the starting point was just shy of 3 dollars in january but skyrocketed to over 79 dollars in may. a continouus, but a lot less steeper incline happend in between may and december, finishing at around 100 dollars in december.</t>
         </is>
       </c>
       <c r="W177" t="n">
@@ -15336,12 +15336,12 @@
       </c>
       <c r="U178" t="inlineStr">
         <is>
-          <t>The total farm production index from the year 2016 is showen by the graph. in Jannuary it starts increasing continously till March, decreas a little bit in April and increase again till it reach the annual maximum of  around 1375 in June. The folowing monthes the index decrease rapidly till October and reaches the minimum value of about 1245. in November and December it increases again.</t>
+          <t>the total farm production index from the year 2016 is showen by the graph. in jannuary it starts increasing continously till march, decreas a little bit in april and increase again till it reach the annual maximum of  around 1375 in june. the folowing monthes the index decrease rapidly till october and reaches the minimum value of about 1245. in november and december it increases again.</t>
         </is>
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>The TKN_About  from the year  TKN_Year  is showen by the graph. in Jannuary it starts increasing continously till March, decreas a little bit in April and increase again till it reach the annual maximum of  around 103 in June. The folowing monthes the index decrease rapidly till October and reaches the minimum value of about 0. in November and December it increases again.</t>
+          <t>the TKN_About  from the year  TKN_Year  is showen by the graph. in jannuary it starts increasing continously till march, decreas a little bit in april and increase again till it reach the annual maximum of  around 103 in june. the folowing monthes the index decrease rapidly till october and reaches the minimum value of about 0. in november and december it increases again.</t>
         </is>
       </c>
       <c r="W178" t="n">
@@ -15420,12 +15420,12 @@
       </c>
       <c r="U179" t="inlineStr">
         <is>
-          <t>This is a canola production graph, showing the amount produced in tonnes for the year 2016. Production stayed within the range of 600000 to about 1125000 tonnes during the year. Production started just under 800000 tonnes in January and rose to above 1000000 tonnes in March. It then dips to under 600000 tonnes in August, with acute increases in May and July, before experiencing a continuous rise to above 1100000 tonnes in December.</t>
+          <t>this is a canola production graph, showing the amount produced in tonnes for the year 2016. production stayed within the range of 600000 to about 1125000 tonnes during the year. production started just under 800000 tonnes in january and rose to above 1000000 tonnes in march. it then dips to under 600000 tonnes in august, with acute increases in may and july, before experiencing a continuous rise to above 1100000 tonnes in december.</t>
         </is>
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>This is a TKN_About  graph, showing the amount produced in TKN_UOM  for the year  TKN_Year . Production stayed within the range of 6 to about 99 TKN_UOM  during the year. Production started just under 41 TKN_UOM  in January and rose to above 77 TKN_UOM  in March. It then dips to under 6 TKN_UOM  in August, with acute increases in May and July, before experiencing a continuous rise to above 95 TKN_UOM  in December.</t>
+          <t>this is a TKN_About  graph, showing the amount produced in TKN_UOM  for the year  TKN_Year . production stayed within the range of 6 to about 99 TKN_UOM  during the year. production started just under 41 TKN_UOM  in january and rose to above 77 TKN_UOM  in march. it then dips to under 6 TKN_UOM  in august, with acute increases in may and july, before experiencing a continuous rise to above 95 TKN_UOM  in december.</t>
         </is>
       </c>
       <c r="W179" t="n">
@@ -15504,12 +15504,12 @@
       </c>
       <c r="U180" t="inlineStr">
         <is>
-          <t>The graph shows the production of wheat flour (in tonnes) in Canada in the year 2018. Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 42000 tonnes. This is followed by a more or less constant decline, until in December with 10000 tonnes the minimum of production is reached.</t>
+          <t>the graph shows the production of wheat flour (in tonnes) in canada in the year 2018. production is very different over the year. while a significant decline in production can be observed from january to february, production continues to rise until april, reaching its annual maximum of more than 42000 tonnes. this is followed by a more or less constant decline, until in december with 10000 tonnes the minimum of production is reached.</t>
         </is>
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  (in TKN_UOM ) in  TKN_Geo  in the year  TKN_Year . Production is very different over the year. While a significant decline in production can be observed from January to February, production continues to rise until April, reaching its annual maximum of more than 99 TKN_UOM . This is followed by a more or less constant decline, until in December with -32 TKN_UOM  the minimum of production is reached.</t>
+          <t>the graph shows the TKN_About  (in TKN_UOM ) in canada in the year  TKN_Year . production is very different over the year. while a significant decline in production can be observed from january to february, production continues to rise until april, reaching its annual maximum of more than 99 TKN_UOM . this is followed by a more or less constant decline, until in december with -32 TKN_UOM  the minimum of production is reached.</t>
         </is>
       </c>
       <c r="W180" t="n">
@@ -15588,12 +15588,12 @@
       </c>
       <c r="U181" t="inlineStr">
         <is>
-          <t>The given graph shows the house and land price index development in Canada in the year 2018, devided by month. The index started out at 1033 january and then decreased to 1031 in february and staying constant until may, giving way to a rise back to 1033 between may and july, again staying at 1033 dollars till the end of the year.</t>
+          <t>the given graph shows the house and land price index development in canada in the year 2018, devided by month. the index started out at 1033 january and then decreased to 1031 in february and staying constant until may, giving way to a rise back to 1033 between may and july, again staying at 1033 dollars till the end of the year.</t>
         </is>
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>The given graph shows TKN_About  TKN_UOM  development in  TKN_Geo  in the year  TKN_Year , devided by month. The index started out at 100 january and then decreased to 0 in february and staying constant until may, giving way to a rise back to 100 between may and july, again staying at 100 dollars till the end of the year.</t>
+          <t>the given graph shows TKN_About  TKN_UOM  development in canada in the year  TKN_Year , devided by month. the index started out at 100 january and then decreased to 0 in february and staying constant until may, giving way to a rise back to 100 between may and july, again staying at 100 dollars till the end of the year.</t>
         </is>
       </c>
       <c r="W181" t="n">
@@ -15672,12 +15672,12 @@
       </c>
       <c r="U182" t="inlineStr">
         <is>
-          <t>The graph showes the price index of servers in 2016. It starts with the maximum value in January and falls massive till to the minimum in March. Afterwards it increases till June while dropping a little bit in May. In June it drops again and increase afterwards slowly till october. It fall again rapidly in November and stays constant in December.</t>
+          <t>the graph showes the price index of servers in 2016. it starts with the maximum value in january and falls massive till to the minimum in march. afterwards it increases till june while dropping a little bit in may. in june it drops again and increase afterwards slowly till october. it fall again rapidly in november and stays constant in december.</t>
         </is>
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>The graph showes the TKN_About  in  TKN_Year . It starts with the maximum value in January and falls massive till to the minimum in March. Afterwards it increases till June while dropping a little bit in May. In June it drops again and increase afterwards slowly till october. It fall again rapidly in November and stays constant in December.</t>
+          <t>the graph showes the TKN_About  in  TKN_Year . it starts with the maximum value in january and falls massive till to the minimum in march. afterwards it increases till june while dropping a little bit in may. in june it drops again and increase afterwards slowly till october. it fall again rapidly in november and stays constant in december.</t>
         </is>
       </c>
       <c r="W182" t="n">
@@ -15756,12 +15756,12 @@
       </c>
       <c r="U183" t="inlineStr">
         <is>
-          <t>The graphs shows the total softwood and hardwood production in Canada in the year 2017. As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over 60000 cubic meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
+          <t>the graphs shows the total softwood and hardwood production in canada in the year 2017. as can be seen in the graph, the production changes very much over the year. initially, the value falls to february before rising in march and reaching a maximum of over 60000 cubic meters. it is also noticeable that production is lower in the summer months. however, the minimum is reached in december.</t>
         </is>
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>The graphs shows the TKN_About  in  TKN_Geo  in the year  TKN_Year . As can be seen in the graph, the production changes very much over the year. Initially, the value falls to February before rising in March and reaching a maximum of over TKN_UOM  meters. It is also noticeable that production is lower in the summer months. However, the minimum is reached in December.</t>
+          <t>the graphs shows the TKN_About  in canada in the year  TKN_Year . as can be seen in the graph, the production changes very much over the year. initially, the value falls to february before rising in march and reaching a maximum of over TKN_UOM  meters. it is also noticeable that production is lower in the summer months. however, the minimum is reached in december.</t>
         </is>
       </c>
       <c r="W183" t="n">
@@ -15840,12 +15840,12 @@
       </c>
       <c r="U184" t="inlineStr">
         <is>
-          <t>The graph showes production of creamery butter in tonnes in the year 2017. The highest production is in January with around 11450 tonnes. It decreases in February and stay nearly constant till April. Afterwards it drops constanously and rapidly till june. It increase agin in july till it drop again in August to the minimal production of creamery butter. Till the end of the year it increase beside a small drop in November.</t>
+          <t>the graph showes production of creamery butter in tonnes in the year 2017. the highest production is in january with around 11450 tonnes. it decreases in february and stay nearly constant till april. afterwards it drops constanously and rapidly till june. it increase agin in july till it drop again in august to the minimal production of creamery butter. till the end of the year it increase beside a small drop in november.</t>
         </is>
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>The graph showes TKN_About  in TKN_UOM  in the year  TKN_Year . The highest production is in January with around 104 TKN_UOM . It decreases in February and stay nearly constant till April. Afterwards it drops constanously and rapidly till june. It increase agin in july till it drop again in August to the minimal TKN_About . Till the end of the year it increase beside a small drop in November.</t>
+          <t>the graph showes TKN_About  in TKN_UOM  in the year  TKN_Year . the highest production is in january with around 104 TKN_UOM . it decreases in february and stay nearly constant till april. afterwards it drops constanously and rapidly till june. it increase agin in july till it drop again in august to the minimal TKN_About . till the end of the year it increase beside a small drop in november.</t>
         </is>
       </c>
       <c r="W184" t="n">
@@ -15924,12 +15924,12 @@
       </c>
       <c r="U185" t="inlineStr">
         <is>
-          <t>This shows the price index of servers in 2017. it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. There was also a dip in April. The price is an index that does not reflect absolute pricing.</t>
+          <t>this shows the price index of servers in 2017. it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. there was also a dip in april. the price is an index that does not reflect absolute pricing.</t>
         </is>
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>This shows the TKN_About  in  TKN_Year . it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. There was also a dip in April. The price is an index that does not reflect absolute pricing.</t>
+          <t>this shows the TKN_About  in  TKN_Year . it stayed relatively stable from the start of year into the third quarter before experiencing a decrease in the last quarter. there was also a dip in april. the price is an index that does not reflect absolute pricing.</t>
         </is>
       </c>
       <c r="W185" t="n">
@@ -16008,12 +16008,12 @@
       </c>
       <c r="U186" t="inlineStr">
         <is>
-          <t>The aforementioned graph shows the production of grains in FPPI units divided by months of the year 2016. Starting point is at 1100 in January and after some slight ups and downs it increased to around 1115 in May only to plummet over the next few months to its lowest point around 970 in September just to increase to 1030 in December again.</t>
+          <t>the aforementioned graph shows the production of grains in fppi units divided by months of the year 2016. starting point is at 1100 in january and after some slight ups and downs it increased to around 1115 in may only to plummet over the next few months to its lowest point around 970 in september just to increase to 1030 in december again.</t>
         </is>
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>The aforementioned graph shows the TKN_About  in FPPI units divided by months of the year  TKN_Year . Starting point is at 93 in January and after some slight ups and downs it increased to around 104 in May only to plummet over the next few months to its lowest point around 1 in September just to increase to 44 in December again.</t>
+          <t>the aforementioned graph shows the TKN_About  in fppi units divided by months of the year  TKN_Year . starting point is at 93 in january and after some slight ups and downs it increased to around 104 in may only to plummet over the next few months to its lowest point around 1 in september just to increase to 44 in december again.</t>
         </is>
       </c>
       <c r="W186" t="n">
@@ -16092,12 +16092,12 @@
       </c>
       <c r="U187" t="inlineStr">
         <is>
-          <t>The graph shows the house and land price index in canada in the year of 2018. It is striking that the value only changes twice a year. It falls from January to February, and from May to July it rises back to the original amount of 1033. For the rest of the year, the value remains constant.</t>
+          <t>the graph shows the house and land price index in canada in the year of 2018. it is striking that the value only changes twice a year. it falls from january to february, and from may to july it rises back to the original amount of 1033. for the rest of the year, the value remains constant.</t>
         </is>
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  TKN_UOM  in canada in the year of  TKN_Year . It is striking that the value only changes twice a year. It falls from January to February, and from May to July it rises back to the original amount of 100. For the rest of the year, the value remains constant.</t>
+          <t>the graph shows TKN_About  TKN_UOM  in canada in the year of  TKN_Year . it is striking that the value only changes twice a year. it falls from january to february, and from may to july it rises back to the original amount of 100. for the rest of the year, the value remains constant.</t>
         </is>
       </c>
       <c r="W187" t="n">
@@ -16176,12 +16176,12 @@
       </c>
       <c r="U188" t="inlineStr">
         <is>
-          <t>The accompanying shows the monthly development of total livestock and animal products production in the year 2016 in Canada, measured in FPPI. It starts out at 1450 in January, increases slightly to just shy of 1475 in March, falls to 1430 in April and increases again to 1460 in June. After that it constantly decreases until reaching its lowest point of 1260 in October. It continues to rise afterwards.</t>
+          <t>the accompanying shows the monthly development of total livestock and animal products production in the year 2016 in canada, measured in fppi. it starts out at 1450 in january, increases slightly to just shy of 1475 in march, falls to 1430 in april and increases again to 1460 in june. after that it constantly decreases until reaching its lowest point of 1260 in october. it continues to rise afterwards.</t>
         </is>
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>The accompanying shows the monthly development of TKN_About  production in the year  TKN_Year  in  TKN_Geo , measured in FPPI. It starts out at 90 in January, increases slightly to just shy of 102 in March, falls to 80 in April and increases again to 95 in June. After that it constantly decreases until reaching its lowest point of -3 in October. It continues to rise afterwards.</t>
+          <t>the accompanying shows the monthly development of TKN_About  production in the year  TKN_Year  in canada, measured in fppi. it starts out at 90 in january, increases slightly to just shy of 102 in march, falls to 80 in april and increases again to 95 in june. after that it constantly decreases until reaching its lowest point of -3 in october. it continues to rise afterwards.</t>
         </is>
       </c>
       <c r="W188" t="n">
@@ -16260,12 +16260,12 @@
       </c>
       <c r="U189" t="inlineStr">
         <is>
-          <t>The grapg shows the production of rye in canada in the year of 2016. While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 25000 tonnes is reached. A lot of work for the farmers in this season of the year I guess.</t>
+          <t>the grapg shows the production of rye in canada in the year of 2016. while production is very low during the winter months, more is produced during the summer months. in september, the annual maximum of almost 25000 tonnes is reached. a lot of work for the farmers in this season of the year i guess.</t>
         </is>
       </c>
       <c r="V189" t="inlineStr">
         <is>
-          <t>The grapg shows the TKN_About  in canada in the year of  TKN_Year . While production is very low during the winter months, more is produced during the summer months. In September, the annual maximum of almost 102 TKN_UOM  is reached. A lot of work for the farmers in this season of the year I guess.</t>
+          <t>the grapg shows the TKN_About  in canada in the year of  TKN_Year . while production is very low during the winter months, more is produced during the summer months. in september, the annual maximum of almost 102 TKN_UOM  is reached. a lot of work for the farmers in this season of the year i guess.</t>
         </is>
       </c>
       <c r="W189" t="n">
@@ -16344,12 +16344,12 @@
       </c>
       <c r="U190" t="inlineStr">
         <is>
-          <t>The graph illustrates the production of Grains in Canada in in 2016. The first few monthes till May the production fluctuate at around 1100. In june it starts to decrease a little bit and in july and august there is a massive drop. In September the graph keeps going decreasing and reach the annual minimum. The last monthes of the year the graph is increasing again.</t>
+          <t>the graph illustrates the production of grains in canada in in 2016. the first few monthes till may the production fluctuate at around 1100. in june it starts to decrease a little bit and in july and august there is a massive drop. in september the graph keeps going decreasing and reach the annual minimum. the last monthes of the year the graph is increasing again.</t>
         </is>
       </c>
       <c r="V190" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About  in  TKN_Geo  in in  TKN_Year . The first few monthes till May the production fluctuate at around 93. In june it starts to decrease a little bit and in july and august there is a massive drop. In September the graph keeps going decreasing and reach the annual minimum. The last monthes of the year the graph is increasing again.</t>
+          <t>the graph illustrates the TKN_About  in canada in in  TKN_Year . the first few monthes till may the production fluctuate at around 93. in june it starts to decrease a little bit and in july and august there is a massive drop. in september the graph keeps going decreasing and reach the annual minimum. the last monthes of the year the graph is increasing again.</t>
         </is>
       </c>
       <c r="W190" t="n">
@@ -16428,12 +16428,12 @@
       </c>
       <c r="U191" t="inlineStr">
         <is>
-          <t>The graph shows the production of wood in 2016. It stayed at within above 54000 and about 58000 cubic meters except for two dips in July with 51000 cubic meters and December with below 48000 cubic meters.</t>
+          <t>the graph shows the production of wood in 2016. it stayed at within above 54000 and about 58000 cubic meters except for two dips in july with 51000 cubic meters and december with below 48000 cubic meters.</t>
         </is>
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>The TKN_About  of wood in  TKN_Year . It stayed at within above 61 and about TKN_UOM  meters except for two dips in July with 34 cubic meters and December with below 7 cubic meters.</t>
+          <t>the TKN_About  of wood in  TKN_Year . it stayed at within above 61 and about TKN_UOM  meters except for two dips in july with 34 cubic meters and december with below 7 cubic meters.</t>
         </is>
       </c>
       <c r="W191" t="n">
@@ -16512,12 +16512,12 @@
       </c>
       <c r="U192" t="inlineStr">
         <is>
-          <t>The given graph shows the monthly development of the production of fresh vegetables in Farm product price index in 2016 in Canada. After starting out at 1402 in January it immediately starts falling to 1360 in May, rising again to 1375 in June and then falling to 1343 in August. After staying pretty flat until October it starts skyrocketing to its highest point of 1410 in December.</t>
+          <t>the given graph shows the monthly development of the production of fresh vegetables in farm product price index in 2016 in canada. after starting out at 1402 in january it immediately starts falling to 1360 in may, rising again to 1375 in june and then falling to 1343 in august. after staying pretty flat until october it starts skyrocketing to its highest point of 1410 in december.</t>
         </is>
       </c>
       <c r="V192" t="inlineStr">
         <is>
-          <t>The given graph shows the monthly development of the TKN_About  TKN_UOM  in  TKN_Year  in  TKN_Geo . After starting out at 88 in January it immediately starts falling to 25 in May, rising again to 48 in June and then falling to 0 in August. After staying pretty flat until October it starts skyrocketing to its highest point of 100 in December.</t>
+          <t>the given graph shows the monthly development of the TKN_About  TKN_UOM  in  TKN_Year  in canada. after starting out at 88 in january it immediately starts falling to 25 in may, rising again to 48 in june and then falling to 0 in august. after staying pretty flat until october it starts skyrocketing to its highest point of 100 in december.</t>
         </is>
       </c>
       <c r="W192" t="n">
@@ -16596,12 +16596,12 @@
       </c>
       <c r="U193" t="inlineStr">
         <is>
-          <t>Graph elucidates the grain production in the year 2018. Production experienced a general increase over the year, with a sharp spike in August and dips in the months of February, July and November.</t>
+          <t>graph elucidates the grain production in the year 2018. production experienced a general increase over the year, with a sharp spike in august and dips in the months of february, july and november.</t>
         </is>
       </c>
       <c r="V193" t="inlineStr">
         <is>
-          <t>Graph elucidates the TKN_About  in the year  TKN_Year . Production experienced a general increase over the year, with a sharp spike in August and dips in the months of February, July and November.</t>
+          <t>graph elucidates the TKN_About  in the year  TKN_Year . production experienced a general increase over the year, with a sharp spike in august and dips in the months of february, july and november.</t>
         </is>
       </c>
       <c r="W193" t="n">
@@ -16680,12 +16680,12 @@
       </c>
       <c r="U194" t="inlineStr">
         <is>
-          <t>The graph illustrates the productioin of Rye in tonnes in 2016. The first few montes till May the graph stays quite constant at a low level of about 5000 tonnes, besides a small peak in March up to nearly 10000 tonnes. The graph starts to increase continusly from May to July. Afterwards it increase rapidly till the maxumum value in September. The next few monthes till the end of the year ithe graph decreases.</t>
+          <t>the graph illustrates the productioin of rye in tonnes in 2016. the first few montes till may the graph stays quite constant at a low level of about 5000 tonnes, besides a small peak in march up to nearly 10000 tonnes. the graph starts to increase continusly from may to july. afterwards it increase rapidly till the maxumum value in september. the next few monthes till the end of the year ithe graph decreases.</t>
         </is>
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>The graph illustrates the productioin TKN_About  in TKN_UOM  in  TKN_Year . The first few montes till May the graph stays quite constant at a low level of about 2 TKN_UOM , besides a small peak in March up to nearly 27 TKN_UOM . The graph starts to increase continusly from May to July. Afterwards it increase rapidly till the maxumum value in September. The next few monthes till the end of the year ithe graph decreases.</t>
+          <t>the graph illustrates the productioin TKN_About  in TKN_UOM  in  TKN_Year . the first few montes till may the graph stays quite constant at a low level of about 2 TKN_UOM , besides a small peak in march up to nearly 27 TKN_UOM . the graph starts to increase continusly from may to july. afterwards it increase rapidly till the maxumum value in september. the next few monthes till the end of the year ithe graph decreases.</t>
         </is>
       </c>
       <c r="W194" t="n">
@@ -16764,12 +16764,12 @@
       </c>
       <c r="U195" t="inlineStr">
         <is>
-          <t>The graph highlights the production of fresh vegetables over the course of a year. It follow a "U" shape with a local increase in the month of June.</t>
+          <t>the graph highlights the production of fresh vegetables over the course of a year. it follow a "u" shape with a local increase in the month of june.</t>
         </is>
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>The graph highlights the TKN_About  over the course of a year. It follow a "U" shape with a local increase in the month of June.</t>
+          <t>the graph highlights the TKN_About  over the course of a year. it follow a "u" shape with a local increase in the month of june.</t>
         </is>
       </c>
       <c r="W195" t="n">
@@ -16848,12 +16848,12 @@
       </c>
       <c r="U196" t="inlineStr">
         <is>
-          <t>The provided graph depicts the development of the price index for tablet computers in Canada in 2016, divided by month. After a slow decline from 943 in January to 938 in February it crashes, reaching a low point of 897 in March. Afterwards it rises to 924 in April and then slowly but constantly declines to 876 in December.</t>
+          <t>the provided graph depicts the development of the price index for tablet computers in canada in 2016, divided by month. after a slow decline from 943 in january to 938 in february it crashes, reaching a low point of 897 in march. afterwards it rises to 924 in april and then slowly but constantly declines to 876 in december.</t>
         </is>
       </c>
       <c r="V196" t="inlineStr">
         <is>
-          <t>The provided graph depicts the development of the TKN_About  in  TKN_Geo  in  TKN_Year , divided by month. After a slow decline from 100 in January to 92 in February it crashes, reaching a low point of 30 in March. Afterwards it rises to 71 in April and then slowly but constantly declines to -2 in December.</t>
+          <t>the provided graph depicts the development of the TKN_About  in canada in  TKN_Year , divided by month. after a slow decline from 100 in january to 92 in february it crashes, reaching a low point of 30 in march. afterwards it rises to 71 in april and then slowly but constantly declines to -2 in december.</t>
         </is>
       </c>
       <c r="W196" t="n">
@@ -16932,12 +16932,12 @@
       </c>
       <c r="U197" t="inlineStr">
         <is>
-          <t>The graph shows the house price index increasing over the year. It stayed the same for the mon of May and September but was increasing continuously throughout the year otherwise.</t>
+          <t>the graph shows the house price index increasing over the year. it stayed the same for the mon of may and september but was increasing continuously throughout the year otherwise.</t>
         </is>
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  TKN_UOM  increasing over the year. It stayed the same for the mon of May and September but was increasing continuously throughout the year otherwise.</t>
+          <t>the graph shows TKN_About  TKN_UOM  increasing over the year. it stayed the same for the mon of may and september but was increasing continuously throughout the year otherwise.</t>
         </is>
       </c>
       <c r="W197" t="n">
@@ -17016,12 +17016,12 @@
       </c>
       <c r="U198" t="inlineStr">
         <is>
-          <t>The graph showes the total vehicles entering canada in 2017. The graph decreases in February. From february till August it starts to increase continously and reaches the maximum of over 3400000. From August till December the graph decrease continuslie till a total number of 2400000 in December.</t>
+          <t>the graph showes the total vehicles entering canada in 2017. the graph decreases in february. from february till august it starts to increase continously and reaches the maximum of over 3400000. from august till december the graph decrease continuslie till a total number of 2400000 in december.</t>
         </is>
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>The graph showes the TKN_About  in  TKN_Year . The graph decreases in February. From february till August it starts to increase continously and reaches the maximum of over 94. From August till December the graph decrease continuslie till a total TKN_UOM  of 28 in December.</t>
+          <t>the graph showes the TKN_About  in  TKN_Year . the graph decreases in february. from february till august it starts to increase continously and reaches the maximum of over 94. from august till december the graph decrease continuslie till a total TKN_UOM  of 28 in december.</t>
         </is>
       </c>
       <c r="W198" t="n">
@@ -17100,12 +17100,12 @@
       </c>
       <c r="U199" t="inlineStr">
         <is>
-          <t>The provided graph depicts the changes in the production of unprocessed milk in Canada in 2016. The first value sits at 1045 in January, giving way to a slight increase to 1068 that is followed by a decline back to 1046 in April. A short rise follows in may but its crashing to 1010 in July. The following months show a steep increase till October, followed by a slow and steady rise till December.</t>
+          <t>the provided graph depicts the changes in the production of unprocessed milk in canada in 2016. the first value sits at 1045 in january, giving way to a slight increase to 1068 that is followed by a decline back to 1046 in april. a short rise follows in may but its crashing to 1010 in july. the following months show a steep increase till october, followed by a slow and steady rise till december.</t>
         </is>
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>The provided graph depicts the changes in the TKN_About  in  TKN_Geo  in  TKN_Year . The first value sits at 34 in January, giving way to a slight increase to 56 that is followed by a decline back to 35 in April. A short rise follows in may but its crashing to -1 in July. The following months show a steep increase till October, followed by a slow and steady rise till December.</t>
+          <t>the provided graph depicts the changes in the TKN_About  in canada in  TKN_Year . the first value sits at 34 in january, giving way to a slight increase to 56 that is followed by a decline back to 35 in april. a short rise follows in may but its crashing to -1 in july. the following months show a steep increase till october, followed by a slow and steady rise till december.</t>
         </is>
       </c>
       <c r="W199" t="n">
@@ -17184,12 +17184,12 @@
       </c>
       <c r="U200" t="inlineStr">
         <is>
-          <t>The graph illustrates the production of rye in canada in the year 2017. The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 20000 tonnes. Then the production decrease again for the remaining months of the year.</t>
+          <t>the graph illustrates the production of rye in canada in the year 2017. the production is very low in the first third of the year, before it rises sharply until october, reaching a maximum of 20000 tonnes. then the production decrease again for the remaining months of the year.</t>
         </is>
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About  in canada in the year  TKN_Year . The production is very low in the first third of the year, before it rises sharply until October, reaching a maximum of 100 tonnes. Then the production decrease again for the remaining months of the year.</t>
+          <t>the graph illustrates the TKN_About  in canada in the year  TKN_Year . the production is very low in the first third of the year, before it rises sharply until october, reaching a maximum of 100 tonnes. then the production decrease again for the remaining months of the year.</t>
         </is>
       </c>
       <c r="W200" t="n">
@@ -17268,12 +17268,12 @@
       </c>
       <c r="U201" t="inlineStr">
         <is>
-          <t>It describes the price index of laptop computer in Canada during 2016. It's clearly possible to see how the values are strongly fluctuating over the year. The maximum values have been recorded during the may of February and May. The minimum value was in August 2016.</t>
+          <t>it describes the price index of laptop computer in canada during 2016. it's clearly possible to see how the values are strongly fluctuating over the year. the maximum values have been recorded during the may of february and may. the minimum value was in august 2016.</t>
         </is>
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>It describes the TKN_About  computer in  TKN_Geo  during  TKN_Year . It's clearly possible to see how the values are strongly fluctuating over the year. The maximum values have been recorded during the may of February and May. The minimum value was in August  TKN_Year .</t>
+          <t>it describes the TKN_About  computer in canada during  TKN_Year . it's clearly possible to see how the values are strongly fluctuating over the year. the maximum values have been recorded during the may of february and may. the minimum value was in august  TKN_Year .</t>
         </is>
       </c>
       <c r="W201" t="n">
@@ -17352,12 +17352,12 @@
       </c>
       <c r="U202" t="inlineStr">
         <is>
-          <t>The graph shoes the overall decrease in tablet computer prices throughout the year. The months of March, June, September and December experienced more sharp drops than the others. The price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
+          <t>the graph shoes the overall decrease in tablet computer prices throughout the year. the months of march, june, september and december experienced more sharp drops than the others. the price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
         </is>
       </c>
       <c r="V202" t="inlineStr">
         <is>
-          <t>The graph shoes the overall TKN_About  computer prices throughout the year. The months of March, June, September and December experienced more sharp drops than the others. The price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
+          <t>the graph shoes the overall TKN_About  computer prices throughout the year. the months of march, june, september and december experienced more sharp drops than the others. the price index climbed slghtly after each sharp drop, but proceeded to slide again.</t>
         </is>
       </c>
       <c r="W202" t="n">
@@ -17436,12 +17436,12 @@
       </c>
       <c r="U203" t="inlineStr">
         <is>
-          <t>The graph shows the production of wheat flour in tonnes in Canada in 2017. The lowest production is in Jannuary. From February till July the graph oscillate. in August it drops and rise again in September. It stay constant in October before it decrease in November again. In december it jump to the highest production of around 40000.</t>
+          <t>the graph shows the production of wheat flour in tonnes in canada in 2017. the lowest production is in jannuary. from february till july the graph oscillate. in august it drops and rise again in september. it stay constant in october before it decrease in november again. in december it jump to the highest production of around 40000.</t>
         </is>
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  in TKN_UOM  in  TKN_Geo  in  TKN_Year . The lowest production is in Jannuary. From February till July the graph oscillate. in August it drops and rise again in September. It stay constant in October before it decrease in November again. In december it jump to the highest production of around 101.</t>
+          <t>the graph shows the TKN_About  in TKN_UOM  in canada in  TKN_Year . the lowest production is in jannuary. from february till july the graph oscillate. in august it drops and rise again in september. it stay constant in october before it decrease in november again. in december it jump to the highest production of around 101.</t>
         </is>
       </c>
       <c r="W203" t="n">
@@ -17520,12 +17520,12 @@
       </c>
       <c r="U204" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the fluctuation in oat production in tons in Canada in the year 2016 divided by months. Between January and July it fluctuates heavily followed by a rise to over 200000 tons in September. The next few months show a continuous decline to the end point at 140000 tons in December.</t>
+          <t>the accompanying graph shows the fluctuation in oat production in tons in canada in the year 2016 divided by months. between january and july it fluctuates heavily followed by a rise to over 200000 tons in september. the next few months show a continuous decline to the end point at 140000 tons in december.</t>
         </is>
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>The accompanying graph shows the fluctuation in TKN_About  in tons in  TKN_Geo  in the year  TKN_Year  divided by months. Between January and July it fluctuates heavily followed by a rise to over 94 tons in September. The next few months show a continuous decline to the end point at 48 tons in December.</t>
+          <t>the accompanying graph shows the fluctuation in TKN_About  in tons in canada in the year  TKN_Year  divided by months. between january and july it fluctuates heavily followed by a rise to over 94 tons in september. the next few months show a continuous decline to the end point at 48 tons in december.</t>
         </is>
       </c>
       <c r="W204" t="n">
@@ -17604,12 +17604,12 @@
       </c>
       <c r="U205" t="inlineStr">
         <is>
-          <t>It shows the data about supply of creamery butter in Canada during 2016. The displayed values are in tones. It's possible to see how the value rapidly increase from January over, reaching its peaks during the month of July with approximately 29000 tonnes. After that, the values decrease until September and then rise up again during last 3 months of the year.</t>
+          <t>it shows the data about supply of creamery butter in canada during 2016. the displayed values are in tones. it's possible to see how the value rapidly increase from january over, reaching its peaks during the month of july with approximately 29000 tonnes. after that, the values decrease until september and then rise up again during last 3 months of the year.</t>
         </is>
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>It shows the data about TKN_About  in  TKN_Geo  during  TKN_Year . The displayed values are in tones. It's possible to see how the value rapidly increase from January over, reaching its peaks during the month of July with approximately 101 tonnes. After that, the values decrease until September and then rise up again during last 3 months of the year.</t>
+          <t>it shows the data about TKN_About  in canada during  TKN_Year . the displayed values are in tones. it's possible to see how the value rapidly increase from january over, reaching its peaks during the month of july with approximately 101 tonnes. after that, the values decrease until september and then rise up again during last 3 months of the year.</t>
         </is>
       </c>
       <c r="W205" t="n">
@@ -17688,12 +17688,12 @@
       </c>
       <c r="U206" t="inlineStr">
         <is>
-          <t>The graph indicates the house price index in canada in the year 2016. As shown the index increases during the hole year until he reaches the maximum of 1000 in December. Unfortunately, you can not say more about this graph.</t>
+          <t>the graph indicates the house price index in canada in the year 2016. as shown the index increases during the hole year until he reaches the maximum of 1000 in december. unfortunately, you can not say more about this graph.</t>
         </is>
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>The graph indicates TKN_About  TKN_UOM  in canada in the year  TKN_Year . As shown the index increases during the hole year until he reaches the maximum of 100 in December. Unfortunately, you can not say more about this graph.</t>
+          <t>the graph indicates TKN_About  TKN_UOM  in canada in the year  TKN_Year . as shown the index increases during the hole year until he reaches the maximum of 100 in december. unfortunately, you can not say more about this graph.</t>
         </is>
       </c>
       <c r="W206" t="n">
@@ -17772,12 +17772,12 @@
       </c>
       <c r="U207" t="inlineStr">
         <is>
-          <t>The graph shows the price index of laptop computer in the year 2016 in Canada. The price index fluctuates hugely the first four monthes and reach the maximum in May. It falls in June and July and drop massivly in August. it rise again in September and October and stays constant in Novermber. In December it drop again.</t>
+          <t>the graph shows the price index of laptop computer in the year 2016 in canada. the price index fluctuates hugely the first four monthes and reach the maximum in may. it falls in june and july and drop massivly in august. it rise again in september and october and stays constant in novermber. in december it drop again.</t>
         </is>
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  computer in the year  TKN_Year  in  TKN_Geo . The price index fluctuates hugely the first four monthes and reach the maximum in May. It falls in June and July and drop massivly in August. it rise again in September and October and stays constant in Novermber. In December it drop again.</t>
+          <t>the graph shows the TKN_About  computer in the year  TKN_Year  in canada. the price index fluctuates hugely the first four monthes and reach the maximum in may. it falls in june and july and drop massivly in august. it rise again in september and october and stays constant in novermber. in december it drop again.</t>
         </is>
       </c>
       <c r="W207" t="n">
@@ -17856,12 +17856,12 @@
       </c>
       <c r="U208" t="inlineStr">
         <is>
-          <t>The provided graph displays the number of Canadian vehicles returning to Canada over the year 2016 divided by month. It starts out at around 1500000 vehicles in January, falls to 1350000 in February and rises continuously to over 2200000 in August. The following month show a steady decrease to its second lowest point of just under 1600000 in December.</t>
+          <t>the provided graph displays the number of canadian vehicles returning to canada over the year 2016 divided by month. it starts out at around 1500000 vehicles in january, falls to 1350000 in february and rises continuously to over 2200000 in august. the following month show a steady decrease to its second lowest point of just under 1600000 in december.</t>
         </is>
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>The provided graph displays the TKN_UOM  of Canadian vehicles returning to  TKN_Geo  over the year  TKN_Year  divided by month. It starts out at around 18 vehicles in January, falls to 1 in February and rises continuously to over 97 in August. The following month show a steady decrease to its second lowest point of just under 29 in December.</t>
+          <t>the provided graph displays the TKN_UOM  of canadian vehicles returning to canada over the year  TKN_Year  divided by month. it starts out at around 18 vehicles in january, falls to 1 in february and rises continuously to over 97 in august. the following month show a steady decrease to its second lowest point of just under 29 in december.</t>
         </is>
       </c>
       <c r="W208" t="n">
@@ -17940,12 +17940,12 @@
       </c>
       <c r="U209" t="inlineStr">
         <is>
-          <t>The graph shows the number of Canadian vehicles returning in 2016. The graph follows an uphill climb from January until August, except for dips in the months of Feburary and June. After August, the graph has a falling trend to the end of the year.</t>
+          <t>the graph shows the number of canadian vehicles returning in 2016. the graph follows an uphill climb from january until august, except for dips in the months of feburary and june. after august, the graph has a falling trend to the end of the year.</t>
         </is>
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_UOM  of Canadian vehicles returning in  TKN_Year . The graph follows an uphill climb from January until August, except for dips in the months of Feburary and June. After August, the graph has a falling trend to the end of the year.</t>
+          <t>the graph shows the TKN_UOM  of canadian vehicles returning in  TKN_Year . the graph follows an uphill climb from january until august, except for dips in the months of feburary and june. after august, the graph has a falling trend to the end of the year.</t>
         </is>
       </c>
       <c r="W209" t="n">
@@ -18024,12 +18024,12 @@
       </c>
       <c r="U210" t="inlineStr">
         <is>
-          <t>The line chart is displaying the recorded data about production of wheat flour in Canada during 2017. The minimum value of production have been recorded during the months of January, August and November. From January to February has been recorded a significant growth. The maximum value of production over the year was recorded during December.</t>
+          <t>the line chart is displaying the recorded data about production of wheat flour in canada during 2017. the minimum value of production have been recorded during the months of january, august and november. from january to february has been recorded a significant growth. the maximum value of production over the year was recorded during december.</t>
         </is>
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>The line chart is displaying the recorded data about TKN_About  in  TKN_Geo  during  TKN_Year . The minimum value of production have been recorded during the months of January, August and November. From January to February has been recorded a significant growth. The maximum value of production over the year was recorded during December.</t>
+          <t>the line chart is displaying the recorded data about TKN_About  in canada during  TKN_Year . the minimum value of production have been recorded during the months of january, august and november. from january to february has been recorded a significant growth. the maximum value of production over the year was recorded during december.</t>
         </is>
       </c>
       <c r="W210" t="n">
@@ -18108,12 +18108,12 @@
       </c>
       <c r="U211" t="inlineStr">
         <is>
-          <t>The graph indicates the production of eggs in shell in canada in the year of 2016. As the graph rises from January to February, it drops sharply until July, before reaching a minimum of 1340. Subsequently, the value rises continuously until the end of the year, reaching a maximum of 1365 in December.</t>
+          <t>the graph indicates the production of eggs in shell in canada in the year of 2016. as the graph rises from january to february, it drops sharply until july, before reaching a minimum of 1340. subsequently, the value rises continuously until the end of the year, reaching a maximum of 1365 in december.</t>
         </is>
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>The graph indicates the TKN_About  in canada in the year of  TKN_Year . As the graph rises from January to February, it drops sharply until July, before reaching a minimum of 4. Subsequently, the value rises continuously until the end of the year, reaching a maximum of 96 in December.</t>
+          <t>the graph indicates the TKN_About  in canada in the year of  TKN_Year . as the graph rises from january to february, it drops sharply until july, before reaching a minimum of 4. subsequently, the value rises continuously until the end of the year, reaching a maximum of 96 in december.</t>
         </is>
       </c>
       <c r="W211" t="n">
@@ -18192,12 +18192,12 @@
       </c>
       <c r="U212" t="inlineStr">
         <is>
-          <t>The displayed chart shows the total number of vehicles entering Canada during 2018. It's possible to see how the highest values have been recorded during the spring and summer months. In particular, the maximum number of cars entering Canada has been reached July and a August. The months with minimum values have been January and February.</t>
+          <t>the displayed chart shows the total number of vehicles entering canada during 2018. it's possible to see how the highest values have been recorded during the spring and summer months. in particular, the maximum number of cars entering canada has been reached july and a august. the months with minimum values have been january and february.</t>
         </is>
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>The displayed chart shows the total TKN_UOM  of vehicles entering  TKN_Geo  during  TKN_Year . It's possible to see how the highest values have been recorded during the spring and summer months. In particular, the maximum TKN_UOM  of cars entering  TKN_Geo  has been reached July and a August. The months with minimum values have been January and February.</t>
+          <t>the displayed chart shows the total TKN_UOM  of vehicles entering canada during  TKN_Year . it's possible to see how the highest values have been recorded during the spring and summer months. in particular, the maximum TKN_UOM  of cars entering canada has been reached july and a august. the months with minimum values have been january and february.</t>
         </is>
       </c>
       <c r="W212" t="n">
@@ -18276,12 +18276,12 @@
       </c>
       <c r="U213" t="inlineStr">
         <is>
-          <t>The graph shows the oats production over the year of 2016. The graph stayed in the range of about 80000 and 200000 tonnes. It has a zig-zag waveform from January to August, before a last peak in September and then decreasing in the last quarter of the year.</t>
+          <t>the graph shows the oats production over the year of 2016. the graph stayed in the range of about 80000 and 200000 tonnes. it has a zig-zag waveform from january to august, before a last peak in september and then decreasing in the last quarter of the year.</t>
         </is>
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  over the year of  TKN_Year . The graph stayed in the range of about 2 and 94 tonnes. It has a zig-zag waveform from January to August, before a last peak in September and then decreasing in the last quarter of the year.</t>
+          <t>the graph shows the TKN_About  over the year of  TKN_Year . the graph stayed in the range of about 2 and 94 tonnes. it has a zig-zag waveform from january to august, before a last peak in september and then decreasing in the last quarter of the year.</t>
         </is>
       </c>
       <c r="W213" t="n">
@@ -18360,12 +18360,12 @@
       </c>
       <c r="U214" t="inlineStr">
         <is>
-          <t>The given graph shows the malt production in tons in Canada in 2017. The Graph continuously rises from 52000 tons in January to 60000 in May, falls back to 53000 in June and rises to 63000 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 40000 tons.</t>
+          <t>the given graph shows the malt production in tons in canada in 2017. the graph continuously rises from 52000 tons in january to 60000 in may, falls back to 53000 in june and rises to 63000 in july. the following months just show a steady decrease of production. the lowest point is reached in december with under 40000 tons.</t>
         </is>
       </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>The given graph shows the TKN_About  in tons in  TKN_Geo  in  TKN_Year . The Graph continuously rises from 56 tons in January to 91 in May, falls back to 60 in June and rises to 104 in July. The following months just show a steady decrease of production. The lowest point is reached in December with under 4 tons.</t>
+          <t>the given graph shows the TKN_About  in tons in canada in  TKN_Year . the graph continuously rises from 56 tons in january to 91 in may, falls back to 60 in june and rises to 104 in july. the following months just show a steady decrease of production. the lowest point is reached in december with under 4 tons.</t>
         </is>
       </c>
       <c r="W214" t="n">
@@ -18444,12 +18444,12 @@
       </c>
       <c r="U215" t="inlineStr">
         <is>
-          <t>The graph shows the production of Grains in Canada in 2017. The first five monthes of the year it oscillates at around 1010. the next two months the production increase. It drop a little bit in August and rise again in September to the annual maximum of 1095. in October, November and December there is a slightly and continously decrease.</t>
+          <t>the graph shows the production of grains in canada in 2017. the first five monthes of the year it oscillates at around 1010. the next two months the production increase. it drop a little bit in august and rise again in september to the annual maximum of 1095. in october, november and december there is a slightly and continously decrease.</t>
         </is>
       </c>
       <c r="V215" t="inlineStr">
         <is>
-          <t>The graph shows the TKN_About  in  TKN_Geo  in  TKN_Year . The first five monthes of the year it oscillates at around 4. the next two months the production increase. It drop a little bit in August and rise again in September to the annual maximum of 105. in October, November and December there is a slightly and continously decrease.</t>
+          <t>the graph shows the TKN_About  in canada in  TKN_Year . the first five monthes of the year it oscillates at around 4. the next two months the production increase. it drop a little bit in august and rise again in september to the annual maximum of 105. in october, november and december there is a slightly and continously decrease.</t>
         </is>
       </c>
       <c r="W215" t="n">
@@ -18528,12 +18528,12 @@
       </c>
       <c r="U216" t="inlineStr">
         <is>
-          <t>The graph indicates the entering vehicles from the united states in canada in the year of 2018. It is noticeable that the number is rising sharply by the middle of the year, reaching a maximum of 1200000 in August. Then the value is strong again until the end of the year.</t>
+          <t>the graph indicates the entering vehicles from the united states in canada in the year of 2018. it is noticeable that the number is rising sharply by the middle of the year, reaching a maximum of 1200000 in august. then the value is strong again until the end of the year.</t>
         </is>
       </c>
       <c r="V216" t="inlineStr">
         <is>
-          <t>The graph indicates the TKN_About  in canada in the year of  TKN_Year . It is noticeable that the TKN_UOM  is rising sharply by the middle of the year, reaching a maximum of 101 in August. Then the value is strong again until the end of the year.</t>
+          <t>the graph indicates the TKN_About  in canada in the year of  TKN_Year . it is noticeable that the TKN_UOM  is rising sharply by the middle of the year, reaching a maximum of 101 in august. then the value is strong again until the end of the year.</t>
         </is>
       </c>
       <c r="W216" t="n">
@@ -18612,12 +18612,12 @@
       </c>
       <c r="U217" t="inlineStr">
         <is>
-          <t>The grain production index of the year 2017 saw a zig-zag pattern from January to May before increasing in July and remained relatively stable for the rest of the year at the increased price.</t>
+          <t>the grain production index of the year 2017 saw a zig-zag pattern from january to may before increasing in july and remained relatively stable for the rest of the year at the increased price.</t>
         </is>
       </c>
       <c r="V217" t="inlineStr">
         <is>
-          <t>The grain TKN_About  the year  TKN_Year  saw a zig-zag pattern from January to May before increasing in July and remained relatively stable for the rest of the year at the increased price.</t>
+          <t>the grain TKN_About  the year  TKN_Year  saw a zig-zag pattern from january to may before increasing in july and remained relatively stable for the rest of the year at the increased price.</t>
         </is>
       </c>
       <c r="W217" t="n">
@@ -18696,12 +18696,12 @@
       </c>
       <c r="U218" t="inlineStr">
         <is>
-          <t>The graph is showing the production's trend of total hardwood in Canada during 2017. The values are in cubic metres. It's clearly possible to see how the values are strongly fluctuating over the year. There are several peaks, in particular during March, May and Novembe. At the same time, the minimum values have been recorded during the months of January, July and August.</t>
+          <t>the graph is showing the production's trend of total hardwood in canada during 2017. the values are in cubic metres. it's clearly possible to see how the values are strongly fluctuating over the year. there are several peaks, in particular during march, may and novembe. at the same time, the minimum values have been recorded during the months of january, july and august.</t>
         </is>
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>The graph is showing the production's trend TKN_About  hardwood in  TKN_Geo  during  TKN_Year . The values are TKN_UOM  metres. It's clearly possible to see how the values are strongly fluctuating over the year. There are several peaks, in particular during March, May and Novembe. At the same time, the minimum values have been recorded during the months of January, July and August.</t>
+          <t>the graph is showing the production's trend TKN_About  hardwood in canada during  TKN_Year . the values are TKN_UOM  metres. it's clearly possible to see how the values are strongly fluctuating over the year. there are several peaks, in particular during march, may and novembe. at the same time, the minimum values have been recorded during the months of january, july and august.</t>
         </is>
       </c>
       <c r="W218" t="n">
@@ -18780,12 +18780,12 @@
       </c>
       <c r="U219" t="inlineStr">
         <is>
-          <t>The following graph is showing the recorded values about production of fresh potatoes in Canada during 2016. The values have been reported using the farm product price index (FPPI). As it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of August. After the summer, the production value drop, reaching its minimum value in October.</t>
+          <t>the following graph is showing the recorded values about production of fresh potatoes in canada during 2016. the values have been reported using the farm product price index (fppi). as it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of august. after the summer, the production value drop, reaching its minimum value in october.</t>
         </is>
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>The following graph is showing the recorded values about TKN_About  in  TKN_Geo  during  TKN_Year . The values have been reported using TKN_UOM  (FPPI). As it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of August. After the summer, the production value drop, reaching its minimum value in October.</t>
+          <t>the following graph is showing the recorded values about TKN_About  in canada during  TKN_Year . the values have been reported using TKN_UOM  (fppi). as it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of august. after the summer, the production value drop, reaching its minimum value in october.</t>
         </is>
       </c>
       <c r="W219" t="n">
@@ -18864,12 +18864,12 @@
       </c>
       <c r="U220" t="inlineStr">
         <is>
-          <t>It illustrates the stocks of softwood and hardwood in Canada during 2016 using cubic metres as unit of measurement. From January to April has been recorded a slightly increase. The value significantly dropped from May to July, and then it remain steady for the last months of the year. The minimum value has been recorded during the month of December.</t>
+          <t>it illustrates the stocks of softwood and hardwood in canada during 2016 using cubic metres as unit of measurement. from january to april has been recorded a slightly increase. the value significantly dropped from may to july, and then it remain steady for the last months of the year. the minimum value has been recorded during the month of december.</t>
         </is>
       </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>It illustrates the TKN_About  hardwood in  TKN_Geo  during  TKN_Year  using TKN_UOM  as unit of measurement. From January to April has been recorded a slightly increase. The value significantly dropped from May to July, and then it remain steady for the last months of the year. The minimum value has been recorded during the month of December.</t>
+          <t>it illustrates the TKN_About  hardwood in canada during  TKN_Year  using TKN_UOM  as unit of measurement. from january to april has been recorded a slightly increase. the value significantly dropped from may to july, and then it remain steady for the last months of the year. the minimum value has been recorded during the month of december.</t>
         </is>
       </c>
       <c r="W220" t="n">
@@ -18948,12 +18948,12 @@
       </c>
       <c r="U221" t="inlineStr">
         <is>
-          <t>The production of fresh fruit in Canada during 2017 has been increasing over the year. Even that, several fluctuations have been recorded, in particular during the first months of the year. The maximum values have been recorded during November and December. During the first months of the year, from January to May, have been recorded the minimum production values.</t>
+          <t>the production of fresh fruit in canada during 2017 has been increasing over the year. even that, several fluctuations have been recorded, in particular during the first months of the year. the maximum values have been recorded during november and december. during the first months of the year, from january to may, have been recorded the minimum production values.</t>
         </is>
       </c>
       <c r="V221" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  has been increasing over the year. Even that, several fluctuations have been recorded, in particular during the first months of the year. The maximum values have been recorded during November and December. During the first months of the year, from January to May, have been recorded the minimum production values.</t>
+          <t>the TKN_About  in canada during  TKN_Year  has been increasing over the year. even that, several fluctuations have been recorded, in particular during the first months of the year. the maximum values have been recorded during november and december. during the first months of the year, from january to may, have been recorded the minimum production values.</t>
         </is>
       </c>
       <c r="W221" t="n">
@@ -19032,12 +19032,12 @@
       </c>
       <c r="U222" t="inlineStr">
         <is>
-          <t>A graph showing the farm product price index over the course of the year 2016 in Canada. It shows a significant price drop in July followed by a steady increase of the FPPPI until October.</t>
+          <t>a graph showing the farm product price index over the course of the year 2016 in canada. it shows a significant price drop in july followed by a steady increase of the fpppi until october.</t>
         </is>
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>A graph showing TKN_UOM  over TKN_About  the year  TKN_Year  in  TKN_Geo . It shows a significant price drop in July followed by a steady increase of the FPPPI until October.</t>
+          <t>a graph showing TKN_UOM  over TKN_About  the year  TKN_Year  in canada. it shows a significant price drop in july followed by a steady increase of the fpppi until october.</t>
         </is>
       </c>
       <c r="W222" t="n">
@@ -19116,12 +19116,12 @@
       </c>
       <c r="U223" t="inlineStr">
         <is>
-          <t>A graph showing the Canadian production of malt in tonnes over the course of the year 2017. The production was highest in August and then steadily decreased.</t>
+          <t>a graph showing the canadian production of malt in tonnes over the course of the year 2017. the production was highest in august and then steadily decreased.</t>
         </is>
       </c>
       <c r="V223" t="inlineStr">
         <is>
-          <t>A graph showing the Canadian TKN_About  in TKN_UOM  over the course of the year  TKN_Year . The production was highest in August and then steadily decreased.</t>
+          <t>a graph showing the canadian TKN_About  in TKN_UOM  over the course of the year  TKN_Year . the production was highest in august and then steadily decreased.</t>
         </is>
       </c>
       <c r="W223" t="n">
@@ -19200,12 +19200,12 @@
       </c>
       <c r="U224" t="inlineStr">
         <is>
-          <t>A graph showing the FPPPI for the production of poultry in Canada over the course of the year 2018. The FPPI has risen steadily until August and then dropped slowly.</t>
+          <t>a graph showing the fpppi for the production of poultry in canada over the course of the year 2018. the fppi has risen steadily until august and then dropped slowly.</t>
         </is>
       </c>
       <c r="V224" t="inlineStr">
         <is>
-          <t>A graph showing the TKN_About  poultry in  TKN_Geo  over the course of the year  TKN_Year . The FPPI has risen steadily until August and then dropped slowly.</t>
+          <t>a graph showing the TKN_About  poultry in canada over the course of the year  TKN_Year . the fppi has risen steadily until august and then dropped slowly.</t>
         </is>
       </c>
       <c r="W224" t="n">
@@ -19284,12 +19284,12 @@
       </c>
       <c r="U225" t="inlineStr">
         <is>
-          <t>the total vehicle entering Canada in 2017 were about 2000000 in Jan and Feb. then, they increased linearly until Aug, reaching 3400000. The they decreased considerably to 2400000, almost back to where they started from.</t>
+          <t>the total vehicle entering canada in 2017 were about 2000000 in jan and feb. then, they increased linearly until aug, reaching 3400000. the they decreased considerably to 2400000, almost back to where they started from.</t>
         </is>
       </c>
       <c r="V225" t="inlineStr">
         <is>
-          <t>the TKN_About   TKN_Geo  in  TKN_Year  were about 1 in Jan and Feb. then, they increased linearly until Aug, reaching 94. The they decreased considerably to 28, almost back to where they started from.</t>
+          <t>the TKN_About  in  TKN_Year  were about 1 in jan and feb. then, they increased linearly until aug, reaching 94. the they decreased considerably to 28, almost back to where they started from.</t>
         </is>
       </c>
       <c r="W225" t="n">
@@ -19368,12 +19368,12 @@
       </c>
       <c r="U226" t="inlineStr">
         <is>
-          <t>The production of fresh vegetables in Canada increased constantly in 2018 (from 1410 to 1450 FPPI), with the exception of the October-December period when it decreased to 1440.</t>
+          <t>the production of fresh vegetables in canada increased constantly in 2018 (from 1410 to 1450 fppi), with the exception of the october-december period when it decreased to 1440.</t>
         </is>
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  increased constantly in  TKN_Year  (from 11 to 96 FPPI), with the exception of the October-December period when it decreased to 74.</t>
+          <t>the TKN_About  in canada increased constantly in  TKN_Year  (from 11 to 96 fppi), with the exception of the october-december period when it decreased to 74.</t>
         </is>
       </c>
       <c r="W226" t="n">
@@ -19452,12 +19452,12 @@
       </c>
       <c r="U227" t="inlineStr">
         <is>
-          <t>Production of creamery decreased sharply in Canada in the period January-June from 11500 to about 8000. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching 10000 by the end of the year.</t>
+          <t>production of creamery decreased sharply in canada in the period january-june from 11500 to about 8000. then it was kind of stable, slightly fluctuating until november, with a rapid growth in december, reaching 10000 by the end of the year.</t>
         </is>
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>Production of creamery decreased sharply in  TKN_Geo  in the period January-June from 105 to about 12. Then it was kind of stable, slightly fluctuating until November, with a rapid growth in December, reaching 65 by the end of the year.</t>
+          <t>production of creamery decreased sharply in canada in the period january-june from 105 to about 12. then it was kind of stable, slightly fluctuating until november, with a rapid growth in december, reaching 65 by the end of the year.</t>
         </is>
       </c>
       <c r="W227" t="n">
@@ -19536,12 +19536,12 @@
       </c>
       <c r="U228" t="inlineStr">
         <is>
-          <t>The supply of creamery in Canada in 2017 grew rapidly from Jan (24000 tons) to May (38000). Then it was stable until July, when it started to drop, reaching 34000 by the end of the year.</t>
+          <t>the supply of creamery in canada in 2017 grew rapidly from jan (24000 tons) to may (38000). then it was stable until july, when it started to drop, reaching 34000 by the end of the year.</t>
         </is>
       </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  grew rapidly from Jan (-1 tons) to May (92). Then it was stable until July, when it started to drop, reaching 66 by the end of the year.</t>
+          <t>the TKN_About  in canada in  TKN_Year  grew rapidly from jan (-1 tons) to may (92). then it was stable until july, when it started to drop, reaching 66 by the end of the year.</t>
         </is>
       </c>
       <c r="W228" t="n">
@@ -19620,12 +19620,12 @@
       </c>
       <c r="U229" t="inlineStr">
         <is>
-          <t>The production of new motor vehicle in Canada in 2017 climbed from 120000 to 220000 from Jan to May. Then it dropped until Jul, was stable until Sep. with a final further decline to 130000 at the end of the year.</t>
+          <t>the production of new motor vehicle in canada in 2017 climbed from 120000 to 220000 from jan to may. then it dropped until jul, was stable until sep. with a final further decline to 130000 at the end of the year.</t>
         </is>
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>The TKN_About  vehicle in  TKN_Geo  in  TKN_Year  climbed from 7 to 100 from Jan to May. Then it dropped until Jul, was stable until Sep. with a final further decline to 16 at the end of the year.</t>
+          <t>the TKN_About  vehicle in canada in  TKN_Year  climbed from 7 to 100 from jan to may. then it dropped until jul, was stable until sep. with a final further decline to 16 at the end of the year.</t>
         </is>
       </c>
       <c r="W229" t="n">
@@ -19704,12 +19704,12 @@
       </c>
       <c r="U230" t="inlineStr">
         <is>
-          <t>The production of new motor vehicles in Canada in 2018 rose sharply until May, from 120000 to 220000 units. Then it started decreasing, reaching the same January level of 120000 in December, at the end of the year.</t>
+          <t>the production of new motor vehicles in canada in 2018 rose sharply until may, from 120000 to 220000 units. then it started decreasing, reaching the same january level of 120000 in december, at the end of the year.</t>
         </is>
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  in  TKN_Year  rose sharply until May, from 2 to 100 units. Then it started decreasing, reaching the same January level of 2 in December, at the end of the year.</t>
+          <t>the TKN_About  in canada in  TKN_Year  rose sharply until may, from 2 to 100 units. then it started decreasing, reaching the same january level of 2 in december, at the end of the year.</t>
         </is>
       </c>
       <c r="W230" t="n">
@@ -19788,12 +19788,12 @@
       </c>
       <c r="U231" t="inlineStr">
         <is>
-          <t>Production of fresh vegetables for 2018 in whole Canada, represented by the farm product price index. It can be seen, that the production rises in the months from february until october and then drops.</t>
+          <t>production of fresh vegetables for 2018 in whole canada, represented by the farm product price index. it can be seen, that the production rises in the months from february until october and then drops.</t>
         </is>
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>Production of fresh vegetables for  TKN_Year  in whole  TKN_Geo , represented TKN_UOM  index. It can be seen, that the production rises in the months from february until october and then drops.</t>
+          <t>production of fresh vegetables for  TKN_Year  in whole canada, represented TKN_UOM  index. it can be seen, that the production rises in the months from february until october and then drops.</t>
         </is>
       </c>
       <c r="W231" t="n">
@@ -19872,12 +19872,12 @@
       </c>
       <c r="U232" t="inlineStr">
         <is>
-          <t>2017: Production of chickens, turkeys, chicks, poults in Canada, with a peak in may and the lowest production in february.</t>
+          <t>2017: production of chickens, turkeys, chicks, poults in canada, with a peak in may and the lowest production in february.</t>
         </is>
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>TKN_Year : TKN_About  in  TKN_Geo , with a peak in may and the lowest production in february.</t>
+          <t>TKN_Year : TKN_About  in canada, with a peak in may and the lowest production in february.</t>
         </is>
       </c>
       <c r="W232" t="n">
@@ -19956,12 +19956,12 @@
       </c>
       <c r="U233" t="inlineStr">
         <is>
-          <t>This is a line graph showing the total 2017 imports of creamery butter to Canada in Tonnes. The graph has significant fluctuations between each month. There is a substantial spike in June, which was the peak month at over 2500 tonnes. There is also a clear dip in September, which was the lowest month at under 750 tonnes.</t>
+          <t>this is a line graph showing the total 2017 imports of creamery butter to canada in tonnes. the graph has significant fluctuations between each month. there is a substantial spike in june, which was the peak month at over 2500 tonnes. there is also a clear dip in september, which was the lowest month at under 750 tonnes.</t>
         </is>
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>This is a line graph showing the total  TKN_Year  imports TKN_About  to  TKN_Geo  in  TKN_UOM . The graph has significant fluctuations between each month. There is a substantial spike in June, which was the peak month at over 97 tonnes. There is also a clear dip in September, which was the lowest month at under 4 tonnes.</t>
+          <t>this is a line graph showing the total  TKN_Year  imports TKN_About  to canada in tonnes. the graph has significant fluctuations between each month. there is a substantial spike in june, which was the peak month at over 97 tonnes. there is also a clear dip in september, which was the lowest month at under 4 tonnes.</t>
         </is>
       </c>
       <c r="W233" t="n">
@@ -20040,12 +20040,12 @@
       </c>
       <c r="U234" t="inlineStr">
         <is>
-          <t>This is a line graph showing the 2017 price index of laptops in Canada. There is a declining trend throughout the year, with a slight spike in October. The graph's peak is in February at 994, and the graph's trough is in December at 970.</t>
+          <t>this is a line graph showing the 2017 price index of laptops in canada. there is a declining trend throughout the year, with a slight spike in october. the graph's peak is in february at 994, and the graph's trough is in december at 970.</t>
         </is>
       </c>
       <c r="V234" t="inlineStr">
         <is>
-          <t>This is a line graph showing the  TKN_Year  price index of laptops in  TKN_Geo . There is a declining trend throughout the year, with a slight spike in October. The graph's peak is in February at 100, and the graph's trough is in December at 0.</t>
+          <t>this is a line graph showing the  TKN_Year  price index of laptops in canada. there is a declining trend throughout the year, with a slight spike in october. the graph's peak is in february at 100, and the graph's trough is in december at 0.</t>
         </is>
       </c>
       <c r="W234" t="n">
@@ -20124,12 +20124,12 @@
       </c>
       <c r="U235" t="inlineStr">
         <is>
-          <t>This is a line graph showing the 2017 house price index in Canada. There is a stable increase from the graph's bottom at under 1000 in January, and peaking at over 1030 in December.</t>
+          <t>this is a line graph showing the 2017 house price index in canada. there is a stable increase from the graph's bottom at under 1000 in january, and peaking at over 1030 in december.</t>
         </is>
       </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>This is a line graph showing the  TKN_Year  house TKN_UOM  in  TKN_Geo . There is a stable increase from the graph's bottom at under 3 in January, and peaking at over 94 in December.</t>
+          <t>this is a line graph showing the  TKN_Year  house TKN_UOM  in canada. there is a stable increase from the graph's bottom at under 3 in january, and peaking at over 94 in december.</t>
         </is>
       </c>
       <c r="W235" t="n">
@@ -20208,12 +20208,12 @@
       </c>
       <c r="U236" t="inlineStr">
         <is>
-          <t>The maximum value of total canadian vehicles returning to the country during 2018 has been reached during the month of August. In particular, the value started to grow in March reaching its peak in August. After that, it slowly decreased. The minimum value was during February 2018.</t>
+          <t>the maximum value of total canadian vehicles returning to the country during 2018 has been reached during the month of august. in particular, the value started to grow in march reaching its peak in august. after that, it slowly decreased. the minimum value was during february 2018.</t>
         </is>
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>The maximum value of TKN_About  during  TKN_Year  has been reached during the month of August. In particular, the value started to grow in March reaching its peak in August. After that, it slowly decreased. The minimum value was during February  TKN_Year .</t>
+          <t>the maximum value of TKN_About  during  TKN_Year  has been reached during the month of august. in particular, the value started to grow in march reaching its peak in august. after that, it slowly decreased. the minimum value was during february  TKN_Year .</t>
         </is>
       </c>
       <c r="W236" t="n">
@@ -20292,12 +20292,12 @@
       </c>
       <c r="U237" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the supply of creamery butter in Canada during 2018 rapidly increased from January over. In particular, it reached its peak during the month of June 2018. After that, it started to decline until September. The last three months of the year it remained quite stable.</t>
+          <t>it's clearly possible to see how the supply of creamery butter in canada during 2018 rapidly increased from january over. in particular, it reached its peak during the month of june 2018. after that, it started to decline until september. the last three months of the year it remained quite stable.</t>
         </is>
       </c>
       <c r="V237" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  during  TKN_Year  rapidly increased from January over. In particular, it reached its peak during the month of June  TKN_Year . After that, it started to decline until September. The last three months of the year it remained quite stable.</t>
+          <t>it's clearly possible to see how the TKN_About  in canada during  TKN_Year  rapidly increased from january over. in particular, it reached its peak during the month of june  TKN_Year . after that, it started to decline until september. the last three months of the year it remained quite stable.</t>
         </is>
       </c>
       <c r="W237" t="n">
@@ -20376,12 +20376,12 @@
       </c>
       <c r="U238" t="inlineStr">
         <is>
-          <t>The production of Malt in Canada during 2016 showed several fluctuations during the year. The production values have been displayed using Tonnes as unit of measurement. The most relevant peaks have been recorded during the months of February and June. At the same time, the minimum values were recorded in January and September 2016.</t>
+          <t>the production of malt in canada during 2016 showed several fluctuations during the year. the production values have been displayed using tonnes as unit of measurement. the most relevant peaks have been recorded during the months of february and june. at the same time, the minimum values were recorded in january and september 2016.</t>
         </is>
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  showed several fluctuations during the year. The production values have been displayed using  TKN_UOM  as unit of measurement. The most relevant peaks have been recorded during the months of February and June. At the same time, the minimum values were recorded in January and September  TKN_Year .</t>
+          <t>the TKN_About  in canada during  TKN_Year  showed several fluctuations during the year. the production values have been displayed using TKN_UOM  as unit of measurement. the most relevant peaks have been recorded during the months of february and june. at the same time, the minimum values were recorded in january and september  TKN_Year .</t>
         </is>
       </c>
       <c r="W238" t="n">
@@ -20460,12 +20460,12 @@
       </c>
       <c r="U239" t="inlineStr">
         <is>
-          <t>The commercial software price index in Canada decreased over 2016. It's clearly possible to see how it rapidly drop from January to April. After that, the price index values have been fluctuating for most of the year.</t>
+          <t>the commercial software price index in canada decreased over 2016. it's clearly possible to see how it rapidly drop from january to april. after that, the price index values have been fluctuating for most of the year.</t>
         </is>
       </c>
       <c r="V239" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  decreased over  TKN_Year . It's clearly possible to see how it rapidly drop from January to April. After that, the price index values have been fluctuating for most of the year.</t>
+          <t>the TKN_About  in canada decreased over  TKN_Year . it's clearly possible to see how it rapidly drop from january to april. after that, the price index values have been fluctuating for most of the year.</t>
         </is>
       </c>
       <c r="W239" t="n">
@@ -20544,12 +20544,12 @@
       </c>
       <c r="U240" t="inlineStr">
         <is>
-          <t>The production of fresh potatoes in Canada during 2016 reached its maximum values during the months of July, August and September. In particular, the maximum value over the year has been registered during the month of August. It's clearly possible to see how the production of fresh potatoes is way higher during the summer months than during the winter one.</t>
+          <t>the production of fresh potatoes in canada during 2016 reached its maximum values during the months of july, august and september. in particular, the maximum value over the year has been registered during the month of august. it's clearly possible to see how the production of fresh potatoes is way higher during the summer months than during the winter one.</t>
         </is>
       </c>
       <c r="V240" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  reached its maximum values during the months of July, August and September. In particular, the maximum value over the year has been registered during the month of August. It's clearly possible to see how the TKN_About  is way higher during the summer months than during the winter one.</t>
+          <t>the TKN_About  in canada during  TKN_Year  reached its maximum values during the months of july, august and september. in particular, the maximum value over the year has been registered during the month of august. it's clearly possible to see how the TKN_About  is way higher during the summer months than during the winter one.</t>
         </is>
       </c>
       <c r="W240" t="n">
@@ -20628,12 +20628,12 @@
       </c>
       <c r="U241" t="inlineStr">
         <is>
-          <t>The production of grains in Canada during 2018 reported several fluctations. Even that, it shows a significant peak during the month of August. The minimum value has been registered during the month of February.</t>
+          <t>the production of grains in canada during 2018 reported several fluctations. even that, it shows a significant peak during the month of august. the minimum value has been registered during the month of february.</t>
         </is>
       </c>
       <c r="V241" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  reported several fluctations. Even that, it shows a significant peak during the month of August. The minimum value has been registered during the month of February.</t>
+          <t>the TKN_About  in canada during  TKN_Year  reported several fluctations. even that, it shows a significant peak during the month of august. the minimum value has been registered during the month of february.</t>
         </is>
       </c>
       <c r="W241" t="n">
@@ -20712,12 +20712,12 @@
       </c>
       <c r="U242" t="inlineStr">
         <is>
-          <t>The line chart describes the Servers price index trend in Canada during 2017. It considerably oscillated over the year, with several peaks and dips. The highest values have been recorded during January and June. The minimum value was recorded in November 2017.</t>
+          <t>the line chart describes the servers price index trend in canada during 2017. it considerably oscillated over the year, with several peaks and dips. the highest values have been recorded during january and june. the minimum value was recorded in november 2017.</t>
         </is>
       </c>
       <c r="V242" t="inlineStr">
         <is>
-          <t>The line chart describes the TKN_About  index trend in  TKN_Geo  during  TKN_Year . It considerably oscillated over the year, with several peaks and dips. The highest values have been recorded during January and June. The minimum value was recorded in November  TKN_Year .</t>
+          <t>the line chart describes the TKN_About  index trend in canada during  TKN_Year . it considerably oscillated over the year, with several peaks and dips. the highest values have been recorded during january and june. the minimum value was recorded in november  TKN_Year .</t>
         </is>
       </c>
       <c r="W242" t="n">
@@ -20796,12 +20796,12 @@
       </c>
       <c r="U243" t="inlineStr">
         <is>
-          <t>The production of fresh potatoes in Canada 2017 shows the highest values during the summer months. In particular, the production reports its maximum value during the month of August. It remain quite steady during the other months of the year. The minimum value was during October 2017.</t>
+          <t>the production of fresh potatoes in canada 2017 shows the highest values during the summer months. in particular, the production reports its maximum value during the month of august. it remain quite steady during the other months of the year. the minimum value was during october 2017.</t>
         </is>
       </c>
       <c r="V243" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo   TKN_Year  shows the highest values during the summer months. In particular, the production reports its maximum value during the month of August. It remain quite steady during the other months of the year. The minimum value was during October  TKN_Year .</t>
+          <t>the TKN_About  in canada  TKN_Year  shows the highest values during the summer months. in particular, the production reports its maximum value during the month of august. it remain quite steady during the other months of the year. the minimum value was during october  TKN_Year .</t>
         </is>
       </c>
       <c r="W243" t="n">
@@ -20880,12 +20880,12 @@
       </c>
       <c r="U244" t="inlineStr">
         <is>
-          <t>The commercial software price index in Canada slipped down during the 2017. The highest value has been recorded during March. Then, it significantly dropped between May and September. The minimu value was recorded during the month of September. During last 3 months of the year it slightly started to increase again.</t>
+          <t>the commercial software price index in canada slipped down during the 2017. the highest value has been recorded during march. then, it significantly dropped between may and september. the minimu value was recorded during the month of september. during last 3 months of the year it slightly started to increase again.</t>
         </is>
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  slipped down during the  TKN_Year . The highest value has been recorded during March. Then, it significantly dropped between May and September. The minimu value was recorded during the month of September. During last 3 months of the year it slightly started to increase again.</t>
+          <t>the TKN_About  in canada slipped down during the  TKN_Year . the highest value has been recorded during march. then, it significantly dropped between may and september. the minimu value was recorded during the month of september. during last 3 months of the year it slightly started to increase again.</t>
         </is>
       </c>
       <c r="W244" t="n">
@@ -20964,12 +20964,12 @@
       </c>
       <c r="U245" t="inlineStr">
         <is>
-          <t>The graph is showing the trend about production of chickens, turkeys, chicks and poults in Canada during 2016. The values are illustrated using the farm product price index (FPPI). The values have been fluactuating over the year, with several dips and peaks. The maximum value was in October 2016. During the last two months of the year, Nov and Dec, was recorded the minimum production of the 2016.</t>
+          <t>the graph is showing the trend about production of chickens, turkeys, chicks and poults in canada during 2016. the values are illustrated using the farm product price index (fppi). the values have been fluactuating over the year, with several dips and peaks. the maximum value was in october 2016. during the last two months of the year, nov and dec, was recorded the minimum production of the 2016.</t>
         </is>
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>The graph is showing the trend about TKN_About  in  TKN_Geo  during  TKN_Year . The values are illustrated using TKN_UOM  (FPPI). The values have been fluactuating over the year, with several dips and peaks. The maximum value was in October  TKN_Year . During the last two months of the year, Nov and Dec, was recorded the minimum production of the  TKN_Year .</t>
+          <t>the graph is showing the trend about TKN_About  in canada during  TKN_Year . the values are illustrated using TKN_UOM  (fppi). the values have been fluactuating over the year, with several dips and peaks. the maximum value was in october  TKN_Year . during the last two months of the year, nov and dec, was recorded the minimum production of the  TKN_Year .</t>
         </is>
       </c>
       <c r="W245" t="n">
@@ -21048,12 +21048,12 @@
       </c>
       <c r="U246" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the production of new motor vehicles in Canada during 2016 rapidly increased fom January to April. After that, it slowly slide down from April until the end of the year. The maximum number of new motor vehicles in Canada during 2016 was in April.</t>
+          <t>as it's shown in the graph, the production of new motor vehicles in canada during 2016 rapidly increased fom january to april. after that, it slowly slide down from april until the end of the year. the maximum number of new motor vehicles in canada during 2016 was in april.</t>
         </is>
       </c>
       <c r="V246" t="inlineStr">
         <is>
-          <t>As it's shown in the graph, the TKN_About  in  TKN_Geo  during  TKN_Year  rapidly increased fom January to April. After that, it slowly slide down from April until the end of the year. The maximum number of new motor vehicles in  TKN_Geo  during  TKN_Year  was in April.</t>
+          <t>as it's shown in the graph, the TKN_About  in canada during  TKN_Year  rapidly increased fom january to april. after that, it slowly slide down from april until the end of the year. the maximum number of new motor vehicles in canada during  TKN_Year  was in april.</t>
         </is>
       </c>
       <c r="W246" t="n">
@@ -21132,12 +21132,12 @@
       </c>
       <c r="U247" t="inlineStr">
         <is>
-          <t>It shows the supply of creamery butter in Canada during 2018. The values are described using Tonnes as UOM. It rapidly increase from January for the first half of the year. It reach its maximum value during the month of June. After that, it starts to decline til September. The supply of creamery butter fluctuated over the last few months of 2018.</t>
+          <t>it shows the supply of creamery butter in canada during 2018. the values are described using tonnes as uom. it rapidly increase from january for the first half of the year. it reach its maximum value during the month of june. after that, it starts to decline til september. the supply of creamery butter fluctuated over the last few months of 2018.</t>
         </is>
       </c>
       <c r="V247" t="inlineStr">
         <is>
-          <t>It shows the TKN_About  in  TKN_Geo  during  TKN_Year . The values are described using  TKN_UOM  as UOM. It rapidly increase from January for the first half of the year. It reach its maximum value during the month of June. After that, it starts to decline til September. The TKN_About  fluctuated over the last few months of  TKN_Year .</t>
+          <t>it shows the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  as uom. it rapidly increase from january for the first half of the year. it reach its maximum value during the month of june. after that, it starts to decline til september. the TKN_About  fluctuated over the last few months of  TKN_Year .</t>
         </is>
       </c>
       <c r="W247" t="n">
@@ -21216,12 +21216,12 @@
       </c>
       <c r="U248" t="inlineStr">
         <is>
-          <t>As it's possible to see, the following graph is about the production of eggs in shell in Canada during 2018. The values are reported using the farm product price index (FPPI). The production slightly increase over the first half of the year, so from January until July. After that, it has been recorded a significant jump of the values between July and August. During the last few months of the year it remained steady.</t>
+          <t>as it's possible to see, the following graph is about the production of eggs in shell in canada during 2018. the values are reported using the farm product price index (fppi). the production slightly increase over the first half of the year, so from january until july. after that, it has been recorded a significant jump of the values between july and august. during the last few months of the year it remained steady.</t>
         </is>
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>As it's possible to see, the following graph is about the TKN_About  in  TKN_Geo  during  TKN_Year . The values are reported using TKN_UOM  (FPPI). The production slightly increase over the first half of the year, so from January until July. After that, it has been recorded a significant jump of the values between July and August. During the last few months of the year it remained steady.</t>
+          <t>as it's possible to see, the following graph is about the TKN_About  in canada during  TKN_Year . the values are reported using TKN_UOM  (fppi). the production slightly increase over the first half of the year, so from january until july. after that, it has been recorded a significant jump of the values between july and august. during the last few months of the year it remained steady.</t>
         </is>
       </c>
       <c r="W248" t="n">
@@ -21300,12 +21300,12 @@
       </c>
       <c r="U249" t="inlineStr">
         <is>
-          <t>Production of rye in Canada during 2018 got a considerable peak during August. During most of the year the values have been fluctuating up and down, with several peaks and dips. Even that, the minimum value over 2018 has been recorded in December.</t>
+          <t>production of rye in canada during 2018 got a considerable peak during august. during most of the year the values have been fluctuating up and down, with several peaks and dips. even that, the minimum value over 2018 has been recorded in december.</t>
         </is>
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>Production of rye in  TKN_Geo  during  TKN_Year  got a considerable peak during August. During most of the year the values have been fluctuating up and down, with several peaks and dips. Even that, the minimum value over  TKN_Year  has been recorded in December.</t>
+          <t>production of rye in canada during  TKN_Year  got a considerable peak during august. during most of the year the values have been fluctuating up and down, with several peaks and dips. even that, the minimum value over  TKN_Year  has been recorded in december.</t>
         </is>
       </c>
       <c r="W249" t="n">
@@ -21384,12 +21384,12 @@
       </c>
       <c r="U250" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in Canada during 2017 showed a massive climb from February to March. The production value kept raising up. it reached its maximum value during the month of May. After that, the production of new motor vehicles slightly started to decline, reaching a dip during the month of December 2017.</t>
+          <t>production of new motor vehicles in canada during 2017 showed a massive climb from february to march. the production value kept raising up. it reached its maximum value during the month of may. after that, the production of new motor vehicles slightly started to decline, reaching a dip during the month of december 2017.</t>
         </is>
       </c>
       <c r="V250" t="inlineStr">
         <is>
-          <t>Production of new motor vehicles in  TKN_Geo  during  TKN_Year  showed a massive climb from February to March. The production value kept raising up. it reached its maximum value during the month of May. After that, the production of new motor vehicles slightly started to decline, reaching a dip during the month of December  TKN_Year .</t>
+          <t>production of new motor vehicles in canada during  TKN_Year  showed a massive climb from february to march. the production value kept raising up. it reached its maximum value during the month of may. after that, the TKN_About  slightly started to decline, reaching a dip during the month of december  TKN_Year .</t>
         </is>
       </c>
       <c r="W250" t="n">
@@ -21468,12 +21468,12 @@
       </c>
       <c r="U251" t="inlineStr">
         <is>
-          <t>The production of Canola in Canada strongly oscillated over 2017. It's clearly possible to see how it reported several peaks and dips. The highest value was during October 2017. The minimum value was in August 2017.</t>
+          <t>the production of canola in canada strongly oscillated over 2017. it's clearly possible to see how it reported several peaks and dips. the highest value was during october 2017. the minimum value was in august 2017.</t>
         </is>
       </c>
       <c r="V251" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  strongly oscillated over  TKN_Year . It's clearly possible to see how it reported several peaks and dips. The highest value was during October  TKN_Year . The minimum value was in August  TKN_Year .</t>
+          <t>the TKN_About  in canada strongly oscillated over  TKN_Year . it's clearly possible to see how it reported several peaks and dips. the highest value was during october  TKN_Year . the minimum value was in august  TKN_Year .</t>
         </is>
       </c>
       <c r="W251" t="n">
@@ -21552,12 +21552,12 @@
       </c>
       <c r="U252" t="inlineStr">
         <is>
-          <t>The following graph shows the total farm production index value in Canada during 2017, and the values are described using the farm product price index (FPPI) as UOM. It's possible to see how the production value considerably increased from January until July. After that, it dropped between July and September.</t>
+          <t>the following graph shows the total farm production index value in canada during 2017, and the values are described using the farm product price index (fppi) as uom. it's possible to see how the production value considerably increased from january until july. after that, it dropped between july and september.</t>
         </is>
       </c>
       <c r="V252" t="inlineStr">
         <is>
-          <t>The following graph shows the TKN_About  value in  TKN_Geo  during  TKN_Year , and the values are described using the TKN_UOM  as UOM. It's possible to see how the production value considerably increased from January until July. After that, it dropped between July and September.</t>
+          <t>the following graph shows the TKN_About  value in canada during  TKN_Year , and the values are described using the TKN_UOM  as uom. it's possible to see how the production value considerably increased from january until july. after that, it dropped between july and september.</t>
         </is>
       </c>
       <c r="W252" t="n">
@@ -21636,12 +21636,12 @@
       </c>
       <c r="U253" t="inlineStr">
         <is>
-          <t>The production of oats strongly fluctuated over the 2017 in Canada. It doesn't really have an ascendant or descendant trend. The most significant dip has been recorded in May. The most considerable peak was recorded in September 2017.</t>
+          <t>the production of oats strongly fluctuated over the 2017 in canada. it doesn't really have an ascendant or descendant trend. the most significant dip has been recorded in may. the most considerable peak was recorded in september 2017.</t>
         </is>
       </c>
       <c r="V253" t="inlineStr">
         <is>
-          <t>The TKN_About  strongly fluctuated over the  TKN_Year  in  TKN_Geo . It doesn't really have an ascendant or descendant trend. The most significant dip has been recorded in May. The most considerable peak was recorded in September  TKN_Year .</t>
+          <t>the TKN_About  strongly fluctuated over the  TKN_Year  in canada. it doesn't really have an ascendant or descendant trend. the most significant dip has been recorded in may. the most considerable peak was recorded in september  TKN_Year .</t>
         </is>
       </c>
       <c r="W253" t="n">
@@ -21720,12 +21720,12 @@
       </c>
       <c r="U254" t="inlineStr">
         <is>
-          <t>The number of vehicles entering Canada during 2018 substantially increased over the summer months. In particular, the maximum value was reached during August. The minimum number of vehicles enterin Canada was during February.</t>
+          <t>the number of vehicles entering canada during 2018 substantially increased over the summer months. in particular, the maximum value was reached during august. the minimum number of vehicles enterin canada was during february.</t>
         </is>
       </c>
       <c r="V254" t="inlineStr">
         <is>
-          <t>The TKN_UOM  TKN_About   TKN_Geo  during  TKN_Year  substantially increased over the summer months. In particular, the maximum value was reached during August. The minimum TKN_UOM  of vehicles enterin  TKN_Geo  was during February.</t>
+          <t>the TKN_UOM  of TKN_About  during  TKN_Year  substantially increased over the summer months. in particular, the maximum value was reached during august. the minimum TKN_UOM  of vehicles enterin canada was during february.</t>
         </is>
       </c>
       <c r="W254" t="n">
@@ -21804,12 +21804,12 @@
       </c>
       <c r="U255" t="inlineStr">
         <is>
-          <t>The total softwoord production in Canada during 2017 considerably oscillated up and down over the year.  The maximum value was recorded in May 2017. But at the same time, two other peaks were in May and October. The minimum value over the whole 2017 was during December 2017, with less than 48000 cubic metres producted.</t>
+          <t>the total softwoord production in canada during 2017 considerably oscillated up and down over the year.  the maximum value was recorded in may 2017. but at the same time, two other peaks were in may and october. the minimum value over the whole 2017 was during december 2017, with less than 48000 cubic metres producted.</t>
         </is>
       </c>
       <c r="V255" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  considerably oscillated up and down over the year.  The maximum value was recorded in May  TKN_Year . But at the same time, two other peaks were in May and October. The minimum value over the whole  TKN_Year  was during December  TKN_Year , with less than 9 TKN_UOM  producted.</t>
+          <t>the TKN_About  in canada during  TKN_Year  considerably oscillated up and down over the year.  the maximum value was recorded in may  TKN_Year . but at the same time, two other peaks were in may and october. the minimum value over the whole  TKN_Year  was during december  TKN_Year , with less than 9 TKN_UOM  producted.</t>
         </is>
       </c>
       <c r="W255" t="n">
@@ -21888,12 +21888,12 @@
       </c>
       <c r="U256" t="inlineStr">
         <is>
-          <t>The graph shows the trend about desktop and similar computer price index in Canada over 2016. After a significantly steep rise from January to February, the values started to slightly decline. They have been decreasing from February til September. A significant drop was registered between July and August. The minimum value over the year was in September 2016. During last few months of the year the price index started to slightly grow again.</t>
+          <t>the graph shows the trend about desktop and similar computer price index in canada over 2016. after a significantly steep rise from january to february, the values started to slightly decline. they have been decreasing from february til september. a significant drop was registered between july and august. the minimum value over the year was in september 2016. during last few months of the year the price index started to slightly grow again.</t>
         </is>
       </c>
       <c r="V256" t="inlineStr">
         <is>
-          <t>The graph shows the trend about TKN_About  index in  TKN_Geo  over  TKN_Year . After a significantly steep rise from January to February, the values started to slightly decline. They have been decreasing from February til September. A significant drop was registered between July and August. The minimum value over the year was in September  TKN_Year . During last few months of the year the price index started to slightly grow again.</t>
+          <t>the graph shows the trend about TKN_About  index in canada over  TKN_Year . after a significantly steep rise from january to february, the values started to slightly decline. they have been decreasing from february til september. a significant drop was registered between july and august. the minimum value over the year was in september  TKN_Year . during last few months of the year the price index started to slightly grow again.</t>
         </is>
       </c>
       <c r="W256" t="n">
@@ -21972,12 +21972,12 @@
       </c>
       <c r="U257" t="inlineStr">
         <is>
-          <t>Production of creamery butter in Canada has been rapidly decreasing over from January until August 2016. Even that, couple of peaks have been recorded during that period, in particular April and July. During the last few months of year, the production started to considerably grow again. The minimum value over the year was registered in August 2016.</t>
+          <t>production of creamery butter in canada has been rapidly decreasing over from january until august 2016. even that, couple of peaks have been recorded during that period, in particular april and july. during the last few months of year, the production started to considerably grow again. the minimum value over the year was registered in august 2016.</t>
         </is>
       </c>
       <c r="V257" t="inlineStr">
         <is>
-          <t>Production of creamery butter in  TKN_Geo  has been rapidly decreasing over from January until August  TKN_Year . Even that, couple of peaks have been recorded during that period, in particular April and July. During the last few months of year, the production started to considerably grow again. The minimum value over the year was registered in August  TKN_Year .</t>
+          <t>production of creamery butter in canada has been rapidly decreasing over from january until august  TKN_Year . even that, couple of peaks have been recorded during that period, in particular april and july. during the last few months of year, the production started to considerably grow again. the minimum value over the year was registered in august  TKN_Year .</t>
         </is>
       </c>
       <c r="W257" t="n">
@@ -22056,12 +22056,12 @@
       </c>
       <c r="U258" t="inlineStr">
         <is>
-          <t>The graph shows the price index of serves in Canada during 2016. At the beginning of the year, between January and March, the index considerably dropped down. After that, it has been oscillating over the rest of the year. A peak was recorded in June. The values strongly declined also between October and November.</t>
+          <t>the graph shows the price index of serves in canada during 2016. at the beginning of the year, between january and march, the index considerably dropped down. after that, it has been oscillating over the rest of the year. a peak was recorded in june. the values strongly declined also between october and november.</t>
         </is>
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About  index of serves in  TKN_Geo  during  TKN_Year . At the beginning of the year, between January and March, the index considerably dropped down. After that, it has been oscillating over the rest of the year. A peak was recorded in June. The values strongly declined also between October and November.</t>
+          <t>the graph shows TKN_About  index of serves in canada during  TKN_Year . at the beginning of the year, between january and march, the index considerably dropped down. after that, it has been oscillating over the rest of the year. a peak was recorded in june. the values strongly declined also between october and november.</t>
         </is>
       </c>
       <c r="W258" t="n">
@@ -22140,12 +22140,12 @@
       </c>
       <c r="U259" t="inlineStr">
         <is>
-          <t>As it's possible to see in the shown graph, the total livestock and animal products reported the highest values during the first half of the year. In particular, the maximum value was recorded during June 2017. After that, it rapidly decreased from June until September. The minimum value was during September 2017.</t>
+          <t>as it's possible to see in the shown graph, the total livestock and animal products reported the highest values during the first half of the year. in particular, the maximum value was recorded during june 2017. after that, it rapidly decreased from june until september. the minimum value was during september 2017.</t>
         </is>
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>As it's possible to see in the shown graph, the TKN_About  reported the highest values during the first half of the year. In particular, the maximum value was recorded during June  TKN_Year . After that, it rapidly decreased from June until September. The minimum value was during September  TKN_Year .</t>
+          <t>as it's possible to see in the shown graph, the TKN_About  reported the highest values during the first half of the year. in particular, the maximum value was recorded during june  TKN_Year . after that, it rapidly decreased from june until september. the minimum value was during september  TKN_Year .</t>
         </is>
       </c>
       <c r="W259" t="n">
@@ -22224,12 +22224,12 @@
       </c>
       <c r="U260" t="inlineStr">
         <is>
-          <t>The total softwood and hardwood production in Canada has been strongly fluctuating over 2018. It's clearly possible to identify several peaks and dips. The maximum value was during May. Even that, the production value strongly dropped down from October to December, reaching its minimum value of the year.</t>
+          <t>the total softwood and hardwood production in canada has been strongly fluctuating over 2018. it's clearly possible to identify several peaks and dips. the maximum value was during may. even that, the production value strongly dropped down from october to december, reaching its minimum value of the year.</t>
         </is>
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  has been strongly fluctuating over  TKN_Year . It's clearly possible to identify several peaks and dips. The maximum value was during May. Even that, the production value strongly dropped down from October to December, reaching its minimum value of the year.</t>
+          <t>the TKN_About  in canada has been strongly fluctuating over  TKN_Year . it's clearly possible to identify several peaks and dips. the maximum value was during may. even that, the production value strongly dropped down from october to december, reaching its minimum value of the year.</t>
         </is>
       </c>
       <c r="W260" t="n">
@@ -22308,12 +22308,12 @@
       </c>
       <c r="U261" t="inlineStr">
         <is>
-          <t>The total livestock and animal products in Canada has been quite steady during the first few months of the 2016. After that, it rapidly declined from June until October. During last three months of the year it started to slightly increase again. The highest value of the year was recorded in March and the lowest in October.</t>
+          <t>the total livestock and animal products in canada has been quite steady during the first few months of the 2016. after that, it rapidly declined from june until october. during last three months of the year it started to slightly increase again. the highest value of the year was recorded in march and the lowest in october.</t>
         </is>
       </c>
       <c r="V261" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  has been quite steady during the first few months of the  TKN_Year . After that, it rapidly declined from June until October. During last three months of the year it started to slightly increase again. The highest value of the year was recorded in March and the lowest in October.</t>
+          <t>the TKN_About  in canada has been quite steady during the first few months of the  TKN_Year . after that, it rapidly declined from june until october. during last three months of the year it started to slightly increase again. the highest value of the year was recorded in march and the lowest in october.</t>
         </is>
       </c>
       <c r="W261" t="n">
@@ -22392,12 +22392,12 @@
       </c>
       <c r="U262" t="inlineStr">
         <is>
-          <t>This figure depicts the total Canadian hardwood production in cubic metres of 2018. Whereas it starts off in January at approximately 1050 cubic metres, production fluctuates until reaching its maximum in May at around 1250. There is a sudden drop, reaching the minimum annual value in July at below 800 cubic metres. Production then again rises from July until October and experiences a drop from October until December.</t>
+          <t>this figure depicts the total canadian hardwood production in cubic metres of 2018. whereas it starts off in january at approximately 1050 cubic metres, production fluctuates until reaching its maximum in may at around 1250. there is a sudden drop, reaching the minimum annual value in july at below 800 cubic metres. production then again rises from july until october and experiences a drop from october until december.</t>
         </is>
       </c>
       <c r="V262" t="inlineStr">
         <is>
-          <t>This figure depicts the TKN_About  in TKN_UOM  of  TKN_Year . Whereas it starts off in January at approximately 63 TKN_UOM , production fluctuates until reaching its maximum in May at around 104. There is a sudden drop, reaching the minimum annual value in July at below 11 TKN_UOM . Production then again rises from July until October and experiences a drop from October until December.</t>
+          <t>this figure depicts the TKN_About  in TKN_UOM  of  TKN_Year . whereas it starts off in january at approximately 63 TKN_UOM , production fluctuates until reaching its maximum in may at around 104. there is a sudden drop, reaching the minimum annual value in july at below 11 TKN_UOM . production then again rises from july until october and experiences a drop from october until december.</t>
         </is>
       </c>
       <c r="W262" t="n">
@@ -22476,12 +22476,12 @@
       </c>
       <c r="U263" t="inlineStr">
         <is>
-          <t>The production of new motor vehicles in Canada of 2018 is shown in this figure. The unit given is dollars. Production shows its lowest value in January. Following this production experiences a sharp increase, until reaching its maximum in May. Production gradually decreases from May until July, plateauing from July until September. There is a steady decline from September until December.</t>
+          <t>the production of new motor vehicles in canada of 2018 is shown in this figure. the unit given is dollars. production shows its lowest value in january. following this production experiences a sharp increase, until reaching its maximum in may. production gradually decreases from may until july, plateauing from july until september. there is a steady decline from september until december.</t>
         </is>
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  of  TKN_Year  is shown in this figure. The unit given is dollars. Production shows its lowest value in January. Following this production experiences a sharp increase, until reaching its maximum in May. Production gradually decreases from May until July, plateauing from July until September. There is a steady decline from September until December.</t>
+          <t>the TKN_About  in canada of  TKN_Year  is shown in this figure. the unit given is dollars. production shows its lowest value in january. following this production experiences a sharp increase, until reaching its maximum in may. production gradually decreases from may until july, plateauing from july until september. there is a steady decline from september until december.</t>
         </is>
       </c>
       <c r="W263" t="n">
@@ -22560,12 +22560,12 @@
       </c>
       <c r="U264" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian price index of desktop and similar computers during 2018. Maximum production is reached in the months of January and February at 962. From then on production oscillates in a decreasing manner, plateauing at 959 during April and May and at 956 during June and July. The minimum production is observed during August and October. There is a rise from October until December, reaching a value of 957.</t>
+          <t>this figure represents the canadian price index of desktop and similar computers during 2018. maximum production is reached in the months of january and february at 962. from then on production oscillates in a decreasing manner, plateauing at 959 during april and may and at 956 during june and july. the minimum production is observed during august and october. there is a rise from october until december, reaching a value of 957.</t>
         </is>
       </c>
       <c r="V264" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About  during  TKN_Year . Maximum production is reached in the months of January and February at 100. From then on production oscillates in a decreasing manner, plateauing at 67 during April and May and at 33 during June and July. The minimum production is observed during August and October. There is a rise from October until December, reaching a value of 44.</t>
+          <t>this figure represents the canadian TKN_About  during  TKN_Year . maximum production is reached in the months of january and february at 100. from then on production oscillates in a decreasing manner, plateauing at 67 during april and may and at 33 during june and july. the minimum production is observed during august and october. there is a rise from october until december, reaching a value of 44.</t>
         </is>
       </c>
       <c r="W264" t="n">
@@ -22644,12 +22644,12 @@
       </c>
       <c r="U265" t="inlineStr">
         <is>
-          <t>The number of total vehicles entering Canada in 2016 is depicted in this graph. During January approximately 2100000 vehicles enter. These numbers slightly decrease to 2000000 in February, the lowest value of the year. From then on a steady increase in entering vehicles can be observed, until the maximum value is reached in August at approxiamtely 3400000. From August until December the number of vehicles entering Canada experience a steady decrease, reaching a number of 2300000 at the end of the year.</t>
+          <t>the number of total vehicles entering canada in 2016 is depicted in this graph. during january approximately 2100000 vehicles enter. these numbers slightly decrease to 2000000 in february, the lowest value of the year. from then on a steady increase in entering vehicles can be observed, until the maximum value is reached in august at approxiamtely 3400000. from august until december the number of vehicles entering canada experience a steady decrease, reaching a number of 2300000 at the end of the year.</t>
         </is>
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>The TKN_UOM  of TKN_About   TKN_Geo  in  TKN_Year  is depicted in this graph. During January approximately 8 vehicles enter. These TKN_UOM s slightly decrease to 1 in February, the lowest value of the year. From then on a steady increase in entering vehicles can be observed, until the maximum value is reached in August at approxiamtely 100. From August until December the TKN_UOM  of vehicles entering  TKN_Geo  experience a steady decrease, reaching a TKN_UOM  of 22 at the end of the year.</t>
+          <t>the TKN_UOM  of TKN_About  in  TKN_Year  is depicted in this graph. during january approximately 8 vehicles enter. these TKN_UOM s slightly decrease to 1 in february, the lowest value of the year. from then on a steady increase in entering vehicles can be observed, until the maximum value is reached in august at approxiamtely 100. from august until december the TKN_UOM  of vehicles entering canada experience a steady decrease, reaching a TKN_UOM  of 22 at the end of the year.</t>
         </is>
       </c>
       <c r="W265" t="n">
@@ -22728,12 +22728,12 @@
       </c>
       <c r="U266" t="inlineStr">
         <is>
-          <t>This graph depicts the total number of United States vehicles entering in Canada during 2016. The lowest number of vehicles is observed in January, at approximately 640000. During the following months numbers of entering vehicles steadily increase until reaching the maximum number the year 2016 in July with approximately 1250000. From July until November a sharp drop is experienced, with numbers of around 700000 in November. The number hardly changes in December.</t>
+          <t>this graph depicts the total number of united states vehicles entering in canada during 2016. the lowest number of vehicles is observed in january, at approximately 640000. during the following months numbers of entering vehicles steadily increase until reaching the maximum number the year 2016 in july with approximately 1250000. from july until november a sharp drop is experienced, with numbers of around 700000 in november. the number hardly changes in december.</t>
         </is>
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>This graph depicts the total TKN_UOM  of TKN_About  in  TKN_Geo  during  TKN_Year . The lowest TKN_UOM  of vehicles is observed in January, at approximately 1. During the following months TKN_UOM s of entering vehicles steadily increase until reaching the maximum TKN_UOM  the year  TKN_Year  in July with approximately 101. From July until November a sharp drop is experienced, with TKN_UOM s of around 11 in November. The TKN_UOM  hardly changes in December.</t>
+          <t>this graph depicts the total TKN_UOM  of TKN_About  in canada during  TKN_Year . the lowest TKN_UOM  of vehicles is observed in january, at approximately 1. during the following months TKN_UOM s of entering vehicles steadily increase until reaching the maximum TKN_UOM  the year  TKN_Year  in july with approximately 101. from july until november a sharp drop is experienced, with TKN_UOM s of around 11 in november. the TKN_UOM  hardly changes in december.</t>
         </is>
       </c>
       <c r="W266" t="n">
@@ -22812,12 +22812,12 @@
       </c>
       <c r="U267" t="inlineStr">
         <is>
-          <t>This graph depicts the total Canadian softwood production in cubic metres in 2018. The unit given is cubic metres. Production starts at around 5600 in January and drops to approximately 5180 in February. It then fluctuates around 5800 between the months of March and May, until it drops back to same production numbers of February during July. Production of softwood fluctuates between July until October, reaching around 5600. Afterwards a sharp decline can be observed until December, which marks the lowest production numbers for this year at around 4200.</t>
+          <t>this graph depicts the total canadian softwood production in cubic metres in 2018. the unit given is cubic metres. production starts at around 5600 in january and drops to approximately 5180 in february. it then fluctuates around 5800 between the months of march and may, until it drops back to same production numbers of february during july. production of softwood fluctuates between july until october, reaching around 5600. afterwards a sharp decline can be observed until december, which marks the lowest production numbers for this year at around 4200.</t>
         </is>
       </c>
       <c r="V267" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in TKN_UOM  in  TKN_Year . The unit given is TKN_UOM . Production starts at around 85 in January and drops to approximately 59 in February. It then fluctuates around 98 between the months of March and May, until it drops back to same production numbers of February during July. Production of softwood fluctuates between July until October, reaching around 85. Afterwards a sharp decline can be observed until December, which marks the lowest production numbers for this year at around -2.</t>
+          <t>this graph depicts the TKN_About  in TKN_UOM  in  TKN_Year . the unit given is TKN_UOM . production starts at around 85 in january and drops to approximately 59 in february. it then fluctuates around 98 between the months of march and may, until it drops back to same production numbers of february during july. production of softwood fluctuates between july until october, reaching around 85. afterwards a sharp decline can be observed until december, which marks the lowest production numbers for this year at around -2.</t>
         </is>
       </c>
       <c r="W267" t="n">
@@ -22896,12 +22896,12 @@
       </c>
       <c r="U268" t="inlineStr">
         <is>
-          <t>This figure shows the Canadian production of wheat flour of 2016. Production is measured in tonnes. Production is the lowest during the month of January at approximately 19500. There is a sharp increase for February, reaching 26000 tonnes, after which a drop is experienced during March. The maximum production of wheat flour is taking place in April at above 30500 tonnes. Production is rather low during May. During the following months production fluctuates until a sharp increase in observed for October, reaching nearly 30000 tonnes. Production remains nearly steady throughout November and drops back to 25000 during December.</t>
+          <t>this figure shows the canadian production of wheat flour of 2016. production is measured in tonnes. production is the lowest during the month of january at approximately 19500. there is a sharp increase for february, reaching 26000 tonnes, after which a drop is experienced during march. the maximum production of wheat flour is taking place in april at above 30500 tonnes. production is rather low during may. during the following months production fluctuates until a sharp increase in observed for october, reaching nearly 30000 tonnes. production remains nearly steady throughout november and drops back to 25000 during december.</t>
         </is>
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>This figure shows the Canadian TKN_About  of  TKN_Year . Production is measured in tonnes. Production is the lowest during the month of January at approximately 0. There is a sharp increase for February, reaching 59 tonnes, after which a drop is experienced during March. The maximum TKN_About  is taking place in April at above 100 tonnes. Production is rather low during May. During the following months production fluctuates until a sharp increase in observed for October, reaching nearly 95 tonnes. Production remains nearly steady throughout November and drops back to 50 during December.</t>
+          <t>this figure shows the canadian TKN_About  of  TKN_Year . production is measured in tonnes. production is the lowest during the month of january at approximately 0. there is a sharp increase for february, reaching 59 tonnes, after which a drop is experienced during march. the maximum TKN_About  is taking place in april at above 100 tonnes. production is rather low during may. during the following months production fluctuates until a sharp increase in observed for october, reaching nearly 95 tonnes. production remains nearly steady throughout november and drops back to 50 during december.</t>
         </is>
       </c>
       <c r="W268" t="n">
@@ -22980,12 +22980,12 @@
       </c>
       <c r="U269" t="inlineStr">
         <is>
-          <t>This graph depicts the total Canadian softwood and hardwood production of 2016. The unit used is cubic metres. Production during January lies at approximately 54000 and experiences an increase until reaching the maximum value in March at above 58300. From then production slowly declines until June, after which a sharp drop can be observed in July at approximately 51000. From July until November production levels increase again, reaching a value of nearly 58100. There is a rapid decline of production in December, which marks the lowest production of the year at 47000 cubic metres.</t>
+          <t>this graph depicts the total canadian softwood and hardwood production of 2016. the unit used is cubic metres. production during january lies at approximately 54000 and experiences an increase until reaching the maximum value in march at above 58300. from then production slowly declines until june, after which a sharp drop can be observed in july at approximately 51000. from july until november production levels increase again, reaching a value of nearly 58100. there is a rapid decline of production in december, which marks the lowest production of the year at 47000 cubic metres.</t>
         </is>
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  of  TKN_Year . The unit used TKN_UOM  metres. Production during January lies at approximately 61 and experiences an increase until reaching the maximum value in March at above 99. From then production slowly declines until June, after which a sharp drop can be observed in July at approximately 34. From July until November production levels increase again, reaching a value of nearly 98. There is a rapid decline of production in December, which marks the lowest production of the year at -2 cubic metres.</t>
+          <t>this graph depicts the TKN_About  of  TKN_Year . the unit used TKN_UOM  metres. production during january lies at approximately 61 and experiences an increase until reaching the maximum value in march at above 99. from then production slowly declines until june, after which a sharp drop can be observed in july at approximately 34. from july until november production levels increase again, reaching a value of nearly 98. there is a rapid decline of production in december, which marks the lowest production of the year at -2 cubic metres.</t>
         </is>
       </c>
       <c r="W269" t="n">
@@ -23064,12 +23064,12 @@
       </c>
       <c r="U270" t="inlineStr">
         <is>
-          <t>The production of unprocessed milk in Canada has been substantially growing over 2018. In particular, during the first few months of the year the values have been slightly decreasing. But then from June over it rapidly increased, reaching it peaks on November 2018. The minimum production value during 2018 has been reported during June.</t>
+          <t>the production of unprocessed milk in canada has been substantially growing over 2018. in particular, during the first few months of the year the values have been slightly decreasing. but then from june over it rapidly increased, reaching it peaks on november 2018. the minimum production value during 2018 has been reported during june.</t>
         </is>
       </c>
       <c r="V270" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  has been substantially growing over  TKN_Year . In particular, during the first few months of the year the values have been slightly decreasing. But then from June over it rapidly increased, reaching it peaks on November  TKN_Year . The minimum production value during  TKN_Year  has been reported during June.</t>
+          <t>the TKN_About  in canada has been substantially growing over  TKN_Year . in particular, during the first few months of the year the values have been slightly decreasing. but then from june over it rapidly increased, reaching it peaks on november  TKN_Year . the minimum production value during  TKN_Year  has been reported during june.</t>
         </is>
       </c>
       <c r="W270" t="n">
@@ -23148,12 +23148,12 @@
       </c>
       <c r="U271" t="inlineStr">
         <is>
-          <t>The house price index in Canada during 2018 presents a quite ambiguous trend. Firstly, during the first few months, it slowly decrease. But then, from May to July, it recorded a considerable growth. During the last few months of the year the house price index mainted the same level.</t>
+          <t>the house price index in canada during 2018 presents a quite ambiguous trend. firstly, during the first few months, it slowly decrease. but then, from may to july, it recorded a considerable growth. during the last few months of the year the house price index mainted the same level.</t>
         </is>
       </c>
       <c r="V271" t="inlineStr">
         <is>
-          <t>The house TKN_UOM  in  TKN_Geo  during  TKN_Year  presents a quite ambiguous trend. Firstly, during the first few months, it slowly decrease. But then, from May to July, it recorded a considerable growth. During the last few months of the year the house TKN_UOM  mainted the same level.</t>
+          <t>the house TKN_UOM  in canada during  TKN_Year  presents a quite ambiguous trend. firstly, during the first few months, it slowly decrease. but then, from may to july, it recorded a considerable growth. during the last few months of the year TKN_About  TKN_UOM  mainted the same level.</t>
         </is>
       </c>
       <c r="W271" t="n">
@@ -23232,12 +23232,12 @@
       </c>
       <c r="U272" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the price index of desktop and similar computers in Canada has been significantly decreasing over 2017. Few fluctuations of the value have been recorded, but without any significant peaks or dips. The highest value was in January. The minimum value was in December 2017.</t>
+          <t>it's clearly possible to see how the price index of desktop and similar computers in canada has been significantly decreasing over 2017. few fluctuations of the value have been recorded, but without any significant peaks or dips. the highest value was in january. the minimum value was in december 2017.</t>
         </is>
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the TKN_About  in  TKN_Geo  has been significantly decreasing over  TKN_Year . Few fluctuations of the value have been recorded, but without any significant peaks or dips. The highest value was in January. The minimum value was in December  TKN_Year .</t>
+          <t>it's clearly possible to see how the TKN_About  in canada has been significantly decreasing over  TKN_Year . few fluctuations of the value have been recorded, but without any significant peaks or dips. the highest value was in january. the minimum value was in december  TKN_Year .</t>
         </is>
       </c>
       <c r="W272" t="n">
@@ -23316,12 +23316,12 @@
       </c>
       <c r="U273" t="inlineStr">
         <is>
-          <t>The graph shows how the land price index in Canada rapidly increased during 2017. In particular, it started in January around 1000 and ended up in December with more than 1035. The most significant increase was recorded between March and May.</t>
+          <t>the graph shows how the land price index in canada rapidly increased during 2017. in particular, it started in january around 1000 and ended up in december with more than 1035. the most significant increase was recorded between march and may.</t>
         </is>
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>The graph shows how TKN_About  TKN_UOM  in  TKN_Geo  rapidly increased during  TKN_Year . In particular, it started in January around -12 and ended up in December with more than 94. The most significant increase was recorded between March and May.</t>
+          <t>the graph shows how TKN_About  TKN_UOM  in canada rapidly increased during  TKN_Year . in particular, it started in january around -12 and ended up in december with more than 94. the most significant increase was recorded between march and may.</t>
         </is>
       </c>
       <c r="W273" t="n">
@@ -23400,12 +23400,12 @@
       </c>
       <c r="U274" t="inlineStr">
         <is>
-          <t>Total Canadian livestock and animal products in 2018 are shown in this graph. The unit given is the farm product price index (FPPI). During January products lie at 1385 and the second highes value of the year can be observed in February at approximately 1395. There is a sharp decline from February onwards, reaching a low of 1338 in April. During the following months there is a steep rise, reaching the maximum of 1412 in July. Again, a huge decrease follows until reaching the lowest value in September, which is followed by a significant rise for October. Following this, a rapid drop can be observed until December.</t>
+          <t>total canadian livestock and animal products in 2018 are shown in this graph. the unit given is the farm product price index (fppi). during january products lie at 1385 and the second highes value of the year can be observed in february at approximately 1395. there is a sharp decline from february onwards, reaching a low of 1338 in april. during the following months there is a steep rise, reaching the maximum of 1412 in july. again, a huge decrease follows until reaching the lowest value in september, which is followed by a significant rise for october. following this, a rapid drop can be observed until december.</t>
         </is>
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>Total Canadian livestock and animal products in  TKN_Year  are shown in this graph. The unit given is TKN_UOM  (FPPI). During January products lie at 63 and the second highes value of the year can be observed in February at approximately 76. There is a sharp decline from February onwards, reaching a low of 1 in April. During the following months there is a steep rise, reaching the maximum of 99 in July. Again, a huge decrease follows until reaching the lowest value in September, which is followed by a significant rise for October. Following this, a rapid drop can be observed until December.</t>
+          <t>total canadian livestock and animal products in  TKN_Year  are shown in this graph. the unit given is TKN_UOM  (fppi). during january products lie at 63 and the second highes value of the year can be observed in february at approximately 76. there is a sharp decline from february onwards, reaching a low of 1 in april. during the following months there is a steep rise, reaching the maximum of 99 in july. again, a huge decrease follows until reaching the lowest value in september, which is followed by a significant rise for october. following this, a rapid drop can be observed until december.</t>
         </is>
       </c>
       <c r="W274" t="n">
@@ -23484,12 +23484,12 @@
       </c>
       <c r="U275" t="inlineStr">
         <is>
-          <t>It's possible to see how the import value of creamery butter in Canada presented several fluctuations over the year. In particular during the first few months different peaks and dips have been recorded. Then the import value rapidly increased from August to November. It reached its maximum value during the month of November. The minimum value was in January 2016.</t>
+          <t>it's possible to see how the import value of creamery butter in canada presented several fluctuations over the year. in particular during the first few months different peaks and dips have been recorded. then the import value rapidly increased from august to november. it reached its maximum value during the month of november. the minimum value was in january 2016.</t>
         </is>
       </c>
       <c r="V275" t="inlineStr">
         <is>
-          <t>It's possible to see how the TKN_About  in  TKN_Geo  presented several fluctuations over the year. In particular during the first few months different peaks and dips have been recorded. Then the import value rapidly increased from August to November. It reached its maximum value during the month of November. The minimum value was in January  TKN_Year .</t>
+          <t>it's possible to see how the TKN_About  in canada presented several fluctuations over the year. in particular during the first few months different peaks and dips have been recorded. then the import value rapidly increased from august to november. it reached its maximum value during the month of november. the minimum value was in january  TKN_Year .</t>
         </is>
       </c>
       <c r="W275" t="n">
@@ -23568,12 +23568,12 @@
       </c>
       <c r="U276" t="inlineStr">
         <is>
-          <t>The values about production of fresh fruit in Canada during 2018 show a quite interesting trend. The production remained stable for most of the year. But two big peaks of production have been recorded, one in March and one in August. Even that, the most significant peak was definetely in August 2018. The month with less production was December.</t>
+          <t>the values about production of fresh fruit in canada during 2018 show a quite interesting trend. the production remained stable for most of the year. but two big peaks of production have been recorded, one in march and one in august. even that, the most significant peak was definetely in august 2018. the month with less production was december.</t>
         </is>
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>The values about TKN_About  in  TKN_Geo  during  TKN_Year  show a quite interesting trend. The production remained stable for most of the year. But two big peaks of production have been recorded, one in March and one in August. Even that, the most significant peak was definetely in August  TKN_Year . The month with less production was December.</t>
+          <t>the values about TKN_About  in canada during  TKN_Year  show a quite interesting trend. the production remained stable for most of the year. but two big peaks of production have been recorded, one in march and one in august. even that, the most significant peak was definetely in august  TKN_Year . the month with less production was december.</t>
         </is>
       </c>
       <c r="W276" t="n">
@@ -23652,12 +23652,12 @@
       </c>
       <c r="U277" t="inlineStr">
         <is>
-          <t>This graph depicts the production of unprocessed milk in Canada during 2018. The given unit is the farm product price index (FPPI). The graph represents a parable throughout the year. It starts at 1050 during January, after which a steady decline can be observed, reaching the lowest production value in June at 1003. During the following months production rapidly increases until the maximum is reached in November at approximately 1140. There is a small decrease in December.</t>
+          <t>this graph depicts the production of unprocessed milk in canada during 2018. the given unit is the farm product price index (fppi). the graph represents a parable throughout the year. it starts at 1050 during january, after which a steady decline can be observed, reaching the lowest production value in june at 1003. during the following months production rapidly increases until the maximum is reached in november at approximately 1140. there is a small decrease in december.</t>
         </is>
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in  TKN_Geo  during  TKN_Year . The given unit is TKN_UOM  (FPPI). The graph represents a parable throughout the year. It starts at 34 during January, after which a steady decline can be observed, reaching the lowest production value in June at 0. During the following months production rapidly increases until the maximum is reached in November at approximately 100. There is a small decrease in December.</t>
+          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the given unit is TKN_UOM  (fppi). the graph represents a parable throughout the year. it starts at 34 during january, after which a steady decline can be observed, reaching the lowest production value in june at 0. during the following months production rapidly increases until the maximum is reached in november at approximately 100. there is a small decrease in december.</t>
         </is>
       </c>
       <c r="W277" t="n">
@@ -23736,12 +23736,12 @@
       </c>
       <c r="U278" t="inlineStr">
         <is>
-          <t>This graph illustrates values about the total farm production index in Canada during 2018. Those values are described using the farm product price index (FPPI). It's clearly possible to see how the maximum values of production are registered during the summer months. In particular, the highest production value was during July 2018. At the same time, the lowest one was in December.</t>
+          <t>this graph illustrates values about the total farm production index in canada during 2018. those values are described using the farm product price index (fppi). it's clearly possible to see how the maximum values of production are registered during the summer months. in particular, the highest production value was during july 2018. at the same time, the lowest one was in december.</t>
         </is>
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>This graph illustrates values about the TKN_About  in  TKN_Geo  during  TKN_Year . Those values are described using TKN_UOM  (FPPI). It's clearly possible to see how the maximum values of production are registered during the summer months. In particular, the highest production value was during July  TKN_Year . At the same time, the lowest one was in December.</t>
+          <t>this graph illustrates values about the TKN_About  in canada during  TKN_Year . those values are described using TKN_UOM  (fppi). it's clearly possible to see how the maximum values of production are registered during the summer months. in particular, the highest production value was during july  TKN_Year . at the same time, the lowest one was in december.</t>
         </is>
       </c>
       <c r="W278" t="n">
@@ -23820,12 +23820,12 @@
       </c>
       <c r="U279" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian production of rye during 2017. The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 6000 to 8000 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 15000 tonnes. The highest production can be observed during October with nearly 20000. Rye production experiences a sharp drop in November, reaching around 7500 tonnes. There is a minimal increase during December.</t>
+          <t>this figure represents the canadian production of rye during 2017. the given unit are tonnes. production remains mostly stable throughout the months of january until may, around 6000 to 8000 tonnes. following this there is a sharp increase in june, with the production plateauing throughout august at approximately 15000 tonnes. the highest production can be observed during october with nearly 20000. rye production experiences a sharp drop in november, reaching around 7500 tonnes. there is a minimal increase during december.</t>
         </is>
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About  during  TKN_Year . The given unit are tonnes. Production remains mostly stable throughout the months of January until May, around 3 to 17 tonnes. Following this there is a sharp increase in June, with the production plateauing throughout August at approximately 65 tonnes. The highest production can be observed during October with nearly 100. Rye production experiences a sharp drop in November, reaching around 13 tonnes. There is a minimal increase during December.</t>
+          <t>this figure represents the canadian TKN_About  during  TKN_Year . the given unit are tonnes. production remains mostly stable throughout the months of january until may, around 3 to 17 tonnes. following this there is a sharp increase in june, with the production plateauing throughout august at approximately 65 tonnes. the highest production can be observed during october with nearly 100. rye production experiences a sharp drop in november, reaching around 13 tonnes. there is a minimal increase during december.</t>
         </is>
       </c>
       <c r="W279" t="n">
@@ -23904,12 +23904,12 @@
       </c>
       <c r="U280" t="inlineStr">
         <is>
-          <t>The production of fresh fruit in Canada clearly showed an ascendant trend during 2017. The values have been oscillating up and down several times over the year, even if the trend kept growing up. The production reached its maximum value during the month of December, and its minimum values during the first months of the year.</t>
+          <t>the production of fresh fruit in canada clearly showed an ascendant trend during 2017. the values have been oscillating up and down several times over the year, even if the trend kept growing up. the production reached its maximum value during the month of december, and its minimum values during the first months of the year.</t>
         </is>
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  clearly showed an ascendant trend during  TKN_Year . The values have been oscillating up and down several times over the year, even if the trend kept growing up. The production reached its maximum value during the month of December, and its minimum values during the first months of the year.</t>
+          <t>the TKN_About  in canada clearly showed an ascendant trend during  TKN_Year . the values have been oscillating up and down several times over the year, even if the trend kept growing up. the production reached its maximum value during the month of december, and its minimum values during the first months of the year.</t>
         </is>
       </c>
       <c r="W280" t="n">
@@ -23988,12 +23988,12 @@
       </c>
       <c r="U281" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from this graph how the production of grains in Canada had a big drop from June to August 2016. During the first few months, from January to June, the value remained quite stable. But then it dramatically dropped down. Even that, during the last few months of the year the production of value slightly started to grow up again.</t>
+          <t>it's clearly possible to see from this graph how the production of grains in canada had a big drop from june to august 2016. during the first few months, from january to june, the value remained quite stable. but then it dramatically dropped down. even that, during the last few months of the year the production of value slightly started to grow up again.</t>
         </is>
       </c>
       <c r="V281" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from this graph how the TKN_About  in  TKN_Geo  had a big drop from June to August  TKN_Year . During the first few months, from January to June, the value remained quite stable. But then it dramatically dropped down. Even that, during the last few months of the year the production of value slightly started to grow up again.</t>
+          <t>it's clearly possible to see from this graph how the TKN_About  in canada had a big drop from june to august  TKN_Year . during the first few months, from january to june, the value remained quite stable. but then it dramatically dropped down. even that, during the last few months of the year the production of value slightly started to grow up again.</t>
         </is>
       </c>
       <c r="W281" t="n">
@@ -24072,12 +24072,12 @@
       </c>
       <c r="U282" t="inlineStr">
         <is>
-          <t>This graph depicts the production of eggs in shell in Canada during 2017. The unit is farm product price index (FPPI). Production starts off at approximately 1363 in January and goes down to the lowest production at 1362 during February. During the months of March and May the production remains unchanged at 1365. There is a slight increase of production during June, until it remain stable throughout July until September at 1367. Then, a small drop can be observed, which is followed by a sharp increase, until it peaks during December at 1371.</t>
+          <t>this graph depicts the production of eggs in shell in canada during 2017. the unit is farm product price index (fppi). production starts off at approximately 1363 in january and goes down to the lowest production at 1362 during february. during the months of march and may the production remains unchanged at 1365. there is a slight increase of production during june, until it remain stable throughout july until september at 1367. then, a small drop can be observed, which is followed by a sharp increase, until it peaks during december at 1371.</t>
         </is>
       </c>
       <c r="V282" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About  in  TKN_Geo  during  TKN_Year . The unit TKN_UOM  (FPPI). Production starts off at approximately 11 in January and goes down to the lowest production at 0 during February. During the months of March and May the production remains unchanged at 33. There is a slight increase of production during June, until it remain stable throughout July until September at 56. Then, a small drop can be observed, which is followed by a sharp increase, until it peaks during December at 100.</t>
+          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the unit TKN_UOM  (fppi). production starts off at approximately 11 in january and goes down to the lowest production at 0 during february. during the months of march and may the production remains unchanged at 33. there is a slight increase of production during june, until it remain stable throughout july until september at 56. then, a small drop can be observed, which is followed by a sharp increase, until it peaks during december at 100.</t>
         </is>
       </c>
       <c r="W282" t="n">
@@ -24156,12 +24156,12 @@
       </c>
       <c r="U283" t="inlineStr">
         <is>
-          <t>The land price index in Canada during 2016 has been showing a slight but constant ascendant trend. In particular, from January to April the index value remained exactly the same. But then, after that, it started to grow up with few fluctuations in between. The maximum values were reached during the months of November and December 2016.</t>
+          <t>the land price index in canada during 2016 has been showing a slight but constant ascendant trend. in particular, from january to april the index value remained exactly the same. but then, after that, it started to grow up with few fluctuations in between. the maximum values were reached during the months of november and december 2016.</t>
         </is>
       </c>
       <c r="V283" t="inlineStr">
         <is>
-          <t>The land TKN_UOM  in  TKN_Geo  during  TKN_Year  has been showing a slight but constant ascendant trend. In particular, from January to April the index value remained exactly the same. But then, after that, it started to grow up with few fluctuations in between. The maximum values were reached during the months of November and December  TKN_Year .</t>
+          <t>the land TKN_UOM  in canada during  TKN_Year  has been showing a slight but constant ascendant trend. in particular, from january to april the index value remained exactly the same. but then, after that, it started to grow up with few fluctuations in between. the maximum values were reached during the months of november and december  TKN_Year .</t>
         </is>
       </c>
       <c r="W283" t="n">
@@ -24240,12 +24240,12 @@
       </c>
       <c r="U284" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from the graph that the production of fresh potatoes in Canada during 2018 reached its maximum values during the summer months. In particular, the most significant peak of the values was registered during August 2018. Despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
+          <t>it's clearly possible to see from the graph that the production of fresh potatoes in canada during 2018 reached its maximum values during the summer months. in particular, the most significant peak of the values was registered during august 2018. despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
         </is>
       </c>
       <c r="V284" t="inlineStr">
         <is>
-          <t>It's clearly possible to see from the graph that the TKN_About  in  TKN_Geo  during  TKN_Year  reached its maximum values during the summer months. In particular, the most significant peak of the values was registered during August  TKN_Year . Despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
+          <t>it's clearly possible to see from the graph that the TKN_About  in canada during  TKN_Year  reached its maximum values during the summer months. in particular, the most significant peak of the values was registered during august  TKN_Year . despite of that, during the rest of the year the production value remained quite stable with few and not significant fluctuations.</t>
         </is>
       </c>
       <c r="W284" t="n">
@@ -24324,12 +24324,12 @@
       </c>
       <c r="U285" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian production of Canola in 2018. The given unit are tonnes. Production starts off at approximately 1150000 during January, after which a sharp decline is observed during February, reaching below 600000. Production fluctuates between March and June, after which a rapid decline takes place again, reaching the lowest production values of the year in August at 500000. Staying mostly constant in September, there is a significant rise peaking in October above 1400000. Production of Canola declines again during November, and hardly changes for December at around 900000.</t>
+          <t>this graph represents the canadian production of canola in 2018. the given unit are tonnes. production starts off at approximately 1150000 during january, after which a sharp decline is observed during february, reaching below 600000. production fluctuates between march and june, after which a rapid decline takes place again, reaching the lowest production values of the year in august at 500000. staying mostly constant in september, there is a significant rise peaking in october above 1400000. production of canola declines again during november, and hardly changes for december at around 900000.</t>
         </is>
       </c>
       <c r="V285" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian TKN_About  in  TKN_Year . The given unit are tonnes. Production starts off at approximately 70 during January, after which a sharp decline is observed during February, reaching below 10. Production fluctuates between March and June, after which a rapid decline takes place again, reaching the lowest production values of the year in August at -1. Staying mostly constant in September, there is a significant rise peaking in October above 97. Production of Canola declines again during November, and hardly changes for December at around 42.</t>
+          <t>this graph represents the canadian TKN_About  in  TKN_Year . the given unit are tonnes. production starts off at approximately 70 during january, after which a sharp decline is observed during february, reaching below 10. production fluctuates between march and june, after which a rapid decline takes place again, reaching the lowest production values of the year in august at -1. staying mostly constant in september, there is a significant rise peaking in october above 97. TKN_About  declines again during november, and hardly changes for december at around 42.</t>
         </is>
       </c>
       <c r="W285" t="n">
@@ -24408,12 +24408,12 @@
       </c>
       <c r="U286" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian price index of servers in 2018. The price index starts off at 1010 during January, and keeps decreasing throughout the following months, until it reaches its minimum value of below 998 in April. From then on there is a sharp increase, peaking in July at above 1012. During the following months a moderate decrease is experienced until October. The price index remains unchanged during November and December at 1008.</t>
+          <t>this figure represents the canadian price index of servers in 2018. the price index starts off at 1010 during january, and keeps decreasing throughout the following months, until it reaches its minimum value of below 998 in april. from then on there is a sharp increase, peaking in july at above 1012. during the following months a moderate decrease is experienced until october. the price index remains unchanged during november and december at 1008.</t>
         </is>
       </c>
       <c r="V286" t="inlineStr">
         <is>
-          <t>This figure represents the Canadian TKN_About  in  TKN_Year . The price index starts off at 81 during January, and keeps decreasing throughout the following months, until it reaches its minimum value of below 6 in April. From then on there is a sharp increase, peaking in July at above 94. During the following months a moderate decrease is experienced until October. The price index remains unchanged during November and December at 69.</t>
+          <t>this figure represents the canadian TKN_About  in  TKN_Year . the price index starts off at 81 during january, and keeps decreasing throughout the following months, until it reaches its minimum value of below 6 in april. from then on there is a sharp increase, peaking in july at above 94. during the following months a moderate decrease is experienced until october. the price index remains unchanged during november and december at 69.</t>
         </is>
       </c>
       <c r="W286" t="n">
@@ -24492,12 +24492,12 @@
       </c>
       <c r="U287" t="inlineStr">
         <is>
-          <t>The commercial software price index in Canada considerably increased over 2018. The minimum value was in January around 1130. The maximum value was in December around 1167. All over the year there were reported several fluctuations of the index value.</t>
+          <t>the commercial software price index in canada considerably increased over 2018. the minimum value was in january around 1130. the maximum value was in december around 1167. all over the year there were reported several fluctuations of the index value.</t>
         </is>
       </c>
       <c r="V287" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  considerably increased over  TKN_Year . The minimum value was in January around 3. The maximum value was in December around 100. All over the year there were reported several fluctuations of the index value.</t>
+          <t>the TKN_About  in canada considerably increased over  TKN_Year . the minimum value was in january around 3. the maximum value was in december around 100. all over the year there were reported several fluctuations of the index value.</t>
         </is>
       </c>
       <c r="W287" t="n">
@@ -24576,12 +24576,12 @@
       </c>
       <c r="U288" t="inlineStr">
         <is>
-          <t>It shows the price index trend about tablet computers in Canada during 2018. It's possible to see how it considerably declined over the year.  Over the year the values ahs been oscillating several times, in particular during the summer months. Even that, the maximum value was recorded in January and the minimum one in November 2018.</t>
+          <t>it shows the price index trend about tablet computers in canada during 2018. it's possible to see how it considerably declined over the year.  over the year the values ahs been oscillating several times, in particular during the summer months. even that, the maximum value was recorded in january and the minimum one in november 2018.</t>
         </is>
       </c>
       <c r="V288" t="inlineStr">
         <is>
-          <t>It shows the TKN_About  in  TKN_Geo  during  TKN_Year . It's possible to see how it considerably declined over the year.  Over the year the values ahs been oscillating several times, in particular during the summer months. Even that, the maximum value was recorded in January and the minimum one in November  TKN_Year .</t>
+          <t>it shows the TKN_About  in canada during  TKN_Year . it's possible to see how it considerably declined over the year.  over the year the values ahs been oscillating several times, in particular during the summer months. even that, the maximum value was recorded in january and the minimum one in november  TKN_Year .</t>
         </is>
       </c>
       <c r="W288" t="n">
@@ -24660,12 +24660,12 @@
       </c>
       <c r="U289" t="inlineStr">
         <is>
-          <t>The production of malt in Canada reported some strong oscillations of the value during 2018. As it's possible to see from the graph, several peaks and dips have been registered. The most significant peaks were during March and July. The most considerable dips during September and December. Furthermore, a marked drop of the production value was registered between July and August 2018.</t>
+          <t>the production of malt in canada reported some strong oscillations of the value during 2018. as it's possible to see from the graph, several peaks and dips have been registered. the most significant peaks were during march and july. the most considerable dips during september and december. furthermore, a marked drop of the production value was registered between july and august 2018.</t>
         </is>
       </c>
       <c r="V289" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  reported some strong oscillations of the value during  TKN_Year . As it's possible to see from the graph, several peaks and dips have been registered. The most significant peaks were during March and July. The most considerable dips during September and December. Furthermore, a marked drop of the production value was registered between July and August  TKN_Year .</t>
+          <t>the TKN_About  in canada reported some strong oscillations of the value during  TKN_Year . as it's possible to see from the graph, several peaks and dips have been registered. the most significant peaks were during march and july. the most considerable dips during september and december. furthermore, a marked drop of the production value was registered between july and august  TKN_Year .</t>
         </is>
       </c>
       <c r="W289" t="n">
@@ -24744,12 +24744,12 @@
       </c>
       <c r="U290" t="inlineStr">
         <is>
-          <t>This figure represents the land price index in Canada in 2018. Overall the price index increases throughout the year. During January a value of 1037 can be observed, after which it rises up to 1038 during February. It falls back to 1037 during March and April. During the following 2 months there is a steady increase, after which the land price index remains unchanged at 1039 throughout June until August. Also, it remains steady during September and October at 1040. Moreover, the land price index stays constant at the peak value of the year during November and December, reaching up to 1041.</t>
+          <t>this figure represents the land price index in canada in 2018. overall the price index increases throughout the year. during january a value of 1037 can be observed, after which it rises up to 1038 during february. it falls back to 1037 during march and april. during the following 2 months there is a steady increase, after which the land price index remains unchanged at 1039 throughout june until august. also, it remains steady during september and october at 1040. moreover, the land price index stays constant at the peak value of the year during november and december, reaching up to 1041.</t>
         </is>
       </c>
       <c r="V290" t="inlineStr">
         <is>
-          <t>This figure represents TKN_About  TKN_UOM  in  TKN_Geo  in  TKN_Year . Overall the TKN_UOM  increases throughout the year. During January a value of 0 can be observed, after which it rises up to 25 during February. It falls back to 0 during March and April. During the following 2 months there is a steady increase, after which TKN_About  TKN_UOM  remains unchanged at 50 throughout June until August. Also, it remains steady during September and October at 75. Moreover, TKN_About  TKN_UOM  stays constant at the peak value of the year during November and December, reaching up to 100.</t>
+          <t>this figure represents TKN_About  TKN_UOM  in canada in  TKN_Year . overall the TKN_UOM  increases throughout the year. during january a value of 0 can be observed, after which it rises up to 25 during february. it falls back to 0 during march and april. during the following 2 months there is a steady increase, after which TKN_About  TKN_UOM  remains unchanged at 50 throughout june until august. also, it remains steady during september and october at 75. moreover, TKN_About  TKN_UOM  stays constant at the peak value of the year during november and december, reaching up to 100.</t>
         </is>
       </c>
       <c r="W290" t="n">
@@ -24828,12 +24828,12 @@
       </c>
       <c r="U291" t="inlineStr">
         <is>
-          <t>The total number of United States vehicles returning presents a steep growth over the first half of the year. In particular, it starts to grow during the month of February until reaching its peak during July 2017. After that, it slightly start to decrease over the last few months of the year. The lowest value of the year was registered during February 2017.</t>
+          <t>the total number of united states vehicles returning presents a steep growth over the first half of the year. in particular, it starts to grow during the month of february until reaching its peak during july 2017. after that, it slightly start to decrease over the last few months of the year. the lowest value of the year was registered during february 2017.</t>
         </is>
       </c>
       <c r="V291" t="inlineStr">
         <is>
-          <t>The total TKN_UOM  of United States vehicles returning presents a steep growth over the first half of the year. In particular, it starts to grow during the month of February until reaching its peak during July  TKN_Year . After that, it slightly start to decrease over the last few months of the year. The lowest value of the year was registered during February  TKN_Year .</t>
+          <t>the total TKN_UOM  of united states vehicles returning presents a steep growth over the first half of the year. in particular, it starts to grow during the month of february until reaching its peak during july  TKN_Year . after that, it slightly start to decrease over the last few months of the year. the lowest value of the year was registered during february  TKN_Year .</t>
         </is>
       </c>
       <c r="W291" t="n">
@@ -24912,12 +24912,12 @@
       </c>
       <c r="U292" t="inlineStr">
         <is>
-          <t>This graph represents the price index of laptop computers in Canada in 2018. The peak value can be observed during January at 966. During the following months the price index fluctuates, until there is a sharp decline from May to June, reaching the lowest value of 952. There is a sharp increase during the month of July to 961. The price index fluctuates again from August until December.</t>
+          <t>this graph represents the price index of laptop computers in canada in 2018. the peak value can be observed during january at 966. during the following months the price index fluctuates, until there is a sharp decline from may to june, reaching the lowest value of 952. there is a sharp increase during the month of july to 961. the price index fluctuates again from august until december.</t>
         </is>
       </c>
       <c r="V292" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year . The peak value can be observed during January at 100. During the following months the price index fluctuates, until there is a sharp decline from May to June, reaching the lowest value of 0. There is a sharp increase during the month of July to 64. The price index fluctuates again from August until December.</t>
+          <t>this graph represents the TKN_About  in canada in  TKN_Year . the peak value can be observed during january at 100. during the following months the price index fluctuates, until there is a sharp decline from may to june, reaching the lowest value of 0. there is a sharp increase during the month of july to 64. the price index fluctuates again from august until december.</t>
         </is>
       </c>
       <c r="W292" t="n">
@@ -24996,12 +24996,12 @@
       </c>
       <c r="U293" t="inlineStr">
         <is>
-          <t>The amount of import creamery butter in Canada during 2018 presented strong variations in its values over the year. It's possible to identify several peaks, dips and curves. During June and July has been recorded a massive drop of the import value. At the same time, the most significant peak was registered during June. The most considerable dip was reported during July.</t>
+          <t>the amount of import creamery butter in canada during 2018 presented strong variations in its values over the year. it's possible to identify several peaks, dips and curves. during june and july has been recorded a massive drop of the import value. at the same time, the most significant peak was registered during june. the most considerable dip was reported during july.</t>
         </is>
       </c>
       <c r="V293" t="inlineStr">
         <is>
-          <t>The amount TKN_About  in  TKN_Geo  during  TKN_Year  presented strong variations in its values over the year. It's possible to identify several peaks, dips and curves. During June and July has been recorded a massive drop of the import value. At the same time, the most significant peak was registered during June. The most considerable dip was reported during July.</t>
+          <t>the amount TKN_About  in canada during  TKN_Year  presented strong variations in its values over the year. it's possible to identify several peaks, dips and curves. during june and july has been recorded a massive drop of the import value. at the same time, the most significant peak was registered during june. the most considerable dip was reported during july.</t>
         </is>
       </c>
       <c r="W293" t="n">
@@ -25080,12 +25080,12 @@
       </c>
       <c r="U294" t="inlineStr">
         <is>
-          <t>The total softwood and hardwood production in Canada showed an oscillating trend over 2017. In particular, couple of peaks have been registered, mainly during the months of March and May. At the same time, the production value showed its minimum values during the months of July and December. The most considerable drop of the value was registered between the months of November and December.</t>
+          <t>the total softwood and hardwood production in canada showed an oscillating trend over 2017. in particular, couple of peaks have been registered, mainly during the months of march and may. at the same time, the production value showed its minimum values during the months of july and december. the most considerable drop of the value was registered between the months of november and december.</t>
         </is>
       </c>
       <c r="V294" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  showed an oscillating trend over  TKN_Year . In particular, couple of peaks have been registered, mainly during the months of March and May. At the same time, the production value showed its minimum values during the months of July and December. The most considerable drop of the value was registered between the months of November and December.</t>
+          <t>the TKN_About  in canada showed an oscillating trend over  TKN_Year . in particular, couple of peaks have been registered, mainly during the months of march and may. at the same time, the production value showed its minimum values during the months of july and december. the most considerable drop of the value was registered between the months of november and december.</t>
         </is>
       </c>
       <c r="W294" t="n">
@@ -25164,12 +25164,12 @@
       </c>
       <c r="U295" t="inlineStr">
         <is>
-          <t>The following graph depicts the Canadian production of oats in tonnes during 2018. In January approximately 160000 tonnes were produced, after which a sharp drop can be observed for February, reaching slightly below 100000. Production remain mostly stable throughout March to May, with the lowest production coming up in July at 80000. Production sharply increases during the following months, until it peaks in October at approximately 210000. Following this there is a drop, and production remains almost unchanged during November and December at 140000.</t>
+          <t>the following graph depicts the canadian production of oats in tonnes during 2018. in january approximately 160000 tonnes were produced, after which a sharp drop can be observed for february, reaching slightly below 100000. production remain mostly stable throughout march to may, with the lowest production coming up in july at 80000. production sharply increases during the following months, until it peaks in october at approximately 210000. following this there is a drop, and production remains almost unchanged during november and december at 140000.</t>
         </is>
       </c>
       <c r="V295" t="inlineStr">
         <is>
-          <t>The following graph depicts the Canadian TKN_About  in TKN_UOM  during  TKN_Year . In January approximately 60 TKN_UOM  were produced, after which a sharp drop can be observed for February, reaching slightly below 15. Production remain mostly stable throughout March to May, with the lowest production coming up in July at 0. Production sharply increases during the following months, until it peaks in October at approximately 97. Following this there is a drop, and production remains almost unchanged during November and December at 45.</t>
+          <t>the following graph depicts the canadian TKN_About  in TKN_UOM  during  TKN_Year . in january approximately 60 TKN_UOM  were produced, after which a sharp drop can be observed for february, reaching slightly below 15. production remain mostly stable throughout march to may, with the lowest production coming up in july at 0. production sharply increases during the following months, until it peaks in october at approximately 97. following this there is a drop, and production remains almost unchanged during november and december at 45.</t>
         </is>
       </c>
       <c r="W295" t="n">
@@ -25248,12 +25248,12 @@
       </c>
       <c r="U296" t="inlineStr">
         <is>
-          <t>The values about hardwood production in Canada have been strongly flactuating over the 2016. The most significant peak was recorded during June. At the same time, the lower value was during December.  It's also possible to see a huge drop of the production value between the months of June and July.</t>
+          <t>the values about hardwood production in canada have been strongly flactuating over the 2016. the most significant peak was recorded during june. at the same time, the lower value was during december.  it's also possible to see a huge drop of the production value between the months of june and july.</t>
         </is>
       </c>
       <c r="V296" t="inlineStr">
         <is>
-          <t>The values about TKN_About  in  TKN_Geo  have been strongly flactuating over the  TKN_Year . The most significant peak was recorded during June. At the same time, the lower value was during December.  It's also possible to see a huge drop of the production value between the months of June and July.</t>
+          <t>the values about TKN_About  in canada have been strongly flactuating over the  TKN_Year . the most significant peak was recorded during june. at the same time, the lower value was during december.  it's also possible to see a huge drop of the production value between the months of june and july.</t>
         </is>
       </c>
       <c r="W296" t="n">
@@ -25332,12 +25332,12 @@
       </c>
       <c r="U297" t="inlineStr">
         <is>
-          <t>This graph represents the production of wheat flour in Canada in 2017 (in tonnes). The lowest production is during January. There is a sharp increase during February and during the following months production levels off between 29000 and 32500. A decrease can be observed in August. For the following 2 months production of wheat flour remains steady at approximately 30000. After a drop in November, production peaks in December with up to 40000 tonnes.</t>
+          <t>this graph represents the production of wheat flour in canada in 2017 (in tonnes). the lowest production is during january. there is a sharp increase during february and during the following months production levels off between 29000 and 32500. a decrease can be observed in august. for the following 2 months production of wheat flour remains steady at approximately 30000. after a drop in november, production peaks in december with up to 40000 tonnes.</t>
         </is>
       </c>
       <c r="V297" t="inlineStr">
         <is>
-          <t>This graph represents the TKN_About  in  TKN_Geo  in  TKN_Year  (in tonnes). The lowest production is during January. There is a sharp increase during February and during the following months production levels off between 42 and 61. A decrease can be observed in August. For the following 2 months TKN_About  remains steady at approximately 47. After a drop in November, production peaks in December with up to 101 tonnes.</t>
+          <t>this graph represents the TKN_About  in canada in  TKN_Year  (in tonnes). the lowest production is during january. there is a sharp increase during february and during the following months production levels off between 42 and 61. a decrease can be observed in august. for the following 2 months TKN_About  remains steady at approximately 47. after a drop in november, production peaks in december with up to 101 tonnes.</t>
         </is>
       </c>
       <c r="W297" t="n">
@@ -25416,12 +25416,12 @@
       </c>
       <c r="U298" t="inlineStr">
         <is>
-          <t>The shown data values are about the production of Eggs in shell in Canada during 2016. They are described using the farm product price index (FPPI). The values slightly increased from January to February. After that, from February over it steeply declined until reaching the minimum value of the year in July. Then, the production value started to rise again until the end of the year. During the last three months the value remained quite stable.</t>
+          <t>the shown data values are about the production of eggs in shell in canada during 2016. they are described using the farm product price index (fppi). the values slightly increased from january to february. after that, from february over it steeply declined until reaching the minimum value of the year in july. then, the production value started to rise again until the end of the year. during the last three months the value remained quite stable.</t>
         </is>
       </c>
       <c r="V298" t="inlineStr">
         <is>
-          <t>The shown data values are about the TKN_About  in  TKN_Geo  during  TKN_Year . They are described using TKN_UOM  (FPPI). The values slightly increased from January to February. After that, from February over it steeply declined until reaching the minimum value of the year in July. Then, the production value started to rise again until the end of the year. During the last three months the value remained quite stable.</t>
+          <t>the shown data values are about the TKN_About  in canada during  TKN_Year . they are described using TKN_UOM  (fppi). the values slightly increased from january to february. after that, from february over it steeply declined until reaching the minimum value of the year in july. then, the production value started to rise again until the end of the year. during the last three months the value remained quite stable.</t>
         </is>
       </c>
       <c r="W298" t="n">
@@ -25500,12 +25500,12 @@
       </c>
       <c r="U299" t="inlineStr">
         <is>
-          <t>This figure represents the production of Canola in Canada during 2016. The unit given is tonnes. In January production lies at approximately 780000 tonnes. During the following 2 months the production increases. From March until August the production fluctuates until reaching the minimum during August with 580000. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 1130000 tonnes.</t>
+          <t>this figure represents the production of canola in canada during 2016. the unit given is tonnes. in january production lies at approximately 780000 tonnes. during the following 2 months the production increases. from march until august the production fluctuates until reaching the minimum during august with 580000. production sharply increases throughout the months august to december, reaching its peak at the end of the year with approximately 1130000 tonnes.</t>
         </is>
       </c>
       <c r="V299" t="inlineStr">
         <is>
-          <t>This figure represents the TKN_About  in  TKN_Geo  during  TKN_Year . The unit given is tonnes. In January production lies at approximately 38 tonnes. During the following 2 months the production increases. From March until August the production fluctuates until reaching the minimum during August with 2. Production sharply increases throughout the months August to December, reaching its peak at the end of the year with approximately 100 tonnes.</t>
+          <t>this figure represents the TKN_About  in canada during  TKN_Year . the unit given is tonnes. in january production lies at approximately 38 tonnes. during the following 2 months the production increases. from march until august the production fluctuates until reaching the minimum during august with 2. production sharply increases throughout the months august to december, reaching its peak at the end of the year with approximately 100 tonnes.</t>
         </is>
       </c>
       <c r="W299" t="n">
@@ -25584,12 +25584,12 @@
       </c>
       <c r="U300" t="inlineStr">
         <is>
-          <t>The number of canadian vehicles returning to the country during 2017 registered the highest values during the summer months. In particular, the maximum number was recorded during August 2017. At the same time, the lowest value of the year was during the month of February. During the last few months of the year the number of vehicles returning to the country slowly decreased.</t>
+          <t>the number of canadian vehicles returning to the country during 2017 registered the highest values during the summer months. in particular, the maximum number was recorded during august 2017. at the same time, the lowest value of the year was during the month of february. during the last few months of the year the number of vehicles returning to the country slowly decreased.</t>
         </is>
       </c>
       <c r="V300" t="inlineStr">
         <is>
-          <t>The TKN_UOM  of TKN_About  during  TKN_Year  registered the highest values during the summer months. In particular, the maximum TKN_UOM  was recorded during August  TKN_Year . At the same time, the lowest value of the year was during the month of February. During the last few months of the year the TKN_UOM  of vehicles returning to the country slowly decreased.</t>
+          <t>the TKN_UOM  of TKN_About  during  TKN_Year  registered the highest values during the summer months. in particular, the maximum TKN_UOM  was recorded during august  TKN_Year . at the same time, the lowest value of the year was during the month of february. during the last few months of the year the TKN_UOM  of vehicles returning to the country slowly decreased.</t>
         </is>
       </c>
       <c r="W300" t="n">
@@ -25668,12 +25668,12 @@
       </c>
       <c r="U301" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how the house and land price index in Canada has been slowly but constantly increasing over 2016. It presented few fluactuations, but none of them are significant.</t>
+          <t>it's clearly possible to see how the house and land price index in canada has been slowly but constantly increasing over 2016. it presented few fluactuations, but none of them are significant.</t>
         </is>
       </c>
       <c r="V301" t="inlineStr">
         <is>
-          <t>It's clearly possible to see how TKN_About  TKN_UOM  in  TKN_Geo  has been slowly but constantly increasing over  TKN_Year . It presented few fluactuations, but none of them are significant.</t>
+          <t>it's clearly possible to see how TKN_About  TKN_UOM  in canada has been slowly but constantly increasing over  TKN_Year . it presented few fluactuations, but none of them are significant.</t>
         </is>
       </c>
       <c r="W301" t="n">
@@ -25752,12 +25752,12 @@
       </c>
       <c r="U302" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian supply of creamery butter (in tonnes) during 2016. The lowest value can be observed in January with 21000 tonnes. Supply increases during February, remains almost unchanged throughout March and sharply increases during the following months until it reaches its peak in July with 29000 tonnes. There is a sharp decline in supply of creamery butter from July until September. The supply remains stable during October and experiences a small rise during November.</t>
+          <t>this graph represents the canadian supply of creamery butter (in tonnes) during 2016. the lowest value can be observed in january with 21000 tonnes. supply increases during february, remains almost unchanged throughout march and sharply increases during the following months until it reaches its peak in july with 29000 tonnes. there is a sharp decline in supply of creamery butter from july until september. the supply remains stable during october and experiences a small rise during november.</t>
         </is>
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>This graph represents the Canadian TKN_About  (in tonnes) during  TKN_Year . The lowest value can be observed in January with 1 tonnes. Supply increases during February, remains almost unchanged throughout March and sharply increases during the following months until it reaches its peak in July with 101 tonnes. There is a sharp decline in TKN_About  from July until September. The supply remains stable during October and experiences a small rise during November.</t>
+          <t>this graph represents the canadian TKN_About  (in tonnes) during  TKN_Year . the lowest value can be observed in january with 1 tonnes. supply increases during february, remains almost unchanged throughout march and sharply increases during the following months until it reaches its peak in july with 101 tonnes. there is a sharp decline in TKN_About  from july until september. the supply remains stable during october and experiences a small rise during november.</t>
         </is>
       </c>
       <c r="W302" t="n">
@@ -25836,12 +25836,12 @@
       </c>
       <c r="U303" t="inlineStr">
         <is>
-          <t>The production of creamery butter in Canada reported a not homogeneous trend over 2018. The maximum value was recorded during January. After that, several oscillations have been recorded over the year. In particular, a big drop was recorded between the months of April and June. The value keep fluactuating over the last few months of the year.</t>
+          <t>the production of creamery butter in canada reported a not homogeneous trend over 2018. the maximum value was recorded during january. after that, several oscillations have been recorded over the year. in particular, a big drop was recorded between the months of april and june. the value keep fluactuating over the last few months of the year.</t>
         </is>
       </c>
       <c r="V303" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  reported a not homogeneous trend over  TKN_Year . The maximum value was recorded during January. After that, several oscillations have been recorded over the year. In particular, a big drop was recorded between the months of April and June. The value keep fluactuating over the last few months of the year.</t>
+          <t>the TKN_About  in canada reported a not homogeneous trend over  TKN_Year . the maximum value was recorded during january. after that, several oscillations have been recorded over the year. in particular, a big drop was recorded between the months of april and june. the value keep fluactuating over the last few months of the year.</t>
         </is>
       </c>
       <c r="W303" t="n">
@@ -25920,12 +25920,12 @@
       </c>
       <c r="U304" t="inlineStr">
         <is>
-          <t>The production of rye in Canada during 2018 is represented in the following graph. The unit given is tonnes. Production remains mainly stable throughout January to March at approximately 13000 tonnes. There is a small increase during April and May, followed by a minor decline during June and July. The maximum production of rye takes place during August with approximately 42000 tonnes. From August to December the production drastically decreases until it reaches its minimum of 7000 in December.</t>
+          <t>the production of rye in canada during 2018 is represented in the following graph. the unit given is tonnes. production remains mainly stable throughout january to march at approximately 13000 tonnes. there is a small increase during april and may, followed by a minor decline during june and july. the maximum production of rye takes place during august with approximately 42000 tonnes. from august to december the production drastically decreases until it reaches its minimum of 7000 in december.</t>
         </is>
       </c>
       <c r="V304" t="inlineStr">
         <is>
-          <t>The TKN_About  in  TKN_Geo  during  TKN_Year  is represented in the following graph. The unit given is tonnes. Production remains mainly stable throughout January to March at approximately 16 tonnes. There is a small increase during April and May, followed by a minor decline during June and July. The maximum TKN_About  takes place during August with approximately 101 tonnes. From August to December the production drastically decreases until it reaches its minimum of -1 in December.</t>
+          <t>the TKN_About  in canada during  TKN_Year  is represented in the following graph. the unit given is tonnes. production remains mainly stable throughout january to march at approximately 16 tonnes. there is a small increase during april and may, followed by a minor decline during june and july. the maximum TKN_About  takes place during august with approximately 101 tonnes. from august to december the production drastically decreases until it reaches its minimum of -1 in december.</t>
         </is>
       </c>
       <c r="W304" t="n">
@@ -26004,12 +26004,12 @@
       </c>
       <c r="U305" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the production of unprocessed milk in Canada reported two significant peaks during 2017, one in February and one in October. Futhermore, from February to July the production value strongly decrease, reaching the yearly minimum value during July. It's clearly possible to see how the summer months are the period with the least production of unprocessed milk.</t>
+          <t>as it's possible to see from the graph, the production of unprocessed milk in canada reported two significant peaks during 2017, one in february and one in october. futhermore, from february to july the production value strongly decrease, reaching the yearly minimum value during july. it's clearly possible to see how the summer months are the period with the least production of unprocessed milk.</t>
         </is>
       </c>
       <c r="V305" t="inlineStr">
         <is>
-          <t>As it's possible to see from the graph, the TKN_About  in  TKN_Geo  reported two significant peaks during  TKN_Year , one in February and one in October. Futhermore, from February to July the production value strongly decrease, reaching the yearly minimum value during July. It's clearly possible to see how the summer months are the period with the least TKN_About .</t>
+          <t>as it's possible to see from the graph, the TKN_About  in canada reported two significant peaks during  TKN_Year , one in february and one in october. futhermore, from february to july the production value strongly decrease, reaching the yearly minimum value during july. it's clearly possible to see how the summer months are the period with the least TKN_About .</t>
         </is>
       </c>
       <c r="W305" t="n">
@@ -26088,12 +26088,12 @@
       </c>
       <c r="U306" t="inlineStr">
         <is>
-          <t>The shown data are about the total farm production index in Canada during 2016. The maximum value was recorded during the month of June. After that, a big drop has been registered between June and September. During the last few months of the year the production value slightly increased.</t>
+          <t>the shown data are about the total farm production index in canada during 2016. the maximum value was recorded during the month of june. after that, a big drop has been registered between june and september. during the last few months of the year the production value slightly increased.</t>
         </is>
       </c>
       <c r="V306" t="inlineStr">
         <is>
-          <t>The shown data are about TKN_UOM  in  TKN_Geo  during  TKN_Year . The maximum value was recorded during the month of June. After that, a big drop has been registered between June and September. During the last few months of the TKN_About  value slightly increased.</t>
+          <t>the shown data are about TKN_UOM  in canada during  TKN_Year . the maximum value was recorded during the month of june. after that, a big drop has been registered between june and september. during the last few months of the TKN_About  value slightly increased.</t>
         </is>
       </c>
       <c r="W306" t="n">
@@ -26172,12 +26172,12 @@
       </c>
       <c r="U307" t="inlineStr">
         <is>
-          <t>The value about softwood and hardwoock stocks in Canada rapidly increased during the first months of 2016. After that, a considerable drop was recorded between the months of May and July. During the last months of the year the softwood and hardwood stocks slowly declined. The minimum value has been reached during the month of December.</t>
+          <t>the value about softwood and hardwoock stocks in canada rapidly increased during the first months of 2016. after that, a considerable drop was recorded between the months of may and july. during the last months of the year the softwood and hardwood stocks slowly declined. the minimum value has been reached during the month of december.</t>
         </is>
       </c>
       <c r="V307" t="inlineStr">
         <is>
-          <t>The value about TKN_About  in  TKN_Geo  rapidly increased during the first months of  TKN_Year . After that, a considerable drop was recorded between the months of May and July. During the last months of the year the softwood and hardwood stocks slowly declined. The minimum value has been reached during the month of December.</t>
+          <t>the value about TKN_About  in canada rapidly increased during the first months of  TKN_Year . after that, a considerable drop was recorded between the months of may and july. during the last months of the year the softwood and hardwood stocks slowly declined. the minimum value has been reached during the month of december.</t>
         </is>
       </c>
       <c r="W307" t="n">

</xml_diff>

<commit_message>
Updated the folder's structure
</commit_message>
<xml_diff>
--- a/Dataset/Captions collection/final_captions_collection.xlsx
+++ b/Dataset/Captions collection/final_captions_collection.xlsx
@@ -2741,7 +2741,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>the following graph is about the TKN_About  in canada during  TKN_Year ; the values are in tonnes. it shows a clearly growth from january over, reaching its maximum value during october. then it's possible to see a significant drop from october to november.</t>
+          <t>the following graph is about the TKN_About  in canada during  TKN_Year ; the values are in TKN_UOM . it shows a clearly growth from january over, reaching its maximum value during october. then it's possible to see a significant drop from october to november.</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>the following line chart is about the TKN_About  in canada during  TKN_Year . the values are reported in tonnes. it shows how the production is actually falling down from january to august, when it reaches its minimum. from september to december the values are slowly rising up.</t>
+          <t>the following line chart is about the TKN_About  in canada during  TKN_Year . the values are reported in TKN_UOM . it shows how the production is actually falling down from january to august, when it reaches its minimum. from september to december the values are slowly rising up.</t>
         </is>
       </c>
       <c r="W29" t="n">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>the graph shows the TKN_About  in canada in the year of  TKN_Year . there is one data entry for each month of the year. production is measured TKN_UOM  index. the x-axis shows the months, the y-axis the index ranging from 4 to 100. there is a high in may (index of 100) and a low in february (a bit below 4).</t>
+          <t>the graph shows the TKN_About  in canada in the year of  TKN_Year . there is one data entry for each month of the year. production is measured by TKN_UOM . the x-axis shows the months, the y-axis the index ranging from 4 to 100. there is a high in may (index of 100) and a low in february (a bit below 4).</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>the line chart illustrates the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it's clearly possible to see two main peaks over the year, one during february and one during october. at the same time, during the summer the production significantly decreased, reaching its minimum value during the month of july.</t>
+          <t>the line chart illustrates the TKN_About  in canada during  TKN_Year . the values are described using the TKN_UOM . it's clearly possible to see two main peaks over the year, one during february and one during october. at the same time, during the summer the production significantly decreased, reaching its minimum value during the month of july.</t>
         </is>
       </c>
       <c r="W38" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>the chart is showing the values about the TKN_About  in canada during  TKN_Year . the values are illustrated using TKN_UOM  (fppi). as can be seen from the graph, from january to may the values have been rapidly decreasing. then, a peak has been recorded during the month of june, but after that the values started to decrease again until october. during the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of december.</t>
+          <t>the chart is showing the values about the TKN_About  in canada during  TKN_Year . the values are illustrated using the TKN_UOM . as can be seen from the graph, from january to may the values have been rapidly decreasing. then, a peak has been recorded during the month of june, but after that the values started to decrease again until october. during the last two months of the year the production significantly jumped up, reaching the maximum value of the year during the month of december.</t>
         </is>
       </c>
       <c r="W49" t="n">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>the graph illustrated the TKN_About  in canada in  TKN_Year . the measurement used is TKN_UOM  (fppi): there is a clear peak in august, reaching an index of more than 96.</t>
+          <t>the graph illustrated the TKN_About  in canada in  TKN_Year . the measurement used is the TKN_UOM : there is a clear peak in august, reaching an index of more than 96.</t>
         </is>
       </c>
       <c r="W59" t="n">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>in this graph, the TKN_About  in canada is illustrated. the x-axis shows the months of the year of  TKN_Year , whereas the y-axis depicts the production in tonnes. values in august and september stand out, reaching almost 102 in september. during the remaining months of the year, production is comparably lower.</t>
+          <t>in this graph, the TKN_About  in canada is illustrated. the x-axis shows the months of the year of  TKN_Year , whereas the y-axis depicts the production in TKN_UOM . values in august and september stand out, reaching almost 102 in september. during the remaining months of the year, production is comparably lower.</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>the shown line chart provides information about the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it's clearly possible to see two significant peaks during the months of march and august. then the overall value of production remain quite stable during the year.</t>
+          <t>the shown line chart provides information about the TKN_About  in canada during  TKN_Year . the values are described using the TKN_UOM . it's clearly possible to see two significant peaks during the months of march and august. then the overall value of production remain quite stable during the year.</t>
         </is>
       </c>
       <c r="W67" t="n">
@@ -6101,7 +6101,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>this graph shows the TKN_About  and poults, measured TKN_UOM  index. the recorded data is from canada,  TKN_Year . the graph's line reaches its high in october, with an index of 100. the decline in the following month stands out, resulting in an index of 0 in november and december.</t>
+          <t>this graph shows the TKN_About  and poults, measured by TKN_UOM . the recorded data is from canada,  TKN_Year . the graph's line reaches its high in october, with an index of 100. the decline in the following month stands out, resulting in an index of 0 in november and december.</t>
         </is>
       </c>
       <c r="W68" t="n">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>the line chart is describing the values about TKN_About  in canada during  TKN_Year . the production amout is described using TKN_UOM  (fppi). the minimum recorded value is during february. the maximum recorded value is during august. furthermore, there are several fluctuations over the year.</t>
+          <t>the line chart is describing the values about TKN_About  in canada during  TKN_Year . the production amout is described using the TKN_UOM . the minimum recorded value is during february. the maximum recorded value is during august. furthermore, there are several fluctuations over the year.</t>
         </is>
       </c>
       <c r="W74" t="n">
@@ -6941,7 +6941,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>the graph describes the TKN_About  in canada during  TKN_Year . the production value is described using TKN_UOM  (fppi). as it can be seen from the graph, the production rapidly increased from january until august. after that, from august to december the production slightly decreased. the maximum value has been registered in august and the minimum one during february.</t>
+          <t>the graph describes the TKN_About  in canada during  TKN_Year . the production value is described using the TKN_UOM . as it can be seen from the graph, the production rapidly increased from january until august. after that, from august to december the production slightly decreased. the maximum value has been registered in august and the minimum one during february.</t>
         </is>
       </c>
       <c r="W78" t="n">
@@ -7025,7 +7025,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>the following line chart is decribing the trend of the TKN_About  in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). it can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. the most significant peak was recorded during the month of july  TKN_Year . the lowest values have been recorded during the months of september and december.</t>
+          <t>the following line chart is decribing the trend of the TKN_About  in canada during  TKN_Year . the values are described using the TKN_UOM . it can be seen from the graph that the values are frequently fluctuating over the year, showing several peaks and dips. the most significant peak was recorded during the month of july  TKN_Year . the lowest values have been recorded during the months of september and december.</t>
         </is>
       </c>
       <c r="W79" t="n">
@@ -8705,7 +8705,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>this line chart illustrates the TKN_About  (in tonnes) of canada in  TKN_Year . production starts very low in january at approximately 0 tonnes. from there on production starts oscillating a lot, having a peak during february, a low in march and reaching the maximum during april. there is a sharp decline from april until may, after which production starts fluctuating again until september. there is a rapid jump in october reaching almost 95 tonnes. a very slight increase can be observed for november, after which the production drops in december.</t>
+          <t>this line chart illustrates the TKN_About  (in TKN_UOM ) of canada in  TKN_Year . production starts very low in january at approximately 0 TKN_UOM . from there on production starts oscillating a lot, having a peak during february, a low in march and reaching the maximum during april. there is a sharp decline from april until may, after which production starts fluctuating again until september. there is a rapid jump in october reaching almost 95 TKN_UOM . a very slight increase can be observed for november, after which the production drops in december.</t>
         </is>
       </c>
       <c r="W99" t="n">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>the graph shows the TKN_About  value in canada during  TKN_Year . the values are described using TKN_UOM  (fppi). the products index shown several fluctuations. in particular, it's clearly possible to see several peaks and dips. in february, july and october the value reached its maximum values. during april and september the value reached its minimum values.</t>
+          <t>the graph shows the TKN_About  value in canada during  TKN_Year . the values are described using the TKN_UOM . the products index shown several fluctuations. in particular, it's clearly possible to see several peaks and dips. in february, july and october the value reached its maximum values. during april and september the value reached its minimum values.</t>
         </is>
       </c>
       <c r="W105" t="n">
@@ -9293,7 +9293,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>the data presented in the graph shows the TKN_About  in canada over the year of  TKN_Year  in tonnes. the lowest TKN_About  can be observed in january. the supply increases constantly over the next months and reaches its highest value in june, after which it decreases with a similar rate and reaches a local minimum in september.</t>
+          <t>the data presented in the graph shows the TKN_About  in canada over the year of  TKN_Year  in TKN_UOM . the lowest TKN_About  can be observed in january. the supply increases constantly over the next months and reaches its highest value in june, after which it decreases with a similar rate and reaches a local minimum in september.</t>
         </is>
       </c>
       <c r="W106" t="n">
@@ -10721,7 +10721,7 @@
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>the following line chart describes the TKN_About  hardwood in canada during  TKN_Year . the unit of measurement of the data TKN_UOM  metres. the production showed several peaks during the year, mainly during march, june and november. furthermore, a significant drop has been recorded between the months of june and july.</t>
+          <t>the following line chart describes the TKN_About  hardwood in canada during  TKN_Year . the unit of measurement of the data is TKN_UOM . the production showed several peaks during the year, mainly during march, june and november. furthermore, a significant drop has been recorded between the months of june and july.</t>
         </is>
       </c>
       <c r="W123" t="n">
@@ -10805,7 +10805,7 @@
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>as it's shown in the graph, the production value of what flour in canada during  TKN_Year  has been strongly fluctuating. the unit of measurement is tonnes. the graph shows several peaks, but the maximum values have been recorded during the months of april, octoeber and november. at the same time, the months with less TKN_About  have been january and july.</t>
+          <t>as it's shown in the graph, the production value of what flour in canada during  TKN_Year  has been strongly fluctuating. the unit of measurement is TKN_UOM . the graph shows several peaks, but the maximum values have been recorded during the months of april, octoeber and november. at the same time, the months with less TKN_About  have been january and july.</t>
         </is>
       </c>
       <c r="W124" t="n">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>this line graph displays the TKN_About  in canada for  TKN_Year  TKN_UOM  index.  a small decrease from january to february is followed by a steady increase until october, where the value again decreases for november and december.</t>
+          <t>this line graph displays the TKN_About  in canada for  TKN_Year  using TKN_UOM .  a small decrease from january to february is followed by a steady increase until october, where the value again decreases for november and december.</t>
         </is>
       </c>
       <c r="W127" t="n">
@@ -11141,7 +11141,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>this line graph displays the TKN_About  in canada for  TKN_Year  TKN_UOM  index.  a slow but steady increase is observed from january to june, where a steep increase is seen from june to august.  a steep decrease follows from august to october, where the value again rises steadily from october to december.</t>
+          <t>this line graph displays the TKN_About  in canada for  TKN_Year  using TKN_UOM .  a slow but steady increase is observed from january to june, where a steep increase is seen from june to august.  a steep decrease follows from august to october, where the value again rises steadily from october to december.</t>
         </is>
       </c>
       <c r="W128" t="n">
@@ -13073,7 +13073,7 @@
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>the following line chart is about the TKN_About  hardwood in canada during  TKN_Year . the described values are TKN_UOM  metres. it's clearly possible to see how the production fluctuated over the year, with several peaks and dips. but at the end of the year, betwewen november and december, has been registered a significant drop of the value.</t>
+          <t>the following line chart is about the TKN_About  hardwood in canada during  TKN_Year . the described values are in TKN_UOM . it's clearly possible to see how the production fluctuated over the year, with several peaks and dips. but at the end of the year, betwewen november and december, has been registered a significant drop of the value.</t>
         </is>
       </c>
       <c r="W151" t="n">
@@ -17189,7 +17189,7 @@
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>the graph illustrates the TKN_About  in canada in the year  TKN_Year . the production is very low in the first third of the year, before it rises sharply until october, reaching a maximum of 100 tonnes. then the production decrease again for the remaining months of the year.</t>
+          <t>the graph illustrates the TKN_About  in canada in the year  TKN_Year . the production is very low in the first third of the year, before it rises sharply until october, reaching a maximum of 100 TKN_UOM . then the production decrease again for the remaining months of the year.</t>
         </is>
       </c>
       <c r="W200" t="n">
@@ -17609,7 +17609,7 @@
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>it shows the data about TKN_About  in canada during  TKN_Year . the displayed values are in tones. it's possible to see how the value rapidly increase from january over, reaching its peaks during the month of july with approximately 101 tonnes. after that, the values decrease until september and then rise up again during last 3 months of the year.</t>
+          <t>it shows the data about TKN_About  in canada during  TKN_Year . the displayed values are in tones. it's possible to see how the value rapidly increase from january over, reaching its peaks during the month of july with approximately 101 TKN_UOM . after that, the values decrease until september and then rise up again during last 3 months of the year.</t>
         </is>
       </c>
       <c r="W205" t="n">
@@ -18281,7 +18281,7 @@
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>the graph shows the TKN_About  over the year of  TKN_Year . the graph stayed in the range of about 2 and 94 tonnes. it has a zig-zag waveform from january to august, before a last peak in september and then decreasing in the last quarter of the year.</t>
+          <t>the graph shows the TKN_About  over the year of  TKN_Year . the graph stayed in the range of about 2 and 94 TKN_UOM . it has a zig-zag waveform from january to august, before a last peak in september and then decreasing in the last quarter of the year.</t>
         </is>
       </c>
       <c r="W213" t="n">
@@ -18701,7 +18701,7 @@
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>the graph is showing the production's trend TKN_About  hardwood in canada during  TKN_Year . the values are TKN_UOM  metres. it's clearly possible to see how the values are strongly fluctuating over the year. there are several peaks, in particular during march, may and novembe. at the same time, the minimum values have been recorded during the months of january, july and august.</t>
+          <t>the graph is showing the production's trend TKN_About  hardwood in canada during  TKN_Year . the values are in TKN_UOM . it's clearly possible to see how the values are strongly fluctuating over the year. there are several peaks, in particular during march, may and novembe. at the same time, the minimum values have been recorded during the months of january, july and august.</t>
         </is>
       </c>
       <c r="W218" t="n">
@@ -18785,7 +18785,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>the following graph is showing the recorded values about TKN_About  in canada during  TKN_Year . the values have been reported using TKN_UOM  (fppi). as it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of august. after the summer, the production value drop, reaching its minimum value in october.</t>
+          <t>the following graph is showing the recorded values about TKN_About  in canada during  TKN_Year . the values have been reported using the TKN_UOM . as it is shown, the production slightly increase during the first half of the year, but then it rapidly grow during the summer months, reaching its maximum value during the month of august. after the summer, the production value drop, reaching its minimum value in october.</t>
         </is>
       </c>
       <c r="W219" t="n">
@@ -19709,7 +19709,7 @@
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>the TKN_About  in canada in  TKN_Year  rose sharply until may, from 2 to 100 units. then it started decreasing, reaching the same january level of 2 in december, at the end of the year.</t>
+          <t>the TKN_About  in canada in  TKN_Year  rose sharply until may, from 2 to 100 TKN_UOM . then it started decreasing, reaching the same january level of 2 in december, at the end of the year.</t>
         </is>
       </c>
       <c r="W230" t="n">
@@ -19793,7 +19793,7 @@
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>production of fresh vegetables for  TKN_Year  in whole canada, represented TKN_UOM  index. it can be seen, that the production rises in the months from february until october and then drops.</t>
+          <t>production of fresh vegetables for  TKN_Year  in whole canada, represented by TKN_UOM . it can be seen, that the production rises in the months from february until october and then drops.</t>
         </is>
       </c>
       <c r="W231" t="n">
@@ -19961,7 +19961,7 @@
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>this is a line graph showing the total  TKN_Year  imports TKN_About  to canada in tonnes. the graph has significant fluctuations between each month. there is a substantial spike in june, which was the peak month at over 97 tonnes. there is also a clear dip in september, which was the lowest month at under 4 tonnes.</t>
+          <t>this is a line graph showing the total  TKN_Year  imports TKN_About  to canada in TKN_UOM . the graph has significant fluctuations between each month. there is a substantial spike in june, which was the peak month at over 97 TKN_UOM . there is also a clear dip in september, which was the lowest month at under 4 TKN_UOM .</t>
         </is>
       </c>
       <c r="W233" t="n">
@@ -20969,7 +20969,7 @@
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>the graph is showing the trend about TKN_About  in canada during  TKN_Year . the values are illustrated using TKN_UOM  (fppi). the values have been fluactuating over the year, with several dips and peaks. the maximum value was in october  TKN_Year . during the last two months of the year, nov and dec, was recorded the minimum production of the  TKN_Year .</t>
+          <t>the graph is showing the trend about TKN_About  in canada during  TKN_Year . the values are illustrated using the TKN_UOM . the values have been fluactuating over the year, with several dips and peaks. the maximum value was in october  TKN_Year . during the last two months of the year, nov and dec, was recorded the minimum production of the  TKN_Year .</t>
         </is>
       </c>
       <c r="W245" t="n">
@@ -21221,7 +21221,7 @@
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>as it's possible to see, the following graph is about the TKN_About  in canada during  TKN_Year . the values are reported using TKN_UOM  (fppi). the production slightly increase over the first half of the year, so from january until july. after that, it has been recorded a significant jump of the values between july and august. during the last few months of the year it remained steady.</t>
+          <t>as it's possible to see, the following graph is about the TKN_About  in canada during  TKN_Year . the values are reported using the TKN_UOM . the production slightly increase over the first half of the year, so from january until july. after that, it has been recorded a significant jump of the values between july and august. during the last few months of the year it remained steady.</t>
         </is>
       </c>
       <c r="W248" t="n">
@@ -22481,7 +22481,7 @@
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>the TKN_About  in canada of  TKN_Year  is shown in this figure. the unit given is dollars. production shows its lowest value in january. following this production experiences a sharp increase, until reaching its maximum in may. production gradually decreases from may until july, plateauing from july until september. there is a steady decline from september until december.</t>
+          <t>the TKN_About  in canada of  TKN_Year  is shown in this figure. the unit given is TKN_UOM . production shows its lowest value in january. following this production experiences a sharp increase, until reaching its maximum in may. production gradually decreases from may until july, plateauing from july until september. there is a steady decline from september until december.</t>
         </is>
       </c>
       <c r="W263" t="n">
@@ -22901,7 +22901,7 @@
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>this figure shows the canadian TKN_About  of  TKN_Year . production is measured in tonnes. production is the lowest during the month of january at approximately 0. there is a sharp increase for february, reaching 59 tonnes, after which a drop is experienced during march. the maximum TKN_About  is taking place in april at above 100 tonnes. production is rather low during may. during the following months production fluctuates until a sharp increase in observed for october, reaching nearly 95 tonnes. production remains nearly steady throughout november and drops back to 50 during december.</t>
+          <t>this figure shows the canadian TKN_About  of  TKN_Year . production is measured in TKN_UOM . production is the lowest during the month of january at approximately 0. there is a sharp increase for february, reaching 59 TKN_UOM , after which a drop is experienced during march. the maximum TKN_About  is taking place in april at above 100 TKN_UOM . production is rather low during may. during the following months production fluctuates until a sharp increase in observed for october, reaching nearly 95 TKN_UOM . production remains nearly steady throughout november and drops back to 50 during december.</t>
         </is>
       </c>
       <c r="W268" t="n">
@@ -22985,7 +22985,7 @@
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>this graph depicts the TKN_About  of  TKN_Year . the unit used TKN_UOM  metres. production during january lies at approximately 61 and experiences an increase until reaching the maximum value in march at above 99. from then production slowly declines until june, after which a sharp drop can be observed in july at approximately 34. from july until november production levels increase again, reaching a value of nearly 98. there is a rapid decline of production in december, which marks the lowest production of the year at -2 cubic metres.</t>
+          <t>this graph depicts the TKN_About  of  TKN_Year . the unit used is TKN_UOM . production during january lies at approximately 61 and experiences an increase until reaching the maximum value in march at above 99. from then production slowly declines until june, after which a sharp drop can be observed in july at approximately 34. from july until november production levels increase again, reaching a value of nearly 98. there is a rapid decline of production in december, which marks the lowest production of the year at -2 TKN_UOM .</t>
         </is>
       </c>
       <c r="W269" t="n">
@@ -23405,7 +23405,7 @@
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>total canadian livestock and animal products in  TKN_Year  are shown in this graph. the unit given is TKN_UOM  (fppi). during january products lie at 63 and the second highes value of the year can be observed in february at approximately 76. there is a sharp decline from february onwards, reaching a low of 1 in april. during the following months there is a steep rise, reaching the maximum of 99 in july. again, a huge decrease follows until reaching the lowest value in september, which is followed by a significant rise for october. following this, a rapid drop can be observed until december.</t>
+          <t>total canadian livestock and animal products in  TKN_Year  are shown in this graph. the unit given is the TKN_UOM . during january products lie at 63 and the second highes value of the year can be observed in february at approximately 76. there is a sharp decline from february onwards, reaching a low of 1 in april. during the following months there is a steep rise, reaching the maximum of 99 in july. again, a huge decrease follows until reaching the lowest value in september, which is followed by a significant rise for october. following this, a rapid drop can be observed until december.</t>
         </is>
       </c>
       <c r="W274" t="n">
@@ -23657,7 +23657,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the given unit is TKN_UOM  (fppi). the graph represents a parable throughout the year. it starts at 34 during january, after which a steady decline can be observed, reaching the lowest production value in june at 0. during the following months production rapidly increases until the maximum is reached in november at approximately 100. there is a small decrease in december.</t>
+          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the given unit is the TKN_UOM . the graph represents a parable throughout the year. it starts at 34 during january, after which a steady decline can be observed, reaching the lowest production value in june at 0. during the following months production rapidly increases until the maximum is reached in november at approximately 100. there is a small decrease in december.</t>
         </is>
       </c>
       <c r="W277" t="n">
@@ -23741,7 +23741,7 @@
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>this graph illustrates values about the TKN_About  in canada during  TKN_Year . those values are described using TKN_UOM  (fppi). it's clearly possible to see how the maximum values of production are registered during the summer months. in particular, the highest production value was during july  TKN_Year . at the same time, the lowest one was in december.</t>
+          <t>this graph illustrates values about the TKN_About  in canada during  TKN_Year . those values are described using the TKN_UOM . it's clearly possible to see how the maximum values of production are registered during the summer months. in particular, the highest production value was during july  TKN_Year . at the same time, the lowest one was in december.</t>
         </is>
       </c>
       <c r="W278" t="n">
@@ -23825,7 +23825,7 @@
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>this figure represents the canadian TKN_About  during  TKN_Year . the given unit are tonnes. production remains mostly stable throughout the months of january until may, around 3 to 17 tonnes. following this there is a sharp increase in june, with the production plateauing throughout august at approximately 65 tonnes. the highest production can be observed during october with nearly 100. rye production experiences a sharp drop in november, reaching around 13 tonnes. there is a minimal increase during december.</t>
+          <t>this figure represents the canadian TKN_About  during  TKN_Year . the given unit are TKN_UOM . production remains mostly stable throughout the months of january until may, around 3 to 17 TKN_UOM . following this there is a sharp increase in june, with the production plateauing throughout august at approximately 65 TKN_UOM . the highest production can be observed during october with nearly 100. rye production experiences a sharp drop in november, reaching around 13 TKN_UOM . there is a minimal increase during december.</t>
         </is>
       </c>
       <c r="W279" t="n">
@@ -24077,7 +24077,7 @@
       </c>
       <c r="V282" t="inlineStr">
         <is>
-          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the unit TKN_UOM  (fppi). production starts off at approximately 11 in january and goes down to the lowest production at 0 during february. during the months of march and may the production remains unchanged at 33. there is a slight increase of production during june, until it remain stable throughout july until september at 56. then, a small drop can be observed, which is followed by a sharp increase, until it peaks during december at 100.</t>
+          <t>this graph depicts the TKN_About  in canada during  TKN_Year . the unit is TKN_UOM . production starts off at approximately 11 in january and goes down to the lowest production at 0 during february. during the months of march and may the production remains unchanged at 33. there is a slight increase of production during june, until it remain stable throughout july until september at 56. then, a small drop can be observed, which is followed by a sharp increase, until it peaks during december at 100.</t>
         </is>
       </c>
       <c r="W282" t="n">
@@ -24329,7 +24329,7 @@
       </c>
       <c r="V285" t="inlineStr">
         <is>
-          <t>this graph represents the canadian TKN_About  in  TKN_Year . the given unit are tonnes. production starts off at approximately 70 during january, after which a sharp decline is observed during february, reaching below 10. production fluctuates between march and june, after which a rapid decline takes place again, reaching the lowest production values of the year in august at -1. staying mostly constant in september, there is a significant rise peaking in october above 97. TKN_About  declines again during november, and hardly changes for december at around 42.</t>
+          <t>this graph represents the canadian TKN_About  in  TKN_Year . the given unit are TKN_UOM . production starts off at approximately 70 during january, after which a sharp decline is observed during february, reaching below 10. production fluctuates between march and june, after which a rapid decline takes place again, reaching the lowest production values of the year in august at -1. staying mostly constant in september, there is a significant rise peaking in october above 97. TKN_About  declines again during november, and hardly changes for december at around 42.</t>
         </is>
       </c>
       <c r="W285" t="n">
@@ -25421,7 +25421,7 @@
       </c>
       <c r="V298" t="inlineStr">
         <is>
-          <t>the shown data values are about the TKN_About  in canada during  TKN_Year . they are described using TKN_UOM  (fppi). the values slightly increased from january to february. after that, from february over it steeply declined until reaching the minimum value of the year in july. then, the production value started to rise again until the end of the year. during the last three months the value remained quite stable.</t>
+          <t>the shown data values are about the TKN_About  in canada during  TKN_Year . they are described using the TKN_UOM . the values slightly increased from january to february. after that, from february over it steeply declined until reaching the minimum value of the year in july. then, the production value started to rise again until the end of the year. during the last three months the value remained quite stable.</t>
         </is>
       </c>
       <c r="W298" t="n">
@@ -25505,7 +25505,7 @@
       </c>
       <c r="V299" t="inlineStr">
         <is>
-          <t>this figure represents the TKN_About  in canada during  TKN_Year . the unit given is tonnes. in january production lies at approximately 38 tonnes. during the following 2 months the production increases. from march until august the production fluctuates until reaching the minimum during august with 2. production sharply increases throughout the months august to december, reaching its peak at the end of the year with approximately 100 tonnes.</t>
+          <t>this figure represents the TKN_About  in canada during  TKN_Year . the unit given is TKN_UOM . in january production lies at approximately 38 TKN_UOM . during the following 2 months the production increases. from march until august the production fluctuates until reaching the minimum during august with 2. production sharply increases throughout the months august to december, reaching its peak at the end of the year with approximately 100 TKN_UOM .</t>
         </is>
       </c>
       <c r="W299" t="n">
@@ -25757,7 +25757,7 @@
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>this graph represents the canadian TKN_About  (in tonnes) during  TKN_Year . the lowest value can be observed in january with 1 tonnes. supply increases during february, remains almost unchanged throughout march and sharply increases during the following months until it reaches its peak in july with 101 tonnes. there is a sharp decline in TKN_About  from july until september. the supply remains stable during october and experiences a small rise during november.</t>
+          <t>this graph represents the canadian TKN_About  (in TKN_UOM ) during  TKN_Year . the lowest value can be observed in january with 1 TKN_UOM . supply increases during february, remains almost unchanged throughout march and sharply increases during the following months until it reaches its peak in july with 101 TKN_UOM . there is a sharp decline in TKN_About  from july until september. the supply remains stable during october and experiences a small rise during november.</t>
         </is>
       </c>
       <c r="W302" t="n">
@@ -25925,7 +25925,7 @@
       </c>
       <c r="V304" t="inlineStr">
         <is>
-          <t>the TKN_About  in canada during  TKN_Year  is represented in the following graph. the unit given is tonnes. production remains mainly stable throughout january to march at approximately 16 tonnes. there is a small increase during april and may, followed by a minor decline during june and july. the maximum TKN_About  takes place during august with approximately 101 tonnes. from august to december the production drastically decreases until it reaches its minimum of -1 in december.</t>
+          <t>the TKN_About  in canada during  TKN_Year  is represented in the following graph. the unit given is TKN_UOM . production remains mainly stable throughout january to march at approximately 16 TKN_UOM . there is a small increase during april and may, followed by a minor decline during june and july. the maximum TKN_About  takes place during august with approximately 101 TKN_UOM . from august to december the production drastically decreases until it reaches its minimum of -1 in december.</t>
         </is>
       </c>
       <c r="W304" t="n">

</xml_diff>